<commit_message>
_context Removed from StudentFeeHead Controller
</commit_message>
<xml_diff>
--- a/Resources/Layout.xlsx
+++ b/Resources/Layout.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24430"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CF2A5D7-B255-4EAE-AD82-32B798A31530}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF86371B-8D8B-41B0-B228-4BD8747FDB67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="24108" yWindow="-108" windowWidth="22080" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
   <si>
     <t>Date</t>
   </si>
@@ -62,9 +62,6 @@
     <t>Automated Receipt No</t>
   </si>
   <si>
-    <t>+Add</t>
-  </si>
-  <si>
     <t>Waiver (If any)</t>
   </si>
   <si>
@@ -72,13 +69,19 @@
   </si>
   <si>
     <t>Image</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>2563/-</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -96,6 +99,13 @@
     <font>
       <sz val="10"/>
       <color theme="0" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="6" tint="0.79998168889431442"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -122,13 +132,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor theme="2" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="2" tint="-0.249977111117893"/>
+        <fgColor theme="6" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -176,6 +186,9 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -192,22 +205,19 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -616,7 +626,7 @@
   <dimension ref="A1:L15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -666,31 +676,31 @@
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="9"/>
-      <c r="C2" s="11" t="s">
+      <c r="B2" s="10"/>
+      <c r="C2" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="15" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" s="12" customFormat="1" ht="3.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F3" s="13"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="18"/>
+    </row>
+    <row r="3" spans="1:12" s="13" customFormat="1" ht="3.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F3" s="14"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="9"/>
-      <c r="C4" s="10"/>
-      <c r="D4" s="10"/>
-      <c r="E4" s="10"/>
-      <c r="F4" s="13"/>
+      <c r="B4" s="10"/>
+      <c r="C4" s="11"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="7" t="s">
+        <v>15</v>
+      </c>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
       <c r="I4" s="2"/>
@@ -698,44 +708,46 @@
       <c r="K4" s="2"/>
       <c r="L4" s="2"/>
     </row>
-    <row r="5" spans="1:12" s="12" customFormat="1" ht="3.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F5" s="13"/>
+    <row r="5" spans="1:12" s="13" customFormat="1" ht="3.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F5" s="7"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="7"/>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8"/>
+      <c r="B6" s="8"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
       <c r="E6" s="17"/>
-      <c r="F6" s="13"/>
-    </row>
-    <row r="7" spans="1:12" s="12" customFormat="1" ht="3.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F6" s="7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" s="13" customFormat="1" ht="3.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="F7" s="14"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A8" s="7" t="s">
+      <c r="A8" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="8"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="16" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" s="13" customFormat="1" ht="3.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F9" s="14"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A10" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="7"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="18" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" s="12" customFormat="1" ht="3.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F9" s="14"/>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A10" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="B10" s="16"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
+      <c r="B10" s="15"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
@@ -803,7 +815,7 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="11">
+  <mergeCells count="10">
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="C10:E10"/>
     <mergeCell ref="C6:D6"/>
@@ -814,7 +826,6 @@
     <mergeCell ref="C2:E2"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="C4:E4"/>
-    <mergeCell ref="F2:F6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Teacher Repository added, Home Index modified
</commit_message>
<xml_diff>
--- a/Resources/Layout.xlsx
+++ b/Resources/Layout.xlsx
@@ -3,12 +3,13 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24430"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF86371B-8D8B-41B0-B228-4BD8747FDB67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{217FE351-EA81-494A-A536-1AEAF87D98D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="24108" yWindow="-108" windowWidth="22080" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="24108" yWindow="-108" windowWidth="22080" windowHeight="13176" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Dashboard" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="30">
   <si>
     <t>Date</t>
   </si>
@@ -75,13 +76,52 @@
   </si>
   <si>
     <t>2563/-</t>
+  </si>
+  <si>
+    <t>Total Student</t>
+  </si>
+  <si>
+    <t>Class 6</t>
+  </si>
+  <si>
+    <t>Class 7</t>
+  </si>
+  <si>
+    <t>Class 8</t>
+  </si>
+  <si>
+    <t>Class 9</t>
+  </si>
+  <si>
+    <t>Class 10</t>
+  </si>
+  <si>
+    <t>Total Teacher</t>
+  </si>
+  <si>
+    <t>Jamal Hossain</t>
+  </si>
+  <si>
+    <t>Shoriful Islam</t>
+  </si>
+  <si>
+    <t>Sajjadur Rahman</t>
+  </si>
+  <si>
+    <t>Golam Faruq</t>
+  </si>
+  <si>
+    <t>Habibur Rahman</t>
+  </si>
+  <si>
+    <t>Atikur Rahman</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -110,8 +150,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -142,8 +188,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -166,11 +224,40 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
@@ -189,36 +276,64 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -625,8 +740,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -676,28 +791,28 @@
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="10"/>
-      <c r="C2" s="12" t="s">
+      <c r="B2" s="16"/>
+      <c r="C2" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="18"/>
-    </row>
-    <row r="3" spans="1:12" s="13" customFormat="1" ht="3.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F3" s="14"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="12"/>
+    </row>
+    <row r="3" spans="1:12" s="8" customFormat="1" ht="3.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F3" s="9"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A4" s="10" t="s">
+      <c r="A4" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="10"/>
-      <c r="C4" s="11"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
+      <c r="B4" s="16"/>
+      <c r="C4" s="18"/>
+      <c r="D4" s="18"/>
+      <c r="E4" s="18"/>
       <c r="F4" s="7" t="s">
         <v>15</v>
       </c>
@@ -708,46 +823,46 @@
       <c r="K4" s="2"/>
       <c r="L4" s="2"/>
     </row>
-    <row r="5" spans="1:12" s="13" customFormat="1" ht="3.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" s="8" customFormat="1" ht="3.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="F5" s="7"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="8"/>
-      <c r="C6" s="9"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="17"/>
+      <c r="B6" s="15"/>
+      <c r="C6" s="14"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="11"/>
       <c r="F6" s="7" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:12" s="13" customFormat="1" ht="3.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F7" s="14"/>
+    <row r="7" spans="1:12" s="8" customFormat="1" ht="3.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F7" s="9"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A8" s="8" t="s">
+      <c r="A8" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="8"/>
-      <c r="C8" s="9"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="16" t="s">
+      <c r="B8" s="15"/>
+      <c r="C8" s="14"/>
+      <c r="D8" s="14"/>
+      <c r="E8" s="10" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:12" s="13" customFormat="1" ht="3.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F9" s="14"/>
+    <row r="9" spans="1:12" s="8" customFormat="1" ht="3.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F9" s="9"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A10" s="15" t="s">
+      <c r="A10" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="15"/>
-      <c r="C10" s="9"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="9"/>
+      <c r="B10" s="13"/>
+      <c r="C10" s="14"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="14"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
@@ -816,19 +931,579 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:E2"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:E4"/>
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="C10:E10"/>
     <mergeCell ref="C6:D6"/>
     <mergeCell ref="C8:D8"/>
     <mergeCell ref="A8:B8"/>
     <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="C2:E2"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:E4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AC9086E-D004-4EA1-8724-804CD1EEFB7F}">
+  <dimension ref="A1:X15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AA15" sqref="AA15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="2.5546875" customWidth="1"/>
+    <col min="3" max="3" width="2.44140625" customWidth="1"/>
+    <col min="4" max="4" width="2.6640625" customWidth="1"/>
+    <col min="5" max="9" width="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="24" width="3" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A1">
+        <v>1</v>
+      </c>
+      <c r="B1">
+        <v>2</v>
+      </c>
+      <c r="C1">
+        <v>3</v>
+      </c>
+      <c r="D1">
+        <v>4</v>
+      </c>
+      <c r="E1">
+        <v>5</v>
+      </c>
+      <c r="F1">
+        <v>6</v>
+      </c>
+      <c r="G1">
+        <v>7</v>
+      </c>
+      <c r="H1">
+        <v>8</v>
+      </c>
+      <c r="I1">
+        <v>9</v>
+      </c>
+      <c r="J1">
+        <v>10</v>
+      </c>
+      <c r="K1">
+        <v>11</v>
+      </c>
+      <c r="L1">
+        <v>12</v>
+      </c>
+      <c r="M1">
+        <v>13</v>
+      </c>
+      <c r="N1">
+        <v>14</v>
+      </c>
+      <c r="O1">
+        <v>15</v>
+      </c>
+      <c r="P1">
+        <v>16</v>
+      </c>
+      <c r="Q1">
+        <v>17</v>
+      </c>
+      <c r="R1">
+        <v>18</v>
+      </c>
+      <c r="S1">
+        <v>19</v>
+      </c>
+      <c r="T1">
+        <v>20</v>
+      </c>
+      <c r="U1">
+        <v>21</v>
+      </c>
+      <c r="V1">
+        <v>22</v>
+      </c>
+      <c r="W1">
+        <v>23</v>
+      </c>
+      <c r="X1">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A2" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="22"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="22"/>
+      <c r="H2" s="22"/>
+      <c r="I2" s="22"/>
+      <c r="J2" s="22"/>
+      <c r="K2" s="22"/>
+      <c r="L2" s="22"/>
+      <c r="M2" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="N2" s="20"/>
+      <c r="O2" s="20"/>
+      <c r="P2" s="20"/>
+      <c r="Q2" s="20"/>
+      <c r="R2" s="20"/>
+      <c r="S2" s="20"/>
+      <c r="T2" s="20"/>
+      <c r="U2" s="20"/>
+      <c r="V2" s="20"/>
+      <c r="W2" s="20"/>
+      <c r="X2" s="20"/>
+    </row>
+    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A3" s="23">
+        <v>1</v>
+      </c>
+      <c r="B3" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="24"/>
+      <c r="D3" s="24"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="25"/>
+      <c r="H3" s="25"/>
+      <c r="I3" s="25"/>
+      <c r="J3" s="25"/>
+      <c r="K3" s="26">
+        <v>45</v>
+      </c>
+      <c r="L3" s="26"/>
+      <c r="M3" s="21">
+        <v>1</v>
+      </c>
+      <c r="N3" s="29" t="s">
+        <v>24</v>
+      </c>
+      <c r="O3" s="29"/>
+      <c r="P3" s="29"/>
+      <c r="Q3" s="29"/>
+      <c r="R3" s="29"/>
+      <c r="S3" s="21">
+        <v>6</v>
+      </c>
+      <c r="T3" s="30" t="s">
+        <v>29</v>
+      </c>
+      <c r="U3" s="30"/>
+      <c r="V3" s="30"/>
+      <c r="W3" s="30"/>
+      <c r="X3" s="30"/>
+    </row>
+    <row r="4" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A4" s="23">
+        <v>2</v>
+      </c>
+      <c r="B4" s="24" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="24"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="23"/>
+      <c r="F4" s="23"/>
+      <c r="G4" s="23"/>
+      <c r="H4" s="23"/>
+      <c r="I4" s="23"/>
+      <c r="J4" s="23"/>
+      <c r="K4" s="26">
+        <v>46</v>
+      </c>
+      <c r="L4" s="26"/>
+      <c r="M4" s="21">
+        <v>2</v>
+      </c>
+      <c r="N4" s="29" t="s">
+        <v>25</v>
+      </c>
+      <c r="O4" s="29"/>
+      <c r="P4" s="29"/>
+      <c r="Q4" s="29"/>
+      <c r="R4" s="29"/>
+      <c r="S4" s="21">
+        <v>7</v>
+      </c>
+      <c r="T4" s="30" t="s">
+        <v>29</v>
+      </c>
+      <c r="U4" s="30"/>
+      <c r="V4" s="30"/>
+      <c r="W4" s="30"/>
+      <c r="X4" s="30"/>
+    </row>
+    <row r="5" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A5" s="23">
+        <v>3</v>
+      </c>
+      <c r="B5" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="27"/>
+      <c r="D5" s="27"/>
+      <c r="E5" s="23"/>
+      <c r="F5" s="23"/>
+      <c r="G5" s="23"/>
+      <c r="H5" s="23"/>
+      <c r="I5" s="23"/>
+      <c r="J5" s="23"/>
+      <c r="K5" s="28">
+        <v>47</v>
+      </c>
+      <c r="L5" s="28"/>
+      <c r="M5" s="21">
+        <v>3</v>
+      </c>
+      <c r="N5" s="29" t="s">
+        <v>26</v>
+      </c>
+      <c r="O5" s="29"/>
+      <c r="P5" s="29"/>
+      <c r="Q5" s="29"/>
+      <c r="R5" s="29"/>
+      <c r="S5" s="21">
+        <v>8</v>
+      </c>
+      <c r="T5" s="30" t="s">
+        <v>29</v>
+      </c>
+      <c r="U5" s="30"/>
+      <c r="V5" s="30"/>
+      <c r="W5" s="30"/>
+      <c r="X5" s="30"/>
+    </row>
+    <row r="6" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A6" s="23">
+        <v>4</v>
+      </c>
+      <c r="B6" s="27" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="27"/>
+      <c r="D6" s="27"/>
+      <c r="E6" s="23"/>
+      <c r="F6" s="23"/>
+      <c r="G6" s="23"/>
+      <c r="H6" s="23"/>
+      <c r="I6" s="23"/>
+      <c r="J6" s="23"/>
+      <c r="K6" s="28">
+        <v>48</v>
+      </c>
+      <c r="L6" s="28"/>
+      <c r="M6" s="21">
+        <v>4</v>
+      </c>
+      <c r="N6" s="29" t="s">
+        <v>27</v>
+      </c>
+      <c r="O6" s="29"/>
+      <c r="P6" s="29"/>
+      <c r="Q6" s="29"/>
+      <c r="R6" s="29"/>
+      <c r="S6" s="21">
+        <v>9</v>
+      </c>
+      <c r="T6" s="30" t="s">
+        <v>29</v>
+      </c>
+      <c r="U6" s="30"/>
+      <c r="V6" s="30"/>
+      <c r="W6" s="30"/>
+      <c r="X6" s="30"/>
+    </row>
+    <row r="7" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A7" s="23">
+        <v>5</v>
+      </c>
+      <c r="B7" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="27"/>
+      <c r="D7" s="27"/>
+      <c r="E7" s="23"/>
+      <c r="F7" s="23"/>
+      <c r="G7" s="23"/>
+      <c r="H7" s="23"/>
+      <c r="I7" s="23"/>
+      <c r="J7" s="23"/>
+      <c r="K7" s="28">
+        <v>49</v>
+      </c>
+      <c r="L7" s="28"/>
+      <c r="M7" s="21">
+        <v>5</v>
+      </c>
+      <c r="N7" s="29" t="s">
+        <v>28</v>
+      </c>
+      <c r="O7" s="29"/>
+      <c r="P7" s="29"/>
+      <c r="Q7" s="29"/>
+      <c r="R7" s="29"/>
+      <c r="S7" s="21">
+        <v>10</v>
+      </c>
+      <c r="T7" s="30" t="s">
+        <v>29</v>
+      </c>
+      <c r="U7" s="30"/>
+      <c r="V7" s="30"/>
+      <c r="W7" s="30"/>
+      <c r="X7" s="30"/>
+    </row>
+    <row r="8" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A8" s="19"/>
+      <c r="B8" s="19"/>
+      <c r="C8" s="19"/>
+      <c r="D8" s="19"/>
+      <c r="E8" s="19"/>
+      <c r="F8" s="19"/>
+      <c r="G8" s="19"/>
+      <c r="H8" s="19"/>
+      <c r="I8" s="19"/>
+      <c r="J8" s="19"/>
+      <c r="K8" s="19"/>
+      <c r="L8" s="19"/>
+      <c r="M8" s="19"/>
+      <c r="N8" s="19"/>
+      <c r="O8" s="19"/>
+      <c r="P8" s="19"/>
+      <c r="Q8" s="19"/>
+      <c r="R8" s="19"/>
+      <c r="S8" s="19"/>
+      <c r="T8" s="19"/>
+      <c r="U8" s="19"/>
+      <c r="V8" s="19"/>
+      <c r="W8" s="19"/>
+      <c r="X8" s="19"/>
+    </row>
+    <row r="9" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A9" s="19"/>
+      <c r="B9" s="19"/>
+      <c r="C9" s="19"/>
+      <c r="D9" s="19"/>
+      <c r="E9" s="19"/>
+      <c r="F9" s="19"/>
+      <c r="G9" s="19"/>
+      <c r="H9" s="19"/>
+      <c r="I9" s="19"/>
+      <c r="J9" s="19"/>
+      <c r="K9" s="19"/>
+      <c r="L9" s="19"/>
+      <c r="M9" s="19"/>
+      <c r="N9" s="19"/>
+      <c r="O9" s="19"/>
+      <c r="P9" s="19"/>
+      <c r="Q9" s="19"/>
+      <c r="R9" s="19"/>
+      <c r="S9" s="19"/>
+      <c r="T9" s="19"/>
+      <c r="U9" s="19"/>
+      <c r="V9" s="19"/>
+      <c r="W9" s="19"/>
+      <c r="X9" s="19"/>
+    </row>
+    <row r="10" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A10" s="19"/>
+      <c r="B10" s="19"/>
+      <c r="C10" s="19"/>
+      <c r="D10" s="19"/>
+      <c r="E10" s="19"/>
+      <c r="F10" s="19"/>
+      <c r="G10" s="19"/>
+      <c r="H10" s="19"/>
+      <c r="I10" s="19"/>
+      <c r="J10" s="19"/>
+      <c r="K10" s="19"/>
+      <c r="L10" s="19"/>
+      <c r="M10" s="19"/>
+      <c r="N10" s="19"/>
+      <c r="O10" s="19"/>
+      <c r="P10" s="19"/>
+      <c r="Q10" s="19"/>
+      <c r="R10" s="19"/>
+      <c r="S10" s="19"/>
+      <c r="T10" s="19"/>
+      <c r="U10" s="19"/>
+      <c r="V10" s="19"/>
+      <c r="W10" s="19"/>
+      <c r="X10" s="19"/>
+    </row>
+    <row r="11" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A11" s="19"/>
+      <c r="B11" s="19"/>
+      <c r="C11" s="19"/>
+      <c r="D11" s="19"/>
+      <c r="E11" s="19"/>
+      <c r="F11" s="19"/>
+      <c r="G11" s="19"/>
+      <c r="H11" s="19"/>
+      <c r="I11" s="19"/>
+      <c r="J11" s="19"/>
+      <c r="K11" s="19"/>
+      <c r="L11" s="19"/>
+      <c r="M11" s="19"/>
+      <c r="N11" s="19"/>
+      <c r="O11" s="19"/>
+      <c r="P11" s="19"/>
+      <c r="Q11" s="19"/>
+      <c r="R11" s="19"/>
+      <c r="S11" s="19"/>
+      <c r="T11" s="19"/>
+      <c r="U11" s="19"/>
+      <c r="V11" s="19"/>
+      <c r="W11" s="19"/>
+      <c r="X11" s="19"/>
+    </row>
+    <row r="12" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A12" s="19"/>
+      <c r="B12" s="19"/>
+      <c r="C12" s="19"/>
+      <c r="D12" s="19"/>
+      <c r="E12" s="19"/>
+      <c r="F12" s="19"/>
+      <c r="G12" s="19"/>
+      <c r="H12" s="19"/>
+      <c r="I12" s="19"/>
+      <c r="J12" s="19"/>
+      <c r="K12" s="19"/>
+      <c r="L12" s="19"/>
+      <c r="M12" s="19"/>
+      <c r="N12" s="19"/>
+      <c r="O12" s="19"/>
+      <c r="P12" s="19"/>
+      <c r="Q12" s="19"/>
+      <c r="R12" s="19"/>
+      <c r="S12" s="19"/>
+      <c r="T12" s="19"/>
+      <c r="U12" s="19"/>
+      <c r="V12" s="19"/>
+      <c r="W12" s="19"/>
+      <c r="X12" s="19"/>
+    </row>
+    <row r="13" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A13" s="19"/>
+      <c r="B13" s="19"/>
+      <c r="C13" s="19"/>
+      <c r="D13" s="19"/>
+      <c r="E13" s="19"/>
+      <c r="F13" s="19"/>
+      <c r="G13" s="19"/>
+      <c r="H13" s="19"/>
+      <c r="I13" s="19"/>
+      <c r="J13" s="19"/>
+      <c r="K13" s="19"/>
+      <c r="L13" s="19"/>
+      <c r="M13" s="19"/>
+      <c r="N13" s="19"/>
+      <c r="O13" s="19"/>
+      <c r="P13" s="19"/>
+      <c r="Q13" s="19"/>
+      <c r="R13" s="19"/>
+      <c r="S13" s="19"/>
+      <c r="T13" s="19"/>
+      <c r="U13" s="19"/>
+      <c r="V13" s="19"/>
+      <c r="W13" s="19"/>
+      <c r="X13" s="19"/>
+    </row>
+    <row r="14" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A14" s="19"/>
+      <c r="B14" s="19"/>
+      <c r="C14" s="19"/>
+      <c r="D14" s="19"/>
+      <c r="E14" s="19"/>
+      <c r="F14" s="19"/>
+      <c r="G14" s="19"/>
+      <c r="H14" s="19"/>
+      <c r="I14" s="19"/>
+      <c r="J14" s="19"/>
+      <c r="K14" s="19"/>
+      <c r="L14" s="19"/>
+      <c r="M14" s="19"/>
+      <c r="N14" s="19"/>
+      <c r="O14" s="19"/>
+      <c r="P14" s="19"/>
+      <c r="Q14" s="19"/>
+      <c r="R14" s="19"/>
+      <c r="S14" s="19"/>
+      <c r="T14" s="19"/>
+      <c r="U14" s="19"/>
+      <c r="V14" s="19"/>
+      <c r="W14" s="19"/>
+      <c r="X14" s="19"/>
+    </row>
+    <row r="15" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A15" s="19"/>
+      <c r="B15" s="19"/>
+      <c r="C15" s="19"/>
+      <c r="D15" s="19"/>
+      <c r="E15" s="19"/>
+      <c r="F15" s="19"/>
+      <c r="G15" s="19"/>
+      <c r="H15" s="19"/>
+      <c r="I15" s="19"/>
+      <c r="J15" s="19"/>
+      <c r="K15" s="19"/>
+      <c r="L15" s="19"/>
+      <c r="M15" s="19"/>
+      <c r="N15" s="19"/>
+      <c r="O15" s="19"/>
+      <c r="P15" s="19"/>
+      <c r="Q15" s="19"/>
+      <c r="R15" s="19"/>
+      <c r="S15" s="19"/>
+      <c r="T15" s="19"/>
+      <c r="U15" s="19"/>
+      <c r="V15" s="19"/>
+      <c r="W15" s="19"/>
+      <c r="X15" s="19"/>
+    </row>
+  </sheetData>
+  <mergeCells count="22">
+    <mergeCell ref="T7:X7"/>
+    <mergeCell ref="M2:X2"/>
+    <mergeCell ref="N3:R3"/>
+    <mergeCell ref="N4:R4"/>
+    <mergeCell ref="N5:R5"/>
+    <mergeCell ref="N6:R6"/>
+    <mergeCell ref="N7:R7"/>
+    <mergeCell ref="T3:X3"/>
+    <mergeCell ref="T4:X4"/>
+    <mergeCell ref="T5:X5"/>
+    <mergeCell ref="T6:X6"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="K6:L6"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="K7:L7"/>
+    <mergeCell ref="A2:L2"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="K4:L4"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="K5:L5"/>
+  </mergeCells>
+  <phoneticPr fontId="4" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
sms create realted (Guardian phone sms)
</commit_message>
<xml_diff>
--- a/Resources/Layout.xlsx
+++ b/Resources/Layout.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24931"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{217FE351-EA81-494A-A536-1AEAF87D98D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{338A20C0-8912-4B9E-B8FC-0DFCD07637A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="24108" yWindow="-108" windowWidth="22080" windowHeight="13176" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Dashboard" sheetId="2" r:id="rId2"/>
+    <sheet name="Class Routine" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="51">
   <si>
     <t>Date</t>
   </si>
@@ -115,13 +116,76 @@
   </si>
   <si>
     <t>Atikur Rahman</t>
+  </si>
+  <si>
+    <t>1st Period</t>
+  </si>
+  <si>
+    <t>2nd Period</t>
+  </si>
+  <si>
+    <t>3rd Period</t>
+  </si>
+  <si>
+    <t>4th Period</t>
+  </si>
+  <si>
+    <t>Sunday</t>
+  </si>
+  <si>
+    <t>Monday</t>
+  </si>
+  <si>
+    <t>Tuesday</t>
+  </si>
+  <si>
+    <t>Wednesday</t>
+  </si>
+  <si>
+    <t>Thursday</t>
+  </si>
+  <si>
+    <t>Friday</t>
+  </si>
+  <si>
+    <t>Saturday</t>
+  </si>
+  <si>
+    <t>Subject 01</t>
+  </si>
+  <si>
+    <t>Subject 02</t>
+  </si>
+  <si>
+    <t>Subject 03</t>
+  </si>
+  <si>
+    <t>Subject 04</t>
+  </si>
+  <si>
+    <t>Subject 05</t>
+  </si>
+  <si>
+    <t>Subject 06</t>
+  </si>
+  <si>
+    <t>Subject 07</t>
+  </si>
+  <si>
+    <t>Subject 08</t>
+  </si>
+  <si>
+    <t>Subject 09</t>
+  </si>
+  <si>
+    <t>Subject 10</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -152,6 +216,22 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -257,7 +337,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
@@ -289,6 +369,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -298,42 +391,38 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -744,15 +833,15 @@
       <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.6640625" customWidth="1"/>
-    <col min="2" max="2" width="10.88671875" customWidth="1"/>
+    <col min="1" max="1" width="3.7109375" customWidth="1"/>
+    <col min="2" max="2" width="10.85546875" customWidth="1"/>
     <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>1</v>
       </c>
@@ -790,29 +879,29 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A2" s="16" t="s">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="16"/>
-      <c r="C2" s="17" t="s">
+      <c r="B2" s="17"/>
+      <c r="C2" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
       <c r="F2" s="12"/>
     </row>
-    <row r="3" spans="1:12" s="8" customFormat="1" ht="3.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" s="8" customFormat="1" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F3" s="9"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A4" s="16" t="s">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="16"/>
-      <c r="C4" s="18"/>
-      <c r="D4" s="18"/>
-      <c r="E4" s="18"/>
+      <c r="B4" s="17"/>
+      <c r="C4" s="19"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="19"/>
       <c r="F4" s="7" t="s">
         <v>15</v>
       </c>
@@ -823,48 +912,48 @@
       <c r="K4" s="2"/>
       <c r="L4" s="2"/>
     </row>
-    <row r="5" spans="1:12" s="8" customFormat="1" ht="3.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" s="8" customFormat="1" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F5" s="7"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A6" s="15" t="s">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="15"/>
-      <c r="C6" s="14"/>
-      <c r="D6" s="14"/>
+      <c r="B6" s="22"/>
+      <c r="C6" s="21"/>
+      <c r="D6" s="21"/>
       <c r="E6" s="11"/>
       <c r="F6" s="7" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:12" s="8" customFormat="1" ht="3.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" s="8" customFormat="1" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F7" s="9"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A8" s="15" t="s">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="15"/>
-      <c r="C8" s="14"/>
-      <c r="D8" s="14"/>
+      <c r="B8" s="22"/>
+      <c r="C8" s="21"/>
+      <c r="D8" s="21"/>
       <c r="E8" s="10" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:12" s="8" customFormat="1" ht="3.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" s="8" customFormat="1" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F9" s="9"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A10" s="13" t="s">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="13"/>
-      <c r="C10" s="14"/>
-      <c r="D10" s="14"/>
-      <c r="E10" s="14"/>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B10" s="20"/>
+      <c r="C10" s="21"/>
+      <c r="D10" s="21"/>
+      <c r="E10" s="21"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>2</v>
       </c>
@@ -884,7 +973,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
         <v>1</v>
       </c>
@@ -904,7 +993,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
         <v>2</v>
       </c>
@@ -924,7 +1013,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="F15" s="6" t="s">
         <v>10</v>
       </c>
@@ -952,21 +1041,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AC9086E-D004-4EA1-8724-804CD1EEFB7F}">
   <dimension ref="A1:X15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="AA15" sqref="AA15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="2.5546875" customWidth="1"/>
-    <col min="3" max="3" width="2.44140625" customWidth="1"/>
-    <col min="4" max="4" width="2.6640625" customWidth="1"/>
+    <col min="2" max="2" width="2.5703125" customWidth="1"/>
+    <col min="3" max="3" width="2.42578125" customWidth="1"/>
+    <col min="4" max="4" width="2.7109375" customWidth="1"/>
     <col min="5" max="9" width="2" bestFit="1" customWidth="1"/>
     <col min="10" max="24" width="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>1</v>
       </c>
@@ -1040,446 +1129,457 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A2" s="22" t="s">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A2" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="22"/>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22"/>
-      <c r="G2" s="22"/>
-      <c r="H2" s="22"/>
-      <c r="I2" s="22"/>
-      <c r="J2" s="22"/>
-      <c r="K2" s="22"/>
-      <c r="L2" s="22"/>
-      <c r="M2" s="20" t="s">
+      <c r="B2" s="28"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
+      <c r="G2" s="28"/>
+      <c r="H2" s="28"/>
+      <c r="I2" s="28"/>
+      <c r="J2" s="28"/>
+      <c r="K2" s="28"/>
+      <c r="L2" s="28"/>
+      <c r="M2" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="N2" s="20"/>
-      <c r="O2" s="20"/>
-      <c r="P2" s="20"/>
-      <c r="Q2" s="20"/>
-      <c r="R2" s="20"/>
-      <c r="S2" s="20"/>
-      <c r="T2" s="20"/>
-      <c r="U2" s="20"/>
-      <c r="V2" s="20"/>
-      <c r="W2" s="20"/>
-      <c r="X2" s="20"/>
-    </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A3" s="23">
+      <c r="N2" s="24"/>
+      <c r="O2" s="24"/>
+      <c r="P2" s="24"/>
+      <c r="Q2" s="24"/>
+      <c r="R2" s="24"/>
+      <c r="S2" s="24"/>
+      <c r="T2" s="24"/>
+      <c r="U2" s="24"/>
+      <c r="V2" s="24"/>
+      <c r="W2" s="24"/>
+      <c r="X2" s="24"/>
+    </row>
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A3" s="15">
         <v>1</v>
       </c>
-      <c r="B3" s="24" t="s">
+      <c r="B3" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="24"/>
-      <c r="D3" s="24"/>
-      <c r="E3" s="25"/>
-      <c r="F3" s="25"/>
-      <c r="G3" s="25"/>
-      <c r="H3" s="25"/>
-      <c r="I3" s="25"/>
-      <c r="J3" s="25"/>
-      <c r="K3" s="26">
+      <c r="C3" s="29"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="16"/>
+      <c r="F3" s="16"/>
+      <c r="G3" s="16"/>
+      <c r="H3" s="16"/>
+      <c r="I3" s="16"/>
+      <c r="J3" s="16"/>
+      <c r="K3" s="30">
         <v>45</v>
       </c>
-      <c r="L3" s="26"/>
-      <c r="M3" s="21">
+      <c r="L3" s="30"/>
+      <c r="M3" s="14">
         <v>1</v>
       </c>
-      <c r="N3" s="29" t="s">
+      <c r="N3" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="O3" s="29"/>
-      <c r="P3" s="29"/>
-      <c r="Q3" s="29"/>
-      <c r="R3" s="29"/>
-      <c r="S3" s="21">
+      <c r="O3" s="25"/>
+      <c r="P3" s="25"/>
+      <c r="Q3" s="25"/>
+      <c r="R3" s="25"/>
+      <c r="S3" s="14">
         <v>6</v>
       </c>
-      <c r="T3" s="30" t="s">
+      <c r="T3" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="U3" s="30"/>
-      <c r="V3" s="30"/>
-      <c r="W3" s="30"/>
-      <c r="X3" s="30"/>
-    </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A4" s="23">
+      <c r="U3" s="23"/>
+      <c r="V3" s="23"/>
+      <c r="W3" s="23"/>
+      <c r="X3" s="23"/>
+    </row>
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A4" s="15">
         <v>2</v>
       </c>
-      <c r="B4" s="24" t="s">
+      <c r="B4" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="24"/>
-      <c r="D4" s="24"/>
-      <c r="E4" s="23"/>
-      <c r="F4" s="23"/>
-      <c r="G4" s="23"/>
-      <c r="H4" s="23"/>
-      <c r="I4" s="23"/>
-      <c r="J4" s="23"/>
-      <c r="K4" s="26">
+      <c r="C4" s="29"/>
+      <c r="D4" s="29"/>
+      <c r="E4" s="15"/>
+      <c r="F4" s="15"/>
+      <c r="G4" s="15"/>
+      <c r="H4" s="15"/>
+      <c r="I4" s="15"/>
+      <c r="J4" s="15"/>
+      <c r="K4" s="30">
         <v>46</v>
       </c>
-      <c r="L4" s="26"/>
-      <c r="M4" s="21">
+      <c r="L4" s="30"/>
+      <c r="M4" s="14">
         <v>2</v>
       </c>
-      <c r="N4" s="29" t="s">
+      <c r="N4" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="O4" s="29"/>
-      <c r="P4" s="29"/>
-      <c r="Q4" s="29"/>
-      <c r="R4" s="29"/>
-      <c r="S4" s="21">
+      <c r="O4" s="25"/>
+      <c r="P4" s="25"/>
+      <c r="Q4" s="25"/>
+      <c r="R4" s="25"/>
+      <c r="S4" s="14">
         <v>7</v>
       </c>
-      <c r="T4" s="30" t="s">
+      <c r="T4" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="U4" s="30"/>
-      <c r="V4" s="30"/>
-      <c r="W4" s="30"/>
-      <c r="X4" s="30"/>
-    </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A5" s="23">
+      <c r="U4" s="23"/>
+      <c r="V4" s="23"/>
+      <c r="W4" s="23"/>
+      <c r="X4" s="23"/>
+    </row>
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A5" s="15">
         <v>3</v>
       </c>
-      <c r="B5" s="27" t="s">
+      <c r="B5" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="27"/>
-      <c r="D5" s="27"/>
-      <c r="E5" s="23"/>
-      <c r="F5" s="23"/>
-      <c r="G5" s="23"/>
-      <c r="H5" s="23"/>
-      <c r="I5" s="23"/>
-      <c r="J5" s="23"/>
-      <c r="K5" s="28">
+      <c r="C5" s="26"/>
+      <c r="D5" s="26"/>
+      <c r="E5" s="15"/>
+      <c r="F5" s="15"/>
+      <c r="G5" s="15"/>
+      <c r="H5" s="15"/>
+      <c r="I5" s="15"/>
+      <c r="J5" s="15"/>
+      <c r="K5" s="27">
         <v>47</v>
       </c>
-      <c r="L5" s="28"/>
-      <c r="M5" s="21">
+      <c r="L5" s="27"/>
+      <c r="M5" s="14">
         <v>3</v>
       </c>
-      <c r="N5" s="29" t="s">
+      <c r="N5" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="O5" s="29"/>
-      <c r="P5" s="29"/>
-      <c r="Q5" s="29"/>
-      <c r="R5" s="29"/>
-      <c r="S5" s="21">
+      <c r="O5" s="25"/>
+      <c r="P5" s="25"/>
+      <c r="Q5" s="25"/>
+      <c r="R5" s="25"/>
+      <c r="S5" s="14">
         <v>8</v>
       </c>
-      <c r="T5" s="30" t="s">
+      <c r="T5" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="U5" s="30"/>
-      <c r="V5" s="30"/>
-      <c r="W5" s="30"/>
-      <c r="X5" s="30"/>
-    </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A6" s="23">
+      <c r="U5" s="23"/>
+      <c r="V5" s="23"/>
+      <c r="W5" s="23"/>
+      <c r="X5" s="23"/>
+    </row>
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A6" s="15">
         <v>4</v>
       </c>
-      <c r="B6" s="27" t="s">
+      <c r="B6" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="27"/>
-      <c r="D6" s="27"/>
-      <c r="E6" s="23"/>
-      <c r="F6" s="23"/>
-      <c r="G6" s="23"/>
-      <c r="H6" s="23"/>
-      <c r="I6" s="23"/>
-      <c r="J6" s="23"/>
-      <c r="K6" s="28">
+      <c r="C6" s="26"/>
+      <c r="D6" s="26"/>
+      <c r="E6" s="15"/>
+      <c r="F6" s="15"/>
+      <c r="G6" s="15"/>
+      <c r="H6" s="15"/>
+      <c r="I6" s="15"/>
+      <c r="J6" s="15"/>
+      <c r="K6" s="27">
         <v>48</v>
       </c>
-      <c r="L6" s="28"/>
-      <c r="M6" s="21">
+      <c r="L6" s="27"/>
+      <c r="M6" s="14">
         <v>4</v>
       </c>
-      <c r="N6" s="29" t="s">
+      <c r="N6" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="O6" s="29"/>
-      <c r="P6" s="29"/>
-      <c r="Q6" s="29"/>
-      <c r="R6" s="29"/>
-      <c r="S6" s="21">
+      <c r="O6" s="25"/>
+      <c r="P6" s="25"/>
+      <c r="Q6" s="25"/>
+      <c r="R6" s="25"/>
+      <c r="S6" s="14">
         <v>9</v>
       </c>
-      <c r="T6" s="30" t="s">
+      <c r="T6" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="U6" s="30"/>
-      <c r="V6" s="30"/>
-      <c r="W6" s="30"/>
-      <c r="X6" s="30"/>
-    </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A7" s="23">
+      <c r="U6" s="23"/>
+      <c r="V6" s="23"/>
+      <c r="W6" s="23"/>
+      <c r="X6" s="23"/>
+    </row>
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A7" s="15">
         <v>5</v>
       </c>
-      <c r="B7" s="27" t="s">
+      <c r="B7" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="C7" s="27"/>
-      <c r="D7" s="27"/>
-      <c r="E7" s="23"/>
-      <c r="F7" s="23"/>
-      <c r="G7" s="23"/>
-      <c r="H7" s="23"/>
-      <c r="I7" s="23"/>
-      <c r="J7" s="23"/>
-      <c r="K7" s="28">
+      <c r="C7" s="26"/>
+      <c r="D7" s="26"/>
+      <c r="E7" s="15"/>
+      <c r="F7" s="15"/>
+      <c r="G7" s="15"/>
+      <c r="H7" s="15"/>
+      <c r="I7" s="15"/>
+      <c r="J7" s="15"/>
+      <c r="K7" s="27">
         <v>49</v>
       </c>
-      <c r="L7" s="28"/>
-      <c r="M7" s="21">
+      <c r="L7" s="27"/>
+      <c r="M7" s="14">
         <v>5</v>
       </c>
-      <c r="N7" s="29" t="s">
+      <c r="N7" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="O7" s="29"/>
-      <c r="P7" s="29"/>
-      <c r="Q7" s="29"/>
-      <c r="R7" s="29"/>
-      <c r="S7" s="21">
+      <c r="O7" s="25"/>
+      <c r="P7" s="25"/>
+      <c r="Q7" s="25"/>
+      <c r="R7" s="25"/>
+      <c r="S7" s="14">
         <v>10</v>
       </c>
-      <c r="T7" s="30" t="s">
+      <c r="T7" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="U7" s="30"/>
-      <c r="V7" s="30"/>
-      <c r="W7" s="30"/>
-      <c r="X7" s="30"/>
-    </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A8" s="19"/>
-      <c r="B8" s="19"/>
-      <c r="C8" s="19"/>
-      <c r="D8" s="19"/>
-      <c r="E8" s="19"/>
-      <c r="F8" s="19"/>
-      <c r="G8" s="19"/>
-      <c r="H8" s="19"/>
-      <c r="I8" s="19"/>
-      <c r="J8" s="19"/>
-      <c r="K8" s="19"/>
-      <c r="L8" s="19"/>
-      <c r="M8" s="19"/>
-      <c r="N8" s="19"/>
-      <c r="O8" s="19"/>
-      <c r="P8" s="19"/>
-      <c r="Q8" s="19"/>
-      <c r="R8" s="19"/>
-      <c r="S8" s="19"/>
-      <c r="T8" s="19"/>
-      <c r="U8" s="19"/>
-      <c r="V8" s="19"/>
-      <c r="W8" s="19"/>
-      <c r="X8" s="19"/>
-    </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A9" s="19"/>
-      <c r="B9" s="19"/>
-      <c r="C9" s="19"/>
-      <c r="D9" s="19"/>
-      <c r="E9" s="19"/>
-      <c r="F9" s="19"/>
-      <c r="G9" s="19"/>
-      <c r="H9" s="19"/>
-      <c r="I9" s="19"/>
-      <c r="J9" s="19"/>
-      <c r="K9" s="19"/>
-      <c r="L9" s="19"/>
-      <c r="M9" s="19"/>
-      <c r="N9" s="19"/>
-      <c r="O9" s="19"/>
-      <c r="P9" s="19"/>
-      <c r="Q9" s="19"/>
-      <c r="R9" s="19"/>
-      <c r="S9" s="19"/>
-      <c r="T9" s="19"/>
-      <c r="U9" s="19"/>
-      <c r="V9" s="19"/>
-      <c r="W9" s="19"/>
-      <c r="X9" s="19"/>
-    </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A10" s="19"/>
-      <c r="B10" s="19"/>
-      <c r="C10" s="19"/>
-      <c r="D10" s="19"/>
-      <c r="E10" s="19"/>
-      <c r="F10" s="19"/>
-      <c r="G10" s="19"/>
-      <c r="H10" s="19"/>
-      <c r="I10" s="19"/>
-      <c r="J10" s="19"/>
-      <c r="K10" s="19"/>
-      <c r="L10" s="19"/>
-      <c r="M10" s="19"/>
-      <c r="N10" s="19"/>
-      <c r="O10" s="19"/>
-      <c r="P10" s="19"/>
-      <c r="Q10" s="19"/>
-      <c r="R10" s="19"/>
-      <c r="S10" s="19"/>
-      <c r="T10" s="19"/>
-      <c r="U10" s="19"/>
-      <c r="V10" s="19"/>
-      <c r="W10" s="19"/>
-      <c r="X10" s="19"/>
-    </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A11" s="19"/>
-      <c r="B11" s="19"/>
-      <c r="C11" s="19"/>
-      <c r="D11" s="19"/>
-      <c r="E11" s="19"/>
-      <c r="F11" s="19"/>
-      <c r="G11" s="19"/>
-      <c r="H11" s="19"/>
-      <c r="I11" s="19"/>
-      <c r="J11" s="19"/>
-      <c r="K11" s="19"/>
-      <c r="L11" s="19"/>
-      <c r="M11" s="19"/>
-      <c r="N11" s="19"/>
-      <c r="O11" s="19"/>
-      <c r="P11" s="19"/>
-      <c r="Q11" s="19"/>
-      <c r="R11" s="19"/>
-      <c r="S11" s="19"/>
-      <c r="T11" s="19"/>
-      <c r="U11" s="19"/>
-      <c r="V11" s="19"/>
-      <c r="W11" s="19"/>
-      <c r="X11" s="19"/>
-    </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A12" s="19"/>
-      <c r="B12" s="19"/>
-      <c r="C12" s="19"/>
-      <c r="D12" s="19"/>
-      <c r="E12" s="19"/>
-      <c r="F12" s="19"/>
-      <c r="G12" s="19"/>
-      <c r="H12" s="19"/>
-      <c r="I12" s="19"/>
-      <c r="J12" s="19"/>
-      <c r="K12" s="19"/>
-      <c r="L12" s="19"/>
-      <c r="M12" s="19"/>
-      <c r="N12" s="19"/>
-      <c r="O12" s="19"/>
-      <c r="P12" s="19"/>
-      <c r="Q12" s="19"/>
-      <c r="R12" s="19"/>
-      <c r="S12" s="19"/>
-      <c r="T12" s="19"/>
-      <c r="U12" s="19"/>
-      <c r="V12" s="19"/>
-      <c r="W12" s="19"/>
-      <c r="X12" s="19"/>
-    </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A13" s="19"/>
-      <c r="B13" s="19"/>
-      <c r="C13" s="19"/>
-      <c r="D13" s="19"/>
-      <c r="E13" s="19"/>
-      <c r="F13" s="19"/>
-      <c r="G13" s="19"/>
-      <c r="H13" s="19"/>
-      <c r="I13" s="19"/>
-      <c r="J13" s="19"/>
-      <c r="K13" s="19"/>
-      <c r="L13" s="19"/>
-      <c r="M13" s="19"/>
-      <c r="N13" s="19"/>
-      <c r="O13" s="19"/>
-      <c r="P13" s="19"/>
-      <c r="Q13" s="19"/>
-      <c r="R13" s="19"/>
-      <c r="S13" s="19"/>
-      <c r="T13" s="19"/>
-      <c r="U13" s="19"/>
-      <c r="V13" s="19"/>
-      <c r="W13" s="19"/>
-      <c r="X13" s="19"/>
-    </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A14" s="19"/>
-      <c r="B14" s="19"/>
-      <c r="C14" s="19"/>
-      <c r="D14" s="19"/>
-      <c r="E14" s="19"/>
-      <c r="F14" s="19"/>
-      <c r="G14" s="19"/>
-      <c r="H14" s="19"/>
-      <c r="I14" s="19"/>
-      <c r="J14" s="19"/>
-      <c r="K14" s="19"/>
-      <c r="L14" s="19"/>
-      <c r="M14" s="19"/>
-      <c r="N14" s="19"/>
-      <c r="O14" s="19"/>
-      <c r="P14" s="19"/>
-      <c r="Q14" s="19"/>
-      <c r="R14" s="19"/>
-      <c r="S14" s="19"/>
-      <c r="T14" s="19"/>
-      <c r="U14" s="19"/>
-      <c r="V14" s="19"/>
-      <c r="W14" s="19"/>
-      <c r="X14" s="19"/>
-    </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A15" s="19"/>
-      <c r="B15" s="19"/>
-      <c r="C15" s="19"/>
-      <c r="D15" s="19"/>
-      <c r="E15" s="19"/>
-      <c r="F15" s="19"/>
-      <c r="G15" s="19"/>
-      <c r="H15" s="19"/>
-      <c r="I15" s="19"/>
-      <c r="J15" s="19"/>
-      <c r="K15" s="19"/>
-      <c r="L15" s="19"/>
-      <c r="M15" s="19"/>
-      <c r="N15" s="19"/>
-      <c r="O15" s="19"/>
-      <c r="P15" s="19"/>
-      <c r="Q15" s="19"/>
-      <c r="R15" s="19"/>
-      <c r="S15" s="19"/>
-      <c r="T15" s="19"/>
-      <c r="U15" s="19"/>
-      <c r="V15" s="19"/>
-      <c r="W15" s="19"/>
-      <c r="X15" s="19"/>
+      <c r="U7" s="23"/>
+      <c r="V7" s="23"/>
+      <c r="W7" s="23"/>
+      <c r="X7" s="23"/>
+    </row>
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A8" s="13"/>
+      <c r="B8" s="13"/>
+      <c r="C8" s="13"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="13"/>
+      <c r="H8" s="13"/>
+      <c r="I8" s="13"/>
+      <c r="J8" s="13"/>
+      <c r="K8" s="13"/>
+      <c r="L8" s="13"/>
+      <c r="M8" s="13"/>
+      <c r="N8" s="13"/>
+      <c r="O8" s="13"/>
+      <c r="P8" s="13"/>
+      <c r="Q8" s="13"/>
+      <c r="R8" s="13"/>
+      <c r="S8" s="13"/>
+      <c r="T8" s="13"/>
+      <c r="U8" s="13"/>
+      <c r="V8" s="13"/>
+      <c r="W8" s="13"/>
+      <c r="X8" s="13"/>
+    </row>
+    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A9" s="13"/>
+      <c r="B9" s="13"/>
+      <c r="C9" s="13"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="13"/>
+      <c r="H9" s="13"/>
+      <c r="I9" s="13"/>
+      <c r="J9" s="13"/>
+      <c r="K9" s="13"/>
+      <c r="L9" s="13"/>
+      <c r="M9" s="13"/>
+      <c r="N9" s="13"/>
+      <c r="O9" s="13"/>
+      <c r="P9" s="13"/>
+      <c r="Q9" s="13"/>
+      <c r="R9" s="13"/>
+      <c r="S9" s="13"/>
+      <c r="T9" s="13"/>
+      <c r="U9" s="13"/>
+      <c r="V9" s="13"/>
+      <c r="W9" s="13"/>
+      <c r="X9" s="13"/>
+    </row>
+    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A10" s="13"/>
+      <c r="B10" s="13"/>
+      <c r="C10" s="13"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="13"/>
+      <c r="H10" s="13"/>
+      <c r="I10" s="13"/>
+      <c r="J10" s="13"/>
+      <c r="K10" s="13"/>
+      <c r="L10" s="13"/>
+      <c r="M10" s="13"/>
+      <c r="N10" s="13"/>
+      <c r="O10" s="13"/>
+      <c r="P10" s="13"/>
+      <c r="Q10" s="13"/>
+      <c r="R10" s="13"/>
+      <c r="S10" s="13"/>
+      <c r="T10" s="13"/>
+      <c r="U10" s="13"/>
+      <c r="V10" s="13"/>
+      <c r="W10" s="13"/>
+      <c r="X10" s="13"/>
+    </row>
+    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A11" s="13"/>
+      <c r="B11" s="13"/>
+      <c r="C11" s="13"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="13"/>
+      <c r="G11" s="13"/>
+      <c r="H11" s="13"/>
+      <c r="I11" s="13"/>
+      <c r="J11" s="13"/>
+      <c r="K11" s="13"/>
+      <c r="L11" s="13"/>
+      <c r="M11" s="13"/>
+      <c r="N11" s="13"/>
+      <c r="O11" s="13"/>
+      <c r="P11" s="13"/>
+      <c r="Q11" s="13"/>
+      <c r="R11" s="13"/>
+      <c r="S11" s="13"/>
+      <c r="T11" s="13"/>
+      <c r="U11" s="13"/>
+      <c r="V11" s="13"/>
+      <c r="W11" s="13"/>
+      <c r="X11" s="13"/>
+    </row>
+    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A12" s="13"/>
+      <c r="B12" s="13"/>
+      <c r="C12" s="13"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="13"/>
+      <c r="G12" s="13"/>
+      <c r="H12" s="13"/>
+      <c r="I12" s="13"/>
+      <c r="J12" s="13"/>
+      <c r="K12" s="13"/>
+      <c r="L12" s="13"/>
+      <c r="M12" s="13"/>
+      <c r="N12" s="13"/>
+      <c r="O12" s="13"/>
+      <c r="P12" s="13"/>
+      <c r="Q12" s="13"/>
+      <c r="R12" s="13"/>
+      <c r="S12" s="13"/>
+      <c r="T12" s="13"/>
+      <c r="U12" s="13"/>
+      <c r="V12" s="13"/>
+      <c r="W12" s="13"/>
+      <c r="X12" s="13"/>
+    </row>
+    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A13" s="13"/>
+      <c r="B13" s="13"/>
+      <c r="C13" s="13"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="13"/>
+      <c r="H13" s="13"/>
+      <c r="I13" s="13"/>
+      <c r="J13" s="13"/>
+      <c r="K13" s="13"/>
+      <c r="L13" s="13"/>
+      <c r="M13" s="13"/>
+      <c r="N13" s="13"/>
+      <c r="O13" s="13"/>
+      <c r="P13" s="13"/>
+      <c r="Q13" s="13"/>
+      <c r="R13" s="13"/>
+      <c r="S13" s="13"/>
+      <c r="T13" s="13"/>
+      <c r="U13" s="13"/>
+      <c r="V13" s="13"/>
+      <c r="W13" s="13"/>
+      <c r="X13" s="13"/>
+    </row>
+    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A14" s="13"/>
+      <c r="B14" s="13"/>
+      <c r="C14" s="13"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="13"/>
+      <c r="G14" s="13"/>
+      <c r="H14" s="13"/>
+      <c r="I14" s="13"/>
+      <c r="J14" s="13"/>
+      <c r="K14" s="13"/>
+      <c r="L14" s="13"/>
+      <c r="M14" s="13"/>
+      <c r="N14" s="13"/>
+      <c r="O14" s="13"/>
+      <c r="P14" s="13"/>
+      <c r="Q14" s="13"/>
+      <c r="R14" s="13"/>
+      <c r="S14" s="13"/>
+      <c r="T14" s="13"/>
+      <c r="U14" s="13"/>
+      <c r="V14" s="13"/>
+      <c r="W14" s="13"/>
+      <c r="X14" s="13"/>
+    </row>
+    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A15" s="13"/>
+      <c r="B15" s="13"/>
+      <c r="C15" s="13"/>
+      <c r="D15" s="13"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="13"/>
+      <c r="G15" s="13"/>
+      <c r="H15" s="13"/>
+      <c r="I15" s="13"/>
+      <c r="J15" s="13"/>
+      <c r="K15" s="13"/>
+      <c r="L15" s="13"/>
+      <c r="M15" s="13"/>
+      <c r="N15" s="13"/>
+      <c r="O15" s="13"/>
+      <c r="P15" s="13"/>
+      <c r="Q15" s="13"/>
+      <c r="R15" s="13"/>
+      <c r="S15" s="13"/>
+      <c r="T15" s="13"/>
+      <c r="U15" s="13"/>
+      <c r="V15" s="13"/>
+      <c r="W15" s="13"/>
+      <c r="X15" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="K6:L6"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="K7:L7"/>
+    <mergeCell ref="A2:L2"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="K4:L4"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="K5:L5"/>
     <mergeCell ref="T7:X7"/>
     <mergeCell ref="M2:X2"/>
     <mergeCell ref="N3:R3"/>
@@ -1491,19 +1591,160 @@
     <mergeCell ref="T4:X4"/>
     <mergeCell ref="T5:X5"/>
     <mergeCell ref="T6:X6"/>
-    <mergeCell ref="B6:D6"/>
-    <mergeCell ref="K6:L6"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="K7:L7"/>
-    <mergeCell ref="A2:L2"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="K3:L3"/>
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="K4:L4"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="K5:L5"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{069E99F5-722A-412E-A4FE-0B3F0CD46943}">
+  <dimension ref="A1:H6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="8" width="20.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="31" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+    </row>
+    <row r="2" spans="1:8" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="32"/>
+      <c r="B2" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2" s="32" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2" s="32" t="s">
+        <v>36</v>
+      </c>
+      <c r="F2" s="32" t="s">
+        <v>37</v>
+      </c>
+      <c r="G2" s="32" t="s">
+        <v>38</v>
+      </c>
+      <c r="H2" s="32" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="32" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" s="33" t="s">
+        <v>41</v>
+      </c>
+      <c r="C3" s="33" t="s">
+        <v>41</v>
+      </c>
+      <c r="D3" s="33" t="s">
+        <v>45</v>
+      </c>
+      <c r="E3" s="33" t="s">
+        <v>45</v>
+      </c>
+      <c r="F3" s="33" t="s">
+        <v>41</v>
+      </c>
+      <c r="G3" s="33"/>
+      <c r="H3" s="33"/>
+    </row>
+    <row r="4" spans="1:8" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="32" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" s="33" t="s">
+        <v>42</v>
+      </c>
+      <c r="C4" s="33" t="s">
+        <v>42</v>
+      </c>
+      <c r="D4" s="33" t="s">
+        <v>46</v>
+      </c>
+      <c r="E4" s="33" t="s">
+        <v>46</v>
+      </c>
+      <c r="F4" s="33" t="s">
+        <v>45</v>
+      </c>
+      <c r="G4" s="33"/>
+      <c r="H4" s="33"/>
+    </row>
+    <row r="5" spans="1:8" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="32" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5" s="33" t="s">
+        <v>43</v>
+      </c>
+      <c r="C5" s="33" t="s">
+        <v>43</v>
+      </c>
+      <c r="D5" s="33" t="s">
+        <v>47</v>
+      </c>
+      <c r="E5" s="33" t="s">
+        <v>47</v>
+      </c>
+      <c r="F5" s="33" t="s">
+        <v>44</v>
+      </c>
+      <c r="G5" s="33" t="s">
+        <v>50</v>
+      </c>
+      <c r="H5" s="33"/>
+    </row>
+    <row r="6" spans="1:8" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="32" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6" s="33" t="s">
+        <v>44</v>
+      </c>
+      <c r="C6" s="33" t="s">
+        <v>44</v>
+      </c>
+      <c r="D6" s="33" t="s">
+        <v>48</v>
+      </c>
+      <c r="E6" s="33" t="s">
+        <v>48</v>
+      </c>
+      <c r="F6" s="33" t="s">
+        <v>49</v>
+      </c>
+      <c r="G6" s="33" t="s">
+        <v>49</v>
+      </c>
+      <c r="H6" s="33"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:H1"/>
+  </mergeCells>
+  <phoneticPr fontId="4" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
attendace Report Modified and call stored procedure form efcore
</commit_message>
<xml_diff>
--- a/Resources/Layout.xlsx
+++ b/Resources/Layout.xlsx
@@ -1,31 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24332"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7ED6608-A84B-464F-A761-C4CEFE040CDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBDC43C8-FBB8-4D92-A02F-22618BF9D235}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11280" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Dashboard" sheetId="2" r:id="rId2"/>
-    <sheet name="Class Routine Teacher" sheetId="6" r:id="rId3"/>
-    <sheet name="Sheet3" sheetId="7" r:id="rId4"/>
-    <sheet name="Student Attendance" sheetId="4" r:id="rId5"/>
-    <sheet name="Employee Attendance" sheetId="5" r:id="rId6"/>
+    <sheet name="Attendance Report" sheetId="8" r:id="rId2"/>
+    <sheet name="Dashboard" sheetId="2" r:id="rId3"/>
+    <sheet name="Class Routine Teacher" sheetId="6" r:id="rId4"/>
+    <sheet name="Sheet3" sheetId="7" r:id="rId5"/>
+    <sheet name="Student Attendance" sheetId="4" r:id="rId6"/>
+    <sheet name="Employee Attendance" sheetId="5" r:id="rId7"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="4">'Student Attendance'!$A$1:$F$20</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="5">'Student Attendance'!$A$1:$F$20</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -33,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="145">
   <si>
     <t>Date</t>
   </si>
@@ -375,6 +377,120 @@
   </si>
   <si>
     <t>ICT</t>
+  </si>
+  <si>
+    <t>Reporting Date: 09 Aug 2022</t>
+  </si>
+  <si>
+    <t>Roll</t>
+  </si>
+  <si>
+    <t>Md. Samsul Alam</t>
+  </si>
+  <si>
+    <t>Md. Jamal Bhuyan</t>
+  </si>
+  <si>
+    <t>Mohammad Yasin</t>
+  </si>
+  <si>
+    <t>Sree Rakesh Chandra</t>
+  </si>
+  <si>
+    <t>Hamidul Islam Azad</t>
+  </si>
+  <si>
+    <t>Abul Kalam Azad</t>
+  </si>
+  <si>
+    <t>Rashidul Islam</t>
+  </si>
+  <si>
+    <t>Miss Sopna Ferdowsi</t>
+  </si>
+  <si>
+    <t>Ten (Humanities)</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Attended (08:48am)</t>
+  </si>
+  <si>
+    <t>Attended (08:49am)</t>
+  </si>
+  <si>
+    <t>Attended (08:44am)</t>
+  </si>
+  <si>
+    <t>Attended (09:04am)</t>
+  </si>
+  <si>
+    <t>Attended (08:56am)</t>
+  </si>
+  <si>
+    <t>Attended (09:07am)</t>
+  </si>
+  <si>
+    <t>Attended (08:39 am)</t>
+  </si>
+  <si>
+    <t>(Daily Attendance Report)</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Noble Residential School</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Pirgacha, Rangpur</t>
+    </r>
+  </si>
+  <si>
+    <t>01652147852</t>
+  </si>
+  <si>
+    <t>01754785412</t>
+  </si>
+  <si>
+    <t>01321456987</t>
+  </si>
+  <si>
+    <t>01574214544</t>
+  </si>
+  <si>
+    <t>01365987412</t>
+  </si>
+  <si>
+    <t>01478521479</t>
+  </si>
+  <si>
+    <t>01956987412</t>
+  </si>
+  <si>
+    <t>01875214321</t>
+  </si>
+  <si>
+    <t>01763635214</t>
+  </si>
+  <si>
+    <t>Academic Class : Six</t>
   </si>
 </sst>
 </file>
@@ -384,7 +500,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-409]mmmm\ d\,\ yyyy;@"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -467,8 +583,24 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -517,8 +649,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="7">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -596,11 +740,72 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="hair">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color indexed="64"/>
+      </left>
+      <right style="hair">
+        <color indexed="64"/>
+      </right>
+      <top style="hair">
+        <color indexed="64"/>
+      </top>
+      <bottom style="hair">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="hair">
+        <color indexed="64"/>
+      </top>
+      <bottom style="hair">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color indexed="64"/>
+      </left>
+      <right style="hair">
+        <color indexed="64"/>
+      </right>
+      <top style="hair">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="hair">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="83">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
@@ -688,81 +893,119 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1170,7 +1413,7 @@
   <dimension ref="A1:L15"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1220,28 +1463,28 @@
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="39" t="s">
+      <c r="A2" s="54" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="39"/>
-      <c r="C2" s="40" t="s">
+      <c r="B2" s="54"/>
+      <c r="C2" s="55" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="40"/>
-      <c r="E2" s="40"/>
+      <c r="D2" s="55"/>
+      <c r="E2" s="55"/>
       <c r="F2" s="12"/>
     </row>
     <row r="3" spans="1:12" s="8" customFormat="1" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F3" s="9"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="39" t="s">
+      <c r="A4" s="54" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="39"/>
-      <c r="C4" s="41"/>
-      <c r="D4" s="41"/>
-      <c r="E4" s="41"/>
+      <c r="B4" s="54"/>
+      <c r="C4" s="56"/>
+      <c r="D4" s="56"/>
+      <c r="E4" s="56"/>
       <c r="F4" s="7" t="s">
         <v>15</v>
       </c>
@@ -1256,12 +1499,12 @@
       <c r="F5" s="7"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="44" t="s">
+      <c r="A6" s="59" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="44"/>
-      <c r="C6" s="43"/>
-      <c r="D6" s="43"/>
+      <c r="B6" s="59"/>
+      <c r="C6" s="58"/>
+      <c r="D6" s="58"/>
       <c r="E6" s="11"/>
       <c r="F6" s="7" t="s">
         <v>16</v>
@@ -1271,12 +1514,12 @@
       <c r="F7" s="9"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="44" t="s">
+      <c r="A8" s="59" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="44"/>
-      <c r="C8" s="43"/>
-      <c r="D8" s="43"/>
+      <c r="B8" s="59"/>
+      <c r="C8" s="58"/>
+      <c r="D8" s="58"/>
       <c r="E8" s="10" t="s">
         <v>14</v>
       </c>
@@ -1285,13 +1528,13 @@
       <c r="F9" s="9"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="42" t="s">
+      <c r="A10" s="57" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="42"/>
-      <c r="C10" s="43"/>
-      <c r="D10" s="43"/>
-      <c r="E10" s="43"/>
+      <c r="B10" s="57"/>
+      <c r="C10" s="58"/>
+      <c r="D10" s="58"/>
+      <c r="E10" s="58"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
@@ -1378,6 +1621,617 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{524DEAA1-1F57-42FE-8A34-A461C043F698}">
+  <dimension ref="A1:I36"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="35.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="60" t="s">
+        <v>134</v>
+      </c>
+      <c r="B1" s="61"/>
+      <c r="C1" s="61"/>
+      <c r="D1" s="61"/>
+      <c r="E1" s="61"/>
+      <c r="F1" s="61"/>
+    </row>
+    <row r="2" spans="1:9" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="61"/>
+      <c r="B2" s="61"/>
+      <c r="C2" s="61"/>
+      <c r="D2" s="61"/>
+      <c r="E2" s="61"/>
+      <c r="F2" s="61"/>
+    </row>
+    <row r="3" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="62" t="s">
+        <v>133</v>
+      </c>
+      <c r="B3" s="62"/>
+      <c r="C3" s="62"/>
+      <c r="D3" s="62"/>
+      <c r="E3" s="62"/>
+      <c r="F3" s="62"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="63" t="s">
+        <v>144</v>
+      </c>
+      <c r="B4" s="63"/>
+      <c r="C4" s="51"/>
+      <c r="D4" s="51"/>
+      <c r="E4" s="64" t="s">
+        <v>114</v>
+      </c>
+      <c r="F4" s="64"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="43" t="s">
+        <v>115</v>
+      </c>
+      <c r="B5" s="45" t="s">
+        <v>36</v>
+      </c>
+      <c r="C5" s="49" t="s">
+        <v>99</v>
+      </c>
+      <c r="D5" s="49" t="s">
+        <v>75</v>
+      </c>
+      <c r="E5" s="48" t="s">
+        <v>125</v>
+      </c>
+      <c r="F5" s="50" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="42">
+        <v>2110001</v>
+      </c>
+      <c r="B6" s="44" t="s">
+        <v>116</v>
+      </c>
+      <c r="C6" s="44" t="s">
+        <v>124</v>
+      </c>
+      <c r="D6" s="53" t="s">
+        <v>135</v>
+      </c>
+      <c r="E6" s="44" t="s">
+        <v>57</v>
+      </c>
+      <c r="F6" s="52"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="42">
+        <v>2110002</v>
+      </c>
+      <c r="B7" s="44" t="s">
+        <v>117</v>
+      </c>
+      <c r="C7" s="44" t="s">
+        <v>124</v>
+      </c>
+      <c r="D7" s="53" t="s">
+        <v>136</v>
+      </c>
+      <c r="E7" s="44" t="s">
+        <v>126</v>
+      </c>
+      <c r="F7" s="52"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="42">
+        <v>2110003</v>
+      </c>
+      <c r="B8" s="44" t="s">
+        <v>118</v>
+      </c>
+      <c r="C8" s="44" t="s">
+        <v>124</v>
+      </c>
+      <c r="D8" s="53" t="s">
+        <v>137</v>
+      </c>
+      <c r="E8" s="44" t="s">
+        <v>127</v>
+      </c>
+      <c r="F8" s="52"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="42">
+        <v>2110004</v>
+      </c>
+      <c r="B9" s="44" t="s">
+        <v>119</v>
+      </c>
+      <c r="C9" s="44" t="s">
+        <v>124</v>
+      </c>
+      <c r="D9" s="53" t="s">
+        <v>138</v>
+      </c>
+      <c r="E9" s="44" t="s">
+        <v>128</v>
+      </c>
+      <c r="F9" s="52"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="42">
+        <v>2110005</v>
+      </c>
+      <c r="B10" s="44" t="s">
+        <v>120</v>
+      </c>
+      <c r="C10" s="44" t="s">
+        <v>124</v>
+      </c>
+      <c r="D10" s="53" t="s">
+        <v>139</v>
+      </c>
+      <c r="E10" s="44" t="s">
+        <v>129</v>
+      </c>
+      <c r="F10" s="52"/>
+      <c r="I10" s="41"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="42">
+        <v>2110006</v>
+      </c>
+      <c r="B11" s="44" t="s">
+        <v>121</v>
+      </c>
+      <c r="C11" s="44" t="s">
+        <v>124</v>
+      </c>
+      <c r="D11" s="53" t="s">
+        <v>140</v>
+      </c>
+      <c r="E11" s="44" t="s">
+        <v>126</v>
+      </c>
+      <c r="F11" s="52"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="42">
+        <v>2110007</v>
+      </c>
+      <c r="B12" s="44" t="s">
+        <v>122</v>
+      </c>
+      <c r="C12" s="44" t="s">
+        <v>124</v>
+      </c>
+      <c r="D12" s="53" t="s">
+        <v>141</v>
+      </c>
+      <c r="E12" s="44" t="s">
+        <v>127</v>
+      </c>
+      <c r="F12" s="52"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="42">
+        <v>2110008</v>
+      </c>
+      <c r="B13" s="44" t="s">
+        <v>123</v>
+      </c>
+      <c r="C13" s="44" t="s">
+        <v>124</v>
+      </c>
+      <c r="D13" s="53" t="s">
+        <v>142</v>
+      </c>
+      <c r="E13" s="44" t="s">
+        <v>128</v>
+      </c>
+      <c r="F13" s="52"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="42">
+        <v>2110009</v>
+      </c>
+      <c r="B14" s="44" t="s">
+        <v>116</v>
+      </c>
+      <c r="C14" s="44" t="s">
+        <v>124</v>
+      </c>
+      <c r="D14" s="53" t="s">
+        <v>143</v>
+      </c>
+      <c r="E14" s="44" t="s">
+        <v>57</v>
+      </c>
+      <c r="F14" s="52"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="42">
+        <v>2110010</v>
+      </c>
+      <c r="B15" s="44" t="s">
+        <v>117</v>
+      </c>
+      <c r="C15" s="44" t="s">
+        <v>124</v>
+      </c>
+      <c r="D15" s="53" t="s">
+        <v>135</v>
+      </c>
+      <c r="E15" s="44" t="s">
+        <v>130</v>
+      </c>
+      <c r="F15" s="52"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="42">
+        <v>2110011</v>
+      </c>
+      <c r="B16" s="44" t="s">
+        <v>118</v>
+      </c>
+      <c r="C16" s="44" t="s">
+        <v>124</v>
+      </c>
+      <c r="D16" s="53" t="s">
+        <v>136</v>
+      </c>
+      <c r="E16" s="44" t="s">
+        <v>131</v>
+      </c>
+      <c r="F16" s="52"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="42">
+        <v>2110012</v>
+      </c>
+      <c r="B17" s="44" t="s">
+        <v>119</v>
+      </c>
+      <c r="C17" s="44" t="s">
+        <v>124</v>
+      </c>
+      <c r="D17" s="53" t="s">
+        <v>137</v>
+      </c>
+      <c r="E17" s="44" t="s">
+        <v>132</v>
+      </c>
+      <c r="F17" s="52"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="42">
+        <v>2110013</v>
+      </c>
+      <c r="B18" s="44" t="s">
+        <v>120</v>
+      </c>
+      <c r="C18" s="44" t="s">
+        <v>124</v>
+      </c>
+      <c r="D18" s="53" t="s">
+        <v>138</v>
+      </c>
+      <c r="E18" s="44" t="s">
+        <v>57</v>
+      </c>
+      <c r="F18" s="52"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="42">
+        <v>2110014</v>
+      </c>
+      <c r="B19" s="44" t="s">
+        <v>121</v>
+      </c>
+      <c r="C19" s="44" t="s">
+        <v>124</v>
+      </c>
+      <c r="D19" s="53" t="s">
+        <v>139</v>
+      </c>
+      <c r="E19" s="44" t="s">
+        <v>57</v>
+      </c>
+      <c r="F19" s="52"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="42">
+        <v>2110015</v>
+      </c>
+      <c r="B20" s="44" t="s">
+        <v>120</v>
+      </c>
+      <c r="C20" s="44" t="s">
+        <v>124</v>
+      </c>
+      <c r="D20" s="53" t="s">
+        <v>140</v>
+      </c>
+      <c r="E20" s="44" t="s">
+        <v>130</v>
+      </c>
+      <c r="F20" s="52"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="42">
+        <v>2110016</v>
+      </c>
+      <c r="B21" s="44" t="s">
+        <v>121</v>
+      </c>
+      <c r="C21" s="44" t="s">
+        <v>124</v>
+      </c>
+      <c r="D21" s="53" t="s">
+        <v>141</v>
+      </c>
+      <c r="E21" s="44" t="s">
+        <v>131</v>
+      </c>
+      <c r="F21" s="52"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="42">
+        <v>2110017</v>
+      </c>
+      <c r="B22" s="44" t="s">
+        <v>122</v>
+      </c>
+      <c r="C22" s="44" t="s">
+        <v>124</v>
+      </c>
+      <c r="D22" s="53" t="s">
+        <v>142</v>
+      </c>
+      <c r="E22" s="44" t="s">
+        <v>132</v>
+      </c>
+      <c r="F22" s="52"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="42">
+        <v>2110018</v>
+      </c>
+      <c r="B23" s="44" t="s">
+        <v>123</v>
+      </c>
+      <c r="C23" s="44" t="s">
+        <v>124</v>
+      </c>
+      <c r="D23" s="53" t="s">
+        <v>143</v>
+      </c>
+      <c r="E23" s="44" t="s">
+        <v>57</v>
+      </c>
+      <c r="F23" s="52"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="42">
+        <v>2110019</v>
+      </c>
+      <c r="B24" s="44" t="s">
+        <v>116</v>
+      </c>
+      <c r="C24" s="44" t="s">
+        <v>124</v>
+      </c>
+      <c r="D24" s="53" t="s">
+        <v>135</v>
+      </c>
+      <c r="E24" s="44" t="s">
+        <v>57</v>
+      </c>
+      <c r="F24" s="52"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="42">
+        <v>2110020</v>
+      </c>
+      <c r="B25" s="44" t="s">
+        <v>117</v>
+      </c>
+      <c r="C25" s="44" t="s">
+        <v>124</v>
+      </c>
+      <c r="D25" s="53" t="s">
+        <v>136</v>
+      </c>
+      <c r="E25" s="44" t="s">
+        <v>57</v>
+      </c>
+      <c r="F25" s="52"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="42">
+        <v>2110021</v>
+      </c>
+      <c r="B26" s="44" t="s">
+        <v>118</v>
+      </c>
+      <c r="C26" s="44" t="s">
+        <v>124</v>
+      </c>
+      <c r="D26" s="53" t="s">
+        <v>137</v>
+      </c>
+      <c r="E26" s="44" t="s">
+        <v>129</v>
+      </c>
+      <c r="F26" s="52"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="42">
+        <v>2110022</v>
+      </c>
+      <c r="B27" s="44" t="s">
+        <v>119</v>
+      </c>
+      <c r="C27" s="44" t="s">
+        <v>124</v>
+      </c>
+      <c r="D27" s="53" t="s">
+        <v>138</v>
+      </c>
+      <c r="E27" s="44" t="s">
+        <v>126</v>
+      </c>
+      <c r="F27" s="52"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="42">
+        <v>2110023</v>
+      </c>
+      <c r="B28" s="44" t="s">
+        <v>120</v>
+      </c>
+      <c r="C28" s="44" t="s">
+        <v>124</v>
+      </c>
+      <c r="D28" s="53" t="s">
+        <v>139</v>
+      </c>
+      <c r="E28" s="44" t="s">
+        <v>127</v>
+      </c>
+      <c r="F28" s="52"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="42">
+        <v>2110024</v>
+      </c>
+      <c r="B29" s="44" t="s">
+        <v>121</v>
+      </c>
+      <c r="C29" s="44" t="s">
+        <v>124</v>
+      </c>
+      <c r="D29" s="53" t="s">
+        <v>140</v>
+      </c>
+      <c r="E29" s="44" t="s">
+        <v>128</v>
+      </c>
+      <c r="F29" s="52"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="42">
+        <v>2110025</v>
+      </c>
+      <c r="B30" s="44" t="s">
+        <v>122</v>
+      </c>
+      <c r="C30" s="44" t="s">
+        <v>124</v>
+      </c>
+      <c r="D30" s="53" t="s">
+        <v>141</v>
+      </c>
+      <c r="E30" s="44" t="s">
+        <v>129</v>
+      </c>
+      <c r="F30" s="52"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="42">
+        <v>2110026</v>
+      </c>
+      <c r="B31" s="44" t="s">
+        <v>123</v>
+      </c>
+      <c r="C31" s="44" t="s">
+        <v>124</v>
+      </c>
+      <c r="D31" s="53" t="s">
+        <v>142</v>
+      </c>
+      <c r="E31" s="44" t="s">
+        <v>126</v>
+      </c>
+      <c r="F31" s="52"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="46">
+        <v>2110027</v>
+      </c>
+      <c r="B32" s="47" t="s">
+        <v>116</v>
+      </c>
+      <c r="C32" s="47" t="s">
+        <v>124</v>
+      </c>
+      <c r="D32" s="53" t="s">
+        <v>143</v>
+      </c>
+      <c r="E32" s="44" t="s">
+        <v>127</v>
+      </c>
+      <c r="F32" s="52"/>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="17"/>
+      <c r="B33" s="17"/>
+      <c r="C33" s="17"/>
+      <c r="D33" s="17"/>
+      <c r="E33" s="44"/>
+      <c r="F33" s="17"/>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="17"/>
+      <c r="B34" s="17"/>
+      <c r="C34" s="17"/>
+      <c r="D34" s="17"/>
+      <c r="E34" s="17"/>
+      <c r="F34" s="17"/>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="17"/>
+      <c r="B35" s="17"/>
+      <c r="C35" s="17"/>
+      <c r="D35" s="17"/>
+      <c r="E35" s="17"/>
+      <c r="F35" s="17"/>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" s="17"/>
+      <c r="B36" s="17"/>
+      <c r="C36" s="17"/>
+      <c r="D36" s="17"/>
+      <c r="E36" s="17"/>
+      <c r="F36" s="17"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A1:F2"/>
+    <mergeCell ref="A3:F3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="E4:F4"/>
+  </mergeCells>
+  <phoneticPr fontId="4" type="noConversion"/>
+  <printOptions horizontalCentered="1"/>
+  <pageMargins left="0.45" right="0.45" top="0.5" bottom="0.5" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="80" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AC9086E-D004-4EA1-8724-804CD1EEFB7F}">
   <dimension ref="A1:X15"/>
   <sheetViews>
@@ -1470,234 +2324,234 @@
       </c>
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A2" s="50" t="s">
+      <c r="A2" s="70" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="50"/>
-      <c r="C2" s="50"/>
-      <c r="D2" s="50"/>
-      <c r="E2" s="50"/>
-      <c r="F2" s="50"/>
-      <c r="G2" s="50"/>
-      <c r="H2" s="50"/>
-      <c r="I2" s="50"/>
-      <c r="J2" s="50"/>
-      <c r="K2" s="50"/>
-      <c r="L2" s="50"/>
-      <c r="M2" s="46" t="s">
+      <c r="B2" s="70"/>
+      <c r="C2" s="70"/>
+      <c r="D2" s="70"/>
+      <c r="E2" s="70"/>
+      <c r="F2" s="70"/>
+      <c r="G2" s="70"/>
+      <c r="H2" s="70"/>
+      <c r="I2" s="70"/>
+      <c r="J2" s="70"/>
+      <c r="K2" s="70"/>
+      <c r="L2" s="70"/>
+      <c r="M2" s="66" t="s">
         <v>23</v>
       </c>
-      <c r="N2" s="46"/>
-      <c r="O2" s="46"/>
-      <c r="P2" s="46"/>
-      <c r="Q2" s="46"/>
-      <c r="R2" s="46"/>
-      <c r="S2" s="46"/>
-      <c r="T2" s="46"/>
-      <c r="U2" s="46"/>
-      <c r="V2" s="46"/>
-      <c r="W2" s="46"/>
-      <c r="X2" s="46"/>
+      <c r="N2" s="66"/>
+      <c r="O2" s="66"/>
+      <c r="P2" s="66"/>
+      <c r="Q2" s="66"/>
+      <c r="R2" s="66"/>
+      <c r="S2" s="66"/>
+      <c r="T2" s="66"/>
+      <c r="U2" s="66"/>
+      <c r="V2" s="66"/>
+      <c r="W2" s="66"/>
+      <c r="X2" s="66"/>
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3" s="15">
         <v>1</v>
       </c>
-      <c r="B3" s="51" t="s">
+      <c r="B3" s="71" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="51"/>
-      <c r="D3" s="51"/>
+      <c r="C3" s="71"/>
+      <c r="D3" s="71"/>
       <c r="E3" s="16"/>
       <c r="F3" s="16"/>
       <c r="G3" s="16"/>
       <c r="H3" s="16"/>
       <c r="I3" s="16"/>
       <c r="J3" s="16"/>
-      <c r="K3" s="52">
+      <c r="K3" s="72">
         <v>45</v>
       </c>
-      <c r="L3" s="52"/>
+      <c r="L3" s="72"/>
       <c r="M3" s="14">
         <v>1</v>
       </c>
-      <c r="N3" s="47" t="s">
+      <c r="N3" s="67" t="s">
         <v>24</v>
       </c>
-      <c r="O3" s="47"/>
-      <c r="P3" s="47"/>
-      <c r="Q3" s="47"/>
-      <c r="R3" s="47"/>
+      <c r="O3" s="67"/>
+      <c r="P3" s="67"/>
+      <c r="Q3" s="67"/>
+      <c r="R3" s="67"/>
       <c r="S3" s="14">
         <v>6</v>
       </c>
-      <c r="T3" s="45" t="s">
+      <c r="T3" s="65" t="s">
         <v>29</v>
       </c>
-      <c r="U3" s="45"/>
-      <c r="V3" s="45"/>
-      <c r="W3" s="45"/>
-      <c r="X3" s="45"/>
+      <c r="U3" s="65"/>
+      <c r="V3" s="65"/>
+      <c r="W3" s="65"/>
+      <c r="X3" s="65"/>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" s="15">
         <v>2</v>
       </c>
-      <c r="B4" s="51" t="s">
+      <c r="B4" s="71" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="51"/>
-      <c r="D4" s="51"/>
+      <c r="C4" s="71"/>
+      <c r="D4" s="71"/>
       <c r="E4" s="15"/>
       <c r="F4" s="15"/>
       <c r="G4" s="15"/>
       <c r="H4" s="15"/>
       <c r="I4" s="15"/>
       <c r="J4" s="15"/>
-      <c r="K4" s="52">
+      <c r="K4" s="72">
         <v>46</v>
       </c>
-      <c r="L4" s="52"/>
+      <c r="L4" s="72"/>
       <c r="M4" s="14">
         <v>2</v>
       </c>
-      <c r="N4" s="47" t="s">
+      <c r="N4" s="67" t="s">
         <v>25</v>
       </c>
-      <c r="O4" s="47"/>
-      <c r="P4" s="47"/>
-      <c r="Q4" s="47"/>
-      <c r="R4" s="47"/>
+      <c r="O4" s="67"/>
+      <c r="P4" s="67"/>
+      <c r="Q4" s="67"/>
+      <c r="R4" s="67"/>
       <c r="S4" s="14">
         <v>7</v>
       </c>
-      <c r="T4" s="45" t="s">
+      <c r="T4" s="65" t="s">
         <v>29</v>
       </c>
-      <c r="U4" s="45"/>
-      <c r="V4" s="45"/>
-      <c r="W4" s="45"/>
-      <c r="X4" s="45"/>
+      <c r="U4" s="65"/>
+      <c r="V4" s="65"/>
+      <c r="W4" s="65"/>
+      <c r="X4" s="65"/>
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5" s="15">
         <v>3</v>
       </c>
-      <c r="B5" s="48" t="s">
+      <c r="B5" s="68" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="48"/>
-      <c r="D5" s="48"/>
+      <c r="C5" s="68"/>
+      <c r="D5" s="68"/>
       <c r="E5" s="15"/>
       <c r="F5" s="15"/>
       <c r="G5" s="15"/>
       <c r="H5" s="15"/>
       <c r="I5" s="15"/>
       <c r="J5" s="15"/>
-      <c r="K5" s="49">
+      <c r="K5" s="69">
         <v>47</v>
       </c>
-      <c r="L5" s="49"/>
+      <c r="L5" s="69"/>
       <c r="M5" s="14">
         <v>3</v>
       </c>
-      <c r="N5" s="47" t="s">
+      <c r="N5" s="67" t="s">
         <v>26</v>
       </c>
-      <c r="O5" s="47"/>
-      <c r="P5" s="47"/>
-      <c r="Q5" s="47"/>
-      <c r="R5" s="47"/>
+      <c r="O5" s="67"/>
+      <c r="P5" s="67"/>
+      <c r="Q5" s="67"/>
+      <c r="R5" s="67"/>
       <c r="S5" s="14">
         <v>8</v>
       </c>
-      <c r="T5" s="45" t="s">
+      <c r="T5" s="65" t="s">
         <v>29</v>
       </c>
-      <c r="U5" s="45"/>
-      <c r="V5" s="45"/>
-      <c r="W5" s="45"/>
-      <c r="X5" s="45"/>
+      <c r="U5" s="65"/>
+      <c r="V5" s="65"/>
+      <c r="W5" s="65"/>
+      <c r="X5" s="65"/>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6" s="15">
         <v>4</v>
       </c>
-      <c r="B6" s="48" t="s">
+      <c r="B6" s="68" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="48"/>
-      <c r="D6" s="48"/>
+      <c r="C6" s="68"/>
+      <c r="D6" s="68"/>
       <c r="E6" s="15"/>
       <c r="F6" s="15"/>
       <c r="G6" s="15"/>
       <c r="H6" s="15"/>
       <c r="I6" s="15"/>
       <c r="J6" s="15"/>
-      <c r="K6" s="49">
+      <c r="K6" s="69">
         <v>48</v>
       </c>
-      <c r="L6" s="49"/>
+      <c r="L6" s="69"/>
       <c r="M6" s="14">
         <v>4</v>
       </c>
-      <c r="N6" s="47" t="s">
+      <c r="N6" s="67" t="s">
         <v>27</v>
       </c>
-      <c r="O6" s="47"/>
-      <c r="P6" s="47"/>
-      <c r="Q6" s="47"/>
-      <c r="R6" s="47"/>
+      <c r="O6" s="67"/>
+      <c r="P6" s="67"/>
+      <c r="Q6" s="67"/>
+      <c r="R6" s="67"/>
       <c r="S6" s="14">
         <v>9</v>
       </c>
-      <c r="T6" s="45" t="s">
+      <c r="T6" s="65" t="s">
         <v>29</v>
       </c>
-      <c r="U6" s="45"/>
-      <c r="V6" s="45"/>
-      <c r="W6" s="45"/>
-      <c r="X6" s="45"/>
+      <c r="U6" s="65"/>
+      <c r="V6" s="65"/>
+      <c r="W6" s="65"/>
+      <c r="X6" s="65"/>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7" s="15">
         <v>5</v>
       </c>
-      <c r="B7" s="48" t="s">
+      <c r="B7" s="68" t="s">
         <v>22</v>
       </c>
-      <c r="C7" s="48"/>
-      <c r="D7" s="48"/>
+      <c r="C7" s="68"/>
+      <c r="D7" s="68"/>
       <c r="E7" s="15"/>
       <c r="F7" s="15"/>
       <c r="G7" s="15"/>
       <c r="H7" s="15"/>
       <c r="I7" s="15"/>
       <c r="J7" s="15"/>
-      <c r="K7" s="49">
+      <c r="K7" s="69">
         <v>49</v>
       </c>
-      <c r="L7" s="49"/>
+      <c r="L7" s="69"/>
       <c r="M7" s="14">
         <v>5</v>
       </c>
-      <c r="N7" s="47" t="s">
+      <c r="N7" s="67" t="s">
         <v>28</v>
       </c>
-      <c r="O7" s="47"/>
-      <c r="P7" s="47"/>
-      <c r="Q7" s="47"/>
-      <c r="R7" s="47"/>
+      <c r="O7" s="67"/>
+      <c r="P7" s="67"/>
+      <c r="Q7" s="67"/>
+      <c r="R7" s="67"/>
       <c r="S7" s="14">
         <v>10</v>
       </c>
-      <c r="T7" s="45" t="s">
+      <c r="T7" s="65" t="s">
         <v>29</v>
       </c>
-      <c r="U7" s="45"/>
-      <c r="V7" s="45"/>
-      <c r="W7" s="45"/>
-      <c r="X7" s="45"/>
+      <c r="U7" s="65"/>
+      <c r="V7" s="65"/>
+      <c r="W7" s="65"/>
+      <c r="X7" s="65"/>
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A8" s="13"/>
@@ -1937,7 +2791,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{889D0D57-1F26-473E-B306-F0F5D3A5E8AC}">
   <dimension ref="A1:I2"/>
   <sheetViews>
@@ -2004,12 +2858,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B9CA3B1-EDA9-4D32-B2CA-E8D9C6600DDC}">
   <dimension ref="A1:J31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S3" sqref="S3"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="T1" sqref="T1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2027,39 +2881,39 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="63" t="s">
+      <c r="A1" s="39" t="s">
         <v>98</v>
       </c>
-      <c r="B1" s="63" t="s">
+      <c r="B1" s="39" t="s">
         <v>99</v>
       </c>
-      <c r="C1" s="64" t="s">
+      <c r="C1" s="40" t="s">
         <v>30</v>
       </c>
-      <c r="D1" s="64" t="s">
+      <c r="D1" s="40" t="s">
         <v>31</v>
       </c>
-      <c r="E1" s="64" t="s">
+      <c r="E1" s="40" t="s">
         <v>32</v>
       </c>
-      <c r="F1" s="64" t="s">
+      <c r="F1" s="40" t="s">
         <v>33</v>
       </c>
-      <c r="G1" s="64" t="s">
+      <c r="G1" s="40" t="s">
         <v>82</v>
       </c>
-      <c r="H1" s="64" t="s">
+      <c r="H1" s="40" t="s">
         <v>83</v>
       </c>
-      <c r="I1" s="64" t="s">
+      <c r="I1" s="40" t="s">
         <v>84</v>
       </c>
-      <c r="J1" s="64" t="s">
+      <c r="J1" s="40" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="62" t="s">
+      <c r="A2" s="73" t="s">
         <v>34</v>
       </c>
       <c r="B2" s="37" t="s">
@@ -2079,7 +2933,7 @@
       <c r="J2" s="37"/>
     </row>
     <row r="3" spans="1:10" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="62"/>
+      <c r="A3" s="73"/>
       <c r="B3" s="38" t="s">
         <v>19</v>
       </c>
@@ -2099,7 +2953,7 @@
       <c r="J3" s="38"/>
     </row>
     <row r="4" spans="1:10" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="62"/>
+      <c r="A4" s="73"/>
       <c r="B4" s="37" t="s">
         <v>20</v>
       </c>
@@ -2119,7 +2973,7 @@
       <c r="J4" s="37"/>
     </row>
     <row r="5" spans="1:10" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="62"/>
+      <c r="A5" s="73"/>
       <c r="B5" s="38" t="s">
         <v>21</v>
       </c>
@@ -2137,7 +2991,7 @@
       <c r="J5" s="38"/>
     </row>
     <row r="6" spans="1:10" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="62"/>
+      <c r="A6" s="73"/>
       <c r="B6" s="37" t="s">
         <v>22</v>
       </c>
@@ -2155,7 +3009,7 @@
       <c r="J6" s="37"/>
     </row>
     <row r="7" spans="1:10" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="62" t="s">
+      <c r="A7" s="73" t="s">
         <v>107</v>
       </c>
       <c r="B7" s="37" t="s">
@@ -2175,7 +3029,7 @@
       <c r="J7" s="37"/>
     </row>
     <row r="8" spans="1:10" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="62"/>
+      <c r="A8" s="73"/>
       <c r="B8" s="38" t="s">
         <v>19</v>
       </c>
@@ -2195,7 +3049,7 @@
       <c r="J8" s="38"/>
     </row>
     <row r="9" spans="1:10" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="62"/>
+      <c r="A9" s="73"/>
       <c r="B9" s="37" t="s">
         <v>20</v>
       </c>
@@ -2215,7 +3069,7 @@
       <c r="J9" s="37"/>
     </row>
     <row r="10" spans="1:10" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="62"/>
+      <c r="A10" s="73"/>
       <c r="B10" s="38" t="s">
         <v>21</v>
       </c>
@@ -2233,7 +3087,7 @@
       <c r="J10" s="38"/>
     </row>
     <row r="11" spans="1:10" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="62"/>
+      <c r="A11" s="73"/>
       <c r="B11" s="37" t="s">
         <v>22</v>
       </c>
@@ -2251,7 +3105,7 @@
       <c r="J11" s="37"/>
     </row>
     <row r="12" spans="1:10" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="62" t="s">
+      <c r="A12" s="73" t="s">
         <v>108</v>
       </c>
       <c r="B12" s="37" t="s">
@@ -2271,7 +3125,7 @@
       <c r="J12" s="37"/>
     </row>
     <row r="13" spans="1:10" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="62"/>
+      <c r="A13" s="73"/>
       <c r="B13" s="38" t="s">
         <v>19</v>
       </c>
@@ -2291,7 +3145,7 @@
       <c r="J13" s="38"/>
     </row>
     <row r="14" spans="1:10" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="62"/>
+      <c r="A14" s="73"/>
       <c r="B14" s="37" t="s">
         <v>20</v>
       </c>
@@ -2311,7 +3165,7 @@
       <c r="J14" s="37"/>
     </row>
     <row r="15" spans="1:10" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="62"/>
+      <c r="A15" s="73"/>
       <c r="B15" s="38" t="s">
         <v>21</v>
       </c>
@@ -2329,7 +3183,7 @@
       <c r="J15" s="38"/>
     </row>
     <row r="16" spans="1:10" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="62"/>
+      <c r="A16" s="73"/>
       <c r="B16" s="37" t="s">
         <v>22</v>
       </c>
@@ -2347,7 +3201,7 @@
       <c r="J16" s="37"/>
     </row>
     <row r="17" spans="1:10" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="62" t="s">
+      <c r="A17" s="73" t="s">
         <v>109</v>
       </c>
       <c r="B17" s="37" t="s">
@@ -2367,7 +3221,7 @@
       <c r="J17" s="37"/>
     </row>
     <row r="18" spans="1:10" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="62"/>
+      <c r="A18" s="73"/>
       <c r="B18" s="38" t="s">
         <v>19</v>
       </c>
@@ -2387,7 +3241,7 @@
       <c r="J18" s="38"/>
     </row>
     <row r="19" spans="1:10" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="62"/>
+      <c r="A19" s="73"/>
       <c r="B19" s="37" t="s">
         <v>20</v>
       </c>
@@ -2407,7 +3261,7 @@
       <c r="J19" s="37"/>
     </row>
     <row r="20" spans="1:10" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="62"/>
+      <c r="A20" s="73"/>
       <c r="B20" s="38" t="s">
         <v>21</v>
       </c>
@@ -2425,7 +3279,7 @@
       <c r="J20" s="38"/>
     </row>
     <row r="21" spans="1:10" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="62"/>
+      <c r="A21" s="73"/>
       <c r="B21" s="37" t="s">
         <v>22</v>
       </c>
@@ -2443,7 +3297,7 @@
       <c r="J21" s="37"/>
     </row>
     <row r="22" spans="1:10" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="62" t="s">
+      <c r="A22" s="73" t="s">
         <v>110</v>
       </c>
       <c r="B22" s="37" t="s">
@@ -2463,7 +3317,7 @@
       <c r="J22" s="37"/>
     </row>
     <row r="23" spans="1:10" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="62"/>
+      <c r="A23" s="73"/>
       <c r="B23" s="38" t="s">
         <v>19</v>
       </c>
@@ -2483,7 +3337,7 @@
       <c r="J23" s="38"/>
     </row>
     <row r="24" spans="1:10" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="62"/>
+      <c r="A24" s="73"/>
       <c r="B24" s="37" t="s">
         <v>20</v>
       </c>
@@ -2503,7 +3357,7 @@
       <c r="J24" s="37"/>
     </row>
     <row r="25" spans="1:10" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="62"/>
+      <c r="A25" s="73"/>
       <c r="B25" s="38" t="s">
         <v>21</v>
       </c>
@@ -2521,7 +3375,7 @@
       <c r="J25" s="38"/>
     </row>
     <row r="26" spans="1:10" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="62"/>
+      <c r="A26" s="73"/>
       <c r="B26" s="37" t="s">
         <v>22</v>
       </c>
@@ -2539,7 +3393,7 @@
       <c r="J26" s="37"/>
     </row>
     <row r="27" spans="1:10" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="62" t="s">
+      <c r="A27" s="73" t="s">
         <v>111</v>
       </c>
       <c r="B27" s="37" t="s">
@@ -2559,7 +3413,7 @@
       <c r="J27" s="37"/>
     </row>
     <row r="28" spans="1:10" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="62"/>
+      <c r="A28" s="73"/>
       <c r="B28" s="38" t="s">
         <v>19</v>
       </c>
@@ -2579,7 +3433,7 @@
       <c r="J28" s="38"/>
     </row>
     <row r="29" spans="1:10" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="62"/>
+      <c r="A29" s="73"/>
       <c r="B29" s="37" t="s">
         <v>20</v>
       </c>
@@ -2599,7 +3453,7 @@
       <c r="J29" s="37"/>
     </row>
     <row r="30" spans="1:10" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="62"/>
+      <c r="A30" s="73"/>
       <c r="B30" s="38" t="s">
         <v>21</v>
       </c>
@@ -2617,7 +3471,7 @@
       <c r="J30" s="38"/>
     </row>
     <row r="31" spans="1:10" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="62"/>
+      <c r="A31" s="73"/>
       <c r="B31" s="37" t="s">
         <v>22</v>
       </c>
@@ -2649,7 +3503,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68C7AB11-C29A-4F36-8877-185A21672CFE}">
   <dimension ref="A1:F20"/>
   <sheetViews>
@@ -2668,24 +3522,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="55" t="s">
+      <c r="A1" s="76" t="s">
         <v>40</v>
       </c>
-      <c r="B1" s="56"/>
-      <c r="C1" s="56"/>
-      <c r="D1" s="56"/>
-      <c r="E1" s="56"/>
-      <c r="F1" s="56"/>
+      <c r="B1" s="77"/>
+      <c r="C1" s="77"/>
+      <c r="D1" s="77"/>
+      <c r="E1" s="77"/>
+      <c r="F1" s="77"/>
     </row>
     <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="57" t="s">
+      <c r="A2" s="78" t="s">
         <v>41</v>
       </c>
-      <c r="B2" s="57"/>
-      <c r="C2" s="57"/>
-      <c r="D2" s="57"/>
-      <c r="E2" s="57"/>
-      <c r="F2" s="57"/>
+      <c r="B2" s="78"/>
+      <c r="C2" s="78"/>
+      <c r="D2" s="78"/>
+      <c r="E2" s="78"/>
+      <c r="F2" s="78"/>
     </row>
     <row r="3" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
@@ -2914,18 +3768,18 @@
       <c r="F15" s="29"/>
     </row>
     <row r="16" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="58" t="s">
+      <c r="A16" s="79" t="s">
         <v>60</v>
       </c>
-      <c r="B16" s="59"/>
-      <c r="C16" s="59"/>
-      <c r="D16" s="59"/>
-      <c r="E16" s="59"/>
-      <c r="F16" s="60"/>
+      <c r="B16" s="80"/>
+      <c r="C16" s="80"/>
+      <c r="D16" s="80"/>
+      <c r="E16" s="80"/>
+      <c r="F16" s="81"/>
     </row>
     <row r="17" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="53"/>
-      <c r="B17" s="54"/>
+      <c r="A17" s="74"/>
+      <c r="B17" s="75"/>
       <c r="C17" s="32" t="s">
         <v>73</v>
       </c>
@@ -2940,10 +3794,10 @@
       </c>
     </row>
     <row r="18" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="53" t="s">
+      <c r="A18" s="74" t="s">
         <v>15</v>
       </c>
-      <c r="B18" s="54"/>
+      <c r="B18" s="75"/>
       <c r="C18" s="32">
         <v>25</v>
       </c>
@@ -2988,7 +3842,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE752E1A-3511-482B-9D5B-C641C60E9654}">
   <dimension ref="A1:G18"/>
   <sheetViews>
@@ -3007,35 +3861,35 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="55" t="s">
+      <c r="A1" s="76" t="s">
         <v>40</v>
       </c>
-      <c r="B1" s="56"/>
-      <c r="C1" s="56"/>
-      <c r="D1" s="56"/>
-      <c r="E1" s="56"/>
-      <c r="F1" s="56"/>
-      <c r="G1" s="56"/>
+      <c r="B1" s="77"/>
+      <c r="C1" s="77"/>
+      <c r="D1" s="77"/>
+      <c r="E1" s="77"/>
+      <c r="F1" s="77"/>
+      <c r="G1" s="77"/>
     </row>
     <row r="2" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="57" t="s">
+      <c r="A2" s="78" t="s">
         <v>41</v>
       </c>
-      <c r="B2" s="57"/>
-      <c r="C2" s="57"/>
-      <c r="D2" s="57"/>
-      <c r="E2" s="57"/>
-      <c r="F2" s="57"/>
-      <c r="G2" s="57"/>
+      <c r="B2" s="78"/>
+      <c r="C2" s="78"/>
+      <c r="D2" s="78"/>
+      <c r="E2" s="78"/>
+      <c r="F2" s="78"/>
+      <c r="G2" s="78"/>
     </row>
     <row r="3" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="61" t="s">
+      <c r="A3" s="82" t="s">
         <v>74</v>
       </c>
-      <c r="B3" s="61"/>
-      <c r="C3" s="61"/>
-      <c r="D3" s="61"/>
-      <c r="E3" s="61"/>
+      <c r="B3" s="82"/>
+      <c r="C3" s="82"/>
+      <c r="D3" s="82"/>
+      <c r="E3" s="82"/>
       <c r="F3" s="21" t="s">
         <v>52</v>
       </c>
@@ -3288,19 +4142,19 @@
       <c r="G15" s="29"/>
     </row>
     <row r="16" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="58" t="s">
+      <c r="A16" s="79" t="s">
         <v>60</v>
       </c>
-      <c r="B16" s="59"/>
-      <c r="C16" s="59"/>
-      <c r="D16" s="59"/>
-      <c r="E16" s="59"/>
-      <c r="F16" s="59"/>
-      <c r="G16" s="60"/>
+      <c r="B16" s="80"/>
+      <c r="C16" s="80"/>
+      <c r="D16" s="80"/>
+      <c r="E16" s="80"/>
+      <c r="F16" s="80"/>
+      <c r="G16" s="81"/>
     </row>
     <row r="17" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="53"/>
-      <c r="B17" s="54"/>
+      <c r="A17" s="74"/>
+      <c r="B17" s="75"/>
       <c r="C17" s="32"/>
       <c r="D17" s="32" t="s">
         <v>76</v>
@@ -3316,10 +4170,10 @@
       </c>
     </row>
     <row r="18" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="53" t="s">
+      <c r="A18" s="74" t="s">
         <v>15</v>
       </c>
-      <c r="B18" s="54"/>
+      <c r="B18" s="75"/>
       <c r="C18" s="32"/>
       <c r="D18" s="32">
         <v>13</v>

</xml_diff>

<commit_message>
Academic Exams Controlle modified and migration added
</commit_message>
<xml_diff>
--- a/Resources/Layout.xlsx
+++ b/Resources/Layout.xlsx
@@ -3,21 +3,23 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24332"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBDC43C8-FBB8-4D92-A02F-22618BF9D235}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A097B59-77A0-4530-87F3-4281ACC094A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11280" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15960" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Attendance Report" sheetId="8" r:id="rId2"/>
-    <sheet name="Dashboard" sheetId="2" r:id="rId3"/>
-    <sheet name="Class Routine Teacher" sheetId="6" r:id="rId4"/>
-    <sheet name="Sheet3" sheetId="7" r:id="rId5"/>
-    <sheet name="Student Attendance" sheetId="4" r:id="rId6"/>
-    <sheet name="Employee Attendance" sheetId="5" r:id="rId7"/>
+    <sheet name="Attendance Report daily" sheetId="8" r:id="rId2"/>
+    <sheet name="Attendance Report Monthly Full" sheetId="10" r:id="rId3"/>
+    <sheet name="Dashboard" sheetId="2" r:id="rId4"/>
+    <sheet name="Class Routine Teacher" sheetId="6" r:id="rId5"/>
+    <sheet name="Sheet3" sheetId="7" r:id="rId6"/>
+    <sheet name="Student Attendance" sheetId="4" r:id="rId7"/>
+    <sheet name="Employee Attendance" sheetId="5" r:id="rId8"/>
+    <sheet name="Exam Create" sheetId="9" r:id="rId9"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="5">'Student Attendance'!$A$1:$F$20</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="6">'Student Attendance'!$A$1:$F$20</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="469" uniqueCount="181">
   <si>
     <t>Date</t>
   </si>
@@ -492,6 +494,114 @@
   <si>
     <t>Academic Class : Six</t>
   </si>
+  <si>
+    <t>Exam Name</t>
+  </si>
+  <si>
+    <t>:</t>
+  </si>
+  <si>
+    <t>Academic Session</t>
+  </si>
+  <si>
+    <t>Academic Class</t>
+  </si>
+  <si>
+    <t>Monthly Exam</t>
+  </si>
+  <si>
+    <t>2022-2023</t>
+  </si>
+  <si>
+    <t>Class six</t>
+  </si>
+  <si>
+    <t>Academic Subject</t>
+  </si>
+  <si>
+    <t>Bangla 1st paper</t>
+  </si>
+  <si>
+    <t>Sohel Rana</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Student Name 1</t>
+  </si>
+  <si>
+    <t>Student Name 2</t>
+  </si>
+  <si>
+    <t>Student Name 3</t>
+  </si>
+  <si>
+    <t>Student Name 4</t>
+  </si>
+  <si>
+    <t>Student Name 5</t>
+  </si>
+  <si>
+    <t>Student Name 6</t>
+  </si>
+  <si>
+    <t>Student Name 7</t>
+  </si>
+  <si>
+    <t>Student Name 8</t>
+  </si>
+  <si>
+    <t>Student Name 9</t>
+  </si>
+  <si>
+    <t>Student Name 10</t>
+  </si>
+  <si>
+    <t>Student Name 11</t>
+  </si>
+  <si>
+    <t>Student Name 12</t>
+  </si>
+  <si>
+    <t>Student Name 13</t>
+  </si>
+  <si>
+    <t>Student Name 14</t>
+  </si>
+  <si>
+    <t>Student Name 15</t>
+  </si>
+  <si>
+    <t>Student Name 16</t>
+  </si>
+  <si>
+    <t>Student Name 17</t>
+  </si>
+  <si>
+    <t>Student Name 18</t>
+  </si>
+  <si>
+    <t>Student Name 19</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>Class: Six</t>
+  </si>
+  <si>
+    <t>Month: February 2023</t>
+  </si>
+  <si>
+    <t>Attended(%)</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
 </sst>
 </file>
 
@@ -500,7 +610,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-409]mmmm\ d\,\ yyyy;@"/>
   </numFmts>
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -599,6 +709,58 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF7030A0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF7030A0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="11">
     <fill>
@@ -662,7 +824,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -801,11 +963,87 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="83">
+  <cellXfs count="102">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
@@ -953,6 +1191,21 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -962,21 +1215,6 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1007,9 +1245,63 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -1413,7 +1705,7 @@
   <dimension ref="A1:L15"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+      <selection activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1624,8 +1916,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{524DEAA1-1F57-42FE-8A34-A461C043F698}">
   <dimension ref="A1:I36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:B4"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="K23" sqref="K23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2232,6 +2524,928 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAB53D77-E889-4E1C-BE59-B510214F2C54}">
+  <dimension ref="A1:AE22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AH8" sqref="AH8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="10" width="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="29" width="3" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="12.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A1" s="90" t="s">
+        <v>177</v>
+      </c>
+      <c r="B1" s="91"/>
+      <c r="C1" s="91"/>
+      <c r="D1" s="91"/>
+      <c r="E1" s="91"/>
+      <c r="F1" s="91"/>
+      <c r="G1" s="91"/>
+      <c r="H1" s="91"/>
+      <c r="I1" s="91"/>
+      <c r="J1" s="91"/>
+      <c r="K1" s="91"/>
+      <c r="L1" s="91"/>
+      <c r="M1" s="91"/>
+      <c r="N1" s="91"/>
+      <c r="O1" s="91"/>
+      <c r="P1" s="91"/>
+      <c r="Q1" s="91"/>
+      <c r="R1" s="91"/>
+      <c r="S1" s="91"/>
+      <c r="T1" s="91"/>
+      <c r="U1" s="91"/>
+      <c r="V1" s="91"/>
+      <c r="W1" s="91"/>
+      <c r="X1" s="91"/>
+      <c r="Y1" s="91"/>
+      <c r="Z1" s="91"/>
+      <c r="AA1" s="91"/>
+      <c r="AB1" s="91"/>
+      <c r="AC1" s="91"/>
+      <c r="AD1" s="91"/>
+      <c r="AE1" s="92"/>
+    </row>
+    <row r="2" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="95" t="s">
+        <v>178</v>
+      </c>
+      <c r="B2" s="96"/>
+      <c r="C2" s="96"/>
+      <c r="D2" s="96"/>
+      <c r="E2" s="96"/>
+      <c r="F2" s="96"/>
+      <c r="G2" s="96"/>
+      <c r="H2" s="96"/>
+      <c r="I2" s="96"/>
+      <c r="J2" s="96"/>
+      <c r="K2" s="96"/>
+      <c r="L2" s="96"/>
+      <c r="M2" s="96"/>
+      <c r="N2" s="96"/>
+      <c r="O2" s="96"/>
+      <c r="P2" s="96"/>
+      <c r="Q2" s="96"/>
+      <c r="R2" s="96"/>
+      <c r="S2" s="96"/>
+      <c r="T2" s="93">
+        <v>24</v>
+      </c>
+      <c r="U2" s="93"/>
+      <c r="V2" s="93"/>
+      <c r="W2" s="93"/>
+      <c r="X2" s="93"/>
+      <c r="Y2" s="93"/>
+      <c r="Z2" s="93"/>
+      <c r="AA2" s="93"/>
+      <c r="AB2" s="93"/>
+      <c r="AC2" s="93"/>
+      <c r="AD2" s="93"/>
+      <c r="AE2" s="94"/>
+    </row>
+    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A3" s="88" t="s">
+        <v>155</v>
+      </c>
+      <c r="B3" s="88">
+        <v>1</v>
+      </c>
+      <c r="C3" s="88">
+        <v>2</v>
+      </c>
+      <c r="D3" s="88">
+        <v>3</v>
+      </c>
+      <c r="E3" s="88">
+        <v>4</v>
+      </c>
+      <c r="F3" s="88">
+        <v>5</v>
+      </c>
+      <c r="G3" s="88">
+        <v>6</v>
+      </c>
+      <c r="H3" s="88">
+        <v>7</v>
+      </c>
+      <c r="I3" s="88">
+        <v>8</v>
+      </c>
+      <c r="J3" s="88">
+        <v>9</v>
+      </c>
+      <c r="K3" s="88">
+        <v>10</v>
+      </c>
+      <c r="L3" s="88">
+        <v>11</v>
+      </c>
+      <c r="M3" s="88">
+        <v>12</v>
+      </c>
+      <c r="N3" s="88">
+        <v>13</v>
+      </c>
+      <c r="O3" s="88">
+        <v>14</v>
+      </c>
+      <c r="P3" s="88">
+        <v>15</v>
+      </c>
+      <c r="Q3" s="88">
+        <v>16</v>
+      </c>
+      <c r="R3" s="88">
+        <v>17</v>
+      </c>
+      <c r="S3" s="88">
+        <v>18</v>
+      </c>
+      <c r="T3" s="88">
+        <v>19</v>
+      </c>
+      <c r="U3" s="88">
+        <v>20</v>
+      </c>
+      <c r="V3" s="88">
+        <v>21</v>
+      </c>
+      <c r="W3" s="88">
+        <v>22</v>
+      </c>
+      <c r="X3" s="88">
+        <v>23</v>
+      </c>
+      <c r="Y3" s="88">
+        <v>24</v>
+      </c>
+      <c r="Z3" s="88">
+        <v>25</v>
+      </c>
+      <c r="AA3" s="88">
+        <v>26</v>
+      </c>
+      <c r="AB3" s="88">
+        <v>27</v>
+      </c>
+      <c r="AC3" s="88">
+        <v>28</v>
+      </c>
+      <c r="AD3" s="89" t="s">
+        <v>55</v>
+      </c>
+      <c r="AE3" s="89" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A4" s="87" t="s">
+        <v>156</v>
+      </c>
+      <c r="B4" s="97" t="s">
+        <v>175</v>
+      </c>
+      <c r="C4" s="97" t="s">
+        <v>175</v>
+      </c>
+      <c r="D4" s="98" t="s">
+        <v>180</v>
+      </c>
+      <c r="E4" s="99" t="s">
+        <v>176</v>
+      </c>
+      <c r="F4" s="86" t="s">
+        <v>175</v>
+      </c>
+      <c r="G4" s="86" t="s">
+        <v>175</v>
+      </c>
+      <c r="H4" s="86" t="s">
+        <v>175</v>
+      </c>
+      <c r="I4" s="86" t="s">
+        <v>175</v>
+      </c>
+      <c r="J4" s="86" t="s">
+        <v>175</v>
+      </c>
+      <c r="K4" s="98" t="s">
+        <v>180</v>
+      </c>
+      <c r="L4" s="86" t="s">
+        <v>175</v>
+      </c>
+      <c r="M4" s="86" t="s">
+        <v>175</v>
+      </c>
+      <c r="N4" s="86" t="s">
+        <v>175</v>
+      </c>
+      <c r="O4" s="86" t="s">
+        <v>175</v>
+      </c>
+      <c r="P4" s="86" t="s">
+        <v>175</v>
+      </c>
+      <c r="Q4" s="86" t="s">
+        <v>175</v>
+      </c>
+      <c r="R4" s="100" t="s">
+        <v>180</v>
+      </c>
+      <c r="S4" s="86" t="s">
+        <v>175</v>
+      </c>
+      <c r="T4" s="86" t="s">
+        <v>175</v>
+      </c>
+      <c r="U4" s="86" t="s">
+        <v>175</v>
+      </c>
+      <c r="V4" s="86" t="s">
+        <v>175</v>
+      </c>
+      <c r="W4" s="86" t="s">
+        <v>175</v>
+      </c>
+      <c r="X4" s="86" t="s">
+        <v>175</v>
+      </c>
+      <c r="Y4" s="98" t="s">
+        <v>180</v>
+      </c>
+      <c r="Z4" s="86" t="s">
+        <v>175</v>
+      </c>
+      <c r="AA4" s="86" t="s">
+        <v>175</v>
+      </c>
+      <c r="AB4" s="86" t="s">
+        <v>175</v>
+      </c>
+      <c r="AC4" s="86" t="s">
+        <v>175</v>
+      </c>
+      <c r="AD4" s="86">
+        <v>23</v>
+      </c>
+      <c r="AE4" s="101">
+        <f>(AD4*100/T2)%</f>
+        <v>0.95833333333333326</v>
+      </c>
+    </row>
+    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A5" s="87" t="s">
+        <v>157</v>
+      </c>
+      <c r="B5" s="86"/>
+      <c r="C5" s="86"/>
+      <c r="D5" s="86"/>
+      <c r="E5" s="86"/>
+      <c r="F5" s="86"/>
+      <c r="G5" s="86"/>
+      <c r="H5" s="86"/>
+      <c r="I5" s="86"/>
+      <c r="J5" s="86"/>
+      <c r="K5" s="86"/>
+      <c r="L5" s="86"/>
+      <c r="M5" s="86"/>
+      <c r="N5" s="86"/>
+      <c r="O5" s="86"/>
+      <c r="P5" s="86"/>
+      <c r="Q5" s="86"/>
+      <c r="R5" s="86"/>
+      <c r="S5" s="86"/>
+      <c r="T5" s="86"/>
+      <c r="U5" s="86"/>
+      <c r="V5" s="86"/>
+      <c r="W5" s="86"/>
+      <c r="X5" s="86"/>
+      <c r="Y5" s="86"/>
+      <c r="Z5" s="86"/>
+      <c r="AA5" s="86"/>
+      <c r="AB5" s="86"/>
+      <c r="AC5" s="86"/>
+      <c r="AD5" s="86"/>
+      <c r="AE5" s="86"/>
+    </row>
+    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A6" s="87" t="s">
+        <v>158</v>
+      </c>
+      <c r="B6" s="86"/>
+      <c r="C6" s="86"/>
+      <c r="D6" s="86"/>
+      <c r="E6" s="86"/>
+      <c r="F6" s="86"/>
+      <c r="G6" s="86"/>
+      <c r="H6" s="86"/>
+      <c r="I6" s="86"/>
+      <c r="J6" s="86"/>
+      <c r="K6" s="86"/>
+      <c r="L6" s="86"/>
+      <c r="M6" s="86"/>
+      <c r="N6" s="86"/>
+      <c r="O6" s="86"/>
+      <c r="P6" s="86"/>
+      <c r="Q6" s="86"/>
+      <c r="R6" s="86"/>
+      <c r="S6" s="86"/>
+      <c r="T6" s="86"/>
+      <c r="U6" s="86"/>
+      <c r="V6" s="86"/>
+      <c r="W6" s="86"/>
+      <c r="X6" s="86"/>
+      <c r="Y6" s="86"/>
+      <c r="Z6" s="86"/>
+      <c r="AA6" s="86"/>
+      <c r="AB6" s="86"/>
+      <c r="AC6" s="86"/>
+      <c r="AD6" s="86"/>
+      <c r="AE6" s="86"/>
+    </row>
+    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A7" s="87" t="s">
+        <v>159</v>
+      </c>
+      <c r="B7" s="86"/>
+      <c r="C7" s="86"/>
+      <c r="D7" s="86"/>
+      <c r="E7" s="86"/>
+      <c r="F7" s="86"/>
+      <c r="G7" s="86"/>
+      <c r="H7" s="86"/>
+      <c r="I7" s="86"/>
+      <c r="J7" s="86"/>
+      <c r="K7" s="86"/>
+      <c r="L7" s="86"/>
+      <c r="M7" s="86"/>
+      <c r="N7" s="86"/>
+      <c r="O7" s="86"/>
+      <c r="P7" s="86"/>
+      <c r="Q7" s="86"/>
+      <c r="R7" s="86"/>
+      <c r="S7" s="86"/>
+      <c r="T7" s="86"/>
+      <c r="U7" s="86"/>
+      <c r="V7" s="86"/>
+      <c r="W7" s="86"/>
+      <c r="X7" s="86"/>
+      <c r="Y7" s="86"/>
+      <c r="Z7" s="86"/>
+      <c r="AA7" s="86"/>
+      <c r="AB7" s="86"/>
+      <c r="AC7" s="86"/>
+      <c r="AD7" s="86"/>
+      <c r="AE7" s="86"/>
+    </row>
+    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A8" s="87" t="s">
+        <v>160</v>
+      </c>
+      <c r="B8" s="86"/>
+      <c r="C8" s="86"/>
+      <c r="D8" s="86"/>
+      <c r="E8" s="86"/>
+      <c r="F8" s="86"/>
+      <c r="G8" s="86"/>
+      <c r="H8" s="86"/>
+      <c r="I8" s="86"/>
+      <c r="J8" s="86"/>
+      <c r="K8" s="86"/>
+      <c r="L8" s="86"/>
+      <c r="M8" s="86"/>
+      <c r="N8" s="86"/>
+      <c r="O8" s="86"/>
+      <c r="P8" s="86"/>
+      <c r="Q8" s="86"/>
+      <c r="R8" s="86"/>
+      <c r="S8" s="86"/>
+      <c r="T8" s="86"/>
+      <c r="U8" s="86"/>
+      <c r="V8" s="86"/>
+      <c r="W8" s="86"/>
+      <c r="X8" s="86"/>
+      <c r="Y8" s="86"/>
+      <c r="Z8" s="86"/>
+      <c r="AA8" s="86"/>
+      <c r="AB8" s="86"/>
+      <c r="AC8" s="86"/>
+      <c r="AD8" s="86"/>
+      <c r="AE8" s="86"/>
+    </row>
+    <row r="9" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A9" s="87" t="s">
+        <v>161</v>
+      </c>
+      <c r="B9" s="86"/>
+      <c r="C9" s="86"/>
+      <c r="D9" s="86"/>
+      <c r="E9" s="86"/>
+      <c r="F9" s="86"/>
+      <c r="G9" s="86"/>
+      <c r="H9" s="86"/>
+      <c r="I9" s="86"/>
+      <c r="J9" s="86"/>
+      <c r="K9" s="86"/>
+      <c r="L9" s="86"/>
+      <c r="M9" s="86"/>
+      <c r="N9" s="86"/>
+      <c r="O9" s="86"/>
+      <c r="P9" s="86"/>
+      <c r="Q9" s="86"/>
+      <c r="R9" s="86"/>
+      <c r="S9" s="86"/>
+      <c r="T9" s="86"/>
+      <c r="U9" s="86"/>
+      <c r="V9" s="86"/>
+      <c r="W9" s="86"/>
+      <c r="X9" s="86"/>
+      <c r="Y9" s="86"/>
+      <c r="Z9" s="86"/>
+      <c r="AA9" s="86"/>
+      <c r="AB9" s="86"/>
+      <c r="AC9" s="86"/>
+      <c r="AD9" s="86"/>
+      <c r="AE9" s="86"/>
+    </row>
+    <row r="10" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A10" s="87" t="s">
+        <v>162</v>
+      </c>
+      <c r="B10" s="86"/>
+      <c r="C10" s="86"/>
+      <c r="D10" s="86"/>
+      <c r="E10" s="86"/>
+      <c r="F10" s="86"/>
+      <c r="G10" s="86"/>
+      <c r="H10" s="86"/>
+      <c r="I10" s="86"/>
+      <c r="J10" s="86"/>
+      <c r="K10" s="86"/>
+      <c r="L10" s="86"/>
+      <c r="M10" s="86"/>
+      <c r="N10" s="86"/>
+      <c r="O10" s="86"/>
+      <c r="P10" s="86"/>
+      <c r="Q10" s="86"/>
+      <c r="R10" s="86"/>
+      <c r="S10" s="86"/>
+      <c r="T10" s="86"/>
+      <c r="U10" s="86"/>
+      <c r="V10" s="86"/>
+      <c r="W10" s="86"/>
+      <c r="X10" s="86"/>
+      <c r="Y10" s="86"/>
+      <c r="Z10" s="86"/>
+      <c r="AA10" s="86"/>
+      <c r="AB10" s="86"/>
+      <c r="AC10" s="86"/>
+      <c r="AD10" s="86"/>
+      <c r="AE10" s="86"/>
+    </row>
+    <row r="11" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A11" s="87" t="s">
+        <v>163</v>
+      </c>
+      <c r="B11" s="86"/>
+      <c r="C11" s="86"/>
+      <c r="D11" s="86"/>
+      <c r="E11" s="86"/>
+      <c r="F11" s="86"/>
+      <c r="G11" s="86"/>
+      <c r="H11" s="86"/>
+      <c r="I11" s="86"/>
+      <c r="J11" s="86"/>
+      <c r="K11" s="86"/>
+      <c r="L11" s="86"/>
+      <c r="M11" s="86"/>
+      <c r="N11" s="86"/>
+      <c r="O11" s="86"/>
+      <c r="P11" s="86"/>
+      <c r="Q11" s="86"/>
+      <c r="R11" s="86"/>
+      <c r="S11" s="86"/>
+      <c r="T11" s="86"/>
+      <c r="U11" s="86"/>
+      <c r="V11" s="86"/>
+      <c r="W11" s="86"/>
+      <c r="X11" s="86"/>
+      <c r="Y11" s="86"/>
+      <c r="Z11" s="86"/>
+      <c r="AA11" s="86"/>
+      <c r="AB11" s="86"/>
+      <c r="AC11" s="86"/>
+      <c r="AD11" s="86"/>
+      <c r="AE11" s="86"/>
+    </row>
+    <row r="12" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A12" s="87" t="s">
+        <v>164</v>
+      </c>
+      <c r="B12" s="86"/>
+      <c r="C12" s="86"/>
+      <c r="D12" s="86"/>
+      <c r="E12" s="86"/>
+      <c r="F12" s="86"/>
+      <c r="G12" s="86"/>
+      <c r="H12" s="86"/>
+      <c r="I12" s="86"/>
+      <c r="J12" s="86"/>
+      <c r="K12" s="86"/>
+      <c r="L12" s="86"/>
+      <c r="M12" s="86"/>
+      <c r="N12" s="86"/>
+      <c r="O12" s="86"/>
+      <c r="P12" s="86"/>
+      <c r="Q12" s="86"/>
+      <c r="R12" s="86"/>
+      <c r="S12" s="86"/>
+      <c r="T12" s="86"/>
+      <c r="U12" s="86"/>
+      <c r="V12" s="86"/>
+      <c r="W12" s="86"/>
+      <c r="X12" s="86"/>
+      <c r="Y12" s="86"/>
+      <c r="Z12" s="86"/>
+      <c r="AA12" s="86"/>
+      <c r="AB12" s="86"/>
+      <c r="AC12" s="86"/>
+      <c r="AD12" s="86"/>
+      <c r="AE12" s="86"/>
+    </row>
+    <row r="13" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A13" s="87" t="s">
+        <v>165</v>
+      </c>
+      <c r="B13" s="86"/>
+      <c r="C13" s="86"/>
+      <c r="D13" s="86"/>
+      <c r="E13" s="86"/>
+      <c r="F13" s="86"/>
+      <c r="G13" s="86"/>
+      <c r="H13" s="86"/>
+      <c r="I13" s="86"/>
+      <c r="J13" s="86"/>
+      <c r="K13" s="86"/>
+      <c r="L13" s="86"/>
+      <c r="M13" s="86"/>
+      <c r="N13" s="86"/>
+      <c r="O13" s="86"/>
+      <c r="P13" s="86"/>
+      <c r="Q13" s="86"/>
+      <c r="R13" s="86"/>
+      <c r="S13" s="86"/>
+      <c r="T13" s="86"/>
+      <c r="U13" s="86"/>
+      <c r="V13" s="86"/>
+      <c r="W13" s="86"/>
+      <c r="X13" s="86"/>
+      <c r="Y13" s="86"/>
+      <c r="Z13" s="86"/>
+      <c r="AA13" s="86"/>
+      <c r="AB13" s="86"/>
+      <c r="AC13" s="86"/>
+      <c r="AD13" s="86"/>
+      <c r="AE13" s="86"/>
+    </row>
+    <row r="14" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A14" s="87" t="s">
+        <v>166</v>
+      </c>
+      <c r="B14" s="86"/>
+      <c r="C14" s="86"/>
+      <c r="D14" s="86"/>
+      <c r="E14" s="86"/>
+      <c r="F14" s="86"/>
+      <c r="G14" s="86"/>
+      <c r="H14" s="86"/>
+      <c r="I14" s="86"/>
+      <c r="J14" s="86"/>
+      <c r="K14" s="86"/>
+      <c r="L14" s="86"/>
+      <c r="M14" s="86"/>
+      <c r="N14" s="86"/>
+      <c r="O14" s="86"/>
+      <c r="P14" s="86"/>
+      <c r="Q14" s="86"/>
+      <c r="R14" s="86"/>
+      <c r="S14" s="86"/>
+      <c r="T14" s="86"/>
+      <c r="U14" s="86"/>
+      <c r="V14" s="86"/>
+      <c r="W14" s="86"/>
+      <c r="X14" s="86"/>
+      <c r="Y14" s="86"/>
+      <c r="Z14" s="86"/>
+      <c r="AA14" s="86"/>
+      <c r="AB14" s="86"/>
+      <c r="AC14" s="86"/>
+      <c r="AD14" s="86"/>
+      <c r="AE14" s="86"/>
+    </row>
+    <row r="15" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A15" s="87" t="s">
+        <v>167</v>
+      </c>
+      <c r="B15" s="86"/>
+      <c r="C15" s="86"/>
+      <c r="D15" s="86"/>
+      <c r="E15" s="86"/>
+      <c r="F15" s="86"/>
+      <c r="G15" s="86"/>
+      <c r="H15" s="86"/>
+      <c r="I15" s="86"/>
+      <c r="J15" s="86"/>
+      <c r="K15" s="86"/>
+      <c r="L15" s="86"/>
+      <c r="M15" s="86"/>
+      <c r="N15" s="86"/>
+      <c r="O15" s="86"/>
+      <c r="P15" s="86"/>
+      <c r="Q15" s="86"/>
+      <c r="R15" s="86"/>
+      <c r="S15" s="86"/>
+      <c r="T15" s="86"/>
+      <c r="U15" s="86"/>
+      <c r="V15" s="86"/>
+      <c r="W15" s="86"/>
+      <c r="X15" s="86"/>
+      <c r="Y15" s="86"/>
+      <c r="Z15" s="86"/>
+      <c r="AA15" s="86"/>
+      <c r="AB15" s="86"/>
+      <c r="AC15" s="86"/>
+      <c r="AD15" s="86"/>
+      <c r="AE15" s="86"/>
+    </row>
+    <row r="16" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A16" s="87" t="s">
+        <v>168</v>
+      </c>
+      <c r="B16" s="86"/>
+      <c r="C16" s="86"/>
+      <c r="D16" s="86"/>
+      <c r="E16" s="86"/>
+      <c r="F16" s="86"/>
+      <c r="G16" s="86"/>
+      <c r="H16" s="86"/>
+      <c r="I16" s="86"/>
+      <c r="J16" s="86"/>
+      <c r="K16" s="86"/>
+      <c r="L16" s="86"/>
+      <c r="M16" s="86"/>
+      <c r="N16" s="86"/>
+      <c r="O16" s="86"/>
+      <c r="P16" s="86"/>
+      <c r="Q16" s="86"/>
+      <c r="R16" s="86"/>
+      <c r="S16" s="86"/>
+      <c r="T16" s="86"/>
+      <c r="U16" s="86"/>
+      <c r="V16" s="86"/>
+      <c r="W16" s="86"/>
+      <c r="X16" s="86"/>
+      <c r="Y16" s="86"/>
+      <c r="Z16" s="86"/>
+      <c r="AA16" s="86"/>
+      <c r="AB16" s="86"/>
+      <c r="AC16" s="86"/>
+      <c r="AD16" s="86"/>
+      <c r="AE16" s="86"/>
+    </row>
+    <row r="17" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A17" s="87" t="s">
+        <v>169</v>
+      </c>
+      <c r="B17" s="86"/>
+      <c r="C17" s="86"/>
+      <c r="D17" s="86"/>
+      <c r="E17" s="86"/>
+      <c r="F17" s="86"/>
+      <c r="G17" s="86"/>
+      <c r="H17" s="86"/>
+      <c r="I17" s="86"/>
+      <c r="J17" s="86"/>
+      <c r="K17" s="86"/>
+      <c r="L17" s="86"/>
+      <c r="M17" s="86"/>
+      <c r="N17" s="86"/>
+      <c r="O17" s="86"/>
+      <c r="P17" s="86"/>
+      <c r="Q17" s="86"/>
+      <c r="R17" s="86"/>
+      <c r="S17" s="86"/>
+      <c r="T17" s="86"/>
+      <c r="U17" s="86"/>
+      <c r="V17" s="86"/>
+      <c r="W17" s="86"/>
+      <c r="X17" s="86"/>
+      <c r="Y17" s="86"/>
+      <c r="Z17" s="86"/>
+      <c r="AA17" s="86"/>
+      <c r="AB17" s="86"/>
+      <c r="AC17" s="86"/>
+      <c r="AD17" s="86"/>
+      <c r="AE17" s="86"/>
+    </row>
+    <row r="18" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A18" s="87" t="s">
+        <v>170</v>
+      </c>
+      <c r="B18" s="86"/>
+      <c r="C18" s="86"/>
+      <c r="D18" s="86"/>
+      <c r="E18" s="86"/>
+      <c r="F18" s="86"/>
+      <c r="G18" s="86"/>
+      <c r="H18" s="86"/>
+      <c r="I18" s="86"/>
+      <c r="J18" s="86"/>
+      <c r="K18" s="86"/>
+      <c r="L18" s="86"/>
+      <c r="M18" s="86"/>
+      <c r="N18" s="86"/>
+      <c r="O18" s="86"/>
+      <c r="P18" s="86"/>
+      <c r="Q18" s="86"/>
+      <c r="R18" s="86"/>
+      <c r="S18" s="86"/>
+      <c r="T18" s="86"/>
+      <c r="U18" s="86"/>
+      <c r="V18" s="86"/>
+      <c r="W18" s="86"/>
+      <c r="X18" s="86"/>
+      <c r="Y18" s="86"/>
+      <c r="Z18" s="86"/>
+      <c r="AA18" s="86"/>
+      <c r="AB18" s="86"/>
+      <c r="AC18" s="86"/>
+      <c r="AD18" s="86"/>
+      <c r="AE18" s="86"/>
+    </row>
+    <row r="19" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A19" s="87" t="s">
+        <v>171</v>
+      </c>
+      <c r="B19" s="86"/>
+      <c r="C19" s="86"/>
+      <c r="D19" s="86"/>
+      <c r="E19" s="86"/>
+      <c r="F19" s="86"/>
+      <c r="G19" s="86"/>
+      <c r="H19" s="86"/>
+      <c r="I19" s="86"/>
+      <c r="J19" s="86"/>
+      <c r="K19" s="86"/>
+      <c r="L19" s="86"/>
+      <c r="M19" s="86"/>
+      <c r="N19" s="86"/>
+      <c r="O19" s="86"/>
+      <c r="P19" s="86"/>
+      <c r="Q19" s="86"/>
+      <c r="R19" s="86"/>
+      <c r="S19" s="86"/>
+      <c r="T19" s="86"/>
+      <c r="U19" s="86"/>
+      <c r="V19" s="86"/>
+      <c r="W19" s="86"/>
+      <c r="X19" s="86"/>
+      <c r="Y19" s="86"/>
+      <c r="Z19" s="86"/>
+      <c r="AA19" s="86"/>
+      <c r="AB19" s="86"/>
+      <c r="AC19" s="86"/>
+      <c r="AD19" s="86"/>
+      <c r="AE19" s="86"/>
+    </row>
+    <row r="20" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A20" s="87" t="s">
+        <v>172</v>
+      </c>
+      <c r="B20" s="86"/>
+      <c r="C20" s="86"/>
+      <c r="D20" s="86"/>
+      <c r="E20" s="86"/>
+      <c r="F20" s="86"/>
+      <c r="G20" s="86"/>
+      <c r="H20" s="86"/>
+      <c r="I20" s="86"/>
+      <c r="J20" s="86"/>
+      <c r="K20" s="86"/>
+      <c r="L20" s="86"/>
+      <c r="M20" s="86"/>
+      <c r="N20" s="86"/>
+      <c r="O20" s="86"/>
+      <c r="P20" s="86"/>
+      <c r="Q20" s="86"/>
+      <c r="R20" s="86"/>
+      <c r="S20" s="86"/>
+      <c r="T20" s="86"/>
+      <c r="U20" s="86"/>
+      <c r="V20" s="86"/>
+      <c r="W20" s="86"/>
+      <c r="X20" s="86"/>
+      <c r="Y20" s="86"/>
+      <c r="Z20" s="86"/>
+      <c r="AA20" s="86"/>
+      <c r="AB20" s="86"/>
+      <c r="AC20" s="86"/>
+      <c r="AD20" s="86"/>
+      <c r="AE20" s="86"/>
+    </row>
+    <row r="21" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A21" s="87" t="s">
+        <v>173</v>
+      </c>
+      <c r="B21" s="86"/>
+      <c r="C21" s="86"/>
+      <c r="D21" s="86"/>
+      <c r="E21" s="86"/>
+      <c r="F21" s="86"/>
+      <c r="G21" s="86"/>
+      <c r="H21" s="86"/>
+      <c r="I21" s="86"/>
+      <c r="J21" s="86"/>
+      <c r="K21" s="86"/>
+      <c r="L21" s="86"/>
+      <c r="M21" s="86"/>
+      <c r="N21" s="86"/>
+      <c r="O21" s="86"/>
+      <c r="P21" s="86"/>
+      <c r="Q21" s="86"/>
+      <c r="R21" s="86"/>
+      <c r="S21" s="86"/>
+      <c r="T21" s="86"/>
+      <c r="U21" s="86"/>
+      <c r="V21" s="86"/>
+      <c r="W21" s="86"/>
+      <c r="X21" s="86"/>
+      <c r="Y21" s="86"/>
+      <c r="Z21" s="86"/>
+      <c r="AA21" s="86"/>
+      <c r="AB21" s="86"/>
+      <c r="AC21" s="86"/>
+      <c r="AD21" s="86"/>
+      <c r="AE21" s="86"/>
+    </row>
+    <row r="22" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A22" s="87" t="s">
+        <v>174</v>
+      </c>
+      <c r="B22" s="86"/>
+      <c r="C22" s="86"/>
+      <c r="D22" s="86"/>
+      <c r="E22" s="86"/>
+      <c r="F22" s="86"/>
+      <c r="G22" s="86"/>
+      <c r="H22" s="86"/>
+      <c r="I22" s="86"/>
+      <c r="J22" s="86"/>
+      <c r="K22" s="86"/>
+      <c r="L22" s="86"/>
+      <c r="M22" s="86"/>
+      <c r="N22" s="86"/>
+      <c r="O22" s="86"/>
+      <c r="P22" s="86"/>
+      <c r="Q22" s="86"/>
+      <c r="R22" s="86"/>
+      <c r="S22" s="86"/>
+      <c r="T22" s="86"/>
+      <c r="U22" s="86"/>
+      <c r="V22" s="86"/>
+      <c r="W22" s="86"/>
+      <c r="X22" s="86"/>
+      <c r="Y22" s="86"/>
+      <c r="Z22" s="86"/>
+      <c r="AA22" s="86"/>
+      <c r="AB22" s="86"/>
+      <c r="AC22" s="86"/>
+      <c r="AD22" s="86"/>
+      <c r="AE22" s="86"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A1:AE1"/>
+    <mergeCell ref="A2:S2"/>
+    <mergeCell ref="T2:AE2"/>
+  </mergeCells>
+  <phoneticPr fontId="4" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AC9086E-D004-4EA1-8724-804CD1EEFB7F}">
   <dimension ref="A1:X15"/>
   <sheetViews>
@@ -2324,234 +3538,234 @@
       </c>
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A2" s="70" t="s">
+      <c r="A2" s="67" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="70"/>
-      <c r="C2" s="70"/>
-      <c r="D2" s="70"/>
-      <c r="E2" s="70"/>
-      <c r="F2" s="70"/>
-      <c r="G2" s="70"/>
-      <c r="H2" s="70"/>
-      <c r="I2" s="70"/>
-      <c r="J2" s="70"/>
-      <c r="K2" s="70"/>
-      <c r="L2" s="70"/>
-      <c r="M2" s="66" t="s">
+      <c r="B2" s="67"/>
+      <c r="C2" s="67"/>
+      <c r="D2" s="67"/>
+      <c r="E2" s="67"/>
+      <c r="F2" s="67"/>
+      <c r="G2" s="67"/>
+      <c r="H2" s="67"/>
+      <c r="I2" s="67"/>
+      <c r="J2" s="67"/>
+      <c r="K2" s="67"/>
+      <c r="L2" s="67"/>
+      <c r="M2" s="71" t="s">
         <v>23</v>
       </c>
-      <c r="N2" s="66"/>
-      <c r="O2" s="66"/>
-      <c r="P2" s="66"/>
-      <c r="Q2" s="66"/>
-      <c r="R2" s="66"/>
-      <c r="S2" s="66"/>
-      <c r="T2" s="66"/>
-      <c r="U2" s="66"/>
-      <c r="V2" s="66"/>
-      <c r="W2" s="66"/>
-      <c r="X2" s="66"/>
+      <c r="N2" s="71"/>
+      <c r="O2" s="71"/>
+      <c r="P2" s="71"/>
+      <c r="Q2" s="71"/>
+      <c r="R2" s="71"/>
+      <c r="S2" s="71"/>
+      <c r="T2" s="71"/>
+      <c r="U2" s="71"/>
+      <c r="V2" s="71"/>
+      <c r="W2" s="71"/>
+      <c r="X2" s="71"/>
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3" s="15">
         <v>1</v>
       </c>
-      <c r="B3" s="71" t="s">
+      <c r="B3" s="68" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="71"/>
-      <c r="D3" s="71"/>
+      <c r="C3" s="68"/>
+      <c r="D3" s="68"/>
       <c r="E3" s="16"/>
       <c r="F3" s="16"/>
       <c r="G3" s="16"/>
       <c r="H3" s="16"/>
       <c r="I3" s="16"/>
       <c r="J3" s="16"/>
-      <c r="K3" s="72">
+      <c r="K3" s="69">
         <v>45</v>
       </c>
-      <c r="L3" s="72"/>
+      <c r="L3" s="69"/>
       <c r="M3" s="14">
         <v>1</v>
       </c>
-      <c r="N3" s="67" t="s">
+      <c r="N3" s="72" t="s">
         <v>24</v>
       </c>
-      <c r="O3" s="67"/>
-      <c r="P3" s="67"/>
-      <c r="Q3" s="67"/>
-      <c r="R3" s="67"/>
+      <c r="O3" s="72"/>
+      <c r="P3" s="72"/>
+      <c r="Q3" s="72"/>
+      <c r="R3" s="72"/>
       <c r="S3" s="14">
         <v>6</v>
       </c>
-      <c r="T3" s="65" t="s">
+      <c r="T3" s="70" t="s">
         <v>29</v>
       </c>
-      <c r="U3" s="65"/>
-      <c r="V3" s="65"/>
-      <c r="W3" s="65"/>
-      <c r="X3" s="65"/>
+      <c r="U3" s="70"/>
+      <c r="V3" s="70"/>
+      <c r="W3" s="70"/>
+      <c r="X3" s="70"/>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" s="15">
         <v>2</v>
       </c>
-      <c r="B4" s="71" t="s">
+      <c r="B4" s="68" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="71"/>
-      <c r="D4" s="71"/>
+      <c r="C4" s="68"/>
+      <c r="D4" s="68"/>
       <c r="E4" s="15"/>
       <c r="F4" s="15"/>
       <c r="G4" s="15"/>
       <c r="H4" s="15"/>
       <c r="I4" s="15"/>
       <c r="J4" s="15"/>
-      <c r="K4" s="72">
+      <c r="K4" s="69">
         <v>46</v>
       </c>
-      <c r="L4" s="72"/>
+      <c r="L4" s="69"/>
       <c r="M4" s="14">
         <v>2</v>
       </c>
-      <c r="N4" s="67" t="s">
+      <c r="N4" s="72" t="s">
         <v>25</v>
       </c>
-      <c r="O4" s="67"/>
-      <c r="P4" s="67"/>
-      <c r="Q4" s="67"/>
-      <c r="R4" s="67"/>
+      <c r="O4" s="72"/>
+      <c r="P4" s="72"/>
+      <c r="Q4" s="72"/>
+      <c r="R4" s="72"/>
       <c r="S4" s="14">
         <v>7</v>
       </c>
-      <c r="T4" s="65" t="s">
+      <c r="T4" s="70" t="s">
         <v>29</v>
       </c>
-      <c r="U4" s="65"/>
-      <c r="V4" s="65"/>
-      <c r="W4" s="65"/>
-      <c r="X4" s="65"/>
+      <c r="U4" s="70"/>
+      <c r="V4" s="70"/>
+      <c r="W4" s="70"/>
+      <c r="X4" s="70"/>
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5" s="15">
         <v>3</v>
       </c>
-      <c r="B5" s="68" t="s">
+      <c r="B5" s="65" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="68"/>
-      <c r="D5" s="68"/>
+      <c r="C5" s="65"/>
+      <c r="D5" s="65"/>
       <c r="E5" s="15"/>
       <c r="F5" s="15"/>
       <c r="G5" s="15"/>
       <c r="H5" s="15"/>
       <c r="I5" s="15"/>
       <c r="J5" s="15"/>
-      <c r="K5" s="69">
+      <c r="K5" s="66">
         <v>47</v>
       </c>
-      <c r="L5" s="69"/>
+      <c r="L5" s="66"/>
       <c r="M5" s="14">
         <v>3</v>
       </c>
-      <c r="N5" s="67" t="s">
+      <c r="N5" s="72" t="s">
         <v>26</v>
       </c>
-      <c r="O5" s="67"/>
-      <c r="P5" s="67"/>
-      <c r="Q5" s="67"/>
-      <c r="R5" s="67"/>
+      <c r="O5" s="72"/>
+      <c r="P5" s="72"/>
+      <c r="Q5" s="72"/>
+      <c r="R5" s="72"/>
       <c r="S5" s="14">
         <v>8</v>
       </c>
-      <c r="T5" s="65" t="s">
+      <c r="T5" s="70" t="s">
         <v>29</v>
       </c>
-      <c r="U5" s="65"/>
-      <c r="V5" s="65"/>
-      <c r="W5" s="65"/>
-      <c r="X5" s="65"/>
+      <c r="U5" s="70"/>
+      <c r="V5" s="70"/>
+      <c r="W5" s="70"/>
+      <c r="X5" s="70"/>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6" s="15">
         <v>4</v>
       </c>
-      <c r="B6" s="68" t="s">
+      <c r="B6" s="65" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="68"/>
-      <c r="D6" s="68"/>
+      <c r="C6" s="65"/>
+      <c r="D6" s="65"/>
       <c r="E6" s="15"/>
       <c r="F6" s="15"/>
       <c r="G6" s="15"/>
       <c r="H6" s="15"/>
       <c r="I6" s="15"/>
       <c r="J6" s="15"/>
-      <c r="K6" s="69">
+      <c r="K6" s="66">
         <v>48</v>
       </c>
-      <c r="L6" s="69"/>
+      <c r="L6" s="66"/>
       <c r="M6" s="14">
         <v>4</v>
       </c>
-      <c r="N6" s="67" t="s">
+      <c r="N6" s="72" t="s">
         <v>27</v>
       </c>
-      <c r="O6" s="67"/>
-      <c r="P6" s="67"/>
-      <c r="Q6" s="67"/>
-      <c r="R6" s="67"/>
+      <c r="O6" s="72"/>
+      <c r="P6" s="72"/>
+      <c r="Q6" s="72"/>
+      <c r="R6" s="72"/>
       <c r="S6" s="14">
         <v>9</v>
       </c>
-      <c r="T6" s="65" t="s">
+      <c r="T6" s="70" t="s">
         <v>29</v>
       </c>
-      <c r="U6" s="65"/>
-      <c r="V6" s="65"/>
-      <c r="W6" s="65"/>
-      <c r="X6" s="65"/>
+      <c r="U6" s="70"/>
+      <c r="V6" s="70"/>
+      <c r="W6" s="70"/>
+      <c r="X6" s="70"/>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7" s="15">
         <v>5</v>
       </c>
-      <c r="B7" s="68" t="s">
+      <c r="B7" s="65" t="s">
         <v>22</v>
       </c>
-      <c r="C7" s="68"/>
-      <c r="D7" s="68"/>
+      <c r="C7" s="65"/>
+      <c r="D7" s="65"/>
       <c r="E7" s="15"/>
       <c r="F7" s="15"/>
       <c r="G7" s="15"/>
       <c r="H7" s="15"/>
       <c r="I7" s="15"/>
       <c r="J7" s="15"/>
-      <c r="K7" s="69">
+      <c r="K7" s="66">
         <v>49</v>
       </c>
-      <c r="L7" s="69"/>
+      <c r="L7" s="66"/>
       <c r="M7" s="14">
         <v>5</v>
       </c>
-      <c r="N7" s="67" t="s">
+      <c r="N7" s="72" t="s">
         <v>28</v>
       </c>
-      <c r="O7" s="67"/>
-      <c r="P7" s="67"/>
-      <c r="Q7" s="67"/>
-      <c r="R7" s="67"/>
+      <c r="O7" s="72"/>
+      <c r="P7" s="72"/>
+      <c r="Q7" s="72"/>
+      <c r="R7" s="72"/>
       <c r="S7" s="14">
         <v>10</v>
       </c>
-      <c r="T7" s="65" t="s">
+      <c r="T7" s="70" t="s">
         <v>29</v>
       </c>
-      <c r="U7" s="65"/>
-      <c r="V7" s="65"/>
-      <c r="W7" s="65"/>
-      <c r="X7" s="65"/>
+      <c r="U7" s="70"/>
+      <c r="V7" s="70"/>
+      <c r="W7" s="70"/>
+      <c r="X7" s="70"/>
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A8" s="13"/>
@@ -2763,6 +3977,17 @@
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="T7:X7"/>
+    <mergeCell ref="M2:X2"/>
+    <mergeCell ref="N3:R3"/>
+    <mergeCell ref="N4:R4"/>
+    <mergeCell ref="N5:R5"/>
+    <mergeCell ref="N6:R6"/>
+    <mergeCell ref="N7:R7"/>
+    <mergeCell ref="T3:X3"/>
+    <mergeCell ref="T4:X4"/>
+    <mergeCell ref="T5:X5"/>
+    <mergeCell ref="T6:X6"/>
     <mergeCell ref="B6:D6"/>
     <mergeCell ref="K6:L6"/>
     <mergeCell ref="B7:D7"/>
@@ -2774,24 +3999,13 @@
     <mergeCell ref="K4:L4"/>
     <mergeCell ref="B5:D5"/>
     <mergeCell ref="K5:L5"/>
-    <mergeCell ref="T7:X7"/>
-    <mergeCell ref="M2:X2"/>
-    <mergeCell ref="N3:R3"/>
-    <mergeCell ref="N4:R4"/>
-    <mergeCell ref="N5:R5"/>
-    <mergeCell ref="N6:R6"/>
-    <mergeCell ref="N7:R7"/>
-    <mergeCell ref="T3:X3"/>
-    <mergeCell ref="T4:X4"/>
-    <mergeCell ref="T5:X5"/>
-    <mergeCell ref="T6:X6"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{889D0D57-1F26-473E-B306-F0F5D3A5E8AC}">
   <dimension ref="A1:I2"/>
   <sheetViews>
@@ -2858,7 +4072,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B9CA3B1-EDA9-4D32-B2CA-E8D9C6600DDC}">
   <dimension ref="A1:J31"/>
   <sheetViews>
@@ -3503,7 +4717,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68C7AB11-C29A-4F36-8877-185A21672CFE}">
   <dimension ref="A1:F20"/>
   <sheetViews>
@@ -3842,7 +5056,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE752E1A-3511-482B-9D5B-C641C60E9654}">
   <dimension ref="A1:G18"/>
   <sheetViews>
@@ -4200,4 +5414,80 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C002464B-D256-4EB5-A012-8EB2C2D144F6}">
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="1.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="83" t="s">
+        <v>145</v>
+      </c>
+      <c r="B1" s="84" t="s">
+        <v>146</v>
+      </c>
+      <c r="C1" s="85" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="83" t="s">
+        <v>147</v>
+      </c>
+      <c r="B2" s="84" t="s">
+        <v>146</v>
+      </c>
+      <c r="C2" s="85" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="83" t="s">
+        <v>148</v>
+      </c>
+      <c r="B3" s="84" t="s">
+        <v>146</v>
+      </c>
+      <c r="C3" s="85" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="83" t="s">
+        <v>152</v>
+      </c>
+      <c r="B4" s="84" t="s">
+        <v>146</v>
+      </c>
+      <c r="C4" s="85" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="83" t="s">
+        <v>81</v>
+      </c>
+      <c r="B5" s="84" t="s">
+        <v>146</v>
+      </c>
+      <c r="C5" s="85" t="s">
+        <v>154</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Offday type index and create page created and migration added successfully
</commit_message>
<xml_diff>
--- a/Resources/Layout.xlsx
+++ b/Resources/Layout.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24332"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A097B59-77A0-4530-87F3-4281ACC094A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81D82C1D-1DFC-4B12-B2F8-34D36D79A82D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15960" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1950" yWindow="1950" windowWidth="21600" windowHeight="11475" firstSheet="5" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -17,6 +17,7 @@
     <sheet name="Student Attendance" sheetId="4" r:id="rId7"/>
     <sheet name="Employee Attendance" sheetId="5" r:id="rId8"/>
     <sheet name="Exam Create" sheetId="9" r:id="rId9"/>
+    <sheet name="OffDays" sheetId="11" r:id="rId10"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="6">'Student Attendance'!$A$1:$F$20</definedName>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="469" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="473" uniqueCount="184">
   <si>
     <t>Date</t>
   </si>
@@ -601,6 +602,15 @@
   </si>
   <si>
     <t>X</t>
+  </si>
+  <si>
+    <t>Id</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>OffDay Type</t>
   </si>
 </sst>
 </file>
@@ -1158,93 +1168,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1262,6 +1185,54 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1271,32 +1242,71 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1755,28 +1765,28 @@
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="54" t="s">
+      <c r="A2" s="66" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="54"/>
-      <c r="C2" s="55" t="s">
+      <c r="B2" s="66"/>
+      <c r="C2" s="67" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="55"/>
-      <c r="E2" s="55"/>
+      <c r="D2" s="67"/>
+      <c r="E2" s="67"/>
       <c r="F2" s="12"/>
     </row>
     <row r="3" spans="1:12" s="8" customFormat="1" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F3" s="9"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="54" t="s">
+      <c r="A4" s="66" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="54"/>
-      <c r="C4" s="56"/>
-      <c r="D4" s="56"/>
-      <c r="E4" s="56"/>
+      <c r="B4" s="66"/>
+      <c r="C4" s="68"/>
+      <c r="D4" s="68"/>
+      <c r="E4" s="68"/>
       <c r="F4" s="7" t="s">
         <v>15</v>
       </c>
@@ -1791,12 +1801,12 @@
       <c r="F5" s="7"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="59" t="s">
+      <c r="A6" s="71" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="59"/>
-      <c r="C6" s="58"/>
-      <c r="D6" s="58"/>
+      <c r="B6" s="71"/>
+      <c r="C6" s="70"/>
+      <c r="D6" s="70"/>
       <c r="E6" s="11"/>
       <c r="F6" s="7" t="s">
         <v>16</v>
@@ -1806,12 +1816,12 @@
       <c r="F7" s="9"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="59" t="s">
+      <c r="A8" s="71" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="59"/>
-      <c r="C8" s="58"/>
-      <c r="D8" s="58"/>
+      <c r="B8" s="71"/>
+      <c r="C8" s="70"/>
+      <c r="D8" s="70"/>
       <c r="E8" s="10" t="s">
         <v>14</v>
       </c>
@@ -1820,13 +1830,13 @@
       <c r="F9" s="9"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="57" t="s">
+      <c r="A10" s="69" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="57"/>
-      <c r="C10" s="58"/>
-      <c r="D10" s="58"/>
-      <c r="E10" s="58"/>
+      <c r="B10" s="69"/>
+      <c r="C10" s="70"/>
+      <c r="D10" s="70"/>
+      <c r="E10" s="70"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
@@ -1909,6 +1919,40 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{057F0B6F-9818-44F5-AA5B-A10992AB9C3A}">
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="2.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="11.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>181</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>183</v>
+      </c>
+      <c r="D1" t="s">
+        <v>182</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -1931,44 +1975,44 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="60" t="s">
+      <c r="A1" s="72" t="s">
         <v>134</v>
       </c>
-      <c r="B1" s="61"/>
-      <c r="C1" s="61"/>
-      <c r="D1" s="61"/>
-      <c r="E1" s="61"/>
-      <c r="F1" s="61"/>
+      <c r="B1" s="73"/>
+      <c r="C1" s="73"/>
+      <c r="D1" s="73"/>
+      <c r="E1" s="73"/>
+      <c r="F1" s="73"/>
     </row>
     <row r="2" spans="1:9" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="61"/>
-      <c r="B2" s="61"/>
-      <c r="C2" s="61"/>
-      <c r="D2" s="61"/>
-      <c r="E2" s="61"/>
-      <c r="F2" s="61"/>
+      <c r="A2" s="73"/>
+      <c r="B2" s="73"/>
+      <c r="C2" s="73"/>
+      <c r="D2" s="73"/>
+      <c r="E2" s="73"/>
+      <c r="F2" s="73"/>
     </row>
     <row r="3" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="62" t="s">
+      <c r="A3" s="74" t="s">
         <v>133</v>
       </c>
-      <c r="B3" s="62"/>
-      <c r="C3" s="62"/>
-      <c r="D3" s="62"/>
-      <c r="E3" s="62"/>
-      <c r="F3" s="62"/>
+      <c r="B3" s="74"/>
+      <c r="C3" s="74"/>
+      <c r="D3" s="74"/>
+      <c r="E3" s="74"/>
+      <c r="F3" s="74"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="63" t="s">
+      <c r="A4" s="75" t="s">
         <v>144</v>
       </c>
-      <c r="B4" s="63"/>
+      <c r="B4" s="75"/>
       <c r="C4" s="51"/>
       <c r="D4" s="51"/>
-      <c r="E4" s="64" t="s">
+      <c r="E4" s="76" t="s">
         <v>114</v>
       </c>
-      <c r="F4" s="64"/>
+      <c r="F4" s="76"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="43" t="s">
@@ -2527,8 +2571,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAB53D77-E889-4E1C-BE59-B510214F2C54}">
   <dimension ref="A1:AE22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AH8" sqref="AH8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="AG10" sqref="AG10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2541,897 +2585,897 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A1" s="90" t="s">
+      <c r="A1" s="77" t="s">
         <v>177</v>
       </c>
-      <c r="B1" s="91"/>
-      <c r="C1" s="91"/>
-      <c r="D1" s="91"/>
-      <c r="E1" s="91"/>
-      <c r="F1" s="91"/>
-      <c r="G1" s="91"/>
-      <c r="H1" s="91"/>
-      <c r="I1" s="91"/>
-      <c r="J1" s="91"/>
-      <c r="K1" s="91"/>
-      <c r="L1" s="91"/>
-      <c r="M1" s="91"/>
-      <c r="N1" s="91"/>
-      <c r="O1" s="91"/>
-      <c r="P1" s="91"/>
-      <c r="Q1" s="91"/>
-      <c r="R1" s="91"/>
-      <c r="S1" s="91"/>
-      <c r="T1" s="91"/>
-      <c r="U1" s="91"/>
-      <c r="V1" s="91"/>
-      <c r="W1" s="91"/>
-      <c r="X1" s="91"/>
-      <c r="Y1" s="91"/>
-      <c r="Z1" s="91"/>
-      <c r="AA1" s="91"/>
-      <c r="AB1" s="91"/>
-      <c r="AC1" s="91"/>
-      <c r="AD1" s="91"/>
-      <c r="AE1" s="92"/>
+      <c r="B1" s="78"/>
+      <c r="C1" s="78"/>
+      <c r="D1" s="78"/>
+      <c r="E1" s="78"/>
+      <c r="F1" s="78"/>
+      <c r="G1" s="78"/>
+      <c r="H1" s="78"/>
+      <c r="I1" s="78"/>
+      <c r="J1" s="78"/>
+      <c r="K1" s="78"/>
+      <c r="L1" s="78"/>
+      <c r="M1" s="78"/>
+      <c r="N1" s="78"/>
+      <c r="O1" s="78"/>
+      <c r="P1" s="78"/>
+      <c r="Q1" s="78"/>
+      <c r="R1" s="78"/>
+      <c r="S1" s="78"/>
+      <c r="T1" s="78"/>
+      <c r="U1" s="78"/>
+      <c r="V1" s="78"/>
+      <c r="W1" s="78"/>
+      <c r="X1" s="78"/>
+      <c r="Y1" s="78"/>
+      <c r="Z1" s="78"/>
+      <c r="AA1" s="78"/>
+      <c r="AB1" s="78"/>
+      <c r="AC1" s="78"/>
+      <c r="AD1" s="78"/>
+      <c r="AE1" s="79"/>
     </row>
     <row r="2" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="95" t="s">
+      <c r="A2" s="80" t="s">
         <v>178</v>
       </c>
-      <c r="B2" s="96"/>
-      <c r="C2" s="96"/>
-      <c r="D2" s="96"/>
-      <c r="E2" s="96"/>
-      <c r="F2" s="96"/>
-      <c r="G2" s="96"/>
-      <c r="H2" s="96"/>
-      <c r="I2" s="96"/>
-      <c r="J2" s="96"/>
-      <c r="K2" s="96"/>
-      <c r="L2" s="96"/>
-      <c r="M2" s="96"/>
-      <c r="N2" s="96"/>
-      <c r="O2" s="96"/>
-      <c r="P2" s="96"/>
-      <c r="Q2" s="96"/>
-      <c r="R2" s="96"/>
-      <c r="S2" s="96"/>
-      <c r="T2" s="93">
+      <c r="B2" s="81"/>
+      <c r="C2" s="81"/>
+      <c r="D2" s="81"/>
+      <c r="E2" s="81"/>
+      <c r="F2" s="81"/>
+      <c r="G2" s="81"/>
+      <c r="H2" s="81"/>
+      <c r="I2" s="81"/>
+      <c r="J2" s="81"/>
+      <c r="K2" s="81"/>
+      <c r="L2" s="81"/>
+      <c r="M2" s="81"/>
+      <c r="N2" s="81"/>
+      <c r="O2" s="81"/>
+      <c r="P2" s="81"/>
+      <c r="Q2" s="81"/>
+      <c r="R2" s="81"/>
+      <c r="S2" s="81"/>
+      <c r="T2" s="82">
         <v>24</v>
       </c>
-      <c r="U2" s="93"/>
-      <c r="V2" s="93"/>
-      <c r="W2" s="93"/>
-      <c r="X2" s="93"/>
-      <c r="Y2" s="93"/>
-      <c r="Z2" s="93"/>
-      <c r="AA2" s="93"/>
-      <c r="AB2" s="93"/>
-      <c r="AC2" s="93"/>
-      <c r="AD2" s="93"/>
-      <c r="AE2" s="94"/>
+      <c r="U2" s="82"/>
+      <c r="V2" s="82"/>
+      <c r="W2" s="82"/>
+      <c r="X2" s="82"/>
+      <c r="Y2" s="82"/>
+      <c r="Z2" s="82"/>
+      <c r="AA2" s="82"/>
+      <c r="AB2" s="82"/>
+      <c r="AC2" s="82"/>
+      <c r="AD2" s="82"/>
+      <c r="AE2" s="83"/>
     </row>
     <row r="3" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A3" s="88" t="s">
+      <c r="A3" s="59" t="s">
         <v>155</v>
       </c>
-      <c r="B3" s="88">
+      <c r="B3" s="59">
         <v>1</v>
       </c>
-      <c r="C3" s="88">
+      <c r="C3" s="59">
         <v>2</v>
       </c>
-      <c r="D3" s="88">
+      <c r="D3" s="59">
         <v>3</v>
       </c>
-      <c r="E3" s="88">
+      <c r="E3" s="59">
         <v>4</v>
       </c>
-      <c r="F3" s="88">
+      <c r="F3" s="59">
         <v>5</v>
       </c>
-      <c r="G3" s="88">
+      <c r="G3" s="59">
         <v>6</v>
       </c>
-      <c r="H3" s="88">
+      <c r="H3" s="59">
         <v>7</v>
       </c>
-      <c r="I3" s="88">
+      <c r="I3" s="59">
         <v>8</v>
       </c>
-      <c r="J3" s="88">
+      <c r="J3" s="59">
         <v>9</v>
       </c>
-      <c r="K3" s="88">
+      <c r="K3" s="59">
         <v>10</v>
       </c>
-      <c r="L3" s="88">
+      <c r="L3" s="59">
         <v>11</v>
       </c>
-      <c r="M3" s="88">
+      <c r="M3" s="59">
         <v>12</v>
       </c>
-      <c r="N3" s="88">
+      <c r="N3" s="59">
         <v>13</v>
       </c>
-      <c r="O3" s="88">
+      <c r="O3" s="59">
         <v>14</v>
       </c>
-      <c r="P3" s="88">
+      <c r="P3" s="59">
         <v>15</v>
       </c>
-      <c r="Q3" s="88">
+      <c r="Q3" s="59">
         <v>16</v>
       </c>
-      <c r="R3" s="88">
+      <c r="R3" s="59">
         <v>17</v>
       </c>
-      <c r="S3" s="88">
+      <c r="S3" s="59">
         <v>18</v>
       </c>
-      <c r="T3" s="88">
+      <c r="T3" s="59">
         <v>19</v>
       </c>
-      <c r="U3" s="88">
+      <c r="U3" s="59">
         <v>20</v>
       </c>
-      <c r="V3" s="88">
+      <c r="V3" s="59">
         <v>21</v>
       </c>
-      <c r="W3" s="88">
+      <c r="W3" s="59">
         <v>22</v>
       </c>
-      <c r="X3" s="88">
+      <c r="X3" s="59">
         <v>23</v>
       </c>
-      <c r="Y3" s="88">
+      <c r="Y3" s="59">
         <v>24</v>
       </c>
-      <c r="Z3" s="88">
+      <c r="Z3" s="59">
         <v>25</v>
       </c>
-      <c r="AA3" s="88">
+      <c r="AA3" s="59">
         <v>26</v>
       </c>
-      <c r="AB3" s="88">
+      <c r="AB3" s="59">
         <v>27</v>
       </c>
-      <c r="AC3" s="88">
+      <c r="AC3" s="59">
         <v>28</v>
       </c>
-      <c r="AD3" s="89" t="s">
+      <c r="AD3" s="60" t="s">
         <v>55</v>
       </c>
-      <c r="AE3" s="89" t="s">
+      <c r="AE3" s="60" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="4" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A4" s="87" t="s">
+      <c r="A4" s="58" t="s">
         <v>156</v>
       </c>
-      <c r="B4" s="97" t="s">
+      <c r="B4" s="61" t="s">
         <v>175</v>
       </c>
-      <c r="C4" s="97" t="s">
+      <c r="C4" s="61" t="s">
         <v>175</v>
       </c>
-      <c r="D4" s="98" t="s">
+      <c r="D4" s="62" t="s">
         <v>180</v>
       </c>
-      <c r="E4" s="99" t="s">
+      <c r="E4" s="63" t="s">
         <v>176</v>
       </c>
-      <c r="F4" s="86" t="s">
+      <c r="F4" s="57" t="s">
         <v>175</v>
       </c>
-      <c r="G4" s="86" t="s">
+      <c r="G4" s="57" t="s">
         <v>175</v>
       </c>
-      <c r="H4" s="86" t="s">
+      <c r="H4" s="57" t="s">
         <v>175</v>
       </c>
-      <c r="I4" s="86" t="s">
+      <c r="I4" s="57" t="s">
         <v>175</v>
       </c>
-      <c r="J4" s="86" t="s">
+      <c r="J4" s="57" t="s">
         <v>175</v>
       </c>
-      <c r="K4" s="98" t="s">
+      <c r="K4" s="62" t="s">
         <v>180</v>
       </c>
-      <c r="L4" s="86" t="s">
+      <c r="L4" s="57" t="s">
         <v>175</v>
       </c>
-      <c r="M4" s="86" t="s">
+      <c r="M4" s="57" t="s">
         <v>175</v>
       </c>
-      <c r="N4" s="86" t="s">
+      <c r="N4" s="57" t="s">
         <v>175</v>
       </c>
-      <c r="O4" s="86" t="s">
+      <c r="O4" s="57" t="s">
         <v>175</v>
       </c>
-      <c r="P4" s="86" t="s">
+      <c r="P4" s="57" t="s">
         <v>175</v>
       </c>
-      <c r="Q4" s="86" t="s">
+      <c r="Q4" s="57" t="s">
         <v>175</v>
       </c>
-      <c r="R4" s="100" t="s">
+      <c r="R4" s="64" t="s">
         <v>180</v>
       </c>
-      <c r="S4" s="86" t="s">
+      <c r="S4" s="57" t="s">
         <v>175</v>
       </c>
-      <c r="T4" s="86" t="s">
+      <c r="T4" s="57" t="s">
         <v>175</v>
       </c>
-      <c r="U4" s="86" t="s">
+      <c r="U4" s="57" t="s">
         <v>175</v>
       </c>
-      <c r="V4" s="86" t="s">
+      <c r="V4" s="57" t="s">
         <v>175</v>
       </c>
-      <c r="W4" s="86" t="s">
+      <c r="W4" s="57" t="s">
         <v>175</v>
       </c>
-      <c r="X4" s="86" t="s">
+      <c r="X4" s="57" t="s">
         <v>175</v>
       </c>
-      <c r="Y4" s="98" t="s">
+      <c r="Y4" s="62" t="s">
         <v>180</v>
       </c>
-      <c r="Z4" s="86" t="s">
+      <c r="Z4" s="57" t="s">
         <v>175</v>
       </c>
-      <c r="AA4" s="86" t="s">
+      <c r="AA4" s="57" t="s">
         <v>175</v>
       </c>
-      <c r="AB4" s="86" t="s">
+      <c r="AB4" s="57" t="s">
         <v>175</v>
       </c>
-      <c r="AC4" s="86" t="s">
+      <c r="AC4" s="57" t="s">
         <v>175</v>
       </c>
-      <c r="AD4" s="86">
+      <c r="AD4" s="57">
         <v>23</v>
       </c>
-      <c r="AE4" s="101">
+      <c r="AE4" s="65">
         <f>(AD4*100/T2)%</f>
         <v>0.95833333333333326</v>
       </c>
     </row>
     <row r="5" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A5" s="87" t="s">
+      <c r="A5" s="58" t="s">
         <v>157</v>
       </c>
-      <c r="B5" s="86"/>
-      <c r="C5" s="86"/>
-      <c r="D5" s="86"/>
-      <c r="E5" s="86"/>
-      <c r="F5" s="86"/>
-      <c r="G5" s="86"/>
-      <c r="H5" s="86"/>
-      <c r="I5" s="86"/>
-      <c r="J5" s="86"/>
-      <c r="K5" s="86"/>
-      <c r="L5" s="86"/>
-      <c r="M5" s="86"/>
-      <c r="N5" s="86"/>
-      <c r="O5" s="86"/>
-      <c r="P5" s="86"/>
-      <c r="Q5" s="86"/>
-      <c r="R5" s="86"/>
-      <c r="S5" s="86"/>
-      <c r="T5" s="86"/>
-      <c r="U5" s="86"/>
-      <c r="V5" s="86"/>
-      <c r="W5" s="86"/>
-      <c r="X5" s="86"/>
-      <c r="Y5" s="86"/>
-      <c r="Z5" s="86"/>
-      <c r="AA5" s="86"/>
-      <c r="AB5" s="86"/>
-      <c r="AC5" s="86"/>
-      <c r="AD5" s="86"/>
-      <c r="AE5" s="86"/>
+      <c r="B5" s="57"/>
+      <c r="C5" s="57"/>
+      <c r="D5" s="57"/>
+      <c r="E5" s="57"/>
+      <c r="F5" s="57"/>
+      <c r="G5" s="57"/>
+      <c r="H5" s="57"/>
+      <c r="I5" s="57"/>
+      <c r="J5" s="57"/>
+      <c r="K5" s="57"/>
+      <c r="L5" s="57"/>
+      <c r="M5" s="57"/>
+      <c r="N5" s="57"/>
+      <c r="O5" s="57"/>
+      <c r="P5" s="57"/>
+      <c r="Q5" s="57"/>
+      <c r="R5" s="57"/>
+      <c r="S5" s="57"/>
+      <c r="T5" s="57"/>
+      <c r="U5" s="57"/>
+      <c r="V5" s="57"/>
+      <c r="W5" s="57"/>
+      <c r="X5" s="57"/>
+      <c r="Y5" s="57"/>
+      <c r="Z5" s="57"/>
+      <c r="AA5" s="57"/>
+      <c r="AB5" s="57"/>
+      <c r="AC5" s="57"/>
+      <c r="AD5" s="57"/>
+      <c r="AE5" s="57"/>
     </row>
     <row r="6" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A6" s="87" t="s">
+      <c r="A6" s="58" t="s">
         <v>158</v>
       </c>
-      <c r="B6" s="86"/>
-      <c r="C6" s="86"/>
-      <c r="D6" s="86"/>
-      <c r="E6" s="86"/>
-      <c r="F6" s="86"/>
-      <c r="G6" s="86"/>
-      <c r="H6" s="86"/>
-      <c r="I6" s="86"/>
-      <c r="J6" s="86"/>
-      <c r="K6" s="86"/>
-      <c r="L6" s="86"/>
-      <c r="M6" s="86"/>
-      <c r="N6" s="86"/>
-      <c r="O6" s="86"/>
-      <c r="P6" s="86"/>
-      <c r="Q6" s="86"/>
-      <c r="R6" s="86"/>
-      <c r="S6" s="86"/>
-      <c r="T6" s="86"/>
-      <c r="U6" s="86"/>
-      <c r="V6" s="86"/>
-      <c r="W6" s="86"/>
-      <c r="X6" s="86"/>
-      <c r="Y6" s="86"/>
-      <c r="Z6" s="86"/>
-      <c r="AA6" s="86"/>
-      <c r="AB6" s="86"/>
-      <c r="AC6" s="86"/>
-      <c r="AD6" s="86"/>
-      <c r="AE6" s="86"/>
+      <c r="B6" s="57"/>
+      <c r="C6" s="57"/>
+      <c r="D6" s="57"/>
+      <c r="E6" s="57"/>
+      <c r="F6" s="57"/>
+      <c r="G6" s="57"/>
+      <c r="H6" s="57"/>
+      <c r="I6" s="57"/>
+      <c r="J6" s="57"/>
+      <c r="K6" s="57"/>
+      <c r="L6" s="57"/>
+      <c r="M6" s="57"/>
+      <c r="N6" s="57"/>
+      <c r="O6" s="57"/>
+      <c r="P6" s="57"/>
+      <c r="Q6" s="57"/>
+      <c r="R6" s="57"/>
+      <c r="S6" s="57"/>
+      <c r="T6" s="57"/>
+      <c r="U6" s="57"/>
+      <c r="V6" s="57"/>
+      <c r="W6" s="57"/>
+      <c r="X6" s="57"/>
+      <c r="Y6" s="57"/>
+      <c r="Z6" s="57"/>
+      <c r="AA6" s="57"/>
+      <c r="AB6" s="57"/>
+      <c r="AC6" s="57"/>
+      <c r="AD6" s="57"/>
+      <c r="AE6" s="57"/>
     </row>
     <row r="7" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A7" s="87" t="s">
+      <c r="A7" s="58" t="s">
         <v>159</v>
       </c>
-      <c r="B7" s="86"/>
-      <c r="C7" s="86"/>
-      <c r="D7" s="86"/>
-      <c r="E7" s="86"/>
-      <c r="F7" s="86"/>
-      <c r="G7" s="86"/>
-      <c r="H7" s="86"/>
-      <c r="I7" s="86"/>
-      <c r="J7" s="86"/>
-      <c r="K7" s="86"/>
-      <c r="L7" s="86"/>
-      <c r="M7" s="86"/>
-      <c r="N7" s="86"/>
-      <c r="O7" s="86"/>
-      <c r="P7" s="86"/>
-      <c r="Q7" s="86"/>
-      <c r="R7" s="86"/>
-      <c r="S7" s="86"/>
-      <c r="T7" s="86"/>
-      <c r="U7" s="86"/>
-      <c r="V7" s="86"/>
-      <c r="W7" s="86"/>
-      <c r="X7" s="86"/>
-      <c r="Y7" s="86"/>
-      <c r="Z7" s="86"/>
-      <c r="AA7" s="86"/>
-      <c r="AB7" s="86"/>
-      <c r="AC7" s="86"/>
-      <c r="AD7" s="86"/>
-      <c r="AE7" s="86"/>
+      <c r="B7" s="57"/>
+      <c r="C7" s="57"/>
+      <c r="D7" s="57"/>
+      <c r="E7" s="57"/>
+      <c r="F7" s="57"/>
+      <c r="G7" s="57"/>
+      <c r="H7" s="57"/>
+      <c r="I7" s="57"/>
+      <c r="J7" s="57"/>
+      <c r="K7" s="57"/>
+      <c r="L7" s="57"/>
+      <c r="M7" s="57"/>
+      <c r="N7" s="57"/>
+      <c r="O7" s="57"/>
+      <c r="P7" s="57"/>
+      <c r="Q7" s="57"/>
+      <c r="R7" s="57"/>
+      <c r="S7" s="57"/>
+      <c r="T7" s="57"/>
+      <c r="U7" s="57"/>
+      <c r="V7" s="57"/>
+      <c r="W7" s="57"/>
+      <c r="X7" s="57"/>
+      <c r="Y7" s="57"/>
+      <c r="Z7" s="57"/>
+      <c r="AA7" s="57"/>
+      <c r="AB7" s="57"/>
+      <c r="AC7" s="57"/>
+      <c r="AD7" s="57"/>
+      <c r="AE7" s="57"/>
     </row>
     <row r="8" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A8" s="87" t="s">
+      <c r="A8" s="58" t="s">
         <v>160</v>
       </c>
-      <c r="B8" s="86"/>
-      <c r="C8" s="86"/>
-      <c r="D8" s="86"/>
-      <c r="E8" s="86"/>
-      <c r="F8" s="86"/>
-      <c r="G8" s="86"/>
-      <c r="H8" s="86"/>
-      <c r="I8" s="86"/>
-      <c r="J8" s="86"/>
-      <c r="K8" s="86"/>
-      <c r="L8" s="86"/>
-      <c r="M8" s="86"/>
-      <c r="N8" s="86"/>
-      <c r="O8" s="86"/>
-      <c r="P8" s="86"/>
-      <c r="Q8" s="86"/>
-      <c r="R8" s="86"/>
-      <c r="S8" s="86"/>
-      <c r="T8" s="86"/>
-      <c r="U8" s="86"/>
-      <c r="V8" s="86"/>
-      <c r="W8" s="86"/>
-      <c r="X8" s="86"/>
-      <c r="Y8" s="86"/>
-      <c r="Z8" s="86"/>
-      <c r="AA8" s="86"/>
-      <c r="AB8" s="86"/>
-      <c r="AC8" s="86"/>
-      <c r="AD8" s="86"/>
-      <c r="AE8" s="86"/>
+      <c r="B8" s="57"/>
+      <c r="C8" s="57"/>
+      <c r="D8" s="57"/>
+      <c r="E8" s="57"/>
+      <c r="F8" s="57"/>
+      <c r="G8" s="57"/>
+      <c r="H8" s="57"/>
+      <c r="I8" s="57"/>
+      <c r="J8" s="57"/>
+      <c r="K8" s="57"/>
+      <c r="L8" s="57"/>
+      <c r="M8" s="57"/>
+      <c r="N8" s="57"/>
+      <c r="O8" s="57"/>
+      <c r="P8" s="57"/>
+      <c r="Q8" s="57"/>
+      <c r="R8" s="57"/>
+      <c r="S8" s="57"/>
+      <c r="T8" s="57"/>
+      <c r="U8" s="57"/>
+      <c r="V8" s="57"/>
+      <c r="W8" s="57"/>
+      <c r="X8" s="57"/>
+      <c r="Y8" s="57"/>
+      <c r="Z8" s="57"/>
+      <c r="AA8" s="57"/>
+      <c r="AB8" s="57"/>
+      <c r="AC8" s="57"/>
+      <c r="AD8" s="57"/>
+      <c r="AE8" s="57"/>
     </row>
     <row r="9" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A9" s="87" t="s">
+      <c r="A9" s="58" t="s">
         <v>161</v>
       </c>
-      <c r="B9" s="86"/>
-      <c r="C9" s="86"/>
-      <c r="D9" s="86"/>
-      <c r="E9" s="86"/>
-      <c r="F9" s="86"/>
-      <c r="G9" s="86"/>
-      <c r="H9" s="86"/>
-      <c r="I9" s="86"/>
-      <c r="J9" s="86"/>
-      <c r="K9" s="86"/>
-      <c r="L9" s="86"/>
-      <c r="M9" s="86"/>
-      <c r="N9" s="86"/>
-      <c r="O9" s="86"/>
-      <c r="P9" s="86"/>
-      <c r="Q9" s="86"/>
-      <c r="R9" s="86"/>
-      <c r="S9" s="86"/>
-      <c r="T9" s="86"/>
-      <c r="U9" s="86"/>
-      <c r="V9" s="86"/>
-      <c r="W9" s="86"/>
-      <c r="X9" s="86"/>
-      <c r="Y9" s="86"/>
-      <c r="Z9" s="86"/>
-      <c r="AA9" s="86"/>
-      <c r="AB9" s="86"/>
-      <c r="AC9" s="86"/>
-      <c r="AD9" s="86"/>
-      <c r="AE9" s="86"/>
+      <c r="B9" s="57"/>
+      <c r="C9" s="57"/>
+      <c r="D9" s="57"/>
+      <c r="E9" s="57"/>
+      <c r="F9" s="57"/>
+      <c r="G9" s="57"/>
+      <c r="H9" s="57"/>
+      <c r="I9" s="57"/>
+      <c r="J9" s="57"/>
+      <c r="K9" s="57"/>
+      <c r="L9" s="57"/>
+      <c r="M9" s="57"/>
+      <c r="N9" s="57"/>
+      <c r="O9" s="57"/>
+      <c r="P9" s="57"/>
+      <c r="Q9" s="57"/>
+      <c r="R9" s="57"/>
+      <c r="S9" s="57"/>
+      <c r="T9" s="57"/>
+      <c r="U9" s="57"/>
+      <c r="V9" s="57"/>
+      <c r="W9" s="57"/>
+      <c r="X9" s="57"/>
+      <c r="Y9" s="57"/>
+      <c r="Z9" s="57"/>
+      <c r="AA9" s="57"/>
+      <c r="AB9" s="57"/>
+      <c r="AC9" s="57"/>
+      <c r="AD9" s="57"/>
+      <c r="AE9" s="57"/>
     </row>
     <row r="10" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A10" s="87" t="s">
+      <c r="A10" s="58" t="s">
         <v>162</v>
       </c>
-      <c r="B10" s="86"/>
-      <c r="C10" s="86"/>
-      <c r="D10" s="86"/>
-      <c r="E10" s="86"/>
-      <c r="F10" s="86"/>
-      <c r="G10" s="86"/>
-      <c r="H10" s="86"/>
-      <c r="I10" s="86"/>
-      <c r="J10" s="86"/>
-      <c r="K10" s="86"/>
-      <c r="L10" s="86"/>
-      <c r="M10" s="86"/>
-      <c r="N10" s="86"/>
-      <c r="O10" s="86"/>
-      <c r="P10" s="86"/>
-      <c r="Q10" s="86"/>
-      <c r="R10" s="86"/>
-      <c r="S10" s="86"/>
-      <c r="T10" s="86"/>
-      <c r="U10" s="86"/>
-      <c r="V10" s="86"/>
-      <c r="W10" s="86"/>
-      <c r="X10" s="86"/>
-      <c r="Y10" s="86"/>
-      <c r="Z10" s="86"/>
-      <c r="AA10" s="86"/>
-      <c r="AB10" s="86"/>
-      <c r="AC10" s="86"/>
-      <c r="AD10" s="86"/>
-      <c r="AE10" s="86"/>
+      <c r="B10" s="57"/>
+      <c r="C10" s="57"/>
+      <c r="D10" s="57"/>
+      <c r="E10" s="57"/>
+      <c r="F10" s="57"/>
+      <c r="G10" s="57"/>
+      <c r="H10" s="57"/>
+      <c r="I10" s="57"/>
+      <c r="J10" s="57"/>
+      <c r="K10" s="57"/>
+      <c r="L10" s="57"/>
+      <c r="M10" s="57"/>
+      <c r="N10" s="57"/>
+      <c r="O10" s="57"/>
+      <c r="P10" s="57"/>
+      <c r="Q10" s="57"/>
+      <c r="R10" s="57"/>
+      <c r="S10" s="57"/>
+      <c r="T10" s="57"/>
+      <c r="U10" s="57"/>
+      <c r="V10" s="57"/>
+      <c r="W10" s="57"/>
+      <c r="X10" s="57"/>
+      <c r="Y10" s="57"/>
+      <c r="Z10" s="57"/>
+      <c r="AA10" s="57"/>
+      <c r="AB10" s="57"/>
+      <c r="AC10" s="57"/>
+      <c r="AD10" s="57"/>
+      <c r="AE10" s="57"/>
     </row>
     <row r="11" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A11" s="87" t="s">
+      <c r="A11" s="58" t="s">
         <v>163</v>
       </c>
-      <c r="B11" s="86"/>
-      <c r="C11" s="86"/>
-      <c r="D11" s="86"/>
-      <c r="E11" s="86"/>
-      <c r="F11" s="86"/>
-      <c r="G11" s="86"/>
-      <c r="H11" s="86"/>
-      <c r="I11" s="86"/>
-      <c r="J11" s="86"/>
-      <c r="K11" s="86"/>
-      <c r="L11" s="86"/>
-      <c r="M11" s="86"/>
-      <c r="N11" s="86"/>
-      <c r="O11" s="86"/>
-      <c r="P11" s="86"/>
-      <c r="Q11" s="86"/>
-      <c r="R11" s="86"/>
-      <c r="S11" s="86"/>
-      <c r="T11" s="86"/>
-      <c r="U11" s="86"/>
-      <c r="V11" s="86"/>
-      <c r="W11" s="86"/>
-      <c r="X11" s="86"/>
-      <c r="Y11" s="86"/>
-      <c r="Z11" s="86"/>
-      <c r="AA11" s="86"/>
-      <c r="AB11" s="86"/>
-      <c r="AC11" s="86"/>
-      <c r="AD11" s="86"/>
-      <c r="AE11" s="86"/>
+      <c r="B11" s="57"/>
+      <c r="C11" s="57"/>
+      <c r="D11" s="57"/>
+      <c r="E11" s="57"/>
+      <c r="F11" s="57"/>
+      <c r="G11" s="57"/>
+      <c r="H11" s="57"/>
+      <c r="I11" s="57"/>
+      <c r="J11" s="57"/>
+      <c r="K11" s="57"/>
+      <c r="L11" s="57"/>
+      <c r="M11" s="57"/>
+      <c r="N11" s="57"/>
+      <c r="O11" s="57"/>
+      <c r="P11" s="57"/>
+      <c r="Q11" s="57"/>
+      <c r="R11" s="57"/>
+      <c r="S11" s="57"/>
+      <c r="T11" s="57"/>
+      <c r="U11" s="57"/>
+      <c r="V11" s="57"/>
+      <c r="W11" s="57"/>
+      <c r="X11" s="57"/>
+      <c r="Y11" s="57"/>
+      <c r="Z11" s="57"/>
+      <c r="AA11" s="57"/>
+      <c r="AB11" s="57"/>
+      <c r="AC11" s="57"/>
+      <c r="AD11" s="57"/>
+      <c r="AE11" s="57"/>
     </row>
     <row r="12" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A12" s="87" t="s">
+      <c r="A12" s="58" t="s">
         <v>164</v>
       </c>
-      <c r="B12" s="86"/>
-      <c r="C12" s="86"/>
-      <c r="D12" s="86"/>
-      <c r="E12" s="86"/>
-      <c r="F12" s="86"/>
-      <c r="G12" s="86"/>
-      <c r="H12" s="86"/>
-      <c r="I12" s="86"/>
-      <c r="J12" s="86"/>
-      <c r="K12" s="86"/>
-      <c r="L12" s="86"/>
-      <c r="M12" s="86"/>
-      <c r="N12" s="86"/>
-      <c r="O12" s="86"/>
-      <c r="P12" s="86"/>
-      <c r="Q12" s="86"/>
-      <c r="R12" s="86"/>
-      <c r="S12" s="86"/>
-      <c r="T12" s="86"/>
-      <c r="U12" s="86"/>
-      <c r="V12" s="86"/>
-      <c r="W12" s="86"/>
-      <c r="X12" s="86"/>
-      <c r="Y12" s="86"/>
-      <c r="Z12" s="86"/>
-      <c r="AA12" s="86"/>
-      <c r="AB12" s="86"/>
-      <c r="AC12" s="86"/>
-      <c r="AD12" s="86"/>
-      <c r="AE12" s="86"/>
+      <c r="B12" s="57"/>
+      <c r="C12" s="57"/>
+      <c r="D12" s="57"/>
+      <c r="E12" s="57"/>
+      <c r="F12" s="57"/>
+      <c r="G12" s="57"/>
+      <c r="H12" s="57"/>
+      <c r="I12" s="57"/>
+      <c r="J12" s="57"/>
+      <c r="K12" s="57"/>
+      <c r="L12" s="57"/>
+      <c r="M12" s="57"/>
+      <c r="N12" s="57"/>
+      <c r="O12" s="57"/>
+      <c r="P12" s="57"/>
+      <c r="Q12" s="57"/>
+      <c r="R12" s="57"/>
+      <c r="S12" s="57"/>
+      <c r="T12" s="57"/>
+      <c r="U12" s="57"/>
+      <c r="V12" s="57"/>
+      <c r="W12" s="57"/>
+      <c r="X12" s="57"/>
+      <c r="Y12" s="57"/>
+      <c r="Z12" s="57"/>
+      <c r="AA12" s="57"/>
+      <c r="AB12" s="57"/>
+      <c r="AC12" s="57"/>
+      <c r="AD12" s="57"/>
+      <c r="AE12" s="57"/>
     </row>
     <row r="13" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A13" s="87" t="s">
+      <c r="A13" s="58" t="s">
         <v>165</v>
       </c>
-      <c r="B13" s="86"/>
-      <c r="C13" s="86"/>
-      <c r="D13" s="86"/>
-      <c r="E13" s="86"/>
-      <c r="F13" s="86"/>
-      <c r="G13" s="86"/>
-      <c r="H13" s="86"/>
-      <c r="I13" s="86"/>
-      <c r="J13" s="86"/>
-      <c r="K13" s="86"/>
-      <c r="L13" s="86"/>
-      <c r="M13" s="86"/>
-      <c r="N13" s="86"/>
-      <c r="O13" s="86"/>
-      <c r="P13" s="86"/>
-      <c r="Q13" s="86"/>
-      <c r="R13" s="86"/>
-      <c r="S13" s="86"/>
-      <c r="T13" s="86"/>
-      <c r="U13" s="86"/>
-      <c r="V13" s="86"/>
-      <c r="W13" s="86"/>
-      <c r="X13" s="86"/>
-      <c r="Y13" s="86"/>
-      <c r="Z13" s="86"/>
-      <c r="AA13" s="86"/>
-      <c r="AB13" s="86"/>
-      <c r="AC13" s="86"/>
-      <c r="AD13" s="86"/>
-      <c r="AE13" s="86"/>
+      <c r="B13" s="57"/>
+      <c r="C13" s="57"/>
+      <c r="D13" s="57"/>
+      <c r="E13" s="57"/>
+      <c r="F13" s="57"/>
+      <c r="G13" s="57"/>
+      <c r="H13" s="57"/>
+      <c r="I13" s="57"/>
+      <c r="J13" s="57"/>
+      <c r="K13" s="57"/>
+      <c r="L13" s="57"/>
+      <c r="M13" s="57"/>
+      <c r="N13" s="57"/>
+      <c r="O13" s="57"/>
+      <c r="P13" s="57"/>
+      <c r="Q13" s="57"/>
+      <c r="R13" s="57"/>
+      <c r="S13" s="57"/>
+      <c r="T13" s="57"/>
+      <c r="U13" s="57"/>
+      <c r="V13" s="57"/>
+      <c r="W13" s="57"/>
+      <c r="X13" s="57"/>
+      <c r="Y13" s="57"/>
+      <c r="Z13" s="57"/>
+      <c r="AA13" s="57"/>
+      <c r="AB13" s="57"/>
+      <c r="AC13" s="57"/>
+      <c r="AD13" s="57"/>
+      <c r="AE13" s="57"/>
     </row>
     <row r="14" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A14" s="87" t="s">
+      <c r="A14" s="58" t="s">
         <v>166</v>
       </c>
-      <c r="B14" s="86"/>
-      <c r="C14" s="86"/>
-      <c r="D14" s="86"/>
-      <c r="E14" s="86"/>
-      <c r="F14" s="86"/>
-      <c r="G14" s="86"/>
-      <c r="H14" s="86"/>
-      <c r="I14" s="86"/>
-      <c r="J14" s="86"/>
-      <c r="K14" s="86"/>
-      <c r="L14" s="86"/>
-      <c r="M14" s="86"/>
-      <c r="N14" s="86"/>
-      <c r="O14" s="86"/>
-      <c r="P14" s="86"/>
-      <c r="Q14" s="86"/>
-      <c r="R14" s="86"/>
-      <c r="S14" s="86"/>
-      <c r="T14" s="86"/>
-      <c r="U14" s="86"/>
-      <c r="V14" s="86"/>
-      <c r="W14" s="86"/>
-      <c r="X14" s="86"/>
-      <c r="Y14" s="86"/>
-      <c r="Z14" s="86"/>
-      <c r="AA14" s="86"/>
-      <c r="AB14" s="86"/>
-      <c r="AC14" s="86"/>
-      <c r="AD14" s="86"/>
-      <c r="AE14" s="86"/>
+      <c r="B14" s="57"/>
+      <c r="C14" s="57"/>
+      <c r="D14" s="57"/>
+      <c r="E14" s="57"/>
+      <c r="F14" s="57"/>
+      <c r="G14" s="57"/>
+      <c r="H14" s="57"/>
+      <c r="I14" s="57"/>
+      <c r="J14" s="57"/>
+      <c r="K14" s="57"/>
+      <c r="L14" s="57"/>
+      <c r="M14" s="57"/>
+      <c r="N14" s="57"/>
+      <c r="O14" s="57"/>
+      <c r="P14" s="57"/>
+      <c r="Q14" s="57"/>
+      <c r="R14" s="57"/>
+      <c r="S14" s="57"/>
+      <c r="T14" s="57"/>
+      <c r="U14" s="57"/>
+      <c r="V14" s="57"/>
+      <c r="W14" s="57"/>
+      <c r="X14" s="57"/>
+      <c r="Y14" s="57"/>
+      <c r="Z14" s="57"/>
+      <c r="AA14" s="57"/>
+      <c r="AB14" s="57"/>
+      <c r="AC14" s="57"/>
+      <c r="AD14" s="57"/>
+      <c r="AE14" s="57"/>
     </row>
     <row r="15" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A15" s="87" t="s">
+      <c r="A15" s="58" t="s">
         <v>167</v>
       </c>
-      <c r="B15" s="86"/>
-      <c r="C15" s="86"/>
-      <c r="D15" s="86"/>
-      <c r="E15" s="86"/>
-      <c r="F15" s="86"/>
-      <c r="G15" s="86"/>
-      <c r="H15" s="86"/>
-      <c r="I15" s="86"/>
-      <c r="J15" s="86"/>
-      <c r="K15" s="86"/>
-      <c r="L15" s="86"/>
-      <c r="M15" s="86"/>
-      <c r="N15" s="86"/>
-      <c r="O15" s="86"/>
-      <c r="P15" s="86"/>
-      <c r="Q15" s="86"/>
-      <c r="R15" s="86"/>
-      <c r="S15" s="86"/>
-      <c r="T15" s="86"/>
-      <c r="U15" s="86"/>
-      <c r="V15" s="86"/>
-      <c r="W15" s="86"/>
-      <c r="X15" s="86"/>
-      <c r="Y15" s="86"/>
-      <c r="Z15" s="86"/>
-      <c r="AA15" s="86"/>
-      <c r="AB15" s="86"/>
-      <c r="AC15" s="86"/>
-      <c r="AD15" s="86"/>
-      <c r="AE15" s="86"/>
+      <c r="B15" s="57"/>
+      <c r="C15" s="57"/>
+      <c r="D15" s="57"/>
+      <c r="E15" s="57"/>
+      <c r="F15" s="57"/>
+      <c r="G15" s="57"/>
+      <c r="H15" s="57"/>
+      <c r="I15" s="57"/>
+      <c r="J15" s="57"/>
+      <c r="K15" s="57"/>
+      <c r="L15" s="57"/>
+      <c r="M15" s="57"/>
+      <c r="N15" s="57"/>
+      <c r="O15" s="57"/>
+      <c r="P15" s="57"/>
+      <c r="Q15" s="57"/>
+      <c r="R15" s="57"/>
+      <c r="S15" s="57"/>
+      <c r="T15" s="57"/>
+      <c r="U15" s="57"/>
+      <c r="V15" s="57"/>
+      <c r="W15" s="57"/>
+      <c r="X15" s="57"/>
+      <c r="Y15" s="57"/>
+      <c r="Z15" s="57"/>
+      <c r="AA15" s="57"/>
+      <c r="AB15" s="57"/>
+      <c r="AC15" s="57"/>
+      <c r="AD15" s="57"/>
+      <c r="AE15" s="57"/>
     </row>
     <row r="16" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A16" s="87" t="s">
+      <c r="A16" s="58" t="s">
         <v>168</v>
       </c>
-      <c r="B16" s="86"/>
-      <c r="C16" s="86"/>
-      <c r="D16" s="86"/>
-      <c r="E16" s="86"/>
-      <c r="F16" s="86"/>
-      <c r="G16" s="86"/>
-      <c r="H16" s="86"/>
-      <c r="I16" s="86"/>
-      <c r="J16" s="86"/>
-      <c r="K16" s="86"/>
-      <c r="L16" s="86"/>
-      <c r="M16" s="86"/>
-      <c r="N16" s="86"/>
-      <c r="O16" s="86"/>
-      <c r="P16" s="86"/>
-      <c r="Q16" s="86"/>
-      <c r="R16" s="86"/>
-      <c r="S16" s="86"/>
-      <c r="T16" s="86"/>
-      <c r="U16" s="86"/>
-      <c r="V16" s="86"/>
-      <c r="W16" s="86"/>
-      <c r="X16" s="86"/>
-      <c r="Y16" s="86"/>
-      <c r="Z16" s="86"/>
-      <c r="AA16" s="86"/>
-      <c r="AB16" s="86"/>
-      <c r="AC16" s="86"/>
-      <c r="AD16" s="86"/>
-      <c r="AE16" s="86"/>
+      <c r="B16" s="57"/>
+      <c r="C16" s="57"/>
+      <c r="D16" s="57"/>
+      <c r="E16" s="57"/>
+      <c r="F16" s="57"/>
+      <c r="G16" s="57"/>
+      <c r="H16" s="57"/>
+      <c r="I16" s="57"/>
+      <c r="J16" s="57"/>
+      <c r="K16" s="57"/>
+      <c r="L16" s="57"/>
+      <c r="M16" s="57"/>
+      <c r="N16" s="57"/>
+      <c r="O16" s="57"/>
+      <c r="P16" s="57"/>
+      <c r="Q16" s="57"/>
+      <c r="R16" s="57"/>
+      <c r="S16" s="57"/>
+      <c r="T16" s="57"/>
+      <c r="U16" s="57"/>
+      <c r="V16" s="57"/>
+      <c r="W16" s="57"/>
+      <c r="X16" s="57"/>
+      <c r="Y16" s="57"/>
+      <c r="Z16" s="57"/>
+      <c r="AA16" s="57"/>
+      <c r="AB16" s="57"/>
+      <c r="AC16" s="57"/>
+      <c r="AD16" s="57"/>
+      <c r="AE16" s="57"/>
     </row>
     <row r="17" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A17" s="87" t="s">
+      <c r="A17" s="58" t="s">
         <v>169</v>
       </c>
-      <c r="B17" s="86"/>
-      <c r="C17" s="86"/>
-      <c r="D17" s="86"/>
-      <c r="E17" s="86"/>
-      <c r="F17" s="86"/>
-      <c r="G17" s="86"/>
-      <c r="H17" s="86"/>
-      <c r="I17" s="86"/>
-      <c r="J17" s="86"/>
-      <c r="K17" s="86"/>
-      <c r="L17" s="86"/>
-      <c r="M17" s="86"/>
-      <c r="N17" s="86"/>
-      <c r="O17" s="86"/>
-      <c r="P17" s="86"/>
-      <c r="Q17" s="86"/>
-      <c r="R17" s="86"/>
-      <c r="S17" s="86"/>
-      <c r="T17" s="86"/>
-      <c r="U17" s="86"/>
-      <c r="V17" s="86"/>
-      <c r="W17" s="86"/>
-      <c r="X17" s="86"/>
-      <c r="Y17" s="86"/>
-      <c r="Z17" s="86"/>
-      <c r="AA17" s="86"/>
-      <c r="AB17" s="86"/>
-      <c r="AC17" s="86"/>
-      <c r="AD17" s="86"/>
-      <c r="AE17" s="86"/>
+      <c r="B17" s="57"/>
+      <c r="C17" s="57"/>
+      <c r="D17" s="57"/>
+      <c r="E17" s="57"/>
+      <c r="F17" s="57"/>
+      <c r="G17" s="57"/>
+      <c r="H17" s="57"/>
+      <c r="I17" s="57"/>
+      <c r="J17" s="57"/>
+      <c r="K17" s="57"/>
+      <c r="L17" s="57"/>
+      <c r="M17" s="57"/>
+      <c r="N17" s="57"/>
+      <c r="O17" s="57"/>
+      <c r="P17" s="57"/>
+      <c r="Q17" s="57"/>
+      <c r="R17" s="57"/>
+      <c r="S17" s="57"/>
+      <c r="T17" s="57"/>
+      <c r="U17" s="57"/>
+      <c r="V17" s="57"/>
+      <c r="W17" s="57"/>
+      <c r="X17" s="57"/>
+      <c r="Y17" s="57"/>
+      <c r="Z17" s="57"/>
+      <c r="AA17" s="57"/>
+      <c r="AB17" s="57"/>
+      <c r="AC17" s="57"/>
+      <c r="AD17" s="57"/>
+      <c r="AE17" s="57"/>
     </row>
     <row r="18" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A18" s="87" t="s">
+      <c r="A18" s="58" t="s">
         <v>170</v>
       </c>
-      <c r="B18" s="86"/>
-      <c r="C18" s="86"/>
-      <c r="D18" s="86"/>
-      <c r="E18" s="86"/>
-      <c r="F18" s="86"/>
-      <c r="G18" s="86"/>
-      <c r="H18" s="86"/>
-      <c r="I18" s="86"/>
-      <c r="J18" s="86"/>
-      <c r="K18" s="86"/>
-      <c r="L18" s="86"/>
-      <c r="M18" s="86"/>
-      <c r="N18" s="86"/>
-      <c r="O18" s="86"/>
-      <c r="P18" s="86"/>
-      <c r="Q18" s="86"/>
-      <c r="R18" s="86"/>
-      <c r="S18" s="86"/>
-      <c r="T18" s="86"/>
-      <c r="U18" s="86"/>
-      <c r="V18" s="86"/>
-      <c r="W18" s="86"/>
-      <c r="X18" s="86"/>
-      <c r="Y18" s="86"/>
-      <c r="Z18" s="86"/>
-      <c r="AA18" s="86"/>
-      <c r="AB18" s="86"/>
-      <c r="AC18" s="86"/>
-      <c r="AD18" s="86"/>
-      <c r="AE18" s="86"/>
+      <c r="B18" s="57"/>
+      <c r="C18" s="57"/>
+      <c r="D18" s="57"/>
+      <c r="E18" s="57"/>
+      <c r="F18" s="57"/>
+      <c r="G18" s="57"/>
+      <c r="H18" s="57"/>
+      <c r="I18" s="57"/>
+      <c r="J18" s="57"/>
+      <c r="K18" s="57"/>
+      <c r="L18" s="57"/>
+      <c r="M18" s="57"/>
+      <c r="N18" s="57"/>
+      <c r="O18" s="57"/>
+      <c r="P18" s="57"/>
+      <c r="Q18" s="57"/>
+      <c r="R18" s="57"/>
+      <c r="S18" s="57"/>
+      <c r="T18" s="57"/>
+      <c r="U18" s="57"/>
+      <c r="V18" s="57"/>
+      <c r="W18" s="57"/>
+      <c r="X18" s="57"/>
+      <c r="Y18" s="57"/>
+      <c r="Z18" s="57"/>
+      <c r="AA18" s="57"/>
+      <c r="AB18" s="57"/>
+      <c r="AC18" s="57"/>
+      <c r="AD18" s="57"/>
+      <c r="AE18" s="57"/>
     </row>
     <row r="19" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A19" s="87" t="s">
+      <c r="A19" s="58" t="s">
         <v>171</v>
       </c>
-      <c r="B19" s="86"/>
-      <c r="C19" s="86"/>
-      <c r="D19" s="86"/>
-      <c r="E19" s="86"/>
-      <c r="F19" s="86"/>
-      <c r="G19" s="86"/>
-      <c r="H19" s="86"/>
-      <c r="I19" s="86"/>
-      <c r="J19" s="86"/>
-      <c r="K19" s="86"/>
-      <c r="L19" s="86"/>
-      <c r="M19" s="86"/>
-      <c r="N19" s="86"/>
-      <c r="O19" s="86"/>
-      <c r="P19" s="86"/>
-      <c r="Q19" s="86"/>
-      <c r="R19" s="86"/>
-      <c r="S19" s="86"/>
-      <c r="T19" s="86"/>
-      <c r="U19" s="86"/>
-      <c r="V19" s="86"/>
-      <c r="W19" s="86"/>
-      <c r="X19" s="86"/>
-      <c r="Y19" s="86"/>
-      <c r="Z19" s="86"/>
-      <c r="AA19" s="86"/>
-      <c r="AB19" s="86"/>
-      <c r="AC19" s="86"/>
-      <c r="AD19" s="86"/>
-      <c r="AE19" s="86"/>
+      <c r="B19" s="57"/>
+      <c r="C19" s="57"/>
+      <c r="D19" s="57"/>
+      <c r="E19" s="57"/>
+      <c r="F19" s="57"/>
+      <c r="G19" s="57"/>
+      <c r="H19" s="57"/>
+      <c r="I19" s="57"/>
+      <c r="J19" s="57"/>
+      <c r="K19" s="57"/>
+      <c r="L19" s="57"/>
+      <c r="M19" s="57"/>
+      <c r="N19" s="57"/>
+      <c r="O19" s="57"/>
+      <c r="P19" s="57"/>
+      <c r="Q19" s="57"/>
+      <c r="R19" s="57"/>
+      <c r="S19" s="57"/>
+      <c r="T19" s="57"/>
+      <c r="U19" s="57"/>
+      <c r="V19" s="57"/>
+      <c r="W19" s="57"/>
+      <c r="X19" s="57"/>
+      <c r="Y19" s="57"/>
+      <c r="Z19" s="57"/>
+      <c r="AA19" s="57"/>
+      <c r="AB19" s="57"/>
+      <c r="AC19" s="57"/>
+      <c r="AD19" s="57"/>
+      <c r="AE19" s="57"/>
     </row>
     <row r="20" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A20" s="87" t="s">
+      <c r="A20" s="58" t="s">
         <v>172</v>
       </c>
-      <c r="B20" s="86"/>
-      <c r="C20" s="86"/>
-      <c r="D20" s="86"/>
-      <c r="E20" s="86"/>
-      <c r="F20" s="86"/>
-      <c r="G20" s="86"/>
-      <c r="H20" s="86"/>
-      <c r="I20" s="86"/>
-      <c r="J20" s="86"/>
-      <c r="K20" s="86"/>
-      <c r="L20" s="86"/>
-      <c r="M20" s="86"/>
-      <c r="N20" s="86"/>
-      <c r="O20" s="86"/>
-      <c r="P20" s="86"/>
-      <c r="Q20" s="86"/>
-      <c r="R20" s="86"/>
-      <c r="S20" s="86"/>
-      <c r="T20" s="86"/>
-      <c r="U20" s="86"/>
-      <c r="V20" s="86"/>
-      <c r="W20" s="86"/>
-      <c r="X20" s="86"/>
-      <c r="Y20" s="86"/>
-      <c r="Z20" s="86"/>
-      <c r="AA20" s="86"/>
-      <c r="AB20" s="86"/>
-      <c r="AC20" s="86"/>
-      <c r="AD20" s="86"/>
-      <c r="AE20" s="86"/>
+      <c r="B20" s="57"/>
+      <c r="C20" s="57"/>
+      <c r="D20" s="57"/>
+      <c r="E20" s="57"/>
+      <c r="F20" s="57"/>
+      <c r="G20" s="57"/>
+      <c r="H20" s="57"/>
+      <c r="I20" s="57"/>
+      <c r="J20" s="57"/>
+      <c r="K20" s="57"/>
+      <c r="L20" s="57"/>
+      <c r="M20" s="57"/>
+      <c r="N20" s="57"/>
+      <c r="O20" s="57"/>
+      <c r="P20" s="57"/>
+      <c r="Q20" s="57"/>
+      <c r="R20" s="57"/>
+      <c r="S20" s="57"/>
+      <c r="T20" s="57"/>
+      <c r="U20" s="57"/>
+      <c r="V20" s="57"/>
+      <c r="W20" s="57"/>
+      <c r="X20" s="57"/>
+      <c r="Y20" s="57"/>
+      <c r="Z20" s="57"/>
+      <c r="AA20" s="57"/>
+      <c r="AB20" s="57"/>
+      <c r="AC20" s="57"/>
+      <c r="AD20" s="57"/>
+      <c r="AE20" s="57"/>
     </row>
     <row r="21" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A21" s="87" t="s">
+      <c r="A21" s="58" t="s">
         <v>173</v>
       </c>
-      <c r="B21" s="86"/>
-      <c r="C21" s="86"/>
-      <c r="D21" s="86"/>
-      <c r="E21" s="86"/>
-      <c r="F21" s="86"/>
-      <c r="G21" s="86"/>
-      <c r="H21" s="86"/>
-      <c r="I21" s="86"/>
-      <c r="J21" s="86"/>
-      <c r="K21" s="86"/>
-      <c r="L21" s="86"/>
-      <c r="M21" s="86"/>
-      <c r="N21" s="86"/>
-      <c r="O21" s="86"/>
-      <c r="P21" s="86"/>
-      <c r="Q21" s="86"/>
-      <c r="R21" s="86"/>
-      <c r="S21" s="86"/>
-      <c r="T21" s="86"/>
-      <c r="U21" s="86"/>
-      <c r="V21" s="86"/>
-      <c r="W21" s="86"/>
-      <c r="X21" s="86"/>
-      <c r="Y21" s="86"/>
-      <c r="Z21" s="86"/>
-      <c r="AA21" s="86"/>
-      <c r="AB21" s="86"/>
-      <c r="AC21" s="86"/>
-      <c r="AD21" s="86"/>
-      <c r="AE21" s="86"/>
+      <c r="B21" s="57"/>
+      <c r="C21" s="57"/>
+      <c r="D21" s="57"/>
+      <c r="E21" s="57"/>
+      <c r="F21" s="57"/>
+      <c r="G21" s="57"/>
+      <c r="H21" s="57"/>
+      <c r="I21" s="57"/>
+      <c r="J21" s="57"/>
+      <c r="K21" s="57"/>
+      <c r="L21" s="57"/>
+      <c r="M21" s="57"/>
+      <c r="N21" s="57"/>
+      <c r="O21" s="57"/>
+      <c r="P21" s="57"/>
+      <c r="Q21" s="57"/>
+      <c r="R21" s="57"/>
+      <c r="S21" s="57"/>
+      <c r="T21" s="57"/>
+      <c r="U21" s="57"/>
+      <c r="V21" s="57"/>
+      <c r="W21" s="57"/>
+      <c r="X21" s="57"/>
+      <c r="Y21" s="57"/>
+      <c r="Z21" s="57"/>
+      <c r="AA21" s="57"/>
+      <c r="AB21" s="57"/>
+      <c r="AC21" s="57"/>
+      <c r="AD21" s="57"/>
+      <c r="AE21" s="57"/>
     </row>
     <row r="22" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A22" s="87" t="s">
+      <c r="A22" s="58" t="s">
         <v>174</v>
       </c>
-      <c r="B22" s="86"/>
-      <c r="C22" s="86"/>
-      <c r="D22" s="86"/>
-      <c r="E22" s="86"/>
-      <c r="F22" s="86"/>
-      <c r="G22" s="86"/>
-      <c r="H22" s="86"/>
-      <c r="I22" s="86"/>
-      <c r="J22" s="86"/>
-      <c r="K22" s="86"/>
-      <c r="L22" s="86"/>
-      <c r="M22" s="86"/>
-      <c r="N22" s="86"/>
-      <c r="O22" s="86"/>
-      <c r="P22" s="86"/>
-      <c r="Q22" s="86"/>
-      <c r="R22" s="86"/>
-      <c r="S22" s="86"/>
-      <c r="T22" s="86"/>
-      <c r="U22" s="86"/>
-      <c r="V22" s="86"/>
-      <c r="W22" s="86"/>
-      <c r="X22" s="86"/>
-      <c r="Y22" s="86"/>
-      <c r="Z22" s="86"/>
-      <c r="AA22" s="86"/>
-      <c r="AB22" s="86"/>
-      <c r="AC22" s="86"/>
-      <c r="AD22" s="86"/>
-      <c r="AE22" s="86"/>
+      <c r="B22" s="57"/>
+      <c r="C22" s="57"/>
+      <c r="D22" s="57"/>
+      <c r="E22" s="57"/>
+      <c r="F22" s="57"/>
+      <c r="G22" s="57"/>
+      <c r="H22" s="57"/>
+      <c r="I22" s="57"/>
+      <c r="J22" s="57"/>
+      <c r="K22" s="57"/>
+      <c r="L22" s="57"/>
+      <c r="M22" s="57"/>
+      <c r="N22" s="57"/>
+      <c r="O22" s="57"/>
+      <c r="P22" s="57"/>
+      <c r="Q22" s="57"/>
+      <c r="R22" s="57"/>
+      <c r="S22" s="57"/>
+      <c r="T22" s="57"/>
+      <c r="U22" s="57"/>
+      <c r="V22" s="57"/>
+      <c r="W22" s="57"/>
+      <c r="X22" s="57"/>
+      <c r="Y22" s="57"/>
+      <c r="Z22" s="57"/>
+      <c r="AA22" s="57"/>
+      <c r="AB22" s="57"/>
+      <c r="AC22" s="57"/>
+      <c r="AD22" s="57"/>
+      <c r="AE22" s="57"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -3538,234 +3582,234 @@
       </c>
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A2" s="67" t="s">
+      <c r="A2" s="89" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="67"/>
-      <c r="C2" s="67"/>
-      <c r="D2" s="67"/>
-      <c r="E2" s="67"/>
-      <c r="F2" s="67"/>
-      <c r="G2" s="67"/>
-      <c r="H2" s="67"/>
-      <c r="I2" s="67"/>
-      <c r="J2" s="67"/>
-      <c r="K2" s="67"/>
-      <c r="L2" s="67"/>
-      <c r="M2" s="71" t="s">
+      <c r="B2" s="89"/>
+      <c r="C2" s="89"/>
+      <c r="D2" s="89"/>
+      <c r="E2" s="89"/>
+      <c r="F2" s="89"/>
+      <c r="G2" s="89"/>
+      <c r="H2" s="89"/>
+      <c r="I2" s="89"/>
+      <c r="J2" s="89"/>
+      <c r="K2" s="89"/>
+      <c r="L2" s="89"/>
+      <c r="M2" s="85" t="s">
         <v>23</v>
       </c>
-      <c r="N2" s="71"/>
-      <c r="O2" s="71"/>
-      <c r="P2" s="71"/>
-      <c r="Q2" s="71"/>
-      <c r="R2" s="71"/>
-      <c r="S2" s="71"/>
-      <c r="T2" s="71"/>
-      <c r="U2" s="71"/>
-      <c r="V2" s="71"/>
-      <c r="W2" s="71"/>
-      <c r="X2" s="71"/>
+      <c r="N2" s="85"/>
+      <c r="O2" s="85"/>
+      <c r="P2" s="85"/>
+      <c r="Q2" s="85"/>
+      <c r="R2" s="85"/>
+      <c r="S2" s="85"/>
+      <c r="T2" s="85"/>
+      <c r="U2" s="85"/>
+      <c r="V2" s="85"/>
+      <c r="W2" s="85"/>
+      <c r="X2" s="85"/>
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3" s="15">
         <v>1</v>
       </c>
-      <c r="B3" s="68" t="s">
+      <c r="B3" s="90" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="68"/>
-      <c r="D3" s="68"/>
+      <c r="C3" s="90"/>
+      <c r="D3" s="90"/>
       <c r="E3" s="16"/>
       <c r="F3" s="16"/>
       <c r="G3" s="16"/>
       <c r="H3" s="16"/>
       <c r="I3" s="16"/>
       <c r="J3" s="16"/>
-      <c r="K3" s="69">
+      <c r="K3" s="91">
         <v>45</v>
       </c>
-      <c r="L3" s="69"/>
+      <c r="L3" s="91"/>
       <c r="M3" s="14">
         <v>1</v>
       </c>
-      <c r="N3" s="72" t="s">
+      <c r="N3" s="86" t="s">
         <v>24</v>
       </c>
-      <c r="O3" s="72"/>
-      <c r="P3" s="72"/>
-      <c r="Q3" s="72"/>
-      <c r="R3" s="72"/>
+      <c r="O3" s="86"/>
+      <c r="P3" s="86"/>
+      <c r="Q3" s="86"/>
+      <c r="R3" s="86"/>
       <c r="S3" s="14">
         <v>6</v>
       </c>
-      <c r="T3" s="70" t="s">
+      <c r="T3" s="84" t="s">
         <v>29</v>
       </c>
-      <c r="U3" s="70"/>
-      <c r="V3" s="70"/>
-      <c r="W3" s="70"/>
-      <c r="X3" s="70"/>
+      <c r="U3" s="84"/>
+      <c r="V3" s="84"/>
+      <c r="W3" s="84"/>
+      <c r="X3" s="84"/>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" s="15">
         <v>2</v>
       </c>
-      <c r="B4" s="68" t="s">
+      <c r="B4" s="90" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="68"/>
-      <c r="D4" s="68"/>
+      <c r="C4" s="90"/>
+      <c r="D4" s="90"/>
       <c r="E4" s="15"/>
       <c r="F4" s="15"/>
       <c r="G4" s="15"/>
       <c r="H4" s="15"/>
       <c r="I4" s="15"/>
       <c r="J4" s="15"/>
-      <c r="K4" s="69">
+      <c r="K4" s="91">
         <v>46</v>
       </c>
-      <c r="L4" s="69"/>
+      <c r="L4" s="91"/>
       <c r="M4" s="14">
         <v>2</v>
       </c>
-      <c r="N4" s="72" t="s">
+      <c r="N4" s="86" t="s">
         <v>25</v>
       </c>
-      <c r="O4" s="72"/>
-      <c r="P4" s="72"/>
-      <c r="Q4" s="72"/>
-      <c r="R4" s="72"/>
+      <c r="O4" s="86"/>
+      <c r="P4" s="86"/>
+      <c r="Q4" s="86"/>
+      <c r="R4" s="86"/>
       <c r="S4" s="14">
         <v>7</v>
       </c>
-      <c r="T4" s="70" t="s">
+      <c r="T4" s="84" t="s">
         <v>29</v>
       </c>
-      <c r="U4" s="70"/>
-      <c r="V4" s="70"/>
-      <c r="W4" s="70"/>
-      <c r="X4" s="70"/>
+      <c r="U4" s="84"/>
+      <c r="V4" s="84"/>
+      <c r="W4" s="84"/>
+      <c r="X4" s="84"/>
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5" s="15">
         <v>3</v>
       </c>
-      <c r="B5" s="65" t="s">
+      <c r="B5" s="87" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="65"/>
-      <c r="D5" s="65"/>
+      <c r="C5" s="87"/>
+      <c r="D5" s="87"/>
       <c r="E5" s="15"/>
       <c r="F5" s="15"/>
       <c r="G5" s="15"/>
       <c r="H5" s="15"/>
       <c r="I5" s="15"/>
       <c r="J5" s="15"/>
-      <c r="K5" s="66">
+      <c r="K5" s="88">
         <v>47</v>
       </c>
-      <c r="L5" s="66"/>
+      <c r="L5" s="88"/>
       <c r="M5" s="14">
         <v>3</v>
       </c>
-      <c r="N5" s="72" t="s">
+      <c r="N5" s="86" t="s">
         <v>26</v>
       </c>
-      <c r="O5" s="72"/>
-      <c r="P5" s="72"/>
-      <c r="Q5" s="72"/>
-      <c r="R5" s="72"/>
+      <c r="O5" s="86"/>
+      <c r="P5" s="86"/>
+      <c r="Q5" s="86"/>
+      <c r="R5" s="86"/>
       <c r="S5" s="14">
         <v>8</v>
       </c>
-      <c r="T5" s="70" t="s">
+      <c r="T5" s="84" t="s">
         <v>29</v>
       </c>
-      <c r="U5" s="70"/>
-      <c r="V5" s="70"/>
-      <c r="W5" s="70"/>
-      <c r="X5" s="70"/>
+      <c r="U5" s="84"/>
+      <c r="V5" s="84"/>
+      <c r="W5" s="84"/>
+      <c r="X5" s="84"/>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6" s="15">
         <v>4</v>
       </c>
-      <c r="B6" s="65" t="s">
+      <c r="B6" s="87" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="65"/>
-      <c r="D6" s="65"/>
+      <c r="C6" s="87"/>
+      <c r="D6" s="87"/>
       <c r="E6" s="15"/>
       <c r="F6" s="15"/>
       <c r="G6" s="15"/>
       <c r="H6" s="15"/>
       <c r="I6" s="15"/>
       <c r="J6" s="15"/>
-      <c r="K6" s="66">
+      <c r="K6" s="88">
         <v>48</v>
       </c>
-      <c r="L6" s="66"/>
+      <c r="L6" s="88"/>
       <c r="M6" s="14">
         <v>4</v>
       </c>
-      <c r="N6" s="72" t="s">
+      <c r="N6" s="86" t="s">
         <v>27</v>
       </c>
-      <c r="O6" s="72"/>
-      <c r="P6" s="72"/>
-      <c r="Q6" s="72"/>
-      <c r="R6" s="72"/>
+      <c r="O6" s="86"/>
+      <c r="P6" s="86"/>
+      <c r="Q6" s="86"/>
+      <c r="R6" s="86"/>
       <c r="S6" s="14">
         <v>9</v>
       </c>
-      <c r="T6" s="70" t="s">
+      <c r="T6" s="84" t="s">
         <v>29</v>
       </c>
-      <c r="U6" s="70"/>
-      <c r="V6" s="70"/>
-      <c r="W6" s="70"/>
-      <c r="X6" s="70"/>
+      <c r="U6" s="84"/>
+      <c r="V6" s="84"/>
+      <c r="W6" s="84"/>
+      <c r="X6" s="84"/>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7" s="15">
         <v>5</v>
       </c>
-      <c r="B7" s="65" t="s">
+      <c r="B7" s="87" t="s">
         <v>22</v>
       </c>
-      <c r="C7" s="65"/>
-      <c r="D7" s="65"/>
+      <c r="C7" s="87"/>
+      <c r="D7" s="87"/>
       <c r="E7" s="15"/>
       <c r="F7" s="15"/>
       <c r="G7" s="15"/>
       <c r="H7" s="15"/>
       <c r="I7" s="15"/>
       <c r="J7" s="15"/>
-      <c r="K7" s="66">
+      <c r="K7" s="88">
         <v>49</v>
       </c>
-      <c r="L7" s="66"/>
+      <c r="L7" s="88"/>
       <c r="M7" s="14">
         <v>5</v>
       </c>
-      <c r="N7" s="72" t="s">
+      <c r="N7" s="86" t="s">
         <v>28</v>
       </c>
-      <c r="O7" s="72"/>
-      <c r="P7" s="72"/>
-      <c r="Q7" s="72"/>
-      <c r="R7" s="72"/>
+      <c r="O7" s="86"/>
+      <c r="P7" s="86"/>
+      <c r="Q7" s="86"/>
+      <c r="R7" s="86"/>
       <c r="S7" s="14">
         <v>10</v>
       </c>
-      <c r="T7" s="70" t="s">
+      <c r="T7" s="84" t="s">
         <v>29</v>
       </c>
-      <c r="U7" s="70"/>
-      <c r="V7" s="70"/>
-      <c r="W7" s="70"/>
-      <c r="X7" s="70"/>
+      <c r="U7" s="84"/>
+      <c r="V7" s="84"/>
+      <c r="W7" s="84"/>
+      <c r="X7" s="84"/>
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A8" s="13"/>
@@ -3977,6 +4021,17 @@
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="K6:L6"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="K7:L7"/>
+    <mergeCell ref="A2:L2"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="K4:L4"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="K5:L5"/>
     <mergeCell ref="T7:X7"/>
     <mergeCell ref="M2:X2"/>
     <mergeCell ref="N3:R3"/>
@@ -3988,17 +4043,6 @@
     <mergeCell ref="T4:X4"/>
     <mergeCell ref="T5:X5"/>
     <mergeCell ref="T6:X6"/>
-    <mergeCell ref="B6:D6"/>
-    <mergeCell ref="K6:L6"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="K7:L7"/>
-    <mergeCell ref="A2:L2"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="K3:L3"/>
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="K4:L4"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="K5:L5"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4127,7 +4171,7 @@
       </c>
     </row>
     <row r="2" spans="1:10" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="73" t="s">
+      <c r="A2" s="92" t="s">
         <v>34</v>
       </c>
       <c r="B2" s="37" t="s">
@@ -4147,7 +4191,7 @@
       <c r="J2" s="37"/>
     </row>
     <row r="3" spans="1:10" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="73"/>
+      <c r="A3" s="92"/>
       <c r="B3" s="38" t="s">
         <v>19</v>
       </c>
@@ -4167,7 +4211,7 @@
       <c r="J3" s="38"/>
     </row>
     <row r="4" spans="1:10" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="73"/>
+      <c r="A4" s="92"/>
       <c r="B4" s="37" t="s">
         <v>20</v>
       </c>
@@ -4187,7 +4231,7 @@
       <c r="J4" s="37"/>
     </row>
     <row r="5" spans="1:10" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="73"/>
+      <c r="A5" s="92"/>
       <c r="B5" s="38" t="s">
         <v>21</v>
       </c>
@@ -4205,7 +4249,7 @@
       <c r="J5" s="38"/>
     </row>
     <row r="6" spans="1:10" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="73"/>
+      <c r="A6" s="92"/>
       <c r="B6" s="37" t="s">
         <v>22</v>
       </c>
@@ -4223,7 +4267,7 @@
       <c r="J6" s="37"/>
     </row>
     <row r="7" spans="1:10" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="73" t="s">
+      <c r="A7" s="92" t="s">
         <v>107</v>
       </c>
       <c r="B7" s="37" t="s">
@@ -4243,7 +4287,7 @@
       <c r="J7" s="37"/>
     </row>
     <row r="8" spans="1:10" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="73"/>
+      <c r="A8" s="92"/>
       <c r="B8" s="38" t="s">
         <v>19</v>
       </c>
@@ -4263,7 +4307,7 @@
       <c r="J8" s="38"/>
     </row>
     <row r="9" spans="1:10" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="73"/>
+      <c r="A9" s="92"/>
       <c r="B9" s="37" t="s">
         <v>20</v>
       </c>
@@ -4283,7 +4327,7 @@
       <c r="J9" s="37"/>
     </row>
     <row r="10" spans="1:10" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="73"/>
+      <c r="A10" s="92"/>
       <c r="B10" s="38" t="s">
         <v>21</v>
       </c>
@@ -4301,7 +4345,7 @@
       <c r="J10" s="38"/>
     </row>
     <row r="11" spans="1:10" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="73"/>
+      <c r="A11" s="92"/>
       <c r="B11" s="37" t="s">
         <v>22</v>
       </c>
@@ -4319,7 +4363,7 @@
       <c r="J11" s="37"/>
     </row>
     <row r="12" spans="1:10" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="73" t="s">
+      <c r="A12" s="92" t="s">
         <v>108</v>
       </c>
       <c r="B12" s="37" t="s">
@@ -4339,7 +4383,7 @@
       <c r="J12" s="37"/>
     </row>
     <row r="13" spans="1:10" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="73"/>
+      <c r="A13" s="92"/>
       <c r="B13" s="38" t="s">
         <v>19</v>
       </c>
@@ -4359,7 +4403,7 @@
       <c r="J13" s="38"/>
     </row>
     <row r="14" spans="1:10" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="73"/>
+      <c r="A14" s="92"/>
       <c r="B14" s="37" t="s">
         <v>20</v>
       </c>
@@ -4379,7 +4423,7 @@
       <c r="J14" s="37"/>
     </row>
     <row r="15" spans="1:10" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="73"/>
+      <c r="A15" s="92"/>
       <c r="B15" s="38" t="s">
         <v>21</v>
       </c>
@@ -4397,7 +4441,7 @@
       <c r="J15" s="38"/>
     </row>
     <row r="16" spans="1:10" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="73"/>
+      <c r="A16" s="92"/>
       <c r="B16" s="37" t="s">
         <v>22</v>
       </c>
@@ -4415,7 +4459,7 @@
       <c r="J16" s="37"/>
     </row>
     <row r="17" spans="1:10" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="73" t="s">
+      <c r="A17" s="92" t="s">
         <v>109</v>
       </c>
       <c r="B17" s="37" t="s">
@@ -4435,7 +4479,7 @@
       <c r="J17" s="37"/>
     </row>
     <row r="18" spans="1:10" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="73"/>
+      <c r="A18" s="92"/>
       <c r="B18" s="38" t="s">
         <v>19</v>
       </c>
@@ -4455,7 +4499,7 @@
       <c r="J18" s="38"/>
     </row>
     <row r="19" spans="1:10" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="73"/>
+      <c r="A19" s="92"/>
       <c r="B19" s="37" t="s">
         <v>20</v>
       </c>
@@ -4475,7 +4519,7 @@
       <c r="J19" s="37"/>
     </row>
     <row r="20" spans="1:10" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="73"/>
+      <c r="A20" s="92"/>
       <c r="B20" s="38" t="s">
         <v>21</v>
       </c>
@@ -4493,7 +4537,7 @@
       <c r="J20" s="38"/>
     </row>
     <row r="21" spans="1:10" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="73"/>
+      <c r="A21" s="92"/>
       <c r="B21" s="37" t="s">
         <v>22</v>
       </c>
@@ -4511,7 +4555,7 @@
       <c r="J21" s="37"/>
     </row>
     <row r="22" spans="1:10" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="73" t="s">
+      <c r="A22" s="92" t="s">
         <v>110</v>
       </c>
       <c r="B22" s="37" t="s">
@@ -4531,7 +4575,7 @@
       <c r="J22" s="37"/>
     </row>
     <row r="23" spans="1:10" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="73"/>
+      <c r="A23" s="92"/>
       <c r="B23" s="38" t="s">
         <v>19</v>
       </c>
@@ -4551,7 +4595,7 @@
       <c r="J23" s="38"/>
     </row>
     <row r="24" spans="1:10" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="73"/>
+      <c r="A24" s="92"/>
       <c r="B24" s="37" t="s">
         <v>20</v>
       </c>
@@ -4571,7 +4615,7 @@
       <c r="J24" s="37"/>
     </row>
     <row r="25" spans="1:10" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="73"/>
+      <c r="A25" s="92"/>
       <c r="B25" s="38" t="s">
         <v>21</v>
       </c>
@@ -4589,7 +4633,7 @@
       <c r="J25" s="38"/>
     </row>
     <row r="26" spans="1:10" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="73"/>
+      <c r="A26" s="92"/>
       <c r="B26" s="37" t="s">
         <v>22</v>
       </c>
@@ -4607,7 +4651,7 @@
       <c r="J26" s="37"/>
     </row>
     <row r="27" spans="1:10" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="73" t="s">
+      <c r="A27" s="92" t="s">
         <v>111</v>
       </c>
       <c r="B27" s="37" t="s">
@@ -4627,7 +4671,7 @@
       <c r="J27" s="37"/>
     </row>
     <row r="28" spans="1:10" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="73"/>
+      <c r="A28" s="92"/>
       <c r="B28" s="38" t="s">
         <v>19</v>
       </c>
@@ -4647,7 +4691,7 @@
       <c r="J28" s="38"/>
     </row>
     <row r="29" spans="1:10" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="73"/>
+      <c r="A29" s="92"/>
       <c r="B29" s="37" t="s">
         <v>20</v>
       </c>
@@ -4667,7 +4711,7 @@
       <c r="J29" s="37"/>
     </row>
     <row r="30" spans="1:10" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="73"/>
+      <c r="A30" s="92"/>
       <c r="B30" s="38" t="s">
         <v>21</v>
       </c>
@@ -4685,7 +4729,7 @@
       <c r="J30" s="38"/>
     </row>
     <row r="31" spans="1:10" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="73"/>
+      <c r="A31" s="92"/>
       <c r="B31" s="37" t="s">
         <v>22</v>
       </c>
@@ -4736,24 +4780,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="76" t="s">
+      <c r="A1" s="95" t="s">
         <v>40</v>
       </c>
-      <c r="B1" s="77"/>
-      <c r="C1" s="77"/>
-      <c r="D1" s="77"/>
-      <c r="E1" s="77"/>
-      <c r="F1" s="77"/>
+      <c r="B1" s="96"/>
+      <c r="C1" s="96"/>
+      <c r="D1" s="96"/>
+      <c r="E1" s="96"/>
+      <c r="F1" s="96"/>
     </row>
     <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="78" t="s">
+      <c r="A2" s="97" t="s">
         <v>41</v>
       </c>
-      <c r="B2" s="78"/>
-      <c r="C2" s="78"/>
-      <c r="D2" s="78"/>
-      <c r="E2" s="78"/>
-      <c r="F2" s="78"/>
+      <c r="B2" s="97"/>
+      <c r="C2" s="97"/>
+      <c r="D2" s="97"/>
+      <c r="E2" s="97"/>
+      <c r="F2" s="97"/>
     </row>
     <row r="3" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
@@ -4982,18 +5026,18 @@
       <c r="F15" s="29"/>
     </row>
     <row r="16" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="79" t="s">
+      <c r="A16" s="98" t="s">
         <v>60</v>
       </c>
-      <c r="B16" s="80"/>
-      <c r="C16" s="80"/>
-      <c r="D16" s="80"/>
-      <c r="E16" s="80"/>
-      <c r="F16" s="81"/>
+      <c r="B16" s="99"/>
+      <c r="C16" s="99"/>
+      <c r="D16" s="99"/>
+      <c r="E16" s="99"/>
+      <c r="F16" s="100"/>
     </row>
     <row r="17" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="74"/>
-      <c r="B17" s="75"/>
+      <c r="A17" s="93"/>
+      <c r="B17" s="94"/>
       <c r="C17" s="32" t="s">
         <v>73</v>
       </c>
@@ -5008,10 +5052,10 @@
       </c>
     </row>
     <row r="18" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="74" t="s">
+      <c r="A18" s="93" t="s">
         <v>15</v>
       </c>
-      <c r="B18" s="75"/>
+      <c r="B18" s="94"/>
       <c r="C18" s="32">
         <v>25</v>
       </c>
@@ -5075,35 +5119,35 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="76" t="s">
+      <c r="A1" s="95" t="s">
         <v>40</v>
       </c>
-      <c r="B1" s="77"/>
-      <c r="C1" s="77"/>
-      <c r="D1" s="77"/>
-      <c r="E1" s="77"/>
-      <c r="F1" s="77"/>
-      <c r="G1" s="77"/>
+      <c r="B1" s="96"/>
+      <c r="C1" s="96"/>
+      <c r="D1" s="96"/>
+      <c r="E1" s="96"/>
+      <c r="F1" s="96"/>
+      <c r="G1" s="96"/>
     </row>
     <row r="2" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="78" t="s">
+      <c r="A2" s="97" t="s">
         <v>41</v>
       </c>
-      <c r="B2" s="78"/>
-      <c r="C2" s="78"/>
-      <c r="D2" s="78"/>
-      <c r="E2" s="78"/>
-      <c r="F2" s="78"/>
-      <c r="G2" s="78"/>
+      <c r="B2" s="97"/>
+      <c r="C2" s="97"/>
+      <c r="D2" s="97"/>
+      <c r="E2" s="97"/>
+      <c r="F2" s="97"/>
+      <c r="G2" s="97"/>
     </row>
     <row r="3" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="82" t="s">
+      <c r="A3" s="101" t="s">
         <v>74</v>
       </c>
-      <c r="B3" s="82"/>
-      <c r="C3" s="82"/>
-      <c r="D3" s="82"/>
-      <c r="E3" s="82"/>
+      <c r="B3" s="101"/>
+      <c r="C3" s="101"/>
+      <c r="D3" s="101"/>
+      <c r="E3" s="101"/>
       <c r="F3" s="21" t="s">
         <v>52</v>
       </c>
@@ -5356,19 +5400,19 @@
       <c r="G15" s="29"/>
     </row>
     <row r="16" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="79" t="s">
+      <c r="A16" s="98" t="s">
         <v>60</v>
       </c>
-      <c r="B16" s="80"/>
-      <c r="C16" s="80"/>
-      <c r="D16" s="80"/>
-      <c r="E16" s="80"/>
-      <c r="F16" s="80"/>
-      <c r="G16" s="81"/>
+      <c r="B16" s="99"/>
+      <c r="C16" s="99"/>
+      <c r="D16" s="99"/>
+      <c r="E16" s="99"/>
+      <c r="F16" s="99"/>
+      <c r="G16" s="100"/>
     </row>
     <row r="17" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="74"/>
-      <c r="B17" s="75"/>
+      <c r="A17" s="93"/>
+      <c r="B17" s="94"/>
       <c r="C17" s="32"/>
       <c r="D17" s="32" t="s">
         <v>76</v>
@@ -5384,10 +5428,10 @@
       </c>
     </row>
     <row r="18" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="74" t="s">
+      <c r="A18" s="93" t="s">
         <v>15</v>
       </c>
-      <c r="B18" s="75"/>
+      <c r="B18" s="94"/>
       <c r="C18" s="32"/>
       <c r="D18" s="32">
         <v>13</v>
@@ -5421,7 +5465,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5432,57 +5476,57 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="83" t="s">
+      <c r="A1" s="54" t="s">
         <v>145</v>
       </c>
-      <c r="B1" s="84" t="s">
+      <c r="B1" s="55" t="s">
         <v>146</v>
       </c>
-      <c r="C1" s="85" t="s">
+      <c r="C1" s="56" t="s">
         <v>149</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="83" t="s">
+      <c r="A2" s="54" t="s">
         <v>147</v>
       </c>
-      <c r="B2" s="84" t="s">
+      <c r="B2" s="55" t="s">
         <v>146</v>
       </c>
-      <c r="C2" s="85" t="s">
+      <c r="C2" s="56" t="s">
         <v>150</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="83" t="s">
+      <c r="A3" s="54" t="s">
         <v>148</v>
       </c>
-      <c r="B3" s="84" t="s">
+      <c r="B3" s="55" t="s">
         <v>146</v>
       </c>
-      <c r="C3" s="85" t="s">
+      <c r="C3" s="56" t="s">
         <v>151</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="83" t="s">
+      <c r="A4" s="54" t="s">
         <v>152</v>
       </c>
-      <c r="B4" s="84" t="s">
+      <c r="B4" s="55" t="s">
         <v>146</v>
       </c>
-      <c r="C4" s="85" t="s">
+      <c r="C4" s="56" t="s">
         <v>153</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="83" t="s">
+      <c r="A5" s="54" t="s">
         <v>81</v>
       </c>
-      <c r="B5" s="84" t="s">
+      <c r="B5" s="55" t="s">
         <v>146</v>
       </c>
-      <c r="C5" s="85" t="s">
+      <c r="C5" s="56" t="s">
         <v>154</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Academic Exam and Result created and modified
</commit_message>
<xml_diff>
--- a/Resources/Layout.xlsx
+++ b/Resources/Layout.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24332"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81D82C1D-1DFC-4B12-B2F8-34D36D79A82D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09C768F6-C7A1-4003-90B5-CFBD0C8C5C5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1950" yWindow="1950" windowWidth="21600" windowHeight="11475" firstSheet="5" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15960" firstSheet="3" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,8 @@
     <sheet name="Student Attendance" sheetId="4" r:id="rId7"/>
     <sheet name="Employee Attendance" sheetId="5" r:id="rId8"/>
     <sheet name="Exam Create" sheetId="9" r:id="rId9"/>
-    <sheet name="OffDays" sheetId="11" r:id="rId10"/>
+    <sheet name="Rpt Student List" sheetId="12" r:id="rId10"/>
+    <sheet name="OffDays" sheetId="11" r:id="rId11"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="6">'Student Attendance'!$A$1:$F$20</definedName>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="473" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="515" uniqueCount="214">
   <si>
     <t>Date</t>
   </si>
@@ -612,6 +613,96 @@
   <si>
     <t>OffDay Type</t>
   </si>
+  <si>
+    <t>Pirgacha, Rangpur</t>
+  </si>
+  <si>
+    <t>Student List</t>
+  </si>
+  <si>
+    <t>Session</t>
+  </si>
+  <si>
+    <t>Section</t>
+  </si>
+  <si>
+    <t>Father Name</t>
+  </si>
+  <si>
+    <t>Mother Name</t>
+  </si>
+  <si>
+    <t>Gender</t>
+  </si>
+  <si>
+    <t>DOB</t>
+  </si>
+  <si>
+    <t>Religion</t>
+  </si>
+  <si>
+    <t>Blood Group</t>
+  </si>
+  <si>
+    <t>Class Six(6)</t>
+  </si>
+  <si>
+    <t>Total = 100</t>
+  </si>
+  <si>
+    <t>ANURADHA CHOWHAN</t>
+  </si>
+  <si>
+    <t>PORESH CHOWHAN</t>
+  </si>
+  <si>
+    <t>1717259984</t>
+  </si>
+  <si>
+    <t>MUNNI CHOWHAN</t>
+  </si>
+  <si>
+    <t>Female</t>
+  </si>
+  <si>
+    <t>Hindu</t>
+  </si>
+  <si>
+    <t>SAFIYA AFRIN JEMI</t>
+  </si>
+  <si>
+    <t>MD SHOFIQUL ISLAM</t>
+  </si>
+  <si>
+    <t>01767295693</t>
+  </si>
+  <si>
+    <t>MST NURUNNAHAR BEGUM</t>
+  </si>
+  <si>
+    <t>01714627094</t>
+  </si>
+  <si>
+    <t>Islam</t>
+  </si>
+  <si>
+    <t>Class Six</t>
+  </si>
+  <si>
+    <t>Section A</t>
+  </si>
+  <si>
+    <t>A+</t>
+  </si>
+  <si>
+    <t>Active</t>
+  </si>
+  <si>
+    <t>2022-2024</t>
+  </si>
+  <si>
+    <t>B+</t>
+  </si>
 </sst>
 </file>
 
@@ -620,7 +711,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-409]mmmm\ d\,\ yyyy;@"/>
   </numFmts>
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -771,6 +862,27 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="11">
     <fill>
@@ -834,7 +946,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="19">
+  <borders count="24">
     <border>
       <left/>
       <right/>
@@ -1048,12 +1160,85 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="102">
+  <cellXfs count="118">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
@@ -1254,6 +1439,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1263,21 +1463,6 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1306,6 +1491,58 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" readingOrder="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" readingOrder="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="21" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" readingOrder="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1715,7 +1952,7 @@
   <dimension ref="A1:L15"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="K22" sqref="K22"/>
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1923,11 +2160,480 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8B463AB-5D43-4D17-8047-E3ADE0908B1A}">
+  <dimension ref="A1:N21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I29" sqref="I29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="26.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="6.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="103" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" s="103"/>
+      <c r="C1" s="103"/>
+      <c r="D1" s="103"/>
+      <c r="E1" s="103"/>
+      <c r="F1" s="103"/>
+      <c r="G1" s="103"/>
+      <c r="H1" s="103"/>
+      <c r="I1" s="103"/>
+      <c r="J1" s="103"/>
+      <c r="K1" s="103"/>
+      <c r="L1" s="103"/>
+      <c r="M1" s="103"/>
+      <c r="N1" s="103"/>
+    </row>
+    <row r="2" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="104" t="s">
+        <v>184</v>
+      </c>
+      <c r="B2" s="104"/>
+      <c r="C2" s="104"/>
+      <c r="D2" s="104"/>
+      <c r="E2" s="104"/>
+      <c r="F2" s="104"/>
+      <c r="G2" s="104"/>
+      <c r="H2" s="104"/>
+      <c r="I2" s="104"/>
+      <c r="J2" s="104"/>
+      <c r="K2" s="104"/>
+      <c r="L2" s="104"/>
+      <c r="M2" s="104"/>
+      <c r="N2" s="104"/>
+    </row>
+    <row r="3" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="105" t="s">
+        <v>185</v>
+      </c>
+      <c r="B3" s="106"/>
+      <c r="C3" s="106"/>
+      <c r="D3" s="106"/>
+      <c r="E3" s="106"/>
+      <c r="F3" s="106"/>
+      <c r="G3" s="106"/>
+      <c r="H3" s="106"/>
+      <c r="I3" s="106"/>
+      <c r="J3" s="106"/>
+      <c r="K3" s="106"/>
+      <c r="L3" s="106"/>
+      <c r="M3" s="106"/>
+      <c r="N3" s="107"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" s="108" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" s="108" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4" s="108" t="s">
+        <v>99</v>
+      </c>
+      <c r="D4" s="108" t="s">
+        <v>186</v>
+      </c>
+      <c r="E4" s="108" t="s">
+        <v>187</v>
+      </c>
+      <c r="F4" s="108" t="s">
+        <v>190</v>
+      </c>
+      <c r="G4" s="108" t="s">
+        <v>75</v>
+      </c>
+      <c r="H4" s="108" t="s">
+        <v>188</v>
+      </c>
+      <c r="I4" s="108" t="s">
+        <v>189</v>
+      </c>
+      <c r="J4" s="108" t="s">
+        <v>62</v>
+      </c>
+      <c r="K4" s="108" t="s">
+        <v>191</v>
+      </c>
+      <c r="L4" s="108" t="s">
+        <v>192</v>
+      </c>
+      <c r="M4" s="108" t="s">
+        <v>193</v>
+      </c>
+      <c r="N4" s="108" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="112" t="s">
+        <v>194</v>
+      </c>
+      <c r="B5" s="112"/>
+      <c r="C5" s="112"/>
+      <c r="D5" s="112"/>
+      <c r="E5" s="112"/>
+      <c r="F5" s="112"/>
+      <c r="G5" s="112"/>
+      <c r="H5" s="112"/>
+      <c r="I5" s="112"/>
+      <c r="J5" s="112"/>
+      <c r="K5" s="112"/>
+      <c r="L5" s="112"/>
+      <c r="M5" s="113" t="s">
+        <v>195</v>
+      </c>
+      <c r="N5" s="113"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" s="114">
+        <v>2306001</v>
+      </c>
+      <c r="B6" s="109" t="s">
+        <v>196</v>
+      </c>
+      <c r="C6" s="110" t="s">
+        <v>208</v>
+      </c>
+      <c r="D6" s="102" t="s">
+        <v>150</v>
+      </c>
+      <c r="E6" s="102" t="s">
+        <v>209</v>
+      </c>
+      <c r="F6" s="102" t="s">
+        <v>200</v>
+      </c>
+      <c r="G6" s="110" t="s">
+        <v>198</v>
+      </c>
+      <c r="H6" s="110" t="s">
+        <v>197</v>
+      </c>
+      <c r="I6" s="110" t="s">
+        <v>199</v>
+      </c>
+      <c r="J6" s="114">
+        <v>1717259984</v>
+      </c>
+      <c r="K6" s="111">
+        <v>39165</v>
+      </c>
+      <c r="L6" s="102" t="s">
+        <v>201</v>
+      </c>
+      <c r="M6" s="110" t="s">
+        <v>210</v>
+      </c>
+      <c r="N6" s="110" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7" s="114">
+        <v>2306002</v>
+      </c>
+      <c r="B7" s="114" t="s">
+        <v>202</v>
+      </c>
+      <c r="C7" s="114" t="s">
+        <v>208</v>
+      </c>
+      <c r="D7" s="115" t="s">
+        <v>212</v>
+      </c>
+      <c r="E7" s="115" t="s">
+        <v>209</v>
+      </c>
+      <c r="F7" s="114" t="s">
+        <v>200</v>
+      </c>
+      <c r="G7" s="114" t="s">
+        <v>206</v>
+      </c>
+      <c r="H7" s="114" t="s">
+        <v>203</v>
+      </c>
+      <c r="I7" s="114" t="s">
+        <v>205</v>
+      </c>
+      <c r="J7" s="114" t="s">
+        <v>204</v>
+      </c>
+      <c r="K7" s="116">
+        <v>42686</v>
+      </c>
+      <c r="L7" s="114" t="s">
+        <v>207</v>
+      </c>
+      <c r="M7" s="117" t="s">
+        <v>213</v>
+      </c>
+      <c r="N7" s="117" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8" s="4"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="4"/>
+      <c r="J8" s="4"/>
+      <c r="K8" s="4"/>
+      <c r="L8" s="4"/>
+      <c r="M8" s="4"/>
+      <c r="N8" s="4"/>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A9" s="4"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="4"/>
+      <c r="J9" s="4"/>
+      <c r="K9" s="4"/>
+      <c r="L9" s="4"/>
+      <c r="M9" s="4"/>
+      <c r="N9" s="4"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10" s="4"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
+      <c r="I10" s="4"/>
+      <c r="J10" s="4"/>
+      <c r="K10" s="4"/>
+      <c r="L10" s="4"/>
+      <c r="M10" s="4"/>
+      <c r="N10" s="4"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11" s="4"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
+      <c r="I11" s="4"/>
+      <c r="J11" s="4"/>
+      <c r="K11" s="4"/>
+      <c r="L11" s="4"/>
+      <c r="M11" s="4"/>
+      <c r="N11" s="4"/>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A12" s="4"/>
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
+      <c r="I12" s="4"/>
+      <c r="J12" s="4"/>
+      <c r="K12" s="4"/>
+      <c r="L12" s="4"/>
+      <c r="M12" s="4"/>
+      <c r="N12" s="4"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13" s="4"/>
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4"/>
+      <c r="I13" s="4"/>
+      <c r="J13" s="4"/>
+      <c r="K13" s="4"/>
+      <c r="L13" s="4"/>
+      <c r="M13" s="4"/>
+      <c r="N13" s="4"/>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A14" s="4"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="4"/>
+      <c r="I14" s="4"/>
+      <c r="J14" s="4"/>
+      <c r="K14" s="4"/>
+      <c r="L14" s="4"/>
+      <c r="M14" s="4"/>
+      <c r="N14" s="4"/>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A15" s="4"/>
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="4"/>
+      <c r="H15" s="4"/>
+      <c r="I15" s="4"/>
+      <c r="J15" s="4"/>
+      <c r="K15" s="4"/>
+      <c r="L15" s="4"/>
+      <c r="M15" s="4"/>
+      <c r="N15" s="4"/>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A16" s="4"/>
+      <c r="B16" s="4"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="4"/>
+      <c r="H16" s="4"/>
+      <c r="I16" s="4"/>
+      <c r="J16" s="4"/>
+      <c r="K16" s="4"/>
+      <c r="L16" s="4"/>
+      <c r="M16" s="4"/>
+      <c r="N16" s="4"/>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A17" s="4"/>
+      <c r="B17" s="4"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="4"/>
+      <c r="I17" s="4"/>
+      <c r="J17" s="4"/>
+      <c r="K17" s="4"/>
+      <c r="L17" s="4"/>
+      <c r="M17" s="4"/>
+      <c r="N17" s="4"/>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A18" s="4"/>
+      <c r="B18" s="4"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
+      <c r="G18" s="4"/>
+      <c r="H18" s="4"/>
+      <c r="I18" s="4"/>
+      <c r="J18" s="4"/>
+      <c r="K18" s="4"/>
+      <c r="L18" s="4"/>
+      <c r="M18" s="4"/>
+      <c r="N18" s="4"/>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A19" s="4"/>
+      <c r="B19" s="4"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4"/>
+      <c r="G19" s="4"/>
+      <c r="H19" s="4"/>
+      <c r="I19" s="4"/>
+      <c r="J19" s="4"/>
+      <c r="K19" s="4"/>
+      <c r="L19" s="4"/>
+      <c r="M19" s="4"/>
+      <c r="N19" s="4"/>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A20" s="4"/>
+      <c r="B20" s="4"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="4"/>
+      <c r="G20" s="4"/>
+      <c r="H20" s="4"/>
+      <c r="I20" s="4"/>
+      <c r="J20" s="4"/>
+      <c r="K20" s="4"/>
+      <c r="L20" s="4"/>
+      <c r="M20" s="4"/>
+      <c r="N20" s="4"/>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A21" s="4"/>
+      <c r="B21" s="4"/>
+      <c r="C21" s="4"/>
+      <c r="D21" s="4"/>
+      <c r="E21" s="4"/>
+      <c r="F21" s="4"/>
+      <c r="G21" s="4"/>
+      <c r="H21" s="4"/>
+      <c r="I21" s="4"/>
+      <c r="J21" s="4"/>
+      <c r="K21" s="4"/>
+      <c r="L21" s="4"/>
+      <c r="M21" s="4"/>
+      <c r="N21" s="4"/>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="A1:N1"/>
+    <mergeCell ref="A2:N2"/>
+    <mergeCell ref="A3:N3"/>
+    <mergeCell ref="A5:L5"/>
+    <mergeCell ref="M5:N5"/>
+  </mergeCells>
+  <phoneticPr fontId="4" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{057F0B6F-9818-44F5-AA5B-A10992AB9C3A}">
   <dimension ref="A1:D1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M29" sqref="M29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3582,234 +4288,234 @@
       </c>
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A2" s="89" t="s">
+      <c r="A2" s="86" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="89"/>
-      <c r="C2" s="89"/>
-      <c r="D2" s="89"/>
-      <c r="E2" s="89"/>
-      <c r="F2" s="89"/>
-      <c r="G2" s="89"/>
-      <c r="H2" s="89"/>
-      <c r="I2" s="89"/>
-      <c r="J2" s="89"/>
-      <c r="K2" s="89"/>
-      <c r="L2" s="89"/>
-      <c r="M2" s="85" t="s">
+      <c r="B2" s="86"/>
+      <c r="C2" s="86"/>
+      <c r="D2" s="86"/>
+      <c r="E2" s="86"/>
+      <c r="F2" s="86"/>
+      <c r="G2" s="86"/>
+      <c r="H2" s="86"/>
+      <c r="I2" s="86"/>
+      <c r="J2" s="86"/>
+      <c r="K2" s="86"/>
+      <c r="L2" s="86"/>
+      <c r="M2" s="90" t="s">
         <v>23</v>
       </c>
-      <c r="N2" s="85"/>
-      <c r="O2" s="85"/>
-      <c r="P2" s="85"/>
-      <c r="Q2" s="85"/>
-      <c r="R2" s="85"/>
-      <c r="S2" s="85"/>
-      <c r="T2" s="85"/>
-      <c r="U2" s="85"/>
-      <c r="V2" s="85"/>
-      <c r="W2" s="85"/>
-      <c r="X2" s="85"/>
+      <c r="N2" s="90"/>
+      <c r="O2" s="90"/>
+      <c r="P2" s="90"/>
+      <c r="Q2" s="90"/>
+      <c r="R2" s="90"/>
+      <c r="S2" s="90"/>
+      <c r="T2" s="90"/>
+      <c r="U2" s="90"/>
+      <c r="V2" s="90"/>
+      <c r="W2" s="90"/>
+      <c r="X2" s="90"/>
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3" s="15">
         <v>1</v>
       </c>
-      <c r="B3" s="90" t="s">
+      <c r="B3" s="87" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="90"/>
-      <c r="D3" s="90"/>
+      <c r="C3" s="87"/>
+      <c r="D3" s="87"/>
       <c r="E3" s="16"/>
       <c r="F3" s="16"/>
       <c r="G3" s="16"/>
       <c r="H3" s="16"/>
       <c r="I3" s="16"/>
       <c r="J3" s="16"/>
-      <c r="K3" s="91">
+      <c r="K3" s="88">
         <v>45</v>
       </c>
-      <c r="L3" s="91"/>
+      <c r="L3" s="88"/>
       <c r="M3" s="14">
         <v>1</v>
       </c>
-      <c r="N3" s="86" t="s">
+      <c r="N3" s="91" t="s">
         <v>24</v>
       </c>
-      <c r="O3" s="86"/>
-      <c r="P3" s="86"/>
-      <c r="Q3" s="86"/>
-      <c r="R3" s="86"/>
+      <c r="O3" s="91"/>
+      <c r="P3" s="91"/>
+      <c r="Q3" s="91"/>
+      <c r="R3" s="91"/>
       <c r="S3" s="14">
         <v>6</v>
       </c>
-      <c r="T3" s="84" t="s">
+      <c r="T3" s="89" t="s">
         <v>29</v>
       </c>
-      <c r="U3" s="84"/>
-      <c r="V3" s="84"/>
-      <c r="W3" s="84"/>
-      <c r="X3" s="84"/>
+      <c r="U3" s="89"/>
+      <c r="V3" s="89"/>
+      <c r="W3" s="89"/>
+      <c r="X3" s="89"/>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" s="15">
         <v>2</v>
       </c>
-      <c r="B4" s="90" t="s">
+      <c r="B4" s="87" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="90"/>
-      <c r="D4" s="90"/>
+      <c r="C4" s="87"/>
+      <c r="D4" s="87"/>
       <c r="E4" s="15"/>
       <c r="F4" s="15"/>
       <c r="G4" s="15"/>
       <c r="H4" s="15"/>
       <c r="I4" s="15"/>
       <c r="J4" s="15"/>
-      <c r="K4" s="91">
+      <c r="K4" s="88">
         <v>46</v>
       </c>
-      <c r="L4" s="91"/>
+      <c r="L4" s="88"/>
       <c r="M4" s="14">
         <v>2</v>
       </c>
-      <c r="N4" s="86" t="s">
+      <c r="N4" s="91" t="s">
         <v>25</v>
       </c>
-      <c r="O4" s="86"/>
-      <c r="P4" s="86"/>
-      <c r="Q4" s="86"/>
-      <c r="R4" s="86"/>
+      <c r="O4" s="91"/>
+      <c r="P4" s="91"/>
+      <c r="Q4" s="91"/>
+      <c r="R4" s="91"/>
       <c r="S4" s="14">
         <v>7</v>
       </c>
-      <c r="T4" s="84" t="s">
+      <c r="T4" s="89" t="s">
         <v>29</v>
       </c>
-      <c r="U4" s="84"/>
-      <c r="V4" s="84"/>
-      <c r="W4" s="84"/>
-      <c r="X4" s="84"/>
+      <c r="U4" s="89"/>
+      <c r="V4" s="89"/>
+      <c r="W4" s="89"/>
+      <c r="X4" s="89"/>
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5" s="15">
         <v>3</v>
       </c>
-      <c r="B5" s="87" t="s">
+      <c r="B5" s="84" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="87"/>
-      <c r="D5" s="87"/>
+      <c r="C5" s="84"/>
+      <c r="D5" s="84"/>
       <c r="E5" s="15"/>
       <c r="F5" s="15"/>
       <c r="G5" s="15"/>
       <c r="H5" s="15"/>
       <c r="I5" s="15"/>
       <c r="J5" s="15"/>
-      <c r="K5" s="88">
+      <c r="K5" s="85">
         <v>47</v>
       </c>
-      <c r="L5" s="88"/>
+      <c r="L5" s="85"/>
       <c r="M5" s="14">
         <v>3</v>
       </c>
-      <c r="N5" s="86" t="s">
+      <c r="N5" s="91" t="s">
         <v>26</v>
       </c>
-      <c r="O5" s="86"/>
-      <c r="P5" s="86"/>
-      <c r="Q5" s="86"/>
-      <c r="R5" s="86"/>
+      <c r="O5" s="91"/>
+      <c r="P5" s="91"/>
+      <c r="Q5" s="91"/>
+      <c r="R5" s="91"/>
       <c r="S5" s="14">
         <v>8</v>
       </c>
-      <c r="T5" s="84" t="s">
+      <c r="T5" s="89" t="s">
         <v>29</v>
       </c>
-      <c r="U5" s="84"/>
-      <c r="V5" s="84"/>
-      <c r="W5" s="84"/>
-      <c r="X5" s="84"/>
+      <c r="U5" s="89"/>
+      <c r="V5" s="89"/>
+      <c r="W5" s="89"/>
+      <c r="X5" s="89"/>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6" s="15">
         <v>4</v>
       </c>
-      <c r="B6" s="87" t="s">
+      <c r="B6" s="84" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="87"/>
-      <c r="D6" s="87"/>
+      <c r="C6" s="84"/>
+      <c r="D6" s="84"/>
       <c r="E6" s="15"/>
       <c r="F6" s="15"/>
       <c r="G6" s="15"/>
       <c r="H6" s="15"/>
       <c r="I6" s="15"/>
       <c r="J6" s="15"/>
-      <c r="K6" s="88">
+      <c r="K6" s="85">
         <v>48</v>
       </c>
-      <c r="L6" s="88"/>
+      <c r="L6" s="85"/>
       <c r="M6" s="14">
         <v>4</v>
       </c>
-      <c r="N6" s="86" t="s">
+      <c r="N6" s="91" t="s">
         <v>27</v>
       </c>
-      <c r="O6" s="86"/>
-      <c r="P6" s="86"/>
-      <c r="Q6" s="86"/>
-      <c r="R6" s="86"/>
+      <c r="O6" s="91"/>
+      <c r="P6" s="91"/>
+      <c r="Q6" s="91"/>
+      <c r="R6" s="91"/>
       <c r="S6" s="14">
         <v>9</v>
       </c>
-      <c r="T6" s="84" t="s">
+      <c r="T6" s="89" t="s">
         <v>29</v>
       </c>
-      <c r="U6" s="84"/>
-      <c r="V6" s="84"/>
-      <c r="W6" s="84"/>
-      <c r="X6" s="84"/>
+      <c r="U6" s="89"/>
+      <c r="V6" s="89"/>
+      <c r="W6" s="89"/>
+      <c r="X6" s="89"/>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7" s="15">
         <v>5</v>
       </c>
-      <c r="B7" s="87" t="s">
+      <c r="B7" s="84" t="s">
         <v>22</v>
       </c>
-      <c r="C7" s="87"/>
-      <c r="D7" s="87"/>
+      <c r="C7" s="84"/>
+      <c r="D7" s="84"/>
       <c r="E7" s="15"/>
       <c r="F7" s="15"/>
       <c r="G7" s="15"/>
       <c r="H7" s="15"/>
       <c r="I7" s="15"/>
       <c r="J7" s="15"/>
-      <c r="K7" s="88">
+      <c r="K7" s="85">
         <v>49</v>
       </c>
-      <c r="L7" s="88"/>
+      <c r="L7" s="85"/>
       <c r="M7" s="14">
         <v>5</v>
       </c>
-      <c r="N7" s="86" t="s">
+      <c r="N7" s="91" t="s">
         <v>28</v>
       </c>
-      <c r="O7" s="86"/>
-      <c r="P7" s="86"/>
-      <c r="Q7" s="86"/>
-      <c r="R7" s="86"/>
+      <c r="O7" s="91"/>
+      <c r="P7" s="91"/>
+      <c r="Q7" s="91"/>
+      <c r="R7" s="91"/>
       <c r="S7" s="14">
         <v>10</v>
       </c>
-      <c r="T7" s="84" t="s">
+      <c r="T7" s="89" t="s">
         <v>29</v>
       </c>
-      <c r="U7" s="84"/>
-      <c r="V7" s="84"/>
-      <c r="W7" s="84"/>
-      <c r="X7" s="84"/>
+      <c r="U7" s="89"/>
+      <c r="V7" s="89"/>
+      <c r="W7" s="89"/>
+      <c r="X7" s="89"/>
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A8" s="13"/>
@@ -4021,6 +4727,17 @@
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="T7:X7"/>
+    <mergeCell ref="M2:X2"/>
+    <mergeCell ref="N3:R3"/>
+    <mergeCell ref="N4:R4"/>
+    <mergeCell ref="N5:R5"/>
+    <mergeCell ref="N6:R6"/>
+    <mergeCell ref="N7:R7"/>
+    <mergeCell ref="T3:X3"/>
+    <mergeCell ref="T4:X4"/>
+    <mergeCell ref="T5:X5"/>
+    <mergeCell ref="T6:X6"/>
     <mergeCell ref="B6:D6"/>
     <mergeCell ref="K6:L6"/>
     <mergeCell ref="B7:D7"/>
@@ -4032,17 +4749,6 @@
     <mergeCell ref="K4:L4"/>
     <mergeCell ref="B5:D5"/>
     <mergeCell ref="K5:L5"/>
-    <mergeCell ref="T7:X7"/>
-    <mergeCell ref="M2:X2"/>
-    <mergeCell ref="N3:R3"/>
-    <mergeCell ref="N4:R4"/>
-    <mergeCell ref="N5:R5"/>
-    <mergeCell ref="N6:R6"/>
-    <mergeCell ref="N7:R7"/>
-    <mergeCell ref="T3:X3"/>
-    <mergeCell ref="T4:X4"/>
-    <mergeCell ref="T5:X5"/>
-    <mergeCell ref="T6:X6"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Student payment related work done. yearlyFrequency added in studentFeeHead
</commit_message>
<xml_diff>
--- a/Resources/Layout.xlsx
+++ b/Resources/Layout.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24332"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14633309-BD91-4502-A1AA-20D0DD36E1B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32D032E1-EB80-4CAE-B557-27994395DA4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15960" firstSheet="5" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15960" firstSheet="7" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="Rpt Student List" sheetId="12" r:id="rId10"/>
     <sheet name="Rpt Student Payment " sheetId="11" r:id="rId11"/>
     <sheet name="SingleStudentResult" sheetId="13" r:id="rId12"/>
+    <sheet name="Rpt payment Receipt" sheetId="14" r:id="rId13"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="10">'Rpt Student Payment '!$A$1:$L$17</definedName>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="578" uniqueCount="259">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="596" uniqueCount="271">
   <si>
     <t>Date</t>
   </si>
@@ -873,6 +874,42 @@
   </si>
   <si>
     <t>Name of the Exam</t>
+  </si>
+  <si>
+    <t>Name of the Institutte</t>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t>Payment Receipt</t>
+  </si>
+  <si>
+    <t>Name of the Student</t>
+  </si>
+  <si>
+    <t>Student Name :</t>
+  </si>
+  <si>
+    <t>Class Roll :</t>
+  </si>
+  <si>
+    <t>Receipt No :</t>
+  </si>
+  <si>
+    <t>Academic Class :</t>
+  </si>
+  <si>
+    <t>Division :</t>
+  </si>
+  <si>
+    <t>Signature</t>
+  </si>
+  <si>
+    <t>Tk</t>
+  </si>
+  <si>
+    <t>In word:Taka One Thousand and Five Hundred only.</t>
   </si>
 </sst>
 </file>
@@ -1691,7 +1728,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="177">
+  <cellXfs count="195">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
@@ -1897,253 +1934,10 @@
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="11" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="11" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="11" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="11" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="11" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="11" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2154,8 +1948,299 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="11" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="11" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="11" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="11" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="11" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="11" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2674,28 +2759,28 @@
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="87" t="s">
+      <c r="A2" s="95" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="87"/>
-      <c r="C2" s="88" t="s">
+      <c r="B2" s="95"/>
+      <c r="C2" s="96" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="88"/>
-      <c r="E2" s="88"/>
+      <c r="D2" s="96"/>
+      <c r="E2" s="96"/>
       <c r="F2" s="12"/>
     </row>
     <row r="3" spans="1:12" s="8" customFormat="1" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F3" s="9"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="87" t="s">
+      <c r="A4" s="95" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="87"/>
-      <c r="C4" s="89"/>
-      <c r="D4" s="89"/>
-      <c r="E4" s="89"/>
+      <c r="B4" s="95"/>
+      <c r="C4" s="97"/>
+      <c r="D4" s="97"/>
+      <c r="E4" s="97"/>
       <c r="F4" s="7" t="s">
         <v>15</v>
       </c>
@@ -2710,12 +2795,12 @@
       <c r="F5" s="7"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="92" t="s">
+      <c r="A6" s="100" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="92"/>
-      <c r="C6" s="91"/>
-      <c r="D6" s="91"/>
+      <c r="B6" s="100"/>
+      <c r="C6" s="99"/>
+      <c r="D6" s="99"/>
       <c r="E6" s="11"/>
       <c r="F6" s="7" t="s">
         <v>16</v>
@@ -2725,12 +2810,12 @@
       <c r="F7" s="9"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="92" t="s">
+      <c r="A8" s="100" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="92"/>
-      <c r="C8" s="91"/>
-      <c r="D8" s="91"/>
+      <c r="B8" s="100"/>
+      <c r="C8" s="99"/>
+      <c r="D8" s="99"/>
       <c r="E8" s="10" t="s">
         <v>14</v>
       </c>
@@ -2739,13 +2824,13 @@
       <c r="F9" s="9"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="90" t="s">
+      <c r="A10" s="98" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="90"/>
-      <c r="C10" s="91"/>
-      <c r="D10" s="91"/>
-      <c r="E10" s="91"/>
+      <c r="B10" s="98"/>
+      <c r="C10" s="99"/>
+      <c r="D10" s="99"/>
+      <c r="E10" s="99"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
@@ -2858,58 +2943,58 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="123" t="s">
+      <c r="A1" s="136" t="s">
         <v>40</v>
       </c>
-      <c r="B1" s="123"/>
-      <c r="C1" s="123"/>
-      <c r="D1" s="123"/>
-      <c r="E1" s="123"/>
-      <c r="F1" s="123"/>
-      <c r="G1" s="123"/>
-      <c r="H1" s="123"/>
-      <c r="I1" s="123"/>
-      <c r="J1" s="123"/>
-      <c r="K1" s="123"/>
-      <c r="L1" s="123"/>
-      <c r="M1" s="123"/>
-      <c r="N1" s="123"/>
+      <c r="B1" s="136"/>
+      <c r="C1" s="136"/>
+      <c r="D1" s="136"/>
+      <c r="E1" s="136"/>
+      <c r="F1" s="136"/>
+      <c r="G1" s="136"/>
+      <c r="H1" s="136"/>
+      <c r="I1" s="136"/>
+      <c r="J1" s="136"/>
+      <c r="K1" s="136"/>
+      <c r="L1" s="136"/>
+      <c r="M1" s="136"/>
+      <c r="N1" s="136"/>
     </row>
     <row r="2" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="124" t="s">
+      <c r="A2" s="137" t="s">
         <v>174</v>
       </c>
-      <c r="B2" s="124"/>
-      <c r="C2" s="124"/>
-      <c r="D2" s="124"/>
-      <c r="E2" s="124"/>
-      <c r="F2" s="124"/>
-      <c r="G2" s="124"/>
-      <c r="H2" s="124"/>
-      <c r="I2" s="124"/>
-      <c r="J2" s="124"/>
-      <c r="K2" s="124"/>
-      <c r="L2" s="124"/>
-      <c r="M2" s="124"/>
-      <c r="N2" s="124"/>
+      <c r="B2" s="137"/>
+      <c r="C2" s="137"/>
+      <c r="D2" s="137"/>
+      <c r="E2" s="137"/>
+      <c r="F2" s="137"/>
+      <c r="G2" s="137"/>
+      <c r="H2" s="137"/>
+      <c r="I2" s="137"/>
+      <c r="J2" s="137"/>
+      <c r="K2" s="137"/>
+      <c r="L2" s="137"/>
+      <c r="M2" s="137"/>
+      <c r="N2" s="137"/>
     </row>
     <row r="3" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="125" t="s">
+      <c r="A3" s="138" t="s">
         <v>175</v>
       </c>
-      <c r="B3" s="126"/>
-      <c r="C3" s="126"/>
-      <c r="D3" s="126"/>
-      <c r="E3" s="126"/>
-      <c r="F3" s="126"/>
-      <c r="G3" s="126"/>
-      <c r="H3" s="126"/>
-      <c r="I3" s="126"/>
-      <c r="J3" s="126"/>
-      <c r="K3" s="126"/>
-      <c r="L3" s="126"/>
-      <c r="M3" s="126"/>
-      <c r="N3" s="127"/>
+      <c r="B3" s="139"/>
+      <c r="C3" s="139"/>
+      <c r="D3" s="139"/>
+      <c r="E3" s="139"/>
+      <c r="F3" s="139"/>
+      <c r="G3" s="139"/>
+      <c r="H3" s="139"/>
+      <c r="I3" s="139"/>
+      <c r="J3" s="139"/>
+      <c r="K3" s="139"/>
+      <c r="L3" s="139"/>
+      <c r="M3" s="139"/>
+      <c r="N3" s="140"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="65" t="s">
@@ -2956,24 +3041,24 @@
       </c>
     </row>
     <row r="5" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="128" t="s">
+      <c r="A5" s="141" t="s">
         <v>184</v>
       </c>
-      <c r="B5" s="128"/>
-      <c r="C5" s="128"/>
-      <c r="D5" s="128"/>
-      <c r="E5" s="128"/>
-      <c r="F5" s="128"/>
-      <c r="G5" s="128"/>
-      <c r="H5" s="128"/>
-      <c r="I5" s="128"/>
-      <c r="J5" s="128"/>
-      <c r="K5" s="128"/>
-      <c r="L5" s="128"/>
-      <c r="M5" s="129" t="s">
+      <c r="B5" s="141"/>
+      <c r="C5" s="141"/>
+      <c r="D5" s="141"/>
+      <c r="E5" s="141"/>
+      <c r="F5" s="141"/>
+      <c r="G5" s="141"/>
+      <c r="H5" s="141"/>
+      <c r="I5" s="141"/>
+      <c r="J5" s="141"/>
+      <c r="K5" s="141"/>
+      <c r="L5" s="141"/>
+      <c r="M5" s="142" t="s">
         <v>185</v>
       </c>
-      <c r="N5" s="129"/>
+      <c r="N5" s="142"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="69">
@@ -3327,36 +3412,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="130" t="s">
+      <c r="A1" s="143" t="s">
         <v>221</v>
       </c>
-      <c r="B1" s="131"/>
-      <c r="C1" s="131"/>
-      <c r="D1" s="131"/>
-      <c r="E1" s="131"/>
-      <c r="F1" s="131"/>
-      <c r="G1" s="131"/>
-      <c r="H1" s="131"/>
-      <c r="I1" s="131"/>
-      <c r="J1" s="131"/>
-      <c r="K1" s="131"/>
-      <c r="L1" s="132"/>
+      <c r="B1" s="144"/>
+      <c r="C1" s="144"/>
+      <c r="D1" s="144"/>
+      <c r="E1" s="144"/>
+      <c r="F1" s="144"/>
+      <c r="G1" s="144"/>
+      <c r="H1" s="144"/>
+      <c r="I1" s="144"/>
+      <c r="J1" s="144"/>
+      <c r="K1" s="144"/>
+      <c r="L1" s="145"/>
     </row>
     <row r="2" spans="1:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="133" t="s">
+      <c r="A2" s="146" t="s">
         <v>222</v>
       </c>
-      <c r="B2" s="134"/>
-      <c r="C2" s="134"/>
-      <c r="D2" s="134"/>
-      <c r="E2" s="134"/>
-      <c r="F2" s="134"/>
-      <c r="G2" s="134"/>
-      <c r="H2" s="134"/>
-      <c r="I2" s="134"/>
-      <c r="J2" s="134"/>
-      <c r="K2" s="134"/>
-      <c r="L2" s="135"/>
+      <c r="B2" s="147"/>
+      <c r="C2" s="147"/>
+      <c r="D2" s="147"/>
+      <c r="E2" s="147"/>
+      <c r="F2" s="147"/>
+      <c r="G2" s="147"/>
+      <c r="H2" s="147"/>
+      <c r="I2" s="147"/>
+      <c r="J2" s="147"/>
+      <c r="K2" s="147"/>
+      <c r="L2" s="148"/>
     </row>
     <row r="3" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="74" t="s">
@@ -3377,32 +3462,32 @@
       <c r="F3" s="74" t="s">
         <v>219</v>
       </c>
-      <c r="G3" s="143" t="s">
+      <c r="G3" s="156" t="s">
         <v>39</v>
       </c>
-      <c r="H3" s="144"/>
-      <c r="I3" s="144"/>
-      <c r="J3" s="144"/>
-      <c r="K3" s="145"/>
+      <c r="H3" s="157"/>
+      <c r="I3" s="157"/>
+      <c r="J3" s="157"/>
+      <c r="K3" s="158"/>
       <c r="L3" s="85" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="149" t="s">
+      <c r="A4" s="162" t="s">
         <v>223</v>
       </c>
-      <c r="B4" s="150"/>
-      <c r="C4" s="150"/>
-      <c r="D4" s="150"/>
-      <c r="E4" s="150"/>
-      <c r="F4" s="150"/>
-      <c r="G4" s="150"/>
-      <c r="H4" s="150"/>
-      <c r="I4" s="150"/>
-      <c r="J4" s="150"/>
-      <c r="K4" s="150"/>
-      <c r="L4" s="151"/>
+      <c r="B4" s="163"/>
+      <c r="C4" s="163"/>
+      <c r="D4" s="163"/>
+      <c r="E4" s="163"/>
+      <c r="F4" s="163"/>
+      <c r="G4" s="163"/>
+      <c r="H4" s="163"/>
+      <c r="I4" s="163"/>
+      <c r="J4" s="163"/>
+      <c r="K4" s="163"/>
+      <c r="L4" s="164"/>
     </row>
     <row r="5" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="80">
@@ -3423,13 +3508,13 @@
       <c r="F5" s="83">
         <v>235689</v>
       </c>
-      <c r="G5" s="146" t="s">
+      <c r="G5" s="159" t="s">
         <v>213</v>
       </c>
-      <c r="H5" s="147"/>
-      <c r="I5" s="147"/>
-      <c r="J5" s="147"/>
-      <c r="K5" s="148"/>
+      <c r="H5" s="160"/>
+      <c r="I5" s="160"/>
+      <c r="J5" s="160"/>
+      <c r="K5" s="161"/>
       <c r="L5" s="81">
         <v>800</v>
       </c>
@@ -3453,13 +3538,13 @@
       <c r="F6" s="83">
         <v>235687</v>
       </c>
-      <c r="G6" s="146" t="s">
+      <c r="G6" s="159" t="s">
         <v>9</v>
       </c>
-      <c r="H6" s="147"/>
-      <c r="I6" s="147"/>
-      <c r="J6" s="147"/>
-      <c r="K6" s="148"/>
+      <c r="H6" s="160"/>
+      <c r="I6" s="160"/>
+      <c r="J6" s="160"/>
+      <c r="K6" s="161"/>
       <c r="L6" s="81">
         <v>1500</v>
       </c>
@@ -3483,51 +3568,51 @@
       <c r="F7" s="83">
         <v>235686</v>
       </c>
-      <c r="G7" s="146" t="s">
+      <c r="G7" s="159" t="s">
         <v>217</v>
       </c>
-      <c r="H7" s="147"/>
-      <c r="I7" s="147"/>
-      <c r="J7" s="147"/>
-      <c r="K7" s="148"/>
+      <c r="H7" s="160"/>
+      <c r="I7" s="160"/>
+      <c r="J7" s="160"/>
+      <c r="K7" s="161"/>
       <c r="L7" s="81">
         <v>1600</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="136" t="s">
+      <c r="A8" s="149" t="s">
         <v>212</v>
       </c>
-      <c r="B8" s="136"/>
-      <c r="C8" s="136"/>
-      <c r="D8" s="136"/>
-      <c r="E8" s="136"/>
-      <c r="F8" s="136"/>
-      <c r="G8" s="136"/>
-      <c r="H8" s="136"/>
-      <c r="I8" s="136"/>
-      <c r="J8" s="136"/>
-      <c r="K8" s="136"/>
+      <c r="B8" s="149"/>
+      <c r="C8" s="149"/>
+      <c r="D8" s="149"/>
+      <c r="E8" s="149"/>
+      <c r="F8" s="149"/>
+      <c r="G8" s="149"/>
+      <c r="H8" s="149"/>
+      <c r="I8" s="149"/>
+      <c r="J8" s="149"/>
+      <c r="K8" s="149"/>
       <c r="L8" s="75">
         <f t="shared" ref="L8" si="0">SUM(L5:L7)</f>
         <v>3900</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="149" t="s">
+      <c r="A9" s="162" t="s">
         <v>224</v>
       </c>
-      <c r="B9" s="150"/>
-      <c r="C9" s="150"/>
-      <c r="D9" s="150"/>
-      <c r="E9" s="150"/>
-      <c r="F9" s="150"/>
-      <c r="G9" s="150"/>
-      <c r="H9" s="150"/>
-      <c r="I9" s="150"/>
-      <c r="J9" s="150"/>
-      <c r="K9" s="150"/>
-      <c r="L9" s="151"/>
+      <c r="B9" s="163"/>
+      <c r="C9" s="163"/>
+      <c r="D9" s="163"/>
+      <c r="E9" s="163"/>
+      <c r="F9" s="163"/>
+      <c r="G9" s="163"/>
+      <c r="H9" s="163"/>
+      <c r="I9" s="163"/>
+      <c r="J9" s="163"/>
+      <c r="K9" s="163"/>
+      <c r="L9" s="164"/>
     </row>
     <row r="10" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="80">
@@ -3548,13 +3633,13 @@
       <c r="F10" s="84">
         <v>215496</v>
       </c>
-      <c r="G10" s="146" t="s">
+      <c r="G10" s="159" t="s">
         <v>216</v>
       </c>
-      <c r="H10" s="147"/>
-      <c r="I10" s="147"/>
-      <c r="J10" s="147"/>
-      <c r="K10" s="148"/>
+      <c r="H10" s="160"/>
+      <c r="I10" s="160"/>
+      <c r="J10" s="160"/>
+      <c r="K10" s="161"/>
       <c r="L10" s="81">
         <v>1000</v>
       </c>
@@ -3578,50 +3663,50 @@
       <c r="F11" s="84">
         <v>124586</v>
       </c>
-      <c r="G11" s="146" t="s">
+      <c r="G11" s="159" t="s">
         <v>216</v>
       </c>
-      <c r="H11" s="147"/>
-      <c r="I11" s="147"/>
-      <c r="J11" s="147"/>
-      <c r="K11" s="148"/>
+      <c r="H11" s="160"/>
+      <c r="I11" s="160"/>
+      <c r="J11" s="160"/>
+      <c r="K11" s="161"/>
       <c r="L11" s="81">
         <v>2000</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="152" t="s">
+      <c r="A12" s="165" t="s">
         <v>212</v>
       </c>
-      <c r="B12" s="153"/>
-      <c r="C12" s="153"/>
-      <c r="D12" s="153"/>
-      <c r="E12" s="153"/>
-      <c r="F12" s="153"/>
-      <c r="G12" s="153"/>
-      <c r="H12" s="153"/>
-      <c r="I12" s="153"/>
-      <c r="J12" s="153"/>
-      <c r="K12" s="154"/>
+      <c r="B12" s="166"/>
+      <c r="C12" s="166"/>
+      <c r="D12" s="166"/>
+      <c r="E12" s="166"/>
+      <c r="F12" s="166"/>
+      <c r="G12" s="166"/>
+      <c r="H12" s="166"/>
+      <c r="I12" s="166"/>
+      <c r="J12" s="166"/>
+      <c r="K12" s="167"/>
       <c r="L12" s="76">
         <v>3000</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="149" t="s">
+      <c r="A13" s="162" t="s">
         <v>225</v>
       </c>
-      <c r="B13" s="150"/>
-      <c r="C13" s="150"/>
-      <c r="D13" s="150"/>
-      <c r="E13" s="150"/>
-      <c r="F13" s="150"/>
-      <c r="G13" s="150"/>
-      <c r="H13" s="150"/>
-      <c r="I13" s="150"/>
-      <c r="J13" s="150"/>
-      <c r="K13" s="150"/>
-      <c r="L13" s="151"/>
+      <c r="B13" s="163"/>
+      <c r="C13" s="163"/>
+      <c r="D13" s="163"/>
+      <c r="E13" s="163"/>
+      <c r="F13" s="163"/>
+      <c r="G13" s="163"/>
+      <c r="H13" s="163"/>
+      <c r="I13" s="163"/>
+      <c r="J13" s="163"/>
+      <c r="K13" s="163"/>
+      <c r="L13" s="164"/>
     </row>
     <row r="14" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="80">
@@ -3642,49 +3727,49 @@
       <c r="F14" s="84">
         <v>965241</v>
       </c>
-      <c r="G14" s="146" t="s">
+      <c r="G14" s="159" t="s">
         <v>220</v>
       </c>
-      <c r="H14" s="147"/>
-      <c r="I14" s="147"/>
-      <c r="J14" s="147"/>
-      <c r="K14" s="148"/>
+      <c r="H14" s="160"/>
+      <c r="I14" s="160"/>
+      <c r="J14" s="160"/>
+      <c r="K14" s="161"/>
       <c r="L14" s="81">
         <v>1200</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="137" t="s">
+      <c r="A15" s="150" t="s">
         <v>212</v>
       </c>
-      <c r="B15" s="138"/>
-      <c r="C15" s="138"/>
-      <c r="D15" s="138"/>
-      <c r="E15" s="138"/>
-      <c r="F15" s="138"/>
-      <c r="G15" s="138"/>
-      <c r="H15" s="138"/>
-      <c r="I15" s="138"/>
-      <c r="J15" s="138"/>
-      <c r="K15" s="139"/>
+      <c r="B15" s="151"/>
+      <c r="C15" s="151"/>
+      <c r="D15" s="151"/>
+      <c r="E15" s="151"/>
+      <c r="F15" s="151"/>
+      <c r="G15" s="151"/>
+      <c r="H15" s="151"/>
+      <c r="I15" s="151"/>
+      <c r="J15" s="151"/>
+      <c r="K15" s="152"/>
       <c r="L15" s="79">
         <v>1200</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="21" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="140" t="s">
+      <c r="A16" s="153" t="s">
         <v>226</v>
       </c>
-      <c r="B16" s="141"/>
-      <c r="C16" s="141"/>
-      <c r="D16" s="141"/>
-      <c r="E16" s="141"/>
-      <c r="F16" s="141"/>
-      <c r="G16" s="141"/>
-      <c r="H16" s="141"/>
-      <c r="I16" s="141"/>
-      <c r="J16" s="141"/>
-      <c r="K16" s="142"/>
+      <c r="B16" s="154"/>
+      <c r="C16" s="154"/>
+      <c r="D16" s="154"/>
+      <c r="E16" s="154"/>
+      <c r="F16" s="154"/>
+      <c r="G16" s="154"/>
+      <c r="H16" s="154"/>
+      <c r="I16" s="154"/>
+      <c r="J16" s="154"/>
+      <c r="K16" s="155"/>
       <c r="L16" s="77">
         <f>L8+L12+L15</f>
         <v>8100</v>
@@ -3740,10 +3825,10 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:10" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="161"/>
-      <c r="B1" s="161"/>
-      <c r="C1" s="161"/>
-      <c r="D1" s="161"/>
+      <c r="A1" s="135"/>
+      <c r="B1" s="135"/>
+      <c r="C1" s="135"/>
+      <c r="D1" s="135"/>
       <c r="E1" s="168" t="s">
         <v>227</v>
       </c>
@@ -3754,10 +3839,10 @@
       <c r="J1" s="168"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="161"/>
-      <c r="B2" s="161"/>
-      <c r="C2" s="161"/>
-      <c r="D2" s="161"/>
+      <c r="A2" s="135"/>
+      <c r="B2" s="135"/>
+      <c r="C2" s="135"/>
+      <c r="D2" s="135"/>
       <c r="E2" s="169" t="s">
         <v>257</v>
       </c>
@@ -3768,10 +3853,10 @@
       <c r="J2" s="169"/>
     </row>
     <row r="3" spans="1:10" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="162"/>
-      <c r="B3" s="162"/>
-      <c r="C3" s="162"/>
-      <c r="D3" s="162"/>
+      <c r="A3" s="174"/>
+      <c r="B3" s="174"/>
+      <c r="C3" s="174"/>
+      <c r="D3" s="174"/>
       <c r="E3" s="170" t="s">
         <v>228</v>
       </c>
@@ -3782,92 +3867,92 @@
       <c r="J3" s="170"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="156" t="s">
+      <c r="A4" s="132" t="s">
         <v>229</v>
       </c>
-      <c r="B4" s="156"/>
-      <c r="C4" s="156"/>
-      <c r="D4" s="156"/>
-      <c r="E4" s="156"/>
-      <c r="F4" s="156"/>
-      <c r="G4" s="156"/>
-      <c r="H4" s="156"/>
-      <c r="I4" s="156"/>
-      <c r="J4" s="156"/>
+      <c r="B4" s="132"/>
+      <c r="C4" s="132"/>
+      <c r="D4" s="132"/>
+      <c r="E4" s="132"/>
+      <c r="F4" s="132"/>
+      <c r="G4" s="132"/>
+      <c r="H4" s="132"/>
+      <c r="I4" s="132"/>
+      <c r="J4" s="132"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="157" t="s">
+      <c r="A5" s="172" t="s">
         <v>250</v>
       </c>
-      <c r="B5" s="157"/>
-      <c r="C5" s="157" t="s">
+      <c r="B5" s="172"/>
+      <c r="C5" s="172" t="s">
         <v>255</v>
       </c>
-      <c r="D5" s="157"/>
-      <c r="E5" s="157"/>
-      <c r="F5" s="157"/>
+      <c r="D5" s="172"/>
+      <c r="E5" s="172"/>
+      <c r="F5" s="172"/>
       <c r="G5" s="86"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="155" t="s">
+      <c r="A6" s="171" t="s">
         <v>146</v>
       </c>
-      <c r="B6" s="155"/>
-      <c r="C6" s="155" t="s">
+      <c r="B6" s="171"/>
+      <c r="C6" s="171" t="s">
         <v>251</v>
       </c>
-      <c r="D6" s="155"/>
-      <c r="E6" s="155"/>
-      <c r="F6" s="155"/>
-      <c r="G6" s="155" t="s">
+      <c r="D6" s="171"/>
+      <c r="E6" s="171"/>
+      <c r="F6" s="171"/>
+      <c r="G6" s="171" t="s">
         <v>145</v>
       </c>
-      <c r="H6" s="155"/>
-      <c r="I6" s="155" t="s">
+      <c r="H6" s="171"/>
+      <c r="I6" s="171" t="s">
         <v>256</v>
       </c>
-      <c r="J6" s="155"/>
+      <c r="J6" s="171"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="155" t="s">
+      <c r="A7" s="171" t="s">
         <v>35</v>
       </c>
-      <c r="B7" s="155"/>
-      <c r="C7" s="155" t="s">
+      <c r="B7" s="171"/>
+      <c r="C7" s="171" t="s">
         <v>252</v>
       </c>
-      <c r="D7" s="155"/>
+      <c r="D7" s="171"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="155" t="s">
+      <c r="A8" s="171" t="s">
         <v>230</v>
       </c>
-      <c r="B8" s="155"/>
-      <c r="C8" s="163" t="s">
+      <c r="B8" s="171"/>
+      <c r="C8" s="175" t="s">
         <v>253</v>
       </c>
-      <c r="D8" s="163"/>
+      <c r="D8" s="175"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="155" t="s">
+      <c r="A9" s="171" t="s">
         <v>231</v>
       </c>
-      <c r="B9" s="155"/>
-      <c r="C9" s="164" t="s">
+      <c r="B9" s="171"/>
+      <c r="C9" s="176" t="s">
         <v>254</v>
       </c>
-      <c r="D9" s="164"/>
-      <c r="E9" s="164"/>
+      <c r="D9" s="176"/>
+      <c r="E9" s="176"/>
     </row>
     <row r="10" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="55" t="s">
         <v>233</v>
       </c>
-      <c r="B10" s="165" t="s">
+      <c r="B10" s="177" t="s">
         <v>232</v>
       </c>
-      <c r="C10" s="166"/>
-      <c r="D10" s="167"/>
+      <c r="C10" s="178"/>
+      <c r="D10" s="179"/>
       <c r="E10" s="55" t="s">
         <v>15</v>
       </c>
@@ -3891,11 +3976,11 @@
       <c r="A11" s="55">
         <v>101</v>
       </c>
-      <c r="B11" s="158" t="s">
+      <c r="B11" s="131" t="s">
         <v>234</v>
       </c>
-      <c r="C11" s="156"/>
-      <c r="D11" s="159"/>
+      <c r="C11" s="132"/>
+      <c r="D11" s="133"/>
       <c r="E11" s="55">
         <v>50</v>
       </c>
@@ -3916,11 +4001,11 @@
       <c r="A12" s="55">
         <v>102</v>
       </c>
-      <c r="B12" s="158" t="s">
+      <c r="B12" s="131" t="s">
         <v>235</v>
       </c>
-      <c r="C12" s="156"/>
-      <c r="D12" s="159"/>
+      <c r="C12" s="132"/>
+      <c r="D12" s="133"/>
       <c r="E12" s="55">
         <v>50</v>
       </c>
@@ -3941,11 +4026,11 @@
       <c r="A13" s="55">
         <v>103</v>
       </c>
-      <c r="B13" s="158" t="s">
+      <c r="B13" s="131" t="s">
         <v>236</v>
       </c>
-      <c r="C13" s="156"/>
-      <c r="D13" s="159"/>
+      <c r="C13" s="132"/>
+      <c r="D13" s="133"/>
       <c r="E13" s="55">
         <v>50</v>
       </c>
@@ -3966,11 +4051,11 @@
       <c r="A14" s="55">
         <v>104</v>
       </c>
-      <c r="B14" s="158" t="s">
+      <c r="B14" s="131" t="s">
         <v>237</v>
       </c>
-      <c r="C14" s="156"/>
-      <c r="D14" s="159"/>
+      <c r="C14" s="132"/>
+      <c r="D14" s="133"/>
       <c r="E14" s="55">
         <v>50</v>
       </c>
@@ -3991,11 +4076,11 @@
       <c r="A15" s="55">
         <v>105</v>
       </c>
-      <c r="B15" s="158" t="s">
+      <c r="B15" s="131" t="s">
         <v>238</v>
       </c>
-      <c r="C15" s="156"/>
-      <c r="D15" s="159"/>
+      <c r="C15" s="132"/>
+      <c r="D15" s="133"/>
       <c r="E15" s="55">
         <v>50</v>
       </c>
@@ -4016,11 +4101,11 @@
       <c r="A16" s="55">
         <v>106</v>
       </c>
-      <c r="B16" s="158" t="s">
+      <c r="B16" s="131" t="s">
         <v>239</v>
       </c>
-      <c r="C16" s="156"/>
-      <c r="D16" s="159"/>
+      <c r="C16" s="132"/>
+      <c r="D16" s="133"/>
       <c r="E16" s="55">
         <v>50</v>
       </c>
@@ -4041,11 +4126,11 @@
       <c r="A17" s="55">
         <v>107</v>
       </c>
-      <c r="B17" s="158" t="s">
+      <c r="B17" s="131" t="s">
         <v>240</v>
       </c>
-      <c r="C17" s="156"/>
-      <c r="D17" s="159"/>
+      <c r="C17" s="132"/>
+      <c r="D17" s="133"/>
       <c r="E17" s="55">
         <v>50</v>
       </c>
@@ -4066,11 +4151,11 @@
       <c r="A18" s="55">
         <v>108</v>
       </c>
-      <c r="B18" s="158" t="s">
+      <c r="B18" s="131" t="s">
         <v>241</v>
       </c>
-      <c r="C18" s="156"/>
-      <c r="D18" s="159"/>
+      <c r="C18" s="132"/>
+      <c r="D18" s="133"/>
       <c r="E18" s="55">
         <v>50</v>
       </c>
@@ -4091,11 +4176,11 @@
       <c r="A19" s="55">
         <v>109</v>
       </c>
-      <c r="B19" s="158" t="s">
+      <c r="B19" s="131" t="s">
         <v>242</v>
       </c>
-      <c r="C19" s="156"/>
-      <c r="D19" s="159"/>
+      <c r="C19" s="132"/>
+      <c r="D19" s="133"/>
       <c r="E19" s="55">
         <v>50</v>
       </c>
@@ -4116,11 +4201,11 @@
       <c r="A20" s="55">
         <v>110</v>
       </c>
-      <c r="B20" s="158" t="s">
+      <c r="B20" s="131" t="s">
         <v>243</v>
       </c>
-      <c r="C20" s="156"/>
-      <c r="D20" s="159"/>
+      <c r="C20" s="132"/>
+      <c r="D20" s="133"/>
       <c r="E20" s="55">
         <v>50</v>
       </c>
@@ -4141,11 +4226,11 @@
       <c r="A21" s="55">
         <v>111</v>
       </c>
-      <c r="B21" s="158" t="s">
+      <c r="B21" s="131" t="s">
         <v>244</v>
       </c>
-      <c r="C21" s="156"/>
-      <c r="D21" s="159"/>
+      <c r="C21" s="132"/>
+      <c r="D21" s="133"/>
       <c r="E21" s="55">
         <v>50</v>
       </c>
@@ -4163,12 +4248,12 @@
       <c r="J21" s="4"/>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="160" t="s">
+      <c r="A22" s="173" t="s">
         <v>248</v>
       </c>
-      <c r="B22" s="160"/>
-      <c r="C22" s="160"/>
-      <c r="D22" s="160"/>
+      <c r="B22" s="173"/>
+      <c r="C22" s="173"/>
+      <c r="D22" s="173"/>
       <c r="E22" s="86">
         <f>SUM(E11:E21)</f>
         <v>550</v>
@@ -4180,14 +4265,12 @@
     </row>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="E1:J1"/>
-    <mergeCell ref="E2:J2"/>
-    <mergeCell ref="E3:J3"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="C6:F6"/>
-    <mergeCell ref="C5:F5"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="I6:J6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A6:B6"/>
     <mergeCell ref="B19:D19"/>
     <mergeCell ref="B20:D20"/>
     <mergeCell ref="B21:D21"/>
@@ -4204,17 +4287,254 @@
     <mergeCell ref="B16:D16"/>
     <mergeCell ref="B17:D17"/>
     <mergeCell ref="B18:D18"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="E1:J1"/>
+    <mergeCell ref="E2:J2"/>
+    <mergeCell ref="E3:J3"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="C6:F6"/>
+    <mergeCell ref="C5:F5"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="I6:J6"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0D3CB5C-E45F-4446-A4A9-5BAE1F767FB0}">
+  <dimension ref="A1:J14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O9" sqref="O9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="7.42578125" customWidth="1"/>
+    <col min="3" max="3" width="7.28515625" customWidth="1"/>
+    <col min="4" max="4" width="6.85546875" customWidth="1"/>
+    <col min="6" max="6" width="6.42578125" customWidth="1"/>
+    <col min="7" max="7" width="13.42578125" customWidth="1"/>
+    <col min="8" max="8" width="7.85546875" customWidth="1"/>
+    <col min="10" max="10" width="3" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A1" s="183" t="s">
+        <v>259</v>
+      </c>
+      <c r="B1" s="183"/>
+      <c r="C1" s="183"/>
+      <c r="D1" s="183"/>
+      <c r="E1" s="183"/>
+      <c r="F1" s="183"/>
+      <c r="G1" s="183"/>
+      <c r="H1" s="183"/>
+      <c r="I1" s="183"/>
+      <c r="J1" s="183"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="182" t="s">
+        <v>260</v>
+      </c>
+      <c r="B2" s="182"/>
+      <c r="C2" s="182"/>
+      <c r="D2" s="182"/>
+      <c r="E2" s="182"/>
+      <c r="F2" s="182"/>
+      <c r="G2" s="182"/>
+      <c r="H2" s="182"/>
+      <c r="I2" s="182"/>
+      <c r="J2" s="182"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="132" t="s">
+        <v>261</v>
+      </c>
+      <c r="B3" s="132"/>
+      <c r="C3" s="132"/>
+      <c r="D3" s="132"/>
+      <c r="E3" s="132"/>
+      <c r="F3" s="132"/>
+      <c r="G3" s="132"/>
+      <c r="H3" s="132"/>
+      <c r="I3" s="132"/>
+      <c r="J3" s="132"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="194" t="s">
+        <v>265</v>
+      </c>
+      <c r="B4" s="194"/>
+      <c r="C4" s="185">
+        <v>8563214</v>
+      </c>
+      <c r="D4" s="185"/>
+      <c r="E4" s="185"/>
+      <c r="F4" s="64"/>
+      <c r="G4" s="192" t="s">
+        <v>52</v>
+      </c>
+      <c r="H4" s="187">
+        <v>45280</v>
+      </c>
+      <c r="I4" s="188"/>
+      <c r="J4" s="188"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="194" t="s">
+        <v>263</v>
+      </c>
+      <c r="B5" s="194"/>
+      <c r="C5" s="186" t="s">
+        <v>262</v>
+      </c>
+      <c r="D5" s="186"/>
+      <c r="E5" s="186"/>
+      <c r="F5" s="64"/>
+      <c r="G5" s="192" t="s">
+        <v>264</v>
+      </c>
+      <c r="H5" s="186">
+        <v>230546</v>
+      </c>
+      <c r="I5" s="186"/>
+      <c r="J5" s="186"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="194" t="s">
+        <v>266</v>
+      </c>
+      <c r="B6" s="194"/>
+      <c r="C6" s="186" t="s">
+        <v>198</v>
+      </c>
+      <c r="D6" s="186"/>
+      <c r="E6" s="186"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="193" t="s">
+        <v>267</v>
+      </c>
+      <c r="H6" s="186" t="s">
+        <v>199</v>
+      </c>
+      <c r="I6" s="186"/>
+      <c r="J6" s="186"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="64"/>
+      <c r="B7" s="64"/>
+      <c r="C7" s="64"/>
+      <c r="D7" s="64"/>
+      <c r="E7" s="64"/>
+      <c r="F7" s="190" t="s">
+        <v>210</v>
+      </c>
+      <c r="G7" s="190"/>
+      <c r="H7" s="89"/>
+      <c r="I7" s="189">
+        <v>1500</v>
+      </c>
+      <c r="J7" s="189" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F8" s="132" t="s">
+        <v>15</v>
+      </c>
+      <c r="G8" s="132"/>
+      <c r="H8" s="191"/>
+      <c r="I8" s="191">
+        <v>1500</v>
+      </c>
+      <c r="J8" s="191" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F9" s="180"/>
+      <c r="G9" s="180"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="64"/>
+      <c r="B10" s="64"/>
+      <c r="C10" s="98" t="s">
+        <v>270</v>
+      </c>
+      <c r="D10" s="98"/>
+      <c r="E10" s="98"/>
+      <c r="F10" s="98"/>
+      <c r="G10" s="98"/>
+      <c r="H10" s="98"/>
+      <c r="I10" s="98"/>
+      <c r="J10" s="98"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="87"/>
+      <c r="B11" s="87"/>
+      <c r="C11" s="88"/>
+      <c r="D11" s="88"/>
+      <c r="E11" s="88"/>
+      <c r="F11" s="88"/>
+      <c r="G11" s="88"/>
+      <c r="H11" s="88"/>
+      <c r="I11" s="88"/>
+      <c r="J11" s="88"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="87"/>
+      <c r="B12" s="87"/>
+      <c r="C12" s="88"/>
+      <c r="D12" s="88"/>
+      <c r="E12" s="88"/>
+      <c r="F12" s="181"/>
+      <c r="G12" s="181"/>
+      <c r="H12" s="181"/>
+      <c r="I12" s="181"/>
+      <c r="J12" s="181"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F13" s="174"/>
+      <c r="G13" s="174"/>
+      <c r="H13" s="174"/>
+      <c r="I13" s="174"/>
+      <c r="J13" s="174"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F14" s="184" t="s">
+        <v>268</v>
+      </c>
+      <c r="G14" s="184"/>
+      <c r="H14" s="184"/>
+      <c r="I14" s="184"/>
+      <c r="J14" s="184"/>
+    </row>
+  </sheetData>
+  <mergeCells count="17">
+    <mergeCell ref="F14:J14"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="C10:J10"/>
+    <mergeCell ref="F12:J13"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="H5:J5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="C6:E6"/>
+    <mergeCell ref="H6:J6"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="H4:J4"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -4237,44 +4557,44 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="93" t="s">
+      <c r="A1" s="101" t="s">
         <v>134</v>
       </c>
-      <c r="B1" s="94"/>
-      <c r="C1" s="94"/>
-      <c r="D1" s="94"/>
-      <c r="E1" s="94"/>
-      <c r="F1" s="94"/>
+      <c r="B1" s="102"/>
+      <c r="C1" s="102"/>
+      <c r="D1" s="102"/>
+      <c r="E1" s="102"/>
+      <c r="F1" s="102"/>
     </row>
     <row r="2" spans="1:9" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="94"/>
-      <c r="B2" s="94"/>
-      <c r="C2" s="94"/>
-      <c r="D2" s="94"/>
-      <c r="E2" s="94"/>
-      <c r="F2" s="94"/>
+      <c r="A2" s="102"/>
+      <c r="B2" s="102"/>
+      <c r="C2" s="102"/>
+      <c r="D2" s="102"/>
+      <c r="E2" s="102"/>
+      <c r="F2" s="102"/>
     </row>
     <row r="3" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="95" t="s">
+      <c r="A3" s="103" t="s">
         <v>133</v>
       </c>
-      <c r="B3" s="95"/>
-      <c r="C3" s="95"/>
-      <c r="D3" s="95"/>
-      <c r="E3" s="95"/>
-      <c r="F3" s="95"/>
+      <c r="B3" s="103"/>
+      <c r="C3" s="103"/>
+      <c r="D3" s="103"/>
+      <c r="E3" s="103"/>
+      <c r="F3" s="103"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="96" t="s">
+      <c r="A4" s="104" t="s">
         <v>144</v>
       </c>
-      <c r="B4" s="96"/>
+      <c r="B4" s="104"/>
       <c r="C4" s="51"/>
       <c r="D4" s="51"/>
-      <c r="E4" s="97" t="s">
+      <c r="E4" s="105" t="s">
         <v>114</v>
       </c>
-      <c r="F4" s="97"/>
+      <c r="F4" s="105"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="43" t="s">
@@ -4847,76 +5167,76 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A1" s="98" t="s">
+      <c r="A1" s="106" t="s">
         <v>170</v>
       </c>
-      <c r="B1" s="99"/>
-      <c r="C1" s="99"/>
-      <c r="D1" s="99"/>
-      <c r="E1" s="99"/>
-      <c r="F1" s="99"/>
-      <c r="G1" s="99"/>
-      <c r="H1" s="99"/>
-      <c r="I1" s="99"/>
-      <c r="J1" s="99"/>
-      <c r="K1" s="99"/>
-      <c r="L1" s="99"/>
-      <c r="M1" s="99"/>
-      <c r="N1" s="99"/>
-      <c r="O1" s="99"/>
-      <c r="P1" s="99"/>
-      <c r="Q1" s="99"/>
-      <c r="R1" s="99"/>
-      <c r="S1" s="99"/>
-      <c r="T1" s="99"/>
-      <c r="U1" s="99"/>
-      <c r="V1" s="99"/>
-      <c r="W1" s="99"/>
-      <c r="X1" s="99"/>
-      <c r="Y1" s="99"/>
-      <c r="Z1" s="99"/>
-      <c r="AA1" s="99"/>
-      <c r="AB1" s="99"/>
-      <c r="AC1" s="99"/>
-      <c r="AD1" s="99"/>
-      <c r="AE1" s="100"/>
+      <c r="B1" s="107"/>
+      <c r="C1" s="107"/>
+      <c r="D1" s="107"/>
+      <c r="E1" s="107"/>
+      <c r="F1" s="107"/>
+      <c r="G1" s="107"/>
+      <c r="H1" s="107"/>
+      <c r="I1" s="107"/>
+      <c r="J1" s="107"/>
+      <c r="K1" s="107"/>
+      <c r="L1" s="107"/>
+      <c r="M1" s="107"/>
+      <c r="N1" s="107"/>
+      <c r="O1" s="107"/>
+      <c r="P1" s="107"/>
+      <c r="Q1" s="107"/>
+      <c r="R1" s="107"/>
+      <c r="S1" s="107"/>
+      <c r="T1" s="107"/>
+      <c r="U1" s="107"/>
+      <c r="V1" s="107"/>
+      <c r="W1" s="107"/>
+      <c r="X1" s="107"/>
+      <c r="Y1" s="107"/>
+      <c r="Z1" s="107"/>
+      <c r="AA1" s="107"/>
+      <c r="AB1" s="107"/>
+      <c r="AC1" s="107"/>
+      <c r="AD1" s="107"/>
+      <c r="AE1" s="108"/>
     </row>
     <row r="2" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="101" t="s">
+      <c r="A2" s="109" t="s">
         <v>171</v>
       </c>
-      <c r="B2" s="102"/>
-      <c r="C2" s="102"/>
-      <c r="D2" s="102"/>
-      <c r="E2" s="102"/>
-      <c r="F2" s="102"/>
-      <c r="G2" s="102"/>
-      <c r="H2" s="102"/>
-      <c r="I2" s="102"/>
-      <c r="J2" s="102"/>
-      <c r="K2" s="102"/>
-      <c r="L2" s="102"/>
-      <c r="M2" s="102"/>
-      <c r="N2" s="102"/>
-      <c r="O2" s="102"/>
-      <c r="P2" s="102"/>
-      <c r="Q2" s="102"/>
-      <c r="R2" s="102"/>
-      <c r="S2" s="102"/>
-      <c r="T2" s="103">
+      <c r="B2" s="110"/>
+      <c r="C2" s="110"/>
+      <c r="D2" s="110"/>
+      <c r="E2" s="110"/>
+      <c r="F2" s="110"/>
+      <c r="G2" s="110"/>
+      <c r="H2" s="110"/>
+      <c r="I2" s="110"/>
+      <c r="J2" s="110"/>
+      <c r="K2" s="110"/>
+      <c r="L2" s="110"/>
+      <c r="M2" s="110"/>
+      <c r="N2" s="110"/>
+      <c r="O2" s="110"/>
+      <c r="P2" s="110"/>
+      <c r="Q2" s="110"/>
+      <c r="R2" s="110"/>
+      <c r="S2" s="110"/>
+      <c r="T2" s="111">
         <v>24</v>
       </c>
-      <c r="U2" s="103"/>
-      <c r="V2" s="103"/>
-      <c r="W2" s="103"/>
-      <c r="X2" s="103"/>
-      <c r="Y2" s="103"/>
-      <c r="Z2" s="103"/>
-      <c r="AA2" s="103"/>
-      <c r="AB2" s="103"/>
-      <c r="AC2" s="103"/>
-      <c r="AD2" s="103"/>
-      <c r="AE2" s="104"/>
+      <c r="U2" s="111"/>
+      <c r="V2" s="111"/>
+      <c r="W2" s="111"/>
+      <c r="X2" s="111"/>
+      <c r="Y2" s="111"/>
+      <c r="Z2" s="111"/>
+      <c r="AA2" s="111"/>
+      <c r="AB2" s="111"/>
+      <c r="AC2" s="111"/>
+      <c r="AD2" s="111"/>
+      <c r="AE2" s="112"/>
     </row>
     <row r="3" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A3" s="57" t="s">
@@ -5844,234 +6164,234 @@
       </c>
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A2" s="107" t="s">
+      <c r="A2" s="118" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="107"/>
-      <c r="C2" s="107"/>
-      <c r="D2" s="107"/>
-      <c r="E2" s="107"/>
-      <c r="F2" s="107"/>
-      <c r="G2" s="107"/>
-      <c r="H2" s="107"/>
-      <c r="I2" s="107"/>
-      <c r="J2" s="107"/>
-      <c r="K2" s="107"/>
-      <c r="L2" s="107"/>
-      <c r="M2" s="111" t="s">
+      <c r="B2" s="118"/>
+      <c r="C2" s="118"/>
+      <c r="D2" s="118"/>
+      <c r="E2" s="118"/>
+      <c r="F2" s="118"/>
+      <c r="G2" s="118"/>
+      <c r="H2" s="118"/>
+      <c r="I2" s="118"/>
+      <c r="J2" s="118"/>
+      <c r="K2" s="118"/>
+      <c r="L2" s="118"/>
+      <c r="M2" s="114" t="s">
         <v>23</v>
       </c>
-      <c r="N2" s="111"/>
-      <c r="O2" s="111"/>
-      <c r="P2" s="111"/>
-      <c r="Q2" s="111"/>
-      <c r="R2" s="111"/>
-      <c r="S2" s="111"/>
-      <c r="T2" s="111"/>
-      <c r="U2" s="111"/>
-      <c r="V2" s="111"/>
-      <c r="W2" s="111"/>
-      <c r="X2" s="111"/>
+      <c r="N2" s="114"/>
+      <c r="O2" s="114"/>
+      <c r="P2" s="114"/>
+      <c r="Q2" s="114"/>
+      <c r="R2" s="114"/>
+      <c r="S2" s="114"/>
+      <c r="T2" s="114"/>
+      <c r="U2" s="114"/>
+      <c r="V2" s="114"/>
+      <c r="W2" s="114"/>
+      <c r="X2" s="114"/>
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3" s="15">
         <v>1</v>
       </c>
-      <c r="B3" s="108" t="s">
+      <c r="B3" s="119" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="108"/>
-      <c r="D3" s="108"/>
+      <c r="C3" s="119"/>
+      <c r="D3" s="119"/>
       <c r="E3" s="16"/>
       <c r="F3" s="16"/>
       <c r="G3" s="16"/>
       <c r="H3" s="16"/>
       <c r="I3" s="16"/>
       <c r="J3" s="16"/>
-      <c r="K3" s="109">
+      <c r="K3" s="120">
         <v>45</v>
       </c>
-      <c r="L3" s="109"/>
+      <c r="L3" s="120"/>
       <c r="M3" s="14">
         <v>1</v>
       </c>
-      <c r="N3" s="112" t="s">
+      <c r="N3" s="115" t="s">
         <v>24</v>
       </c>
-      <c r="O3" s="112"/>
-      <c r="P3" s="112"/>
-      <c r="Q3" s="112"/>
-      <c r="R3" s="112"/>
+      <c r="O3" s="115"/>
+      <c r="P3" s="115"/>
+      <c r="Q3" s="115"/>
+      <c r="R3" s="115"/>
       <c r="S3" s="14">
         <v>6</v>
       </c>
-      <c r="T3" s="110" t="s">
+      <c r="T3" s="113" t="s">
         <v>29</v>
       </c>
-      <c r="U3" s="110"/>
-      <c r="V3" s="110"/>
-      <c r="W3" s="110"/>
-      <c r="X3" s="110"/>
+      <c r="U3" s="113"/>
+      <c r="V3" s="113"/>
+      <c r="W3" s="113"/>
+      <c r="X3" s="113"/>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" s="15">
         <v>2</v>
       </c>
-      <c r="B4" s="108" t="s">
+      <c r="B4" s="119" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="108"/>
-      <c r="D4" s="108"/>
+      <c r="C4" s="119"/>
+      <c r="D4" s="119"/>
       <c r="E4" s="15"/>
       <c r="F4" s="15"/>
       <c r="G4" s="15"/>
       <c r="H4" s="15"/>
       <c r="I4" s="15"/>
       <c r="J4" s="15"/>
-      <c r="K4" s="109">
+      <c r="K4" s="120">
         <v>46</v>
       </c>
-      <c r="L4" s="109"/>
+      <c r="L4" s="120"/>
       <c r="M4" s="14">
         <v>2</v>
       </c>
-      <c r="N4" s="112" t="s">
+      <c r="N4" s="115" t="s">
         <v>25</v>
       </c>
-      <c r="O4" s="112"/>
-      <c r="P4" s="112"/>
-      <c r="Q4" s="112"/>
-      <c r="R4" s="112"/>
+      <c r="O4" s="115"/>
+      <c r="P4" s="115"/>
+      <c r="Q4" s="115"/>
+      <c r="R4" s="115"/>
       <c r="S4" s="14">
         <v>7</v>
       </c>
-      <c r="T4" s="110" t="s">
+      <c r="T4" s="113" t="s">
         <v>29</v>
       </c>
-      <c r="U4" s="110"/>
-      <c r="V4" s="110"/>
-      <c r="W4" s="110"/>
-      <c r="X4" s="110"/>
+      <c r="U4" s="113"/>
+      <c r="V4" s="113"/>
+      <c r="W4" s="113"/>
+      <c r="X4" s="113"/>
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5" s="15">
         <v>3</v>
       </c>
-      <c r="B5" s="105" t="s">
+      <c r="B5" s="116" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="105"/>
-      <c r="D5" s="105"/>
+      <c r="C5" s="116"/>
+      <c r="D5" s="116"/>
       <c r="E5" s="15"/>
       <c r="F5" s="15"/>
       <c r="G5" s="15"/>
       <c r="H5" s="15"/>
       <c r="I5" s="15"/>
       <c r="J5" s="15"/>
-      <c r="K5" s="106">
+      <c r="K5" s="117">
         <v>47</v>
       </c>
-      <c r="L5" s="106"/>
+      <c r="L5" s="117"/>
       <c r="M5" s="14">
         <v>3</v>
       </c>
-      <c r="N5" s="112" t="s">
+      <c r="N5" s="115" t="s">
         <v>26</v>
       </c>
-      <c r="O5" s="112"/>
-      <c r="P5" s="112"/>
-      <c r="Q5" s="112"/>
-      <c r="R5" s="112"/>
+      <c r="O5" s="115"/>
+      <c r="P5" s="115"/>
+      <c r="Q5" s="115"/>
+      <c r="R5" s="115"/>
       <c r="S5" s="14">
         <v>8</v>
       </c>
-      <c r="T5" s="110" t="s">
+      <c r="T5" s="113" t="s">
         <v>29</v>
       </c>
-      <c r="U5" s="110"/>
-      <c r="V5" s="110"/>
-      <c r="W5" s="110"/>
-      <c r="X5" s="110"/>
+      <c r="U5" s="113"/>
+      <c r="V5" s="113"/>
+      <c r="W5" s="113"/>
+      <c r="X5" s="113"/>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6" s="15">
         <v>4</v>
       </c>
-      <c r="B6" s="105" t="s">
+      <c r="B6" s="116" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="105"/>
-      <c r="D6" s="105"/>
+      <c r="C6" s="116"/>
+      <c r="D6" s="116"/>
       <c r="E6" s="15"/>
       <c r="F6" s="15"/>
       <c r="G6" s="15"/>
       <c r="H6" s="15"/>
       <c r="I6" s="15"/>
       <c r="J6" s="15"/>
-      <c r="K6" s="106">
+      <c r="K6" s="117">
         <v>48</v>
       </c>
-      <c r="L6" s="106"/>
+      <c r="L6" s="117"/>
       <c r="M6" s="14">
         <v>4</v>
       </c>
-      <c r="N6" s="112" t="s">
+      <c r="N6" s="115" t="s">
         <v>27</v>
       </c>
-      <c r="O6" s="112"/>
-      <c r="P6" s="112"/>
-      <c r="Q6" s="112"/>
-      <c r="R6" s="112"/>
+      <c r="O6" s="115"/>
+      <c r="P6" s="115"/>
+      <c r="Q6" s="115"/>
+      <c r="R6" s="115"/>
       <c r="S6" s="14">
         <v>9</v>
       </c>
-      <c r="T6" s="110" t="s">
+      <c r="T6" s="113" t="s">
         <v>29</v>
       </c>
-      <c r="U6" s="110"/>
-      <c r="V6" s="110"/>
-      <c r="W6" s="110"/>
-      <c r="X6" s="110"/>
+      <c r="U6" s="113"/>
+      <c r="V6" s="113"/>
+      <c r="W6" s="113"/>
+      <c r="X6" s="113"/>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7" s="15">
         <v>5</v>
       </c>
-      <c r="B7" s="105" t="s">
+      <c r="B7" s="116" t="s">
         <v>22</v>
       </c>
-      <c r="C7" s="105"/>
-      <c r="D7" s="105"/>
+      <c r="C7" s="116"/>
+      <c r="D7" s="116"/>
       <c r="E7" s="15"/>
       <c r="F7" s="15"/>
       <c r="G7" s="15"/>
       <c r="H7" s="15"/>
       <c r="I7" s="15"/>
       <c r="J7" s="15"/>
-      <c r="K7" s="106">
+      <c r="K7" s="117">
         <v>49</v>
       </c>
-      <c r="L7" s="106"/>
+      <c r="L7" s="117"/>
       <c r="M7" s="14">
         <v>5</v>
       </c>
-      <c r="N7" s="112" t="s">
+      <c r="N7" s="115" t="s">
         <v>28</v>
       </c>
-      <c r="O7" s="112"/>
-      <c r="P7" s="112"/>
-      <c r="Q7" s="112"/>
-      <c r="R7" s="112"/>
+      <c r="O7" s="115"/>
+      <c r="P7" s="115"/>
+      <c r="Q7" s="115"/>
+      <c r="R7" s="115"/>
       <c r="S7" s="14">
         <v>10</v>
       </c>
-      <c r="T7" s="110" t="s">
+      <c r="T7" s="113" t="s">
         <v>29</v>
       </c>
-      <c r="U7" s="110"/>
-      <c r="V7" s="110"/>
-      <c r="W7" s="110"/>
-      <c r="X7" s="110"/>
+      <c r="U7" s="113"/>
+      <c r="V7" s="113"/>
+      <c r="W7" s="113"/>
+      <c r="X7" s="113"/>
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A8" s="13"/>
@@ -6283,6 +6603,17 @@
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="K6:L6"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="K7:L7"/>
+    <mergeCell ref="A2:L2"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="K4:L4"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="K5:L5"/>
     <mergeCell ref="T7:X7"/>
     <mergeCell ref="M2:X2"/>
     <mergeCell ref="N3:R3"/>
@@ -6294,17 +6625,6 @@
     <mergeCell ref="T4:X4"/>
     <mergeCell ref="T5:X5"/>
     <mergeCell ref="T6:X6"/>
-    <mergeCell ref="B6:D6"/>
-    <mergeCell ref="K6:L6"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="K7:L7"/>
-    <mergeCell ref="A2:L2"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="K3:L3"/>
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="K4:L4"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="K5:L5"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6433,7 +6753,7 @@
       </c>
     </row>
     <row r="2" spans="1:10" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="113" t="s">
+      <c r="A2" s="121" t="s">
         <v>34</v>
       </c>
       <c r="B2" s="37" t="s">
@@ -6453,7 +6773,7 @@
       <c r="J2" s="37"/>
     </row>
     <row r="3" spans="1:10" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="113"/>
+      <c r="A3" s="121"/>
       <c r="B3" s="38" t="s">
         <v>19</v>
       </c>
@@ -6473,7 +6793,7 @@
       <c r="J3" s="38"/>
     </row>
     <row r="4" spans="1:10" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="113"/>
+      <c r="A4" s="121"/>
       <c r="B4" s="37" t="s">
         <v>20</v>
       </c>
@@ -6493,7 +6813,7 @@
       <c r="J4" s="37"/>
     </row>
     <row r="5" spans="1:10" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="113"/>
+      <c r="A5" s="121"/>
       <c r="B5" s="38" t="s">
         <v>21</v>
       </c>
@@ -6511,7 +6831,7 @@
       <c r="J5" s="38"/>
     </row>
     <row r="6" spans="1:10" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="113"/>
+      <c r="A6" s="121"/>
       <c r="B6" s="37" t="s">
         <v>22</v>
       </c>
@@ -6529,7 +6849,7 @@
       <c r="J6" s="37"/>
     </row>
     <row r="7" spans="1:10" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="113" t="s">
+      <c r="A7" s="121" t="s">
         <v>107</v>
       </c>
       <c r="B7" s="37" t="s">
@@ -6549,7 +6869,7 @@
       <c r="J7" s="37"/>
     </row>
     <row r="8" spans="1:10" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="113"/>
+      <c r="A8" s="121"/>
       <c r="B8" s="38" t="s">
         <v>19</v>
       </c>
@@ -6569,7 +6889,7 @@
       <c r="J8" s="38"/>
     </row>
     <row r="9" spans="1:10" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="113"/>
+      <c r="A9" s="121"/>
       <c r="B9" s="37" t="s">
         <v>20</v>
       </c>
@@ -6589,7 +6909,7 @@
       <c r="J9" s="37"/>
     </row>
     <row r="10" spans="1:10" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="113"/>
+      <c r="A10" s="121"/>
       <c r="B10" s="38" t="s">
         <v>21</v>
       </c>
@@ -6607,7 +6927,7 @@
       <c r="J10" s="38"/>
     </row>
     <row r="11" spans="1:10" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="113"/>
+      <c r="A11" s="121"/>
       <c r="B11" s="37" t="s">
         <v>22</v>
       </c>
@@ -6625,7 +6945,7 @@
       <c r="J11" s="37"/>
     </row>
     <row r="12" spans="1:10" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="113" t="s">
+      <c r="A12" s="121" t="s">
         <v>108</v>
       </c>
       <c r="B12" s="37" t="s">
@@ -6645,7 +6965,7 @@
       <c r="J12" s="37"/>
     </row>
     <row r="13" spans="1:10" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="113"/>
+      <c r="A13" s="121"/>
       <c r="B13" s="38" t="s">
         <v>19</v>
       </c>
@@ -6665,7 +6985,7 @@
       <c r="J13" s="38"/>
     </row>
     <row r="14" spans="1:10" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="113"/>
+      <c r="A14" s="121"/>
       <c r="B14" s="37" t="s">
         <v>20</v>
       </c>
@@ -6685,7 +7005,7 @@
       <c r="J14" s="37"/>
     </row>
     <row r="15" spans="1:10" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="113"/>
+      <c r="A15" s="121"/>
       <c r="B15" s="38" t="s">
         <v>21</v>
       </c>
@@ -6703,7 +7023,7 @@
       <c r="J15" s="38"/>
     </row>
     <row r="16" spans="1:10" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="113"/>
+      <c r="A16" s="121"/>
       <c r="B16" s="37" t="s">
         <v>22</v>
       </c>
@@ -6721,7 +7041,7 @@
       <c r="J16" s="37"/>
     </row>
     <row r="17" spans="1:10" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="113" t="s">
+      <c r="A17" s="121" t="s">
         <v>109</v>
       </c>
       <c r="B17" s="37" t="s">
@@ -6741,7 +7061,7 @@
       <c r="J17" s="37"/>
     </row>
     <row r="18" spans="1:10" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="113"/>
+      <c r="A18" s="121"/>
       <c r="B18" s="38" t="s">
         <v>19</v>
       </c>
@@ -6761,7 +7081,7 @@
       <c r="J18" s="38"/>
     </row>
     <row r="19" spans="1:10" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="113"/>
+      <c r="A19" s="121"/>
       <c r="B19" s="37" t="s">
         <v>20</v>
       </c>
@@ -6781,7 +7101,7 @@
       <c r="J19" s="37"/>
     </row>
     <row r="20" spans="1:10" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="113"/>
+      <c r="A20" s="121"/>
       <c r="B20" s="38" t="s">
         <v>21</v>
       </c>
@@ -6799,7 +7119,7 @@
       <c r="J20" s="38"/>
     </row>
     <row r="21" spans="1:10" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="113"/>
+      <c r="A21" s="121"/>
       <c r="B21" s="37" t="s">
         <v>22</v>
       </c>
@@ -6817,7 +7137,7 @@
       <c r="J21" s="37"/>
     </row>
     <row r="22" spans="1:10" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="113" t="s">
+      <c r="A22" s="121" t="s">
         <v>110</v>
       </c>
       <c r="B22" s="37" t="s">
@@ -6837,7 +7157,7 @@
       <c r="J22" s="37"/>
     </row>
     <row r="23" spans="1:10" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="113"/>
+      <c r="A23" s="121"/>
       <c r="B23" s="38" t="s">
         <v>19</v>
       </c>
@@ -6857,7 +7177,7 @@
       <c r="J23" s="38"/>
     </row>
     <row r="24" spans="1:10" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="113"/>
+      <c r="A24" s="121"/>
       <c r="B24" s="37" t="s">
         <v>20</v>
       </c>
@@ -6877,7 +7197,7 @@
       <c r="J24" s="37"/>
     </row>
     <row r="25" spans="1:10" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="113"/>
+      <c r="A25" s="121"/>
       <c r="B25" s="38" t="s">
         <v>21</v>
       </c>
@@ -6895,7 +7215,7 @@
       <c r="J25" s="38"/>
     </row>
     <row r="26" spans="1:10" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="113"/>
+      <c r="A26" s="121"/>
       <c r="B26" s="37" t="s">
         <v>22</v>
       </c>
@@ -6913,7 +7233,7 @@
       <c r="J26" s="37"/>
     </row>
     <row r="27" spans="1:10" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="113" t="s">
+      <c r="A27" s="121" t="s">
         <v>111</v>
       </c>
       <c r="B27" s="37" t="s">
@@ -6933,7 +7253,7 @@
       <c r="J27" s="37"/>
     </row>
     <row r="28" spans="1:10" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="113"/>
+      <c r="A28" s="121"/>
       <c r="B28" s="38" t="s">
         <v>19</v>
       </c>
@@ -6953,7 +7273,7 @@
       <c r="J28" s="38"/>
     </row>
     <row r="29" spans="1:10" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="113"/>
+      <c r="A29" s="121"/>
       <c r="B29" s="37" t="s">
         <v>20</v>
       </c>
@@ -6973,7 +7293,7 @@
       <c r="J29" s="37"/>
     </row>
     <row r="30" spans="1:10" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="113"/>
+      <c r="A30" s="121"/>
       <c r="B30" s="38" t="s">
         <v>21</v>
       </c>
@@ -6991,7 +7311,7 @@
       <c r="J30" s="38"/>
     </row>
     <row r="31" spans="1:10" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="113"/>
+      <c r="A31" s="121"/>
       <c r="B31" s="37" t="s">
         <v>22</v>
       </c>
@@ -7042,24 +7362,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="116" t="s">
+      <c r="A1" s="124" t="s">
         <v>40</v>
       </c>
-      <c r="B1" s="117"/>
-      <c r="C1" s="117"/>
-      <c r="D1" s="117"/>
-      <c r="E1" s="117"/>
-      <c r="F1" s="117"/>
+      <c r="B1" s="125"/>
+      <c r="C1" s="125"/>
+      <c r="D1" s="125"/>
+      <c r="E1" s="125"/>
+      <c r="F1" s="125"/>
     </row>
     <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="118" t="s">
+      <c r="A2" s="126" t="s">
         <v>41</v>
       </c>
-      <c r="B2" s="118"/>
-      <c r="C2" s="118"/>
-      <c r="D2" s="118"/>
-      <c r="E2" s="118"/>
-      <c r="F2" s="118"/>
+      <c r="B2" s="126"/>
+      <c r="C2" s="126"/>
+      <c r="D2" s="126"/>
+      <c r="E2" s="126"/>
+      <c r="F2" s="126"/>
     </row>
     <row r="3" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
@@ -7288,18 +7608,18 @@
       <c r="F15" s="29"/>
     </row>
     <row r="16" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="119" t="s">
+      <c r="A16" s="127" t="s">
         <v>60</v>
       </c>
-      <c r="B16" s="120"/>
-      <c r="C16" s="120"/>
-      <c r="D16" s="120"/>
-      <c r="E16" s="120"/>
-      <c r="F16" s="121"/>
+      <c r="B16" s="128"/>
+      <c r="C16" s="128"/>
+      <c r="D16" s="128"/>
+      <c r="E16" s="128"/>
+      <c r="F16" s="129"/>
     </row>
     <row r="17" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="114"/>
-      <c r="B17" s="115"/>
+      <c r="A17" s="122"/>
+      <c r="B17" s="123"/>
       <c r="C17" s="32" t="s">
         <v>73</v>
       </c>
@@ -7314,10 +7634,10 @@
       </c>
     </row>
     <row r="18" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="114" t="s">
+      <c r="A18" s="122" t="s">
         <v>15</v>
       </c>
-      <c r="B18" s="115"/>
+      <c r="B18" s="123"/>
       <c r="C18" s="32">
         <v>25</v>
       </c>
@@ -7381,35 +7701,35 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="116" t="s">
+      <c r="A1" s="124" t="s">
         <v>40</v>
       </c>
-      <c r="B1" s="117"/>
-      <c r="C1" s="117"/>
-      <c r="D1" s="117"/>
-      <c r="E1" s="117"/>
-      <c r="F1" s="117"/>
-      <c r="G1" s="117"/>
+      <c r="B1" s="125"/>
+      <c r="C1" s="125"/>
+      <c r="D1" s="125"/>
+      <c r="E1" s="125"/>
+      <c r="F1" s="125"/>
+      <c r="G1" s="125"/>
     </row>
     <row r="2" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="118" t="s">
+      <c r="A2" s="126" t="s">
         <v>41</v>
       </c>
-      <c r="B2" s="118"/>
-      <c r="C2" s="118"/>
-      <c r="D2" s="118"/>
-      <c r="E2" s="118"/>
-      <c r="F2" s="118"/>
-      <c r="G2" s="118"/>
+      <c r="B2" s="126"/>
+      <c r="C2" s="126"/>
+      <c r="D2" s="126"/>
+      <c r="E2" s="126"/>
+      <c r="F2" s="126"/>
+      <c r="G2" s="126"/>
     </row>
     <row r="3" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="122" t="s">
+      <c r="A3" s="130" t="s">
         <v>74</v>
       </c>
-      <c r="B3" s="122"/>
-      <c r="C3" s="122"/>
-      <c r="D3" s="122"/>
-      <c r="E3" s="122"/>
+      <c r="B3" s="130"/>
+      <c r="C3" s="130"/>
+      <c r="D3" s="130"/>
+      <c r="E3" s="130"/>
       <c r="F3" s="21" t="s">
         <v>52</v>
       </c>
@@ -7662,19 +7982,19 @@
       <c r="G15" s="29"/>
     </row>
     <row r="16" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="119" t="s">
+      <c r="A16" s="127" t="s">
         <v>60</v>
       </c>
-      <c r="B16" s="120"/>
-      <c r="C16" s="120"/>
-      <c r="D16" s="120"/>
-      <c r="E16" s="120"/>
-      <c r="F16" s="120"/>
-      <c r="G16" s="121"/>
+      <c r="B16" s="128"/>
+      <c r="C16" s="128"/>
+      <c r="D16" s="128"/>
+      <c r="E16" s="128"/>
+      <c r="F16" s="128"/>
+      <c r="G16" s="129"/>
     </row>
     <row r="17" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="114"/>
-      <c r="B17" s="115"/>
+      <c r="A17" s="122"/>
+      <c r="B17" s="123"/>
       <c r="C17" s="32"/>
       <c r="D17" s="32" t="s">
         <v>76</v>
@@ -7690,10 +8010,10 @@
       </c>
     </row>
     <row r="18" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="114" t="s">
+      <c r="A18" s="122" t="s">
         <v>15</v>
       </c>
-      <c r="B18" s="115"/>
+      <c r="B18" s="123"/>
       <c r="C18" s="32"/>
       <c r="D18" s="32">
         <v>13</v>
@@ -7726,28 +8046,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C002464B-D256-4EB5-A012-8EB2C2D144F6}">
   <dimension ref="A1:J20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:B3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="R23" sqref="R23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="98" t="s">
+      <c r="A1" s="106" t="s">
         <v>258</v>
       </c>
-      <c r="B1" s="99"/>
-      <c r="C1" s="99"/>
-      <c r="D1" s="158"/>
-      <c r="E1" s="156"/>
-      <c r="F1" s="156"/>
-      <c r="G1" s="156"/>
-      <c r="H1" s="156"/>
-      <c r="I1" s="156"/>
-      <c r="J1" s="159"/>
+      <c r="B1" s="107"/>
+      <c r="C1" s="107"/>
+      <c r="D1" s="131"/>
+      <c r="E1" s="132"/>
+      <c r="F1" s="132"/>
+      <c r="G1" s="132"/>
+      <c r="H1" s="132"/>
+      <c r="I1" s="132"/>
+      <c r="J1" s="133"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="171"/>
+      <c r="A2" s="90"/>
       <c r="B2" s="17"/>
       <c r="C2" s="17"/>
       <c r="D2" s="17"/>
@@ -7756,30 +8076,30 @@
       <c r="G2" s="17"/>
       <c r="H2" s="17"/>
       <c r="I2" s="17"/>
-      <c r="J2" s="172"/>
+      <c r="J2" s="91"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="176" t="s">
+      <c r="A3" s="134" t="s">
         <v>145</v>
       </c>
-      <c r="B3" s="161"/>
-      <c r="C3" s="161" t="s">
+      <c r="B3" s="135"/>
+      <c r="C3" s="135" t="s">
         <v>147</v>
       </c>
-      <c r="D3" s="161"/>
-      <c r="E3" s="161" t="s">
+      <c r="D3" s="135"/>
+      <c r="E3" s="135" t="s">
         <v>146</v>
       </c>
-      <c r="F3" s="161"/>
-      <c r="G3" s="161" t="s">
+      <c r="F3" s="135"/>
+      <c r="G3" s="135" t="s">
         <v>198</v>
       </c>
-      <c r="H3" s="161"/>
+      <c r="H3" s="135"/>
       <c r="I3" s="17"/>
-      <c r="J3" s="172"/>
+      <c r="J3" s="91"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="171"/>
+      <c r="A4" s="90"/>
       <c r="B4" s="17"/>
       <c r="C4" s="17"/>
       <c r="D4" s="17"/>
@@ -7788,10 +8108,10 @@
       <c r="G4" s="17"/>
       <c r="H4" s="17"/>
       <c r="I4" s="17"/>
-      <c r="J4" s="172"/>
+      <c r="J4" s="91"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="171"/>
+      <c r="A5" s="90"/>
       <c r="B5" s="17"/>
       <c r="C5" s="17"/>
       <c r="D5" s="17"/>
@@ -7800,10 +8120,10 @@
       <c r="G5" s="17"/>
       <c r="H5" s="17"/>
       <c r="I5" s="17"/>
-      <c r="J5" s="172"/>
+      <c r="J5" s="91"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="171"/>
+      <c r="A6" s="90"/>
       <c r="B6" s="17"/>
       <c r="C6" s="17"/>
       <c r="D6" s="17"/>
@@ -7812,10 +8132,10 @@
       <c r="G6" s="17"/>
       <c r="H6" s="17"/>
       <c r="I6" s="17"/>
-      <c r="J6" s="172"/>
+      <c r="J6" s="91"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="171"/>
+      <c r="A7" s="90"/>
       <c r="B7" s="17"/>
       <c r="C7" s="17"/>
       <c r="D7" s="17"/>
@@ -7824,10 +8144,10 @@
       <c r="G7" s="17"/>
       <c r="H7" s="17"/>
       <c r="I7" s="17"/>
-      <c r="J7" s="172"/>
+      <c r="J7" s="91"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="171"/>
+      <c r="A8" s="90"/>
       <c r="B8" s="17"/>
       <c r="C8" s="17"/>
       <c r="D8" s="17"/>
@@ -7836,10 +8156,10 @@
       <c r="G8" s="17"/>
       <c r="H8" s="17"/>
       <c r="I8" s="17"/>
-      <c r="J8" s="172"/>
+      <c r="J8" s="91"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="171"/>
+      <c r="A9" s="90"/>
       <c r="B9" s="17"/>
       <c r="C9" s="17"/>
       <c r="D9" s="17"/>
@@ -7848,10 +8168,10 @@
       <c r="G9" s="17"/>
       <c r="H9" s="17"/>
       <c r="I9" s="17"/>
-      <c r="J9" s="172"/>
+      <c r="J9" s="91"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="171"/>
+      <c r="A10" s="90"/>
       <c r="B10" s="17"/>
       <c r="C10" s="17"/>
       <c r="D10" s="17"/>
@@ -7860,10 +8180,10 @@
       <c r="G10" s="17"/>
       <c r="H10" s="17"/>
       <c r="I10" s="17"/>
-      <c r="J10" s="172"/>
+      <c r="J10" s="91"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="171"/>
+      <c r="A11" s="90"/>
       <c r="B11" s="17"/>
       <c r="C11" s="17"/>
       <c r="D11" s="17"/>
@@ -7872,10 +8192,10 @@
       <c r="G11" s="17"/>
       <c r="H11" s="17"/>
       <c r="I11" s="17"/>
-      <c r="J11" s="172"/>
+      <c r="J11" s="91"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="171"/>
+      <c r="A12" s="90"/>
       <c r="B12" s="17"/>
       <c r="C12" s="17"/>
       <c r="D12" s="17"/>
@@ -7884,10 +8204,10 @@
       <c r="G12" s="17"/>
       <c r="H12" s="17"/>
       <c r="I12" s="17"/>
-      <c r="J12" s="172"/>
+      <c r="J12" s="91"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="171"/>
+      <c r="A13" s="90"/>
       <c r="B13" s="17"/>
       <c r="C13" s="17"/>
       <c r="D13" s="17"/>
@@ -7896,10 +8216,10 @@
       <c r="G13" s="17"/>
       <c r="H13" s="17"/>
       <c r="I13" s="17"/>
-      <c r="J13" s="172"/>
+      <c r="J13" s="91"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="171"/>
+      <c r="A14" s="90"/>
       <c r="B14" s="17"/>
       <c r="C14" s="17"/>
       <c r="D14" s="17"/>
@@ -7908,10 +8228,10 @@
       <c r="G14" s="17"/>
       <c r="H14" s="17"/>
       <c r="I14" s="17"/>
-      <c r="J14" s="172"/>
+      <c r="J14" s="91"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="171"/>
+      <c r="A15" s="90"/>
       <c r="B15" s="17"/>
       <c r="C15" s="17"/>
       <c r="D15" s="17"/>
@@ -7920,10 +8240,10 @@
       <c r="G15" s="17"/>
       <c r="H15" s="17"/>
       <c r="I15" s="17"/>
-      <c r="J15" s="172"/>
+      <c r="J15" s="91"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="171"/>
+      <c r="A16" s="90"/>
       <c r="B16" s="17"/>
       <c r="C16" s="17"/>
       <c r="D16" s="17"/>
@@ -7932,10 +8252,10 @@
       <c r="G16" s="17"/>
       <c r="H16" s="17"/>
       <c r="I16" s="17"/>
-      <c r="J16" s="172"/>
+      <c r="J16" s="91"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="171"/>
+      <c r="A17" s="90"/>
       <c r="B17" s="17"/>
       <c r="C17" s="17"/>
       <c r="D17" s="17"/>
@@ -7944,10 +8264,10 @@
       <c r="G17" s="17"/>
       <c r="H17" s="17"/>
       <c r="I17" s="17"/>
-      <c r="J17" s="172"/>
+      <c r="J17" s="91"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="171"/>
+      <c r="A18" s="90"/>
       <c r="B18" s="17"/>
       <c r="C18" s="17"/>
       <c r="D18" s="17"/>
@@ -7956,10 +8276,10 @@
       <c r="G18" s="17"/>
       <c r="H18" s="17"/>
       <c r="I18" s="17"/>
-      <c r="J18" s="172"/>
+      <c r="J18" s="91"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="171"/>
+      <c r="A19" s="90"/>
       <c r="B19" s="17"/>
       <c r="C19" s="17"/>
       <c r="D19" s="17"/>
@@ -7968,19 +8288,19 @@
       <c r="G19" s="17"/>
       <c r="H19" s="17"/>
       <c r="I19" s="17"/>
-      <c r="J19" s="172"/>
+      <c r="J19" s="91"/>
     </row>
     <row r="20" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="173"/>
-      <c r="B20" s="174"/>
-      <c r="C20" s="174"/>
-      <c r="D20" s="174"/>
-      <c r="E20" s="174"/>
-      <c r="F20" s="174"/>
-      <c r="G20" s="174"/>
-      <c r="H20" s="174"/>
-      <c r="I20" s="174"/>
-      <c r="J20" s="175"/>
+      <c r="A20" s="92"/>
+      <c r="B20" s="93"/>
+      <c r="C20" s="93"/>
+      <c r="D20" s="93"/>
+      <c r="E20" s="93"/>
+      <c r="F20" s="93"/>
+      <c r="G20" s="93"/>
+      <c r="H20" s="93"/>
+      <c r="I20" s="93"/>
+      <c r="J20" s="94"/>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>

<commit_message>
Add sp and modified classFee
</commit_message>
<xml_diff>
--- a/Resources/Layout.xlsx
+++ b/Resources/Layout.xlsx
@@ -3,28 +3,29 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24332"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32D032E1-EB80-4CAE-B557-27994395DA4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{022DAD80-8775-43D7-863A-3371BFAA30C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15960" firstSheet="7" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15960" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Attendance Report daily" sheetId="8" r:id="rId2"/>
-    <sheet name="Attendance Report Monthly Full" sheetId="10" r:id="rId3"/>
-    <sheet name="Dashboard" sheetId="2" r:id="rId4"/>
-    <sheet name="Class Routine Teacher" sheetId="6" r:id="rId5"/>
-    <sheet name="Sheet3" sheetId="7" r:id="rId6"/>
-    <sheet name="Student Attendance" sheetId="4" r:id="rId7"/>
-    <sheet name="Employee Attendance" sheetId="5" r:id="rId8"/>
-    <sheet name="Exam Create" sheetId="9" r:id="rId9"/>
-    <sheet name="Rpt Student List" sheetId="12" r:id="rId10"/>
-    <sheet name="Rpt Student Payment " sheetId="11" r:id="rId11"/>
-    <sheet name="SingleStudentResult" sheetId="13" r:id="rId12"/>
-    <sheet name="Rpt payment Receipt" sheetId="14" r:id="rId13"/>
+    <sheet name="Student Financial" sheetId="15" r:id="rId3"/>
+    <sheet name="Attendance Report Monthly Full" sheetId="10" r:id="rId4"/>
+    <sheet name="Dashboard" sheetId="2" r:id="rId5"/>
+    <sheet name="Class Routine Teacher" sheetId="6" r:id="rId6"/>
+    <sheet name="Sheet3" sheetId="7" r:id="rId7"/>
+    <sheet name="Student Attendance" sheetId="4" r:id="rId8"/>
+    <sheet name="Employee Attendance" sheetId="5" r:id="rId9"/>
+    <sheet name="Exam Create" sheetId="9" r:id="rId10"/>
+    <sheet name="Rpt Student List" sheetId="12" r:id="rId11"/>
+    <sheet name="Rpt Student Payment " sheetId="11" r:id="rId12"/>
+    <sheet name="SingleStudentResult" sheetId="13" r:id="rId13"/>
+    <sheet name="Rpt payment Receipt" sheetId="14" r:id="rId14"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="10">'Rpt Student Payment '!$A$1:$L$17</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="6">'Student Attendance'!$A$1:$F$20</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="11">'Rpt Student Payment '!$A$1:$L$17</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="7">'Student Attendance'!$A$1:$F$20</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="596" uniqueCount="271">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="608" uniqueCount="278">
   <si>
     <t>Date</t>
   </si>
@@ -910,6 +911,27 @@
   </si>
   <si>
     <t>In word:Taka One Thousand and Five Hundred only.</t>
+  </si>
+  <si>
+    <t>Student Image and Info</t>
+  </si>
+  <si>
+    <t>Payment History</t>
+  </si>
+  <si>
+    <t>Payment Schedule</t>
+  </si>
+  <si>
+    <t>Monthly Fee</t>
+  </si>
+  <si>
+    <t>Exam Fee</t>
+  </si>
+  <si>
+    <t>Session Fee</t>
+  </si>
+  <si>
+    <t>Freq.</t>
   </si>
 </sst>
 </file>
@@ -1192,7 +1214,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="44">
+  <borders count="50">
     <border>
       <left/>
       <right/>
@@ -1723,12 +1745,74 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="195">
+  <cellXfs count="224">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
@@ -1948,300 +2032,359 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="11" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="11" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="11" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="11" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="11" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="11" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="11" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="11" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="11" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="11" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="11" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="11" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2759,28 +2902,28 @@
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="95" t="s">
+      <c r="A2" s="100" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="95"/>
-      <c r="C2" s="96" t="s">
+      <c r="B2" s="100"/>
+      <c r="C2" s="101" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="96"/>
-      <c r="E2" s="96"/>
+      <c r="D2" s="101"/>
+      <c r="E2" s="101"/>
       <c r="F2" s="12"/>
     </row>
     <row r="3" spans="1:12" s="8" customFormat="1" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F3" s="9"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="95" t="s">
+      <c r="A4" s="100" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="95"/>
-      <c r="C4" s="97"/>
-      <c r="D4" s="97"/>
-      <c r="E4" s="97"/>
+      <c r="B4" s="100"/>
+      <c r="C4" s="102"/>
+      <c r="D4" s="102"/>
+      <c r="E4" s="102"/>
       <c r="F4" s="7" t="s">
         <v>15</v>
       </c>
@@ -2795,12 +2938,12 @@
       <c r="F5" s="7"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="100" t="s">
+      <c r="A6" s="105" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="100"/>
-      <c r="C6" s="99"/>
-      <c r="D6" s="99"/>
+      <c r="B6" s="105"/>
+      <c r="C6" s="104"/>
+      <c r="D6" s="104"/>
       <c r="E6" s="11"/>
       <c r="F6" s="7" t="s">
         <v>16</v>
@@ -2810,12 +2953,12 @@
       <c r="F7" s="9"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="100" t="s">
+      <c r="A8" s="105" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="100"/>
-      <c r="C8" s="99"/>
-      <c r="D8" s="99"/>
+      <c r="B8" s="105"/>
+      <c r="C8" s="104"/>
+      <c r="D8" s="104"/>
       <c r="E8" s="10" t="s">
         <v>14</v>
       </c>
@@ -2824,13 +2967,13 @@
       <c r="F9" s="9"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="98" t="s">
+      <c r="A10" s="103" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="98"/>
-      <c r="C10" s="99"/>
-      <c r="D10" s="99"/>
-      <c r="E10" s="99"/>
+      <c r="B10" s="103"/>
+      <c r="C10" s="104"/>
+      <c r="D10" s="104"/>
+      <c r="E10" s="104"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
@@ -2917,6 +3060,280 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C002464B-D256-4EB5-A012-8EB2C2D144F6}">
+  <dimension ref="A1:J20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="R23" sqref="R23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="111" t="s">
+        <v>258</v>
+      </c>
+      <c r="B1" s="112"/>
+      <c r="C1" s="112"/>
+      <c r="D1" s="136"/>
+      <c r="E1" s="137"/>
+      <c r="F1" s="137"/>
+      <c r="G1" s="137"/>
+      <c r="H1" s="137"/>
+      <c r="I1" s="137"/>
+      <c r="J1" s="138"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="90"/>
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
+      <c r="I2" s="17"/>
+      <c r="J2" s="91"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="139" t="s">
+        <v>145</v>
+      </c>
+      <c r="B3" s="140"/>
+      <c r="C3" s="140" t="s">
+        <v>147</v>
+      </c>
+      <c r="D3" s="140"/>
+      <c r="E3" s="140" t="s">
+        <v>146</v>
+      </c>
+      <c r="F3" s="140"/>
+      <c r="G3" s="140" t="s">
+        <v>198</v>
+      </c>
+      <c r="H3" s="140"/>
+      <c r="I3" s="17"/>
+      <c r="J3" s="91"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="90"/>
+      <c r="B4" s="17"/>
+      <c r="C4" s="17"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="17"/>
+      <c r="G4" s="17"/>
+      <c r="H4" s="17"/>
+      <c r="I4" s="17"/>
+      <c r="J4" s="91"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="90"/>
+      <c r="B5" s="17"/>
+      <c r="C5" s="17"/>
+      <c r="D5" s="17"/>
+      <c r="E5" s="17"/>
+      <c r="F5" s="17"/>
+      <c r="G5" s="17"/>
+      <c r="H5" s="17"/>
+      <c r="I5" s="17"/>
+      <c r="J5" s="91"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="90"/>
+      <c r="B6" s="17"/>
+      <c r="C6" s="17"/>
+      <c r="D6" s="17"/>
+      <c r="E6" s="17"/>
+      <c r="F6" s="17"/>
+      <c r="G6" s="17"/>
+      <c r="H6" s="17"/>
+      <c r="I6" s="17"/>
+      <c r="J6" s="91"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="90"/>
+      <c r="B7" s="17"/>
+      <c r="C7" s="17"/>
+      <c r="D7" s="17"/>
+      <c r="E7" s="17"/>
+      <c r="F7" s="17"/>
+      <c r="G7" s="17"/>
+      <c r="H7" s="17"/>
+      <c r="I7" s="17"/>
+      <c r="J7" s="91"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="90"/>
+      <c r="B8" s="17"/>
+      <c r="C8" s="17"/>
+      <c r="D8" s="17"/>
+      <c r="E8" s="17"/>
+      <c r="F8" s="17"/>
+      <c r="G8" s="17"/>
+      <c r="H8" s="17"/>
+      <c r="I8" s="17"/>
+      <c r="J8" s="91"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="90"/>
+      <c r="B9" s="17"/>
+      <c r="C9" s="17"/>
+      <c r="D9" s="17"/>
+      <c r="E9" s="17"/>
+      <c r="F9" s="17"/>
+      <c r="G9" s="17"/>
+      <c r="H9" s="17"/>
+      <c r="I9" s="17"/>
+      <c r="J9" s="91"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="90"/>
+      <c r="B10" s="17"/>
+      <c r="C10" s="17"/>
+      <c r="D10" s="17"/>
+      <c r="E10" s="17"/>
+      <c r="F10" s="17"/>
+      <c r="G10" s="17"/>
+      <c r="H10" s="17"/>
+      <c r="I10" s="17"/>
+      <c r="J10" s="91"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="90"/>
+      <c r="B11" s="17"/>
+      <c r="C11" s="17"/>
+      <c r="D11" s="17"/>
+      <c r="E11" s="17"/>
+      <c r="F11" s="17"/>
+      <c r="G11" s="17"/>
+      <c r="H11" s="17"/>
+      <c r="I11" s="17"/>
+      <c r="J11" s="91"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="90"/>
+      <c r="B12" s="17"/>
+      <c r="C12" s="17"/>
+      <c r="D12" s="17"/>
+      <c r="E12" s="17"/>
+      <c r="F12" s="17"/>
+      <c r="G12" s="17"/>
+      <c r="H12" s="17"/>
+      <c r="I12" s="17"/>
+      <c r="J12" s="91"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="90"/>
+      <c r="B13" s="17"/>
+      <c r="C13" s="17"/>
+      <c r="D13" s="17"/>
+      <c r="E13" s="17"/>
+      <c r="F13" s="17"/>
+      <c r="G13" s="17"/>
+      <c r="H13" s="17"/>
+      <c r="I13" s="17"/>
+      <c r="J13" s="91"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="90"/>
+      <c r="B14" s="17"/>
+      <c r="C14" s="17"/>
+      <c r="D14" s="17"/>
+      <c r="E14" s="17"/>
+      <c r="F14" s="17"/>
+      <c r="G14" s="17"/>
+      <c r="H14" s="17"/>
+      <c r="I14" s="17"/>
+      <c r="J14" s="91"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="90"/>
+      <c r="B15" s="17"/>
+      <c r="C15" s="17"/>
+      <c r="D15" s="17"/>
+      <c r="E15" s="17"/>
+      <c r="F15" s="17"/>
+      <c r="G15" s="17"/>
+      <c r="H15" s="17"/>
+      <c r="I15" s="17"/>
+      <c r="J15" s="91"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="90"/>
+      <c r="B16" s="17"/>
+      <c r="C16" s="17"/>
+      <c r="D16" s="17"/>
+      <c r="E16" s="17"/>
+      <c r="F16" s="17"/>
+      <c r="G16" s="17"/>
+      <c r="H16" s="17"/>
+      <c r="I16" s="17"/>
+      <c r="J16" s="91"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" s="90"/>
+      <c r="B17" s="17"/>
+      <c r="C17" s="17"/>
+      <c r="D17" s="17"/>
+      <c r="E17" s="17"/>
+      <c r="F17" s="17"/>
+      <c r="G17" s="17"/>
+      <c r="H17" s="17"/>
+      <c r="I17" s="17"/>
+      <c r="J17" s="91"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" s="90"/>
+      <c r="B18" s="17"/>
+      <c r="C18" s="17"/>
+      <c r="D18" s="17"/>
+      <c r="E18" s="17"/>
+      <c r="F18" s="17"/>
+      <c r="G18" s="17"/>
+      <c r="H18" s="17"/>
+      <c r="I18" s="17"/>
+      <c r="J18" s="91"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" s="90"/>
+      <c r="B19" s="17"/>
+      <c r="C19" s="17"/>
+      <c r="D19" s="17"/>
+      <c r="E19" s="17"/>
+      <c r="F19" s="17"/>
+      <c r="G19" s="17"/>
+      <c r="H19" s="17"/>
+      <c r="I19" s="17"/>
+      <c r="J19" s="91"/>
+    </row>
+    <row r="20" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="92"/>
+      <c r="B20" s="93"/>
+      <c r="C20" s="93"/>
+      <c r="D20" s="93"/>
+      <c r="E20" s="93"/>
+      <c r="F20" s="93"/>
+      <c r="G20" s="93"/>
+      <c r="H20" s="93"/>
+      <c r="I20" s="93"/>
+      <c r="J20" s="94"/>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="D1:J1"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="G3:H3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8B463AB-5D43-4D17-8047-E3ADE0908B1A}">
   <dimension ref="A1:N21"/>
   <sheetViews>
@@ -2943,58 +3360,58 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="136" t="s">
+      <c r="A1" s="141" t="s">
         <v>40</v>
       </c>
-      <c r="B1" s="136"/>
-      <c r="C1" s="136"/>
-      <c r="D1" s="136"/>
-      <c r="E1" s="136"/>
-      <c r="F1" s="136"/>
-      <c r="G1" s="136"/>
-      <c r="H1" s="136"/>
-      <c r="I1" s="136"/>
-      <c r="J1" s="136"/>
-      <c r="K1" s="136"/>
-      <c r="L1" s="136"/>
-      <c r="M1" s="136"/>
-      <c r="N1" s="136"/>
+      <c r="B1" s="141"/>
+      <c r="C1" s="141"/>
+      <c r="D1" s="141"/>
+      <c r="E1" s="141"/>
+      <c r="F1" s="141"/>
+      <c r="G1" s="141"/>
+      <c r="H1" s="141"/>
+      <c r="I1" s="141"/>
+      <c r="J1" s="141"/>
+      <c r="K1" s="141"/>
+      <c r="L1" s="141"/>
+      <c r="M1" s="141"/>
+      <c r="N1" s="141"/>
     </row>
     <row r="2" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="137" t="s">
+      <c r="A2" s="142" t="s">
         <v>174</v>
       </c>
-      <c r="B2" s="137"/>
-      <c r="C2" s="137"/>
-      <c r="D2" s="137"/>
-      <c r="E2" s="137"/>
-      <c r="F2" s="137"/>
-      <c r="G2" s="137"/>
-      <c r="H2" s="137"/>
-      <c r="I2" s="137"/>
-      <c r="J2" s="137"/>
-      <c r="K2" s="137"/>
-      <c r="L2" s="137"/>
-      <c r="M2" s="137"/>
-      <c r="N2" s="137"/>
+      <c r="B2" s="142"/>
+      <c r="C2" s="142"/>
+      <c r="D2" s="142"/>
+      <c r="E2" s="142"/>
+      <c r="F2" s="142"/>
+      <c r="G2" s="142"/>
+      <c r="H2" s="142"/>
+      <c r="I2" s="142"/>
+      <c r="J2" s="142"/>
+      <c r="K2" s="142"/>
+      <c r="L2" s="142"/>
+      <c r="M2" s="142"/>
+      <c r="N2" s="142"/>
     </row>
     <row r="3" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="138" t="s">
+      <c r="A3" s="143" t="s">
         <v>175</v>
       </c>
-      <c r="B3" s="139"/>
-      <c r="C3" s="139"/>
-      <c r="D3" s="139"/>
-      <c r="E3" s="139"/>
-      <c r="F3" s="139"/>
-      <c r="G3" s="139"/>
-      <c r="H3" s="139"/>
-      <c r="I3" s="139"/>
-      <c r="J3" s="139"/>
-      <c r="K3" s="139"/>
-      <c r="L3" s="139"/>
-      <c r="M3" s="139"/>
-      <c r="N3" s="140"/>
+      <c r="B3" s="144"/>
+      <c r="C3" s="144"/>
+      <c r="D3" s="144"/>
+      <c r="E3" s="144"/>
+      <c r="F3" s="144"/>
+      <c r="G3" s="144"/>
+      <c r="H3" s="144"/>
+      <c r="I3" s="144"/>
+      <c r="J3" s="144"/>
+      <c r="K3" s="144"/>
+      <c r="L3" s="144"/>
+      <c r="M3" s="144"/>
+      <c r="N3" s="145"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="65" t="s">
@@ -3041,24 +3458,24 @@
       </c>
     </row>
     <row r="5" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="141" t="s">
+      <c r="A5" s="146" t="s">
         <v>184</v>
       </c>
-      <c r="B5" s="141"/>
-      <c r="C5" s="141"/>
-      <c r="D5" s="141"/>
-      <c r="E5" s="141"/>
-      <c r="F5" s="141"/>
-      <c r="G5" s="141"/>
-      <c r="H5" s="141"/>
-      <c r="I5" s="141"/>
-      <c r="J5" s="141"/>
-      <c r="K5" s="141"/>
-      <c r="L5" s="141"/>
-      <c r="M5" s="142" t="s">
+      <c r="B5" s="146"/>
+      <c r="C5" s="146"/>
+      <c r="D5" s="146"/>
+      <c r="E5" s="146"/>
+      <c r="F5" s="146"/>
+      <c r="G5" s="146"/>
+      <c r="H5" s="146"/>
+      <c r="I5" s="146"/>
+      <c r="J5" s="146"/>
+      <c r="K5" s="146"/>
+      <c r="L5" s="146"/>
+      <c r="M5" s="147" t="s">
         <v>185</v>
       </c>
-      <c r="N5" s="142"/>
+      <c r="N5" s="147"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="69">
@@ -3385,7 +3802,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{057F0B6F-9818-44F5-AA5B-A10992AB9C3A}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -3412,36 +3829,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="143" t="s">
+      <c r="A1" s="148" t="s">
         <v>221</v>
       </c>
-      <c r="B1" s="144"/>
-      <c r="C1" s="144"/>
-      <c r="D1" s="144"/>
-      <c r="E1" s="144"/>
-      <c r="F1" s="144"/>
-      <c r="G1" s="144"/>
-      <c r="H1" s="144"/>
-      <c r="I1" s="144"/>
-      <c r="J1" s="144"/>
-      <c r="K1" s="144"/>
-      <c r="L1" s="145"/>
+      <c r="B1" s="149"/>
+      <c r="C1" s="149"/>
+      <c r="D1" s="149"/>
+      <c r="E1" s="149"/>
+      <c r="F1" s="149"/>
+      <c r="G1" s="149"/>
+      <c r="H1" s="149"/>
+      <c r="I1" s="149"/>
+      <c r="J1" s="149"/>
+      <c r="K1" s="149"/>
+      <c r="L1" s="150"/>
     </row>
     <row r="2" spans="1:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="146" t="s">
+      <c r="A2" s="151" t="s">
         <v>222</v>
       </c>
-      <c r="B2" s="147"/>
-      <c r="C2" s="147"/>
-      <c r="D2" s="147"/>
-      <c r="E2" s="147"/>
-      <c r="F2" s="147"/>
-      <c r="G2" s="147"/>
-      <c r="H2" s="147"/>
-      <c r="I2" s="147"/>
-      <c r="J2" s="147"/>
-      <c r="K2" s="147"/>
-      <c r="L2" s="148"/>
+      <c r="B2" s="152"/>
+      <c r="C2" s="152"/>
+      <c r="D2" s="152"/>
+      <c r="E2" s="152"/>
+      <c r="F2" s="152"/>
+      <c r="G2" s="152"/>
+      <c r="H2" s="152"/>
+      <c r="I2" s="152"/>
+      <c r="J2" s="152"/>
+      <c r="K2" s="152"/>
+      <c r="L2" s="153"/>
     </row>
     <row r="3" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="74" t="s">
@@ -3462,32 +3879,32 @@
       <c r="F3" s="74" t="s">
         <v>219</v>
       </c>
-      <c r="G3" s="156" t="s">
+      <c r="G3" s="161" t="s">
         <v>39</v>
       </c>
-      <c r="H3" s="157"/>
-      <c r="I3" s="157"/>
-      <c r="J3" s="157"/>
-      <c r="K3" s="158"/>
+      <c r="H3" s="162"/>
+      <c r="I3" s="162"/>
+      <c r="J3" s="162"/>
+      <c r="K3" s="163"/>
       <c r="L3" s="85" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="162" t="s">
+      <c r="A4" s="167" t="s">
         <v>223</v>
       </c>
-      <c r="B4" s="163"/>
-      <c r="C4" s="163"/>
-      <c r="D4" s="163"/>
-      <c r="E4" s="163"/>
-      <c r="F4" s="163"/>
-      <c r="G4" s="163"/>
-      <c r="H4" s="163"/>
-      <c r="I4" s="163"/>
-      <c r="J4" s="163"/>
-      <c r="K4" s="163"/>
-      <c r="L4" s="164"/>
+      <c r="B4" s="168"/>
+      <c r="C4" s="168"/>
+      <c r="D4" s="168"/>
+      <c r="E4" s="168"/>
+      <c r="F4" s="168"/>
+      <c r="G4" s="168"/>
+      <c r="H4" s="168"/>
+      <c r="I4" s="168"/>
+      <c r="J4" s="168"/>
+      <c r="K4" s="168"/>
+      <c r="L4" s="169"/>
     </row>
     <row r="5" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="80">
@@ -3508,13 +3925,13 @@
       <c r="F5" s="83">
         <v>235689</v>
       </c>
-      <c r="G5" s="159" t="s">
+      <c r="G5" s="164" t="s">
         <v>213</v>
       </c>
-      <c r="H5" s="160"/>
-      <c r="I5" s="160"/>
-      <c r="J5" s="160"/>
-      <c r="K5" s="161"/>
+      <c r="H5" s="165"/>
+      <c r="I5" s="165"/>
+      <c r="J5" s="165"/>
+      <c r="K5" s="166"/>
       <c r="L5" s="81">
         <v>800</v>
       </c>
@@ -3538,13 +3955,13 @@
       <c r="F6" s="83">
         <v>235687</v>
       </c>
-      <c r="G6" s="159" t="s">
+      <c r="G6" s="164" t="s">
         <v>9</v>
       </c>
-      <c r="H6" s="160"/>
-      <c r="I6" s="160"/>
-      <c r="J6" s="160"/>
-      <c r="K6" s="161"/>
+      <c r="H6" s="165"/>
+      <c r="I6" s="165"/>
+      <c r="J6" s="165"/>
+      <c r="K6" s="166"/>
       <c r="L6" s="81">
         <v>1500</v>
       </c>
@@ -3568,51 +3985,51 @@
       <c r="F7" s="83">
         <v>235686</v>
       </c>
-      <c r="G7" s="159" t="s">
+      <c r="G7" s="164" t="s">
         <v>217</v>
       </c>
-      <c r="H7" s="160"/>
-      <c r="I7" s="160"/>
-      <c r="J7" s="160"/>
-      <c r="K7" s="161"/>
+      <c r="H7" s="165"/>
+      <c r="I7" s="165"/>
+      <c r="J7" s="165"/>
+      <c r="K7" s="166"/>
       <c r="L7" s="81">
         <v>1600</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="149" t="s">
+      <c r="A8" s="154" t="s">
         <v>212</v>
       </c>
-      <c r="B8" s="149"/>
-      <c r="C8" s="149"/>
-      <c r="D8" s="149"/>
-      <c r="E8" s="149"/>
-      <c r="F8" s="149"/>
-      <c r="G8" s="149"/>
-      <c r="H8" s="149"/>
-      <c r="I8" s="149"/>
-      <c r="J8" s="149"/>
-      <c r="K8" s="149"/>
+      <c r="B8" s="154"/>
+      <c r="C8" s="154"/>
+      <c r="D8" s="154"/>
+      <c r="E8" s="154"/>
+      <c r="F8" s="154"/>
+      <c r="G8" s="154"/>
+      <c r="H8" s="154"/>
+      <c r="I8" s="154"/>
+      <c r="J8" s="154"/>
+      <c r="K8" s="154"/>
       <c r="L8" s="75">
         <f t="shared" ref="L8" si="0">SUM(L5:L7)</f>
         <v>3900</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="162" t="s">
+      <c r="A9" s="167" t="s">
         <v>224</v>
       </c>
-      <c r="B9" s="163"/>
-      <c r="C9" s="163"/>
-      <c r="D9" s="163"/>
-      <c r="E9" s="163"/>
-      <c r="F9" s="163"/>
-      <c r="G9" s="163"/>
-      <c r="H9" s="163"/>
-      <c r="I9" s="163"/>
-      <c r="J9" s="163"/>
-      <c r="K9" s="163"/>
-      <c r="L9" s="164"/>
+      <c r="B9" s="168"/>
+      <c r="C9" s="168"/>
+      <c r="D9" s="168"/>
+      <c r="E9" s="168"/>
+      <c r="F9" s="168"/>
+      <c r="G9" s="168"/>
+      <c r="H9" s="168"/>
+      <c r="I9" s="168"/>
+      <c r="J9" s="168"/>
+      <c r="K9" s="168"/>
+      <c r="L9" s="169"/>
     </row>
     <row r="10" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="80">
@@ -3633,13 +4050,13 @@
       <c r="F10" s="84">
         <v>215496</v>
       </c>
-      <c r="G10" s="159" t="s">
+      <c r="G10" s="164" t="s">
         <v>216</v>
       </c>
-      <c r="H10" s="160"/>
-      <c r="I10" s="160"/>
-      <c r="J10" s="160"/>
-      <c r="K10" s="161"/>
+      <c r="H10" s="165"/>
+      <c r="I10" s="165"/>
+      <c r="J10" s="165"/>
+      <c r="K10" s="166"/>
       <c r="L10" s="81">
         <v>1000</v>
       </c>
@@ -3663,50 +4080,50 @@
       <c r="F11" s="84">
         <v>124586</v>
       </c>
-      <c r="G11" s="159" t="s">
+      <c r="G11" s="164" t="s">
         <v>216</v>
       </c>
-      <c r="H11" s="160"/>
-      <c r="I11" s="160"/>
-      <c r="J11" s="160"/>
-      <c r="K11" s="161"/>
+      <c r="H11" s="165"/>
+      <c r="I11" s="165"/>
+      <c r="J11" s="165"/>
+      <c r="K11" s="166"/>
       <c r="L11" s="81">
         <v>2000</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="165" t="s">
+      <c r="A12" s="170" t="s">
         <v>212</v>
       </c>
-      <c r="B12" s="166"/>
-      <c r="C12" s="166"/>
-      <c r="D12" s="166"/>
-      <c r="E12" s="166"/>
-      <c r="F12" s="166"/>
-      <c r="G12" s="166"/>
-      <c r="H12" s="166"/>
-      <c r="I12" s="166"/>
-      <c r="J12" s="166"/>
-      <c r="K12" s="167"/>
+      <c r="B12" s="171"/>
+      <c r="C12" s="171"/>
+      <c r="D12" s="171"/>
+      <c r="E12" s="171"/>
+      <c r="F12" s="171"/>
+      <c r="G12" s="171"/>
+      <c r="H12" s="171"/>
+      <c r="I12" s="171"/>
+      <c r="J12" s="171"/>
+      <c r="K12" s="172"/>
       <c r="L12" s="76">
         <v>3000</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="162" t="s">
+      <c r="A13" s="167" t="s">
         <v>225</v>
       </c>
-      <c r="B13" s="163"/>
-      <c r="C13" s="163"/>
-      <c r="D13" s="163"/>
-      <c r="E13" s="163"/>
-      <c r="F13" s="163"/>
-      <c r="G13" s="163"/>
-      <c r="H13" s="163"/>
-      <c r="I13" s="163"/>
-      <c r="J13" s="163"/>
-      <c r="K13" s="163"/>
-      <c r="L13" s="164"/>
+      <c r="B13" s="168"/>
+      <c r="C13" s="168"/>
+      <c r="D13" s="168"/>
+      <c r="E13" s="168"/>
+      <c r="F13" s="168"/>
+      <c r="G13" s="168"/>
+      <c r="H13" s="168"/>
+      <c r="I13" s="168"/>
+      <c r="J13" s="168"/>
+      <c r="K13" s="168"/>
+      <c r="L13" s="169"/>
     </row>
     <row r="14" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="80">
@@ -3727,49 +4144,49 @@
       <c r="F14" s="84">
         <v>965241</v>
       </c>
-      <c r="G14" s="159" t="s">
+      <c r="G14" s="164" t="s">
         <v>220</v>
       </c>
-      <c r="H14" s="160"/>
-      <c r="I14" s="160"/>
-      <c r="J14" s="160"/>
-      <c r="K14" s="161"/>
+      <c r="H14" s="165"/>
+      <c r="I14" s="165"/>
+      <c r="J14" s="165"/>
+      <c r="K14" s="166"/>
       <c r="L14" s="81">
         <v>1200</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="150" t="s">
+      <c r="A15" s="155" t="s">
         <v>212</v>
       </c>
-      <c r="B15" s="151"/>
-      <c r="C15" s="151"/>
-      <c r="D15" s="151"/>
-      <c r="E15" s="151"/>
-      <c r="F15" s="151"/>
-      <c r="G15" s="151"/>
-      <c r="H15" s="151"/>
-      <c r="I15" s="151"/>
-      <c r="J15" s="151"/>
-      <c r="K15" s="152"/>
+      <c r="B15" s="156"/>
+      <c r="C15" s="156"/>
+      <c r="D15" s="156"/>
+      <c r="E15" s="156"/>
+      <c r="F15" s="156"/>
+      <c r="G15" s="156"/>
+      <c r="H15" s="156"/>
+      <c r="I15" s="156"/>
+      <c r="J15" s="156"/>
+      <c r="K15" s="157"/>
       <c r="L15" s="79">
         <v>1200</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="21" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="153" t="s">
+      <c r="A16" s="158" t="s">
         <v>226</v>
       </c>
-      <c r="B16" s="154"/>
-      <c r="C16" s="154"/>
-      <c r="D16" s="154"/>
-      <c r="E16" s="154"/>
-      <c r="F16" s="154"/>
-      <c r="G16" s="154"/>
-      <c r="H16" s="154"/>
-      <c r="I16" s="154"/>
-      <c r="J16" s="154"/>
-      <c r="K16" s="155"/>
+      <c r="B16" s="159"/>
+      <c r="C16" s="159"/>
+      <c r="D16" s="159"/>
+      <c r="E16" s="159"/>
+      <c r="F16" s="159"/>
+      <c r="G16" s="159"/>
+      <c r="H16" s="159"/>
+      <c r="I16" s="159"/>
+      <c r="J16" s="159"/>
+      <c r="K16" s="160"/>
       <c r="L16" s="77">
         <f>L8+L12+L15</f>
         <v>8100</v>
@@ -3814,145 +4231,145 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7E8279C-BD17-431E-B47D-C2804D5BC3A3}">
   <dimension ref="A1:J22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L30" sqref="L30"/>
+      <selection activeCell="N20" sqref="N20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:10" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="135"/>
-      <c r="B1" s="135"/>
-      <c r="C1" s="135"/>
-      <c r="D1" s="135"/>
-      <c r="E1" s="168" t="s">
+      <c r="A1" s="140"/>
+      <c r="B1" s="140"/>
+      <c r="C1" s="140"/>
+      <c r="D1" s="140"/>
+      <c r="E1" s="182" t="s">
         <v>227</v>
       </c>
-      <c r="F1" s="168"/>
-      <c r="G1" s="168"/>
-      <c r="H1" s="168"/>
-      <c r="I1" s="168"/>
-      <c r="J1" s="168"/>
+      <c r="F1" s="182"/>
+      <c r="G1" s="182"/>
+      <c r="H1" s="182"/>
+      <c r="I1" s="182"/>
+      <c r="J1" s="182"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="135"/>
-      <c r="B2" s="135"/>
-      <c r="C2" s="135"/>
-      <c r="D2" s="135"/>
-      <c r="E2" s="169" t="s">
+      <c r="A2" s="140"/>
+      <c r="B2" s="140"/>
+      <c r="C2" s="140"/>
+      <c r="D2" s="140"/>
+      <c r="E2" s="183" t="s">
         <v>257</v>
       </c>
-      <c r="F2" s="169"/>
-      <c r="G2" s="169"/>
-      <c r="H2" s="169"/>
-      <c r="I2" s="169"/>
-      <c r="J2" s="169"/>
+      <c r="F2" s="183"/>
+      <c r="G2" s="183"/>
+      <c r="H2" s="183"/>
+      <c r="I2" s="183"/>
+      <c r="J2" s="183"/>
     </row>
     <row r="3" spans="1:10" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="174"/>
-      <c r="B3" s="174"/>
-      <c r="C3" s="174"/>
-      <c r="D3" s="174"/>
-      <c r="E3" s="170" t="s">
+      <c r="A3" s="176"/>
+      <c r="B3" s="176"/>
+      <c r="C3" s="176"/>
+      <c r="D3" s="176"/>
+      <c r="E3" s="184" t="s">
         <v>228</v>
       </c>
-      <c r="F3" s="170"/>
-      <c r="G3" s="170"/>
-      <c r="H3" s="170"/>
-      <c r="I3" s="170"/>
-      <c r="J3" s="170"/>
+      <c r="F3" s="184"/>
+      <c r="G3" s="184"/>
+      <c r="H3" s="184"/>
+      <c r="I3" s="184"/>
+      <c r="J3" s="184"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="132" t="s">
+      <c r="A4" s="137" t="s">
         <v>229</v>
       </c>
-      <c r="B4" s="132"/>
-      <c r="C4" s="132"/>
-      <c r="D4" s="132"/>
-      <c r="E4" s="132"/>
-      <c r="F4" s="132"/>
-      <c r="G4" s="132"/>
-      <c r="H4" s="132"/>
-      <c r="I4" s="132"/>
-      <c r="J4" s="132"/>
+      <c r="B4" s="137"/>
+      <c r="C4" s="137"/>
+      <c r="D4" s="137"/>
+      <c r="E4" s="137"/>
+      <c r="F4" s="137"/>
+      <c r="G4" s="137"/>
+      <c r="H4" s="137"/>
+      <c r="I4" s="137"/>
+      <c r="J4" s="137"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="172" t="s">
+      <c r="A5" s="174" t="s">
         <v>250</v>
       </c>
-      <c r="B5" s="172"/>
-      <c r="C5" s="172" t="s">
+      <c r="B5" s="174"/>
+      <c r="C5" s="174" t="s">
         <v>255</v>
       </c>
-      <c r="D5" s="172"/>
-      <c r="E5" s="172"/>
-      <c r="F5" s="172"/>
+      <c r="D5" s="174"/>
+      <c r="E5" s="174"/>
+      <c r="F5" s="174"/>
       <c r="G5" s="86"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="171" t="s">
+      <c r="A6" s="173" t="s">
         <v>146</v>
       </c>
-      <c r="B6" s="171"/>
-      <c r="C6" s="171" t="s">
+      <c r="B6" s="173"/>
+      <c r="C6" s="173" t="s">
         <v>251</v>
       </c>
-      <c r="D6" s="171"/>
-      <c r="E6" s="171"/>
-      <c r="F6" s="171"/>
-      <c r="G6" s="171" t="s">
+      <c r="D6" s="173"/>
+      <c r="E6" s="173"/>
+      <c r="F6" s="173"/>
+      <c r="G6" s="173" t="s">
         <v>145</v>
       </c>
-      <c r="H6" s="171"/>
-      <c r="I6" s="171" t="s">
+      <c r="H6" s="173"/>
+      <c r="I6" s="173" t="s">
         <v>256</v>
       </c>
-      <c r="J6" s="171"/>
+      <c r="J6" s="173"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="171" t="s">
+      <c r="A7" s="173" t="s">
         <v>35</v>
       </c>
-      <c r="B7" s="171"/>
-      <c r="C7" s="171" t="s">
+      <c r="B7" s="173"/>
+      <c r="C7" s="173" t="s">
         <v>252</v>
       </c>
-      <c r="D7" s="171"/>
+      <c r="D7" s="173"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="171" t="s">
+      <c r="A8" s="173" t="s">
         <v>230</v>
       </c>
-      <c r="B8" s="171"/>
-      <c r="C8" s="175" t="s">
+      <c r="B8" s="173"/>
+      <c r="C8" s="177" t="s">
         <v>253</v>
       </c>
-      <c r="D8" s="175"/>
+      <c r="D8" s="177"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="171" t="s">
+      <c r="A9" s="173" t="s">
         <v>231</v>
       </c>
-      <c r="B9" s="171"/>
-      <c r="C9" s="176" t="s">
+      <c r="B9" s="173"/>
+      <c r="C9" s="178" t="s">
         <v>254</v>
       </c>
-      <c r="D9" s="176"/>
-      <c r="E9" s="176"/>
+      <c r="D9" s="178"/>
+      <c r="E9" s="178"/>
     </row>
     <row r="10" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="55" t="s">
         <v>233</v>
       </c>
-      <c r="B10" s="177" t="s">
+      <c r="B10" s="179" t="s">
         <v>232</v>
       </c>
-      <c r="C10" s="178"/>
-      <c r="D10" s="179"/>
+      <c r="C10" s="180"/>
+      <c r="D10" s="181"/>
       <c r="E10" s="55" t="s">
         <v>15</v>
       </c>
@@ -3976,11 +4393,11 @@
       <c r="A11" s="55">
         <v>101</v>
       </c>
-      <c r="B11" s="131" t="s">
+      <c r="B11" s="136" t="s">
         <v>234</v>
       </c>
-      <c r="C11" s="132"/>
-      <c r="D11" s="133"/>
+      <c r="C11" s="137"/>
+      <c r="D11" s="138"/>
       <c r="E11" s="55">
         <v>50</v>
       </c>
@@ -4001,11 +4418,11 @@
       <c r="A12" s="55">
         <v>102</v>
       </c>
-      <c r="B12" s="131" t="s">
+      <c r="B12" s="136" t="s">
         <v>235</v>
       </c>
-      <c r="C12" s="132"/>
-      <c r="D12" s="133"/>
+      <c r="C12" s="137"/>
+      <c r="D12" s="138"/>
       <c r="E12" s="55">
         <v>50</v>
       </c>
@@ -4026,11 +4443,11 @@
       <c r="A13" s="55">
         <v>103</v>
       </c>
-      <c r="B13" s="131" t="s">
+      <c r="B13" s="136" t="s">
         <v>236</v>
       </c>
-      <c r="C13" s="132"/>
-      <c r="D13" s="133"/>
+      <c r="C13" s="137"/>
+      <c r="D13" s="138"/>
       <c r="E13" s="55">
         <v>50</v>
       </c>
@@ -4051,11 +4468,11 @@
       <c r="A14" s="55">
         <v>104</v>
       </c>
-      <c r="B14" s="131" t="s">
+      <c r="B14" s="136" t="s">
         <v>237</v>
       </c>
-      <c r="C14" s="132"/>
-      <c r="D14" s="133"/>
+      <c r="C14" s="137"/>
+      <c r="D14" s="138"/>
       <c r="E14" s="55">
         <v>50</v>
       </c>
@@ -4076,11 +4493,11 @@
       <c r="A15" s="55">
         <v>105</v>
       </c>
-      <c r="B15" s="131" t="s">
+      <c r="B15" s="136" t="s">
         <v>238</v>
       </c>
-      <c r="C15" s="132"/>
-      <c r="D15" s="133"/>
+      <c r="C15" s="137"/>
+      <c r="D15" s="138"/>
       <c r="E15" s="55">
         <v>50</v>
       </c>
@@ -4101,11 +4518,11 @@
       <c r="A16" s="55">
         <v>106</v>
       </c>
-      <c r="B16" s="131" t="s">
+      <c r="B16" s="136" t="s">
         <v>239</v>
       </c>
-      <c r="C16" s="132"/>
-      <c r="D16" s="133"/>
+      <c r="C16" s="137"/>
+      <c r="D16" s="138"/>
       <c r="E16" s="55">
         <v>50</v>
       </c>
@@ -4126,11 +4543,11 @@
       <c r="A17" s="55">
         <v>107</v>
       </c>
-      <c r="B17" s="131" t="s">
+      <c r="B17" s="136" t="s">
         <v>240</v>
       </c>
-      <c r="C17" s="132"/>
-      <c r="D17" s="133"/>
+      <c r="C17" s="137"/>
+      <c r="D17" s="138"/>
       <c r="E17" s="55">
         <v>50</v>
       </c>
@@ -4151,11 +4568,11 @@
       <c r="A18" s="55">
         <v>108</v>
       </c>
-      <c r="B18" s="131" t="s">
+      <c r="B18" s="136" t="s">
         <v>241</v>
       </c>
-      <c r="C18" s="132"/>
-      <c r="D18" s="133"/>
+      <c r="C18" s="137"/>
+      <c r="D18" s="138"/>
       <c r="E18" s="55">
         <v>50</v>
       </c>
@@ -4176,11 +4593,11 @@
       <c r="A19" s="55">
         <v>109</v>
       </c>
-      <c r="B19" s="131" t="s">
+      <c r="B19" s="136" t="s">
         <v>242</v>
       </c>
-      <c r="C19" s="132"/>
-      <c r="D19" s="133"/>
+      <c r="C19" s="137"/>
+      <c r="D19" s="138"/>
       <c r="E19" s="55">
         <v>50</v>
       </c>
@@ -4201,11 +4618,11 @@
       <c r="A20" s="55">
         <v>110</v>
       </c>
-      <c r="B20" s="131" t="s">
+      <c r="B20" s="136" t="s">
         <v>243</v>
       </c>
-      <c r="C20" s="132"/>
-      <c r="D20" s="133"/>
+      <c r="C20" s="137"/>
+      <c r="D20" s="138"/>
       <c r="E20" s="55">
         <v>50</v>
       </c>
@@ -4226,11 +4643,11 @@
       <c r="A21" s="55">
         <v>111</v>
       </c>
-      <c r="B21" s="131" t="s">
+      <c r="B21" s="136" t="s">
         <v>244</v>
       </c>
-      <c r="C21" s="132"/>
-      <c r="D21" s="133"/>
+      <c r="C21" s="137"/>
+      <c r="D21" s="138"/>
       <c r="E21" s="55">
         <v>50</v>
       </c>
@@ -4248,12 +4665,12 @@
       <c r="J21" s="4"/>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="173" t="s">
+      <c r="A22" s="175" t="s">
         <v>248</v>
       </c>
-      <c r="B22" s="173"/>
-      <c r="C22" s="173"/>
-      <c r="D22" s="173"/>
+      <c r="B22" s="175"/>
+      <c r="C22" s="175"/>
+      <c r="D22" s="175"/>
       <c r="E22" s="86">
         <f>SUM(E11:E21)</f>
         <v>550</v>
@@ -4265,12 +4682,14 @@
     </row>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="E1:J1"/>
+    <mergeCell ref="E2:J2"/>
+    <mergeCell ref="E3:J3"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="C6:F6"/>
+    <mergeCell ref="C5:F5"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="I6:J6"/>
     <mergeCell ref="B19:D19"/>
     <mergeCell ref="B20:D20"/>
     <mergeCell ref="B21:D21"/>
@@ -4287,14 +4706,12 @@
     <mergeCell ref="B16:D16"/>
     <mergeCell ref="B17:D17"/>
     <mergeCell ref="B18:D18"/>
-    <mergeCell ref="E1:J1"/>
-    <mergeCell ref="E2:J2"/>
-    <mergeCell ref="E3:J3"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="C6:F6"/>
-    <mergeCell ref="C5:F5"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="I6:J6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A6:B6"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4303,12 +4720,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0D3CB5C-E45F-4446-A4A9-5BAE1F767FB0}">
   <dimension ref="A1:J14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O9" sqref="O9"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L25" sqref="L25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4323,106 +4740,106 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="183" t="s">
+      <c r="A1" s="190" t="s">
         <v>259</v>
       </c>
-      <c r="B1" s="183"/>
-      <c r="C1" s="183"/>
-      <c r="D1" s="183"/>
-      <c r="E1" s="183"/>
-      <c r="F1" s="183"/>
-      <c r="G1" s="183"/>
-      <c r="H1" s="183"/>
-      <c r="I1" s="183"/>
-      <c r="J1" s="183"/>
+      <c r="B1" s="190"/>
+      <c r="C1" s="190"/>
+      <c r="D1" s="190"/>
+      <c r="E1" s="190"/>
+      <c r="F1" s="190"/>
+      <c r="G1" s="190"/>
+      <c r="H1" s="190"/>
+      <c r="I1" s="190"/>
+      <c r="J1" s="190"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="182" t="s">
+      <c r="A2" s="191" t="s">
         <v>260</v>
       </c>
-      <c r="B2" s="182"/>
-      <c r="C2" s="182"/>
-      <c r="D2" s="182"/>
-      <c r="E2" s="182"/>
-      <c r="F2" s="182"/>
-      <c r="G2" s="182"/>
-      <c r="H2" s="182"/>
-      <c r="I2" s="182"/>
-      <c r="J2" s="182"/>
+      <c r="B2" s="191"/>
+      <c r="C2" s="191"/>
+      <c r="D2" s="191"/>
+      <c r="E2" s="191"/>
+      <c r="F2" s="191"/>
+      <c r="G2" s="191"/>
+      <c r="H2" s="191"/>
+      <c r="I2" s="191"/>
+      <c r="J2" s="191"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="132" t="s">
+      <c r="A3" s="137" t="s">
         <v>261</v>
       </c>
-      <c r="B3" s="132"/>
-      <c r="C3" s="132"/>
-      <c r="D3" s="132"/>
-      <c r="E3" s="132"/>
-      <c r="F3" s="132"/>
-      <c r="G3" s="132"/>
-      <c r="H3" s="132"/>
-      <c r="I3" s="132"/>
-      <c r="J3" s="132"/>
+      <c r="B3" s="137"/>
+      <c r="C3" s="137"/>
+      <c r="D3" s="137"/>
+      <c r="E3" s="137"/>
+      <c r="F3" s="137"/>
+      <c r="G3" s="137"/>
+      <c r="H3" s="137"/>
+      <c r="I3" s="137"/>
+      <c r="J3" s="137"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="194" t="s">
+      <c r="A4" s="188" t="s">
         <v>265</v>
       </c>
-      <c r="B4" s="194"/>
-      <c r="C4" s="185">
+      <c r="B4" s="188"/>
+      <c r="C4" s="192">
         <v>8563214</v>
       </c>
-      <c r="D4" s="185"/>
-      <c r="E4" s="185"/>
+      <c r="D4" s="192"/>
+      <c r="E4" s="192"/>
       <c r="F4" s="64"/>
-      <c r="G4" s="192" t="s">
+      <c r="G4" s="98" t="s">
         <v>52</v>
       </c>
-      <c r="H4" s="187">
+      <c r="H4" s="193">
         <v>45280</v>
       </c>
-      <c r="I4" s="188"/>
-      <c r="J4" s="188"/>
+      <c r="I4" s="194"/>
+      <c r="J4" s="194"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="194" t="s">
+      <c r="A5" s="188" t="s">
         <v>263</v>
       </c>
-      <c r="B5" s="194"/>
-      <c r="C5" s="186" t="s">
+      <c r="B5" s="188"/>
+      <c r="C5" s="189" t="s">
         <v>262</v>
       </c>
-      <c r="D5" s="186"/>
-      <c r="E5" s="186"/>
+      <c r="D5" s="189"/>
+      <c r="E5" s="189"/>
       <c r="F5" s="64"/>
-      <c r="G5" s="192" t="s">
+      <c r="G5" s="98" t="s">
         <v>264</v>
       </c>
-      <c r="H5" s="186">
+      <c r="H5" s="189">
         <v>230546</v>
       </c>
-      <c r="I5" s="186"/>
-      <c r="J5" s="186"/>
+      <c r="I5" s="189"/>
+      <c r="J5" s="189"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="194" t="s">
+      <c r="A6" s="188" t="s">
         <v>266</v>
       </c>
-      <c r="B6" s="194"/>
-      <c r="C6" s="186" t="s">
+      <c r="B6" s="188"/>
+      <c r="C6" s="189" t="s">
         <v>198</v>
       </c>
-      <c r="D6" s="186"/>
-      <c r="E6" s="186"/>
+      <c r="D6" s="189"/>
+      <c r="E6" s="189"/>
       <c r="F6" s="8"/>
-      <c r="G6" s="193" t="s">
+      <c r="G6" s="99" t="s">
         <v>267</v>
       </c>
-      <c r="H6" s="186" t="s">
+      <c r="H6" s="189" t="s">
         <v>199</v>
       </c>
-      <c r="I6" s="186"/>
-      <c r="J6" s="186"/>
+      <c r="I6" s="189"/>
+      <c r="J6" s="189"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="64"/>
@@ -4430,48 +4847,48 @@
       <c r="C7" s="64"/>
       <c r="D7" s="64"/>
       <c r="E7" s="64"/>
-      <c r="F7" s="190" t="s">
+      <c r="F7" s="187" t="s">
         <v>210</v>
       </c>
-      <c r="G7" s="190"/>
+      <c r="G7" s="187"/>
       <c r="H7" s="89"/>
-      <c r="I7" s="189">
+      <c r="I7" s="96">
         <v>1500</v>
       </c>
-      <c r="J7" s="189" t="s">
+      <c r="J7" s="96" t="s">
         <v>269</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="F8" s="132" t="s">
+      <c r="F8" s="137" t="s">
         <v>15</v>
       </c>
-      <c r="G8" s="132"/>
-      <c r="H8" s="191"/>
-      <c r="I8" s="191">
+      <c r="G8" s="137"/>
+      <c r="H8" s="97"/>
+      <c r="I8" s="97">
         <v>1500</v>
       </c>
-      <c r="J8" s="191" t="s">
+      <c r="J8" s="97" t="s">
         <v>269</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="F9" s="180"/>
-      <c r="G9" s="180"/>
+      <c r="F9" s="95"/>
+      <c r="G9" s="95"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="64"/>
       <c r="B10" s="64"/>
-      <c r="C10" s="98" t="s">
+      <c r="C10" s="103" t="s">
         <v>270</v>
       </c>
-      <c r="D10" s="98"/>
-      <c r="E10" s="98"/>
-      <c r="F10" s="98"/>
-      <c r="G10" s="98"/>
-      <c r="H10" s="98"/>
-      <c r="I10" s="98"/>
-      <c r="J10" s="98"/>
+      <c r="D10" s="103"/>
+      <c r="E10" s="103"/>
+      <c r="F10" s="103"/>
+      <c r="G10" s="103"/>
+      <c r="H10" s="103"/>
+      <c r="I10" s="103"/>
+      <c r="J10" s="103"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="87"/>
@@ -4491,47 +4908,47 @@
       <c r="C12" s="88"/>
       <c r="D12" s="88"/>
       <c r="E12" s="88"/>
-      <c r="F12" s="181"/>
-      <c r="G12" s="181"/>
-      <c r="H12" s="181"/>
-      <c r="I12" s="181"/>
-      <c r="J12" s="181"/>
+      <c r="F12" s="186"/>
+      <c r="G12" s="186"/>
+      <c r="H12" s="186"/>
+      <c r="I12" s="186"/>
+      <c r="J12" s="186"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="F13" s="174"/>
-      <c r="G13" s="174"/>
-      <c r="H13" s="174"/>
-      <c r="I13" s="174"/>
-      <c r="J13" s="174"/>
+      <c r="F13" s="176"/>
+      <c r="G13" s="176"/>
+      <c r="H13" s="176"/>
+      <c r="I13" s="176"/>
+      <c r="J13" s="176"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="F14" s="184" t="s">
+      <c r="F14" s="185" t="s">
         <v>268</v>
       </c>
-      <c r="G14" s="184"/>
-      <c r="H14" s="184"/>
-      <c r="I14" s="184"/>
-      <c r="J14" s="184"/>
+      <c r="G14" s="185"/>
+      <c r="H14" s="185"/>
+      <c r="I14" s="185"/>
+      <c r="J14" s="185"/>
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="F14:J14"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="C10:J10"/>
-    <mergeCell ref="F12:J13"/>
-    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="H4:J4"/>
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="C5:E5"/>
     <mergeCell ref="H5:J5"/>
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="C6:E6"/>
     <mergeCell ref="H6:J6"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="H4:J4"/>
+    <mergeCell ref="F14:J14"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="C10:J10"/>
+    <mergeCell ref="F12:J13"/>
+    <mergeCell ref="F7:G7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4543,7 +4960,7 @@
   <dimension ref="A1:I36"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="K23" sqref="K23"/>
+      <selection activeCell="J28" sqref="J28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4557,44 +4974,44 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="101" t="s">
+      <c r="A1" s="106" t="s">
         <v>134</v>
       </c>
-      <c r="B1" s="102"/>
-      <c r="C1" s="102"/>
-      <c r="D1" s="102"/>
-      <c r="E1" s="102"/>
-      <c r="F1" s="102"/>
+      <c r="B1" s="107"/>
+      <c r="C1" s="107"/>
+      <c r="D1" s="107"/>
+      <c r="E1" s="107"/>
+      <c r="F1" s="107"/>
     </row>
     <row r="2" spans="1:9" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="102"/>
-      <c r="B2" s="102"/>
-      <c r="C2" s="102"/>
-      <c r="D2" s="102"/>
-      <c r="E2" s="102"/>
-      <c r="F2" s="102"/>
+      <c r="A2" s="107"/>
+      <c r="B2" s="107"/>
+      <c r="C2" s="107"/>
+      <c r="D2" s="107"/>
+      <c r="E2" s="107"/>
+      <c r="F2" s="107"/>
     </row>
     <row r="3" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="103" t="s">
+      <c r="A3" s="108" t="s">
         <v>133</v>
       </c>
-      <c r="B3" s="103"/>
-      <c r="C3" s="103"/>
-      <c r="D3" s="103"/>
-      <c r="E3" s="103"/>
-      <c r="F3" s="103"/>
+      <c r="B3" s="108"/>
+      <c r="C3" s="108"/>
+      <c r="D3" s="108"/>
+      <c r="E3" s="108"/>
+      <c r="F3" s="108"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="104" t="s">
+      <c r="A4" s="109" t="s">
         <v>144</v>
       </c>
-      <c r="B4" s="104"/>
+      <c r="B4" s="109"/>
       <c r="C4" s="51"/>
       <c r="D4" s="51"/>
-      <c r="E4" s="105" t="s">
+      <c r="E4" s="110" t="s">
         <v>114</v>
       </c>
-      <c r="F4" s="105"/>
+      <c r="F4" s="110"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="43" t="s">
@@ -5150,6 +5567,276 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1D32889-7A1F-4945-8F58-77FCE4F7EEAF}">
+  <dimension ref="A1:J16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K10" sqref="K10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="203" t="s">
+        <v>271</v>
+      </c>
+      <c r="B1" s="204"/>
+      <c r="C1" s="205"/>
+      <c r="D1" s="195"/>
+      <c r="E1" s="196"/>
+      <c r="F1" s="196"/>
+      <c r="G1" s="196"/>
+      <c r="H1" s="196"/>
+      <c r="I1" s="196"/>
+      <c r="J1" s="197"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="206"/>
+      <c r="B2" s="207"/>
+      <c r="C2" s="208"/>
+      <c r="D2" s="215" t="s">
+        <v>273</v>
+      </c>
+      <c r="E2" s="216"/>
+      <c r="F2" s="216"/>
+      <c r="G2" s="214"/>
+      <c r="H2" s="214" t="s">
+        <v>272</v>
+      </c>
+      <c r="I2" s="214"/>
+      <c r="J2" s="223"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="206"/>
+      <c r="B3" s="207"/>
+      <c r="C3" s="208"/>
+      <c r="D3" s="221" t="s">
+        <v>208</v>
+      </c>
+      <c r="E3" s="217" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" s="217" t="s">
+        <v>277</v>
+      </c>
+      <c r="G3" s="222" t="s">
+        <v>15</v>
+      </c>
+      <c r="H3" s="17"/>
+      <c r="I3" s="17"/>
+      <c r="J3" s="199"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="206"/>
+      <c r="B4" s="207"/>
+      <c r="C4" s="208"/>
+      <c r="D4" s="213" t="s">
+        <v>210</v>
+      </c>
+      <c r="E4" s="17">
+        <v>2000</v>
+      </c>
+      <c r="F4" s="17">
+        <v>1</v>
+      </c>
+      <c r="G4" s="17">
+        <v>2000</v>
+      </c>
+      <c r="H4" s="17"/>
+      <c r="I4" s="17"/>
+      <c r="J4" s="199"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="206"/>
+      <c r="B5" s="207"/>
+      <c r="C5" s="208"/>
+      <c r="D5" s="213" t="s">
+        <v>274</v>
+      </c>
+      <c r="E5" s="17">
+        <v>1200</v>
+      </c>
+      <c r="F5" s="17">
+        <v>12</v>
+      </c>
+      <c r="G5" s="17">
+        <v>14400</v>
+      </c>
+      <c r="H5" s="17"/>
+      <c r="I5" s="17"/>
+      <c r="J5" s="199"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="206"/>
+      <c r="B6" s="207"/>
+      <c r="C6" s="208"/>
+      <c r="D6" s="213" t="s">
+        <v>275</v>
+      </c>
+      <c r="E6" s="17">
+        <v>500</v>
+      </c>
+      <c r="F6" s="17">
+        <v>2</v>
+      </c>
+      <c r="G6" s="17">
+        <v>1000</v>
+      </c>
+      <c r="H6" s="17"/>
+      <c r="I6" s="17"/>
+      <c r="J6" s="199"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="206"/>
+      <c r="B7" s="207"/>
+      <c r="C7" s="208"/>
+      <c r="D7" s="213" t="s">
+        <v>276</v>
+      </c>
+      <c r="E7" s="212">
+        <v>800</v>
+      </c>
+      <c r="F7" s="212">
+        <v>1</v>
+      </c>
+      <c r="G7" s="212">
+        <v>800</v>
+      </c>
+      <c r="H7" s="17"/>
+      <c r="I7" s="17"/>
+      <c r="J7" s="199"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="206"/>
+      <c r="B8" s="207"/>
+      <c r="C8" s="208"/>
+      <c r="D8" s="218" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8" s="219"/>
+      <c r="F8" s="219"/>
+      <c r="G8" s="220">
+        <f>SUM(G4:G7)</f>
+        <v>18200</v>
+      </c>
+      <c r="H8" s="17"/>
+      <c r="I8" s="17"/>
+      <c r="J8" s="199"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="206"/>
+      <c r="B9" s="207"/>
+      <c r="C9" s="208"/>
+      <c r="D9" s="198"/>
+      <c r="E9" s="17"/>
+      <c r="F9" s="17"/>
+      <c r="G9" s="17"/>
+      <c r="H9" s="17"/>
+      <c r="I9" s="17"/>
+      <c r="J9" s="199"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="206"/>
+      <c r="B10" s="207"/>
+      <c r="C10" s="208"/>
+      <c r="D10" s="198"/>
+      <c r="E10" s="17"/>
+      <c r="F10" s="17"/>
+      <c r="G10" s="17"/>
+      <c r="H10" s="17"/>
+      <c r="I10" s="17"/>
+      <c r="J10" s="199"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="206"/>
+      <c r="B11" s="207"/>
+      <c r="C11" s="208"/>
+      <c r="D11" s="198"/>
+      <c r="E11" s="17"/>
+      <c r="F11" s="17"/>
+      <c r="G11" s="17"/>
+      <c r="H11" s="17"/>
+      <c r="I11" s="17"/>
+      <c r="J11" s="199"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="206"/>
+      <c r="B12" s="207"/>
+      <c r="C12" s="208"/>
+      <c r="D12" s="198"/>
+      <c r="E12" s="17"/>
+      <c r="F12" s="17"/>
+      <c r="G12" s="17"/>
+      <c r="H12" s="17"/>
+      <c r="I12" s="17"/>
+      <c r="J12" s="199"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="206"/>
+      <c r="B13" s="207"/>
+      <c r="C13" s="208"/>
+      <c r="D13" s="198"/>
+      <c r="E13" s="17"/>
+      <c r="F13" s="17"/>
+      <c r="G13" s="17"/>
+      <c r="H13" s="17"/>
+      <c r="I13" s="17"/>
+      <c r="J13" s="199"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="206"/>
+      <c r="B14" s="207"/>
+      <c r="C14" s="208"/>
+      <c r="D14" s="198"/>
+      <c r="E14" s="17"/>
+      <c r="F14" s="17"/>
+      <c r="G14" s="17"/>
+      <c r="H14" s="17"/>
+      <c r="I14" s="17"/>
+      <c r="J14" s="199"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="206"/>
+      <c r="B15" s="207"/>
+      <c r="C15" s="208"/>
+      <c r="D15" s="198"/>
+      <c r="E15" s="17"/>
+      <c r="F15" s="17"/>
+      <c r="G15" s="17"/>
+      <c r="H15" s="17"/>
+      <c r="I15" s="17"/>
+      <c r="J15" s="199"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="209"/>
+      <c r="B16" s="210"/>
+      <c r="C16" s="211"/>
+      <c r="D16" s="200"/>
+      <c r="E16" s="201"/>
+      <c r="F16" s="201"/>
+      <c r="G16" s="201"/>
+      <c r="H16" s="201"/>
+      <c r="I16" s="201"/>
+      <c r="J16" s="202"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A1:C16"/>
+    <mergeCell ref="D2:F2"/>
+    <mergeCell ref="D8:F8"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAB53D77-E889-4E1C-BE59-B510214F2C54}">
   <dimension ref="A1:AE22"/>
   <sheetViews>
@@ -5167,76 +5854,76 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A1" s="106" t="s">
+      <c r="A1" s="111" t="s">
         <v>170</v>
       </c>
-      <c r="B1" s="107"/>
-      <c r="C1" s="107"/>
-      <c r="D1" s="107"/>
-      <c r="E1" s="107"/>
-      <c r="F1" s="107"/>
-      <c r="G1" s="107"/>
-      <c r="H1" s="107"/>
-      <c r="I1" s="107"/>
-      <c r="J1" s="107"/>
-      <c r="K1" s="107"/>
-      <c r="L1" s="107"/>
-      <c r="M1" s="107"/>
-      <c r="N1" s="107"/>
-      <c r="O1" s="107"/>
-      <c r="P1" s="107"/>
-      <c r="Q1" s="107"/>
-      <c r="R1" s="107"/>
-      <c r="S1" s="107"/>
-      <c r="T1" s="107"/>
-      <c r="U1" s="107"/>
-      <c r="V1" s="107"/>
-      <c r="W1" s="107"/>
-      <c r="X1" s="107"/>
-      <c r="Y1" s="107"/>
-      <c r="Z1" s="107"/>
-      <c r="AA1" s="107"/>
-      <c r="AB1" s="107"/>
-      <c r="AC1" s="107"/>
-      <c r="AD1" s="107"/>
-      <c r="AE1" s="108"/>
+      <c r="B1" s="112"/>
+      <c r="C1" s="112"/>
+      <c r="D1" s="112"/>
+      <c r="E1" s="112"/>
+      <c r="F1" s="112"/>
+      <c r="G1" s="112"/>
+      <c r="H1" s="112"/>
+      <c r="I1" s="112"/>
+      <c r="J1" s="112"/>
+      <c r="K1" s="112"/>
+      <c r="L1" s="112"/>
+      <c r="M1" s="112"/>
+      <c r="N1" s="112"/>
+      <c r="O1" s="112"/>
+      <c r="P1" s="112"/>
+      <c r="Q1" s="112"/>
+      <c r="R1" s="112"/>
+      <c r="S1" s="112"/>
+      <c r="T1" s="112"/>
+      <c r="U1" s="112"/>
+      <c r="V1" s="112"/>
+      <c r="W1" s="112"/>
+      <c r="X1" s="112"/>
+      <c r="Y1" s="112"/>
+      <c r="Z1" s="112"/>
+      <c r="AA1" s="112"/>
+      <c r="AB1" s="112"/>
+      <c r="AC1" s="112"/>
+      <c r="AD1" s="112"/>
+      <c r="AE1" s="113"/>
     </row>
     <row r="2" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="109" t="s">
+      <c r="A2" s="114" t="s">
         <v>171</v>
       </c>
-      <c r="B2" s="110"/>
-      <c r="C2" s="110"/>
-      <c r="D2" s="110"/>
-      <c r="E2" s="110"/>
-      <c r="F2" s="110"/>
-      <c r="G2" s="110"/>
-      <c r="H2" s="110"/>
-      <c r="I2" s="110"/>
-      <c r="J2" s="110"/>
-      <c r="K2" s="110"/>
-      <c r="L2" s="110"/>
-      <c r="M2" s="110"/>
-      <c r="N2" s="110"/>
-      <c r="O2" s="110"/>
-      <c r="P2" s="110"/>
-      <c r="Q2" s="110"/>
-      <c r="R2" s="110"/>
-      <c r="S2" s="110"/>
-      <c r="T2" s="111">
+      <c r="B2" s="115"/>
+      <c r="C2" s="115"/>
+      <c r="D2" s="115"/>
+      <c r="E2" s="115"/>
+      <c r="F2" s="115"/>
+      <c r="G2" s="115"/>
+      <c r="H2" s="115"/>
+      <c r="I2" s="115"/>
+      <c r="J2" s="115"/>
+      <c r="K2" s="115"/>
+      <c r="L2" s="115"/>
+      <c r="M2" s="115"/>
+      <c r="N2" s="115"/>
+      <c r="O2" s="115"/>
+      <c r="P2" s="115"/>
+      <c r="Q2" s="115"/>
+      <c r="R2" s="115"/>
+      <c r="S2" s="115"/>
+      <c r="T2" s="116">
         <v>24</v>
       </c>
-      <c r="U2" s="111"/>
-      <c r="V2" s="111"/>
-      <c r="W2" s="111"/>
-      <c r="X2" s="111"/>
-      <c r="Y2" s="111"/>
-      <c r="Z2" s="111"/>
-      <c r="AA2" s="111"/>
-      <c r="AB2" s="111"/>
-      <c r="AC2" s="111"/>
-      <c r="AD2" s="111"/>
-      <c r="AE2" s="112"/>
+      <c r="U2" s="116"/>
+      <c r="V2" s="116"/>
+      <c r="W2" s="116"/>
+      <c r="X2" s="116"/>
+      <c r="Y2" s="116"/>
+      <c r="Z2" s="116"/>
+      <c r="AA2" s="116"/>
+      <c r="AB2" s="116"/>
+      <c r="AC2" s="116"/>
+      <c r="AD2" s="116"/>
+      <c r="AE2" s="117"/>
     </row>
     <row r="3" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A3" s="57" t="s">
@@ -6071,7 +6758,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AC9086E-D004-4EA1-8724-804CD1EEFB7F}">
   <dimension ref="A1:X15"/>
   <sheetViews>
@@ -6164,234 +6851,234 @@
       </c>
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A2" s="118" t="s">
+      <c r="A2" s="120" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="118"/>
-      <c r="C2" s="118"/>
-      <c r="D2" s="118"/>
-      <c r="E2" s="118"/>
-      <c r="F2" s="118"/>
-      <c r="G2" s="118"/>
-      <c r="H2" s="118"/>
-      <c r="I2" s="118"/>
-      <c r="J2" s="118"/>
-      <c r="K2" s="118"/>
-      <c r="L2" s="118"/>
-      <c r="M2" s="114" t="s">
+      <c r="B2" s="120"/>
+      <c r="C2" s="120"/>
+      <c r="D2" s="120"/>
+      <c r="E2" s="120"/>
+      <c r="F2" s="120"/>
+      <c r="G2" s="120"/>
+      <c r="H2" s="120"/>
+      <c r="I2" s="120"/>
+      <c r="J2" s="120"/>
+      <c r="K2" s="120"/>
+      <c r="L2" s="120"/>
+      <c r="M2" s="124" t="s">
         <v>23</v>
       </c>
-      <c r="N2" s="114"/>
-      <c r="O2" s="114"/>
-      <c r="P2" s="114"/>
-      <c r="Q2" s="114"/>
-      <c r="R2" s="114"/>
-      <c r="S2" s="114"/>
-      <c r="T2" s="114"/>
-      <c r="U2" s="114"/>
-      <c r="V2" s="114"/>
-      <c r="W2" s="114"/>
-      <c r="X2" s="114"/>
+      <c r="N2" s="124"/>
+      <c r="O2" s="124"/>
+      <c r="P2" s="124"/>
+      <c r="Q2" s="124"/>
+      <c r="R2" s="124"/>
+      <c r="S2" s="124"/>
+      <c r="T2" s="124"/>
+      <c r="U2" s="124"/>
+      <c r="V2" s="124"/>
+      <c r="W2" s="124"/>
+      <c r="X2" s="124"/>
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3" s="15">
         <v>1</v>
       </c>
-      <c r="B3" s="119" t="s">
+      <c r="B3" s="121" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="119"/>
-      <c r="D3" s="119"/>
+      <c r="C3" s="121"/>
+      <c r="D3" s="121"/>
       <c r="E3" s="16"/>
       <c r="F3" s="16"/>
       <c r="G3" s="16"/>
       <c r="H3" s="16"/>
       <c r="I3" s="16"/>
       <c r="J3" s="16"/>
-      <c r="K3" s="120">
+      <c r="K3" s="122">
         <v>45</v>
       </c>
-      <c r="L3" s="120"/>
+      <c r="L3" s="122"/>
       <c r="M3" s="14">
         <v>1</v>
       </c>
-      <c r="N3" s="115" t="s">
+      <c r="N3" s="125" t="s">
         <v>24</v>
       </c>
-      <c r="O3" s="115"/>
-      <c r="P3" s="115"/>
-      <c r="Q3" s="115"/>
-      <c r="R3" s="115"/>
+      <c r="O3" s="125"/>
+      <c r="P3" s="125"/>
+      <c r="Q3" s="125"/>
+      <c r="R3" s="125"/>
       <c r="S3" s="14">
         <v>6</v>
       </c>
-      <c r="T3" s="113" t="s">
+      <c r="T3" s="123" t="s">
         <v>29</v>
       </c>
-      <c r="U3" s="113"/>
-      <c r="V3" s="113"/>
-      <c r="W3" s="113"/>
-      <c r="X3" s="113"/>
+      <c r="U3" s="123"/>
+      <c r="V3" s="123"/>
+      <c r="W3" s="123"/>
+      <c r="X3" s="123"/>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" s="15">
         <v>2</v>
       </c>
-      <c r="B4" s="119" t="s">
+      <c r="B4" s="121" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="119"/>
-      <c r="D4" s="119"/>
+      <c r="C4" s="121"/>
+      <c r="D4" s="121"/>
       <c r="E4" s="15"/>
       <c r="F4" s="15"/>
       <c r="G4" s="15"/>
       <c r="H4" s="15"/>
       <c r="I4" s="15"/>
       <c r="J4" s="15"/>
-      <c r="K4" s="120">
+      <c r="K4" s="122">
         <v>46</v>
       </c>
-      <c r="L4" s="120"/>
+      <c r="L4" s="122"/>
       <c r="M4" s="14">
         <v>2</v>
       </c>
-      <c r="N4" s="115" t="s">
+      <c r="N4" s="125" t="s">
         <v>25</v>
       </c>
-      <c r="O4" s="115"/>
-      <c r="P4" s="115"/>
-      <c r="Q4" s="115"/>
-      <c r="R4" s="115"/>
+      <c r="O4" s="125"/>
+      <c r="P4" s="125"/>
+      <c r="Q4" s="125"/>
+      <c r="R4" s="125"/>
       <c r="S4" s="14">
         <v>7</v>
       </c>
-      <c r="T4" s="113" t="s">
+      <c r="T4" s="123" t="s">
         <v>29</v>
       </c>
-      <c r="U4" s="113"/>
-      <c r="V4" s="113"/>
-      <c r="W4" s="113"/>
-      <c r="X4" s="113"/>
+      <c r="U4" s="123"/>
+      <c r="V4" s="123"/>
+      <c r="W4" s="123"/>
+      <c r="X4" s="123"/>
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5" s="15">
         <v>3</v>
       </c>
-      <c r="B5" s="116" t="s">
+      <c r="B5" s="118" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="116"/>
-      <c r="D5" s="116"/>
+      <c r="C5" s="118"/>
+      <c r="D5" s="118"/>
       <c r="E5" s="15"/>
       <c r="F5" s="15"/>
       <c r="G5" s="15"/>
       <c r="H5" s="15"/>
       <c r="I5" s="15"/>
       <c r="J5" s="15"/>
-      <c r="K5" s="117">
+      <c r="K5" s="119">
         <v>47</v>
       </c>
-      <c r="L5" s="117"/>
+      <c r="L5" s="119"/>
       <c r="M5" s="14">
         <v>3</v>
       </c>
-      <c r="N5" s="115" t="s">
+      <c r="N5" s="125" t="s">
         <v>26</v>
       </c>
-      <c r="O5" s="115"/>
-      <c r="P5" s="115"/>
-      <c r="Q5" s="115"/>
-      <c r="R5" s="115"/>
+      <c r="O5" s="125"/>
+      <c r="P5" s="125"/>
+      <c r="Q5" s="125"/>
+      <c r="R5" s="125"/>
       <c r="S5" s="14">
         <v>8</v>
       </c>
-      <c r="T5" s="113" t="s">
+      <c r="T5" s="123" t="s">
         <v>29</v>
       </c>
-      <c r="U5" s="113"/>
-      <c r="V5" s="113"/>
-      <c r="W5" s="113"/>
-      <c r="X5" s="113"/>
+      <c r="U5" s="123"/>
+      <c r="V5" s="123"/>
+      <c r="W5" s="123"/>
+      <c r="X5" s="123"/>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6" s="15">
         <v>4</v>
       </c>
-      <c r="B6" s="116" t="s">
+      <c r="B6" s="118" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="116"/>
-      <c r="D6" s="116"/>
+      <c r="C6" s="118"/>
+      <c r="D6" s="118"/>
       <c r="E6" s="15"/>
       <c r="F6" s="15"/>
       <c r="G6" s="15"/>
       <c r="H6" s="15"/>
       <c r="I6" s="15"/>
       <c r="J6" s="15"/>
-      <c r="K6" s="117">
+      <c r="K6" s="119">
         <v>48</v>
       </c>
-      <c r="L6" s="117"/>
+      <c r="L6" s="119"/>
       <c r="M6" s="14">
         <v>4</v>
       </c>
-      <c r="N6" s="115" t="s">
+      <c r="N6" s="125" t="s">
         <v>27</v>
       </c>
-      <c r="O6" s="115"/>
-      <c r="P6" s="115"/>
-      <c r="Q6" s="115"/>
-      <c r="R6" s="115"/>
+      <c r="O6" s="125"/>
+      <c r="P6" s="125"/>
+      <c r="Q6" s="125"/>
+      <c r="R6" s="125"/>
       <c r="S6" s="14">
         <v>9</v>
       </c>
-      <c r="T6" s="113" t="s">
+      <c r="T6" s="123" t="s">
         <v>29</v>
       </c>
-      <c r="U6" s="113"/>
-      <c r="V6" s="113"/>
-      <c r="W6" s="113"/>
-      <c r="X6" s="113"/>
+      <c r="U6" s="123"/>
+      <c r="V6" s="123"/>
+      <c r="W6" s="123"/>
+      <c r="X6" s="123"/>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7" s="15">
         <v>5</v>
       </c>
-      <c r="B7" s="116" t="s">
+      <c r="B7" s="118" t="s">
         <v>22</v>
       </c>
-      <c r="C7" s="116"/>
-      <c r="D7" s="116"/>
+      <c r="C7" s="118"/>
+      <c r="D7" s="118"/>
       <c r="E7" s="15"/>
       <c r="F7" s="15"/>
       <c r="G7" s="15"/>
       <c r="H7" s="15"/>
       <c r="I7" s="15"/>
       <c r="J7" s="15"/>
-      <c r="K7" s="117">
+      <c r="K7" s="119">
         <v>49</v>
       </c>
-      <c r="L7" s="117"/>
+      <c r="L7" s="119"/>
       <c r="M7" s="14">
         <v>5</v>
       </c>
-      <c r="N7" s="115" t="s">
+      <c r="N7" s="125" t="s">
         <v>28</v>
       </c>
-      <c r="O7" s="115"/>
-      <c r="P7" s="115"/>
-      <c r="Q7" s="115"/>
-      <c r="R7" s="115"/>
+      <c r="O7" s="125"/>
+      <c r="P7" s="125"/>
+      <c r="Q7" s="125"/>
+      <c r="R7" s="125"/>
       <c r="S7" s="14">
         <v>10</v>
       </c>
-      <c r="T7" s="113" t="s">
+      <c r="T7" s="123" t="s">
         <v>29</v>
       </c>
-      <c r="U7" s="113"/>
-      <c r="V7" s="113"/>
-      <c r="W7" s="113"/>
-      <c r="X7" s="113"/>
+      <c r="U7" s="123"/>
+      <c r="V7" s="123"/>
+      <c r="W7" s="123"/>
+      <c r="X7" s="123"/>
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A8" s="13"/>
@@ -6603,6 +7290,17 @@
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="T7:X7"/>
+    <mergeCell ref="M2:X2"/>
+    <mergeCell ref="N3:R3"/>
+    <mergeCell ref="N4:R4"/>
+    <mergeCell ref="N5:R5"/>
+    <mergeCell ref="N6:R6"/>
+    <mergeCell ref="N7:R7"/>
+    <mergeCell ref="T3:X3"/>
+    <mergeCell ref="T4:X4"/>
+    <mergeCell ref="T5:X5"/>
+    <mergeCell ref="T6:X6"/>
     <mergeCell ref="B6:D6"/>
     <mergeCell ref="K6:L6"/>
     <mergeCell ref="B7:D7"/>
@@ -6614,24 +7312,13 @@
     <mergeCell ref="K4:L4"/>
     <mergeCell ref="B5:D5"/>
     <mergeCell ref="K5:L5"/>
-    <mergeCell ref="T7:X7"/>
-    <mergeCell ref="M2:X2"/>
-    <mergeCell ref="N3:R3"/>
-    <mergeCell ref="N4:R4"/>
-    <mergeCell ref="N5:R5"/>
-    <mergeCell ref="N6:R6"/>
-    <mergeCell ref="N7:R7"/>
-    <mergeCell ref="T3:X3"/>
-    <mergeCell ref="T4:X4"/>
-    <mergeCell ref="T5:X5"/>
-    <mergeCell ref="T6:X6"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{889D0D57-1F26-473E-B306-F0F5D3A5E8AC}">
   <dimension ref="A1:I2"/>
   <sheetViews>
@@ -6698,7 +7385,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B9CA3B1-EDA9-4D32-B2CA-E8D9C6600DDC}">
   <dimension ref="A1:J31"/>
   <sheetViews>
@@ -6753,7 +7440,7 @@
       </c>
     </row>
     <row r="2" spans="1:10" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="121" t="s">
+      <c r="A2" s="126" t="s">
         <v>34</v>
       </c>
       <c r="B2" s="37" t="s">
@@ -6773,7 +7460,7 @@
       <c r="J2" s="37"/>
     </row>
     <row r="3" spans="1:10" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="121"/>
+      <c r="A3" s="126"/>
       <c r="B3" s="38" t="s">
         <v>19</v>
       </c>
@@ -6793,7 +7480,7 @@
       <c r="J3" s="38"/>
     </row>
     <row r="4" spans="1:10" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="121"/>
+      <c r="A4" s="126"/>
       <c r="B4" s="37" t="s">
         <v>20</v>
       </c>
@@ -6813,7 +7500,7 @@
       <c r="J4" s="37"/>
     </row>
     <row r="5" spans="1:10" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="121"/>
+      <c r="A5" s="126"/>
       <c r="B5" s="38" t="s">
         <v>21</v>
       </c>
@@ -6831,7 +7518,7 @@
       <c r="J5" s="38"/>
     </row>
     <row r="6" spans="1:10" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="121"/>
+      <c r="A6" s="126"/>
       <c r="B6" s="37" t="s">
         <v>22</v>
       </c>
@@ -6849,7 +7536,7 @@
       <c r="J6" s="37"/>
     </row>
     <row r="7" spans="1:10" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="121" t="s">
+      <c r="A7" s="126" t="s">
         <v>107</v>
       </c>
       <c r="B7" s="37" t="s">
@@ -6869,7 +7556,7 @@
       <c r="J7" s="37"/>
     </row>
     <row r="8" spans="1:10" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="121"/>
+      <c r="A8" s="126"/>
       <c r="B8" s="38" t="s">
         <v>19</v>
       </c>
@@ -6889,7 +7576,7 @@
       <c r="J8" s="38"/>
     </row>
     <row r="9" spans="1:10" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="121"/>
+      <c r="A9" s="126"/>
       <c r="B9" s="37" t="s">
         <v>20</v>
       </c>
@@ -6909,7 +7596,7 @@
       <c r="J9" s="37"/>
     </row>
     <row r="10" spans="1:10" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="121"/>
+      <c r="A10" s="126"/>
       <c r="B10" s="38" t="s">
         <v>21</v>
       </c>
@@ -6927,7 +7614,7 @@
       <c r="J10" s="38"/>
     </row>
     <row r="11" spans="1:10" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="121"/>
+      <c r="A11" s="126"/>
       <c r="B11" s="37" t="s">
         <v>22</v>
       </c>
@@ -6945,7 +7632,7 @@
       <c r="J11" s="37"/>
     </row>
     <row r="12" spans="1:10" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="121" t="s">
+      <c r="A12" s="126" t="s">
         <v>108</v>
       </c>
       <c r="B12" s="37" t="s">
@@ -6965,7 +7652,7 @@
       <c r="J12" s="37"/>
     </row>
     <row r="13" spans="1:10" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="121"/>
+      <c r="A13" s="126"/>
       <c r="B13" s="38" t="s">
         <v>19</v>
       </c>
@@ -6985,7 +7672,7 @@
       <c r="J13" s="38"/>
     </row>
     <row r="14" spans="1:10" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="121"/>
+      <c r="A14" s="126"/>
       <c r="B14" s="37" t="s">
         <v>20</v>
       </c>
@@ -7005,7 +7692,7 @@
       <c r="J14" s="37"/>
     </row>
     <row r="15" spans="1:10" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="121"/>
+      <c r="A15" s="126"/>
       <c r="B15" s="38" t="s">
         <v>21</v>
       </c>
@@ -7023,7 +7710,7 @@
       <c r="J15" s="38"/>
     </row>
     <row r="16" spans="1:10" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="121"/>
+      <c r="A16" s="126"/>
       <c r="B16" s="37" t="s">
         <v>22</v>
       </c>
@@ -7041,7 +7728,7 @@
       <c r="J16" s="37"/>
     </row>
     <row r="17" spans="1:10" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="121" t="s">
+      <c r="A17" s="126" t="s">
         <v>109</v>
       </c>
       <c r="B17" s="37" t="s">
@@ -7061,7 +7748,7 @@
       <c r="J17" s="37"/>
     </row>
     <row r="18" spans="1:10" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="121"/>
+      <c r="A18" s="126"/>
       <c r="B18" s="38" t="s">
         <v>19</v>
       </c>
@@ -7081,7 +7768,7 @@
       <c r="J18" s="38"/>
     </row>
     <row r="19" spans="1:10" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="121"/>
+      <c r="A19" s="126"/>
       <c r="B19" s="37" t="s">
         <v>20</v>
       </c>
@@ -7101,7 +7788,7 @@
       <c r="J19" s="37"/>
     </row>
     <row r="20" spans="1:10" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="121"/>
+      <c r="A20" s="126"/>
       <c r="B20" s="38" t="s">
         <v>21</v>
       </c>
@@ -7119,7 +7806,7 @@
       <c r="J20" s="38"/>
     </row>
     <row r="21" spans="1:10" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="121"/>
+      <c r="A21" s="126"/>
       <c r="B21" s="37" t="s">
         <v>22</v>
       </c>
@@ -7137,7 +7824,7 @@
       <c r="J21" s="37"/>
     </row>
     <row r="22" spans="1:10" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="121" t="s">
+      <c r="A22" s="126" t="s">
         <v>110</v>
       </c>
       <c r="B22" s="37" t="s">
@@ -7157,7 +7844,7 @@
       <c r="J22" s="37"/>
     </row>
     <row r="23" spans="1:10" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="121"/>
+      <c r="A23" s="126"/>
       <c r="B23" s="38" t="s">
         <v>19</v>
       </c>
@@ -7177,7 +7864,7 @@
       <c r="J23" s="38"/>
     </row>
     <row r="24" spans="1:10" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="121"/>
+      <c r="A24" s="126"/>
       <c r="B24" s="37" t="s">
         <v>20</v>
       </c>
@@ -7197,7 +7884,7 @@
       <c r="J24" s="37"/>
     </row>
     <row r="25" spans="1:10" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="121"/>
+      <c r="A25" s="126"/>
       <c r="B25" s="38" t="s">
         <v>21</v>
       </c>
@@ -7215,7 +7902,7 @@
       <c r="J25" s="38"/>
     </row>
     <row r="26" spans="1:10" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="121"/>
+      <c r="A26" s="126"/>
       <c r="B26" s="37" t="s">
         <v>22</v>
       </c>
@@ -7233,7 +7920,7 @@
       <c r="J26" s="37"/>
     </row>
     <row r="27" spans="1:10" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="121" t="s">
+      <c r="A27" s="126" t="s">
         <v>111</v>
       </c>
       <c r="B27" s="37" t="s">
@@ -7253,7 +7940,7 @@
       <c r="J27" s="37"/>
     </row>
     <row r="28" spans="1:10" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="121"/>
+      <c r="A28" s="126"/>
       <c r="B28" s="38" t="s">
         <v>19</v>
       </c>
@@ -7273,7 +7960,7 @@
       <c r="J28" s="38"/>
     </row>
     <row r="29" spans="1:10" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="121"/>
+      <c r="A29" s="126"/>
       <c r="B29" s="37" t="s">
         <v>20</v>
       </c>
@@ -7293,7 +7980,7 @@
       <c r="J29" s="37"/>
     </row>
     <row r="30" spans="1:10" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="121"/>
+      <c r="A30" s="126"/>
       <c r="B30" s="38" t="s">
         <v>21</v>
       </c>
@@ -7311,7 +7998,7 @@
       <c r="J30" s="38"/>
     </row>
     <row r="31" spans="1:10" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="121"/>
+      <c r="A31" s="126"/>
       <c r="B31" s="37" t="s">
         <v>22</v>
       </c>
@@ -7343,7 +8030,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68C7AB11-C29A-4F36-8877-185A21672CFE}">
   <dimension ref="A1:F20"/>
   <sheetViews>
@@ -7362,24 +8049,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="124" t="s">
+      <c r="A1" s="129" t="s">
         <v>40</v>
       </c>
-      <c r="B1" s="125"/>
-      <c r="C1" s="125"/>
-      <c r="D1" s="125"/>
-      <c r="E1" s="125"/>
-      <c r="F1" s="125"/>
+      <c r="B1" s="130"/>
+      <c r="C1" s="130"/>
+      <c r="D1" s="130"/>
+      <c r="E1" s="130"/>
+      <c r="F1" s="130"/>
     </row>
     <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="126" t="s">
+      <c r="A2" s="131" t="s">
         <v>41</v>
       </c>
-      <c r="B2" s="126"/>
-      <c r="C2" s="126"/>
-      <c r="D2" s="126"/>
-      <c r="E2" s="126"/>
-      <c r="F2" s="126"/>
+      <c r="B2" s="131"/>
+      <c r="C2" s="131"/>
+      <c r="D2" s="131"/>
+      <c r="E2" s="131"/>
+      <c r="F2" s="131"/>
     </row>
     <row r="3" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
@@ -7608,18 +8295,18 @@
       <c r="F15" s="29"/>
     </row>
     <row r="16" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="127" t="s">
+      <c r="A16" s="132" t="s">
         <v>60</v>
       </c>
-      <c r="B16" s="128"/>
-      <c r="C16" s="128"/>
-      <c r="D16" s="128"/>
-      <c r="E16" s="128"/>
-      <c r="F16" s="129"/>
+      <c r="B16" s="133"/>
+      <c r="C16" s="133"/>
+      <c r="D16" s="133"/>
+      <c r="E16" s="133"/>
+      <c r="F16" s="134"/>
     </row>
     <row r="17" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="122"/>
-      <c r="B17" s="123"/>
+      <c r="A17" s="127"/>
+      <c r="B17" s="128"/>
       <c r="C17" s="32" t="s">
         <v>73</v>
       </c>
@@ -7634,10 +8321,10 @@
       </c>
     </row>
     <row r="18" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="122" t="s">
+      <c r="A18" s="127" t="s">
         <v>15</v>
       </c>
-      <c r="B18" s="123"/>
+      <c r="B18" s="128"/>
       <c r="C18" s="32">
         <v>25</v>
       </c>
@@ -7682,7 +8369,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE752E1A-3511-482B-9D5B-C641C60E9654}">
   <dimension ref="A1:G18"/>
   <sheetViews>
@@ -7701,35 +8388,35 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="124" t="s">
+      <c r="A1" s="129" t="s">
         <v>40</v>
       </c>
-      <c r="B1" s="125"/>
-      <c r="C1" s="125"/>
-      <c r="D1" s="125"/>
-      <c r="E1" s="125"/>
-      <c r="F1" s="125"/>
-      <c r="G1" s="125"/>
+      <c r="B1" s="130"/>
+      <c r="C1" s="130"/>
+      <c r="D1" s="130"/>
+      <c r="E1" s="130"/>
+      <c r="F1" s="130"/>
+      <c r="G1" s="130"/>
     </row>
     <row r="2" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="126" t="s">
+      <c r="A2" s="131" t="s">
         <v>41</v>
       </c>
-      <c r="B2" s="126"/>
-      <c r="C2" s="126"/>
-      <c r="D2" s="126"/>
-      <c r="E2" s="126"/>
-      <c r="F2" s="126"/>
-      <c r="G2" s="126"/>
+      <c r="B2" s="131"/>
+      <c r="C2" s="131"/>
+      <c r="D2" s="131"/>
+      <c r="E2" s="131"/>
+      <c r="F2" s="131"/>
+      <c r="G2" s="131"/>
     </row>
     <row r="3" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="130" t="s">
+      <c r="A3" s="135" t="s">
         <v>74</v>
       </c>
-      <c r="B3" s="130"/>
-      <c r="C3" s="130"/>
-      <c r="D3" s="130"/>
-      <c r="E3" s="130"/>
+      <c r="B3" s="135"/>
+      <c r="C3" s="135"/>
+      <c r="D3" s="135"/>
+      <c r="E3" s="135"/>
       <c r="F3" s="21" t="s">
         <v>52</v>
       </c>
@@ -7982,19 +8669,19 @@
       <c r="G15" s="29"/>
     </row>
     <row r="16" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="127" t="s">
+      <c r="A16" s="132" t="s">
         <v>60</v>
       </c>
-      <c r="B16" s="128"/>
-      <c r="C16" s="128"/>
-      <c r="D16" s="128"/>
-      <c r="E16" s="128"/>
-      <c r="F16" s="128"/>
-      <c r="G16" s="129"/>
+      <c r="B16" s="133"/>
+      <c r="C16" s="133"/>
+      <c r="D16" s="133"/>
+      <c r="E16" s="133"/>
+      <c r="F16" s="133"/>
+      <c r="G16" s="134"/>
     </row>
     <row r="17" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="122"/>
-      <c r="B17" s="123"/>
+      <c r="A17" s="127"/>
+      <c r="B17" s="128"/>
       <c r="C17" s="32"/>
       <c r="D17" s="32" t="s">
         <v>76</v>
@@ -8010,10 +8697,10 @@
       </c>
     </row>
     <row r="18" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="122" t="s">
+      <c r="A18" s="127" t="s">
         <v>15</v>
       </c>
-      <c r="B18" s="123"/>
+      <c r="B18" s="128"/>
       <c r="C18" s="32"/>
       <c r="D18" s="32">
         <v>13</v>
@@ -8040,278 +8727,4 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C002464B-D256-4EB5-A012-8EB2C2D144F6}">
-  <dimension ref="A1:J20"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="R23" sqref="R23"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="106" t="s">
-        <v>258</v>
-      </c>
-      <c r="B1" s="107"/>
-      <c r="C1" s="107"/>
-      <c r="D1" s="131"/>
-      <c r="E1" s="132"/>
-      <c r="F1" s="132"/>
-      <c r="G1" s="132"/>
-      <c r="H1" s="132"/>
-      <c r="I1" s="132"/>
-      <c r="J1" s="133"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="90"/>
-      <c r="B2" s="17"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="17"/>
-      <c r="G2" s="17"/>
-      <c r="H2" s="17"/>
-      <c r="I2" s="17"/>
-      <c r="J2" s="91"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="134" t="s">
-        <v>145</v>
-      </c>
-      <c r="B3" s="135"/>
-      <c r="C3" s="135" t="s">
-        <v>147</v>
-      </c>
-      <c r="D3" s="135"/>
-      <c r="E3" s="135" t="s">
-        <v>146</v>
-      </c>
-      <c r="F3" s="135"/>
-      <c r="G3" s="135" t="s">
-        <v>198</v>
-      </c>
-      <c r="H3" s="135"/>
-      <c r="I3" s="17"/>
-      <c r="J3" s="91"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="90"/>
-      <c r="B4" s="17"/>
-      <c r="C4" s="17"/>
-      <c r="D4" s="17"/>
-      <c r="E4" s="17"/>
-      <c r="F4" s="17"/>
-      <c r="G4" s="17"/>
-      <c r="H4" s="17"/>
-      <c r="I4" s="17"/>
-      <c r="J4" s="91"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="90"/>
-      <c r="B5" s="17"/>
-      <c r="C5" s="17"/>
-      <c r="D5" s="17"/>
-      <c r="E5" s="17"/>
-      <c r="F5" s="17"/>
-      <c r="G5" s="17"/>
-      <c r="H5" s="17"/>
-      <c r="I5" s="17"/>
-      <c r="J5" s="91"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="90"/>
-      <c r="B6" s="17"/>
-      <c r="C6" s="17"/>
-      <c r="D6" s="17"/>
-      <c r="E6" s="17"/>
-      <c r="F6" s="17"/>
-      <c r="G6" s="17"/>
-      <c r="H6" s="17"/>
-      <c r="I6" s="17"/>
-      <c r="J6" s="91"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="90"/>
-      <c r="B7" s="17"/>
-      <c r="C7" s="17"/>
-      <c r="D7" s="17"/>
-      <c r="E7" s="17"/>
-      <c r="F7" s="17"/>
-      <c r="G7" s="17"/>
-      <c r="H7" s="17"/>
-      <c r="I7" s="17"/>
-      <c r="J7" s="91"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="90"/>
-      <c r="B8" s="17"/>
-      <c r="C8" s="17"/>
-      <c r="D8" s="17"/>
-      <c r="E8" s="17"/>
-      <c r="F8" s="17"/>
-      <c r="G8" s="17"/>
-      <c r="H8" s="17"/>
-      <c r="I8" s="17"/>
-      <c r="J8" s="91"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="90"/>
-      <c r="B9" s="17"/>
-      <c r="C9" s="17"/>
-      <c r="D9" s="17"/>
-      <c r="E9" s="17"/>
-      <c r="F9" s="17"/>
-      <c r="G9" s="17"/>
-      <c r="H9" s="17"/>
-      <c r="I9" s="17"/>
-      <c r="J9" s="91"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="90"/>
-      <c r="B10" s="17"/>
-      <c r="C10" s="17"/>
-      <c r="D10" s="17"/>
-      <c r="E10" s="17"/>
-      <c r="F10" s="17"/>
-      <c r="G10" s="17"/>
-      <c r="H10" s="17"/>
-      <c r="I10" s="17"/>
-      <c r="J10" s="91"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="90"/>
-      <c r="B11" s="17"/>
-      <c r="C11" s="17"/>
-      <c r="D11" s="17"/>
-      <c r="E11" s="17"/>
-      <c r="F11" s="17"/>
-      <c r="G11" s="17"/>
-      <c r="H11" s="17"/>
-      <c r="I11" s="17"/>
-      <c r="J11" s="91"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="90"/>
-      <c r="B12" s="17"/>
-      <c r="C12" s="17"/>
-      <c r="D12" s="17"/>
-      <c r="E12" s="17"/>
-      <c r="F12" s="17"/>
-      <c r="G12" s="17"/>
-      <c r="H12" s="17"/>
-      <c r="I12" s="17"/>
-      <c r="J12" s="91"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="90"/>
-      <c r="B13" s="17"/>
-      <c r="C13" s="17"/>
-      <c r="D13" s="17"/>
-      <c r="E13" s="17"/>
-      <c r="F13" s="17"/>
-      <c r="G13" s="17"/>
-      <c r="H13" s="17"/>
-      <c r="I13" s="17"/>
-      <c r="J13" s="91"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="90"/>
-      <c r="B14" s="17"/>
-      <c r="C14" s="17"/>
-      <c r="D14" s="17"/>
-      <c r="E14" s="17"/>
-      <c r="F14" s="17"/>
-      <c r="G14" s="17"/>
-      <c r="H14" s="17"/>
-      <c r="I14" s="17"/>
-      <c r="J14" s="91"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="90"/>
-      <c r="B15" s="17"/>
-      <c r="C15" s="17"/>
-      <c r="D15" s="17"/>
-      <c r="E15" s="17"/>
-      <c r="F15" s="17"/>
-      <c r="G15" s="17"/>
-      <c r="H15" s="17"/>
-      <c r="I15" s="17"/>
-      <c r="J15" s="91"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="90"/>
-      <c r="B16" s="17"/>
-      <c r="C16" s="17"/>
-      <c r="D16" s="17"/>
-      <c r="E16" s="17"/>
-      <c r="F16" s="17"/>
-      <c r="G16" s="17"/>
-      <c r="H16" s="17"/>
-      <c r="I16" s="17"/>
-      <c r="J16" s="91"/>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="90"/>
-      <c r="B17" s="17"/>
-      <c r="C17" s="17"/>
-      <c r="D17" s="17"/>
-      <c r="E17" s="17"/>
-      <c r="F17" s="17"/>
-      <c r="G17" s="17"/>
-      <c r="H17" s="17"/>
-      <c r="I17" s="17"/>
-      <c r="J17" s="91"/>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="90"/>
-      <c r="B18" s="17"/>
-      <c r="C18" s="17"/>
-      <c r="D18" s="17"/>
-      <c r="E18" s="17"/>
-      <c r="F18" s="17"/>
-      <c r="G18" s="17"/>
-      <c r="H18" s="17"/>
-      <c r="I18" s="17"/>
-      <c r="J18" s="91"/>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="90"/>
-      <c r="B19" s="17"/>
-      <c r="C19" s="17"/>
-      <c r="D19" s="17"/>
-      <c r="E19" s="17"/>
-      <c r="F19" s="17"/>
-      <c r="G19" s="17"/>
-      <c r="H19" s="17"/>
-      <c r="I19" s="17"/>
-      <c r="J19" s="91"/>
-    </row>
-    <row r="20" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="92"/>
-      <c r="B20" s="93"/>
-      <c r="C20" s="93"/>
-      <c r="D20" s="93"/>
-      <c r="E20" s="93"/>
-      <c r="F20" s="93"/>
-      <c r="G20" s="93"/>
-      <c r="H20" s="93"/>
-      <c r="I20" s="93"/>
-      <c r="J20" s="94"/>
-    </row>
-  </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="D1:J1"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="G3:H3"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>